<commit_message>
v1: resize image to fit window
</commit_message>
<xml_diff>
--- a/paint_todo.xlsx
+++ b/paint_todo.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="52">
   <si>
     <t>Id</t>
   </si>
@@ -242,6 +242,9 @@
 - minimum is 3 swatches, max is maybe 12
 - save setting and reuse on next progam open
 (maybe instead of drag-n-drop the border, there are little &lt; &gt; arrow buttons that will expand/contract space one swatch at a time)</t>
+  </si>
+  <si>
+    <t>resize image to fit window as it resizes</t>
   </si>
 </sst>
 </file>
@@ -749,7 +752,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -777,10 +780,10 @@
     </row>
     <row r="2">
       <c r="A2" s="0">
-        <v>2</v>
+        <v>30</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>14</v>
+        <v>51</v>
       </c>
       <c r="C2" s="0" t="s">
         <v>5</v>
@@ -797,10 +800,10 @@
     </row>
     <row r="3">
       <c r="A3" s="0">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C3" s="0" t="s">
         <v>5</v>
@@ -812,6 +815,26 @@
         <v>13</v>
       </c>
       <c r="F3" s="0" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="0">
+        <v>1</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="E4" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="F4" s="0" t="s">
         <v>13</v>
       </c>
     </row>
@@ -855,7 +878,7 @@
         <v>9</v>
       </c>
       <c r="F2" s="0">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="3">

</xml_diff>

<commit_message>
v1: zoom in and out; fit to window
</commit_message>
<xml_diff>
--- a/paint_todo.xlsx
+++ b/paint_todo.xlsx
@@ -296,7 +296,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:F26"/>
+  <dimension ref="A1:F25"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -339,10 +339,10 @@
     </row>
     <row r="3">
       <c r="A3" s="0">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C3" s="0" t="s">
         <v>8</v>
@@ -356,10 +356,10 @@
     </row>
     <row r="4">
       <c r="A4" s="0">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>16</v>
+        <v>33</v>
       </c>
       <c r="C4" s="0" t="s">
         <v>8</v>
@@ -373,10 +373,10 @@
     </row>
     <row r="5">
       <c r="A5" s="0">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>33</v>
+        <v>18</v>
       </c>
       <c r="C5" s="0" t="s">
         <v>8</v>
@@ -390,10 +390,10 @@
     </row>
     <row r="6">
       <c r="A6" s="0">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C6" s="0" t="s">
         <v>8</v>
@@ -407,10 +407,10 @@
     </row>
     <row r="7">
       <c r="A7" s="0">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C7" s="0" t="s">
         <v>8</v>
@@ -424,10 +424,10 @@
     </row>
     <row r="8">
       <c r="A8" s="0">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C8" s="0" t="s">
         <v>8</v>
@@ -441,10 +441,10 @@
     </row>
     <row r="9">
       <c r="A9" s="0">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>21</v>
+        <v>28</v>
       </c>
       <c r="C9" s="0" t="s">
         <v>8</v>
@@ -458,10 +458,10 @@
     </row>
     <row r="10">
       <c r="A10" s="0">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="C10" s="0" t="s">
         <v>8</v>
@@ -475,10 +475,10 @@
     </row>
     <row r="11">
       <c r="A11" s="0">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C11" s="0" t="s">
         <v>8</v>
@@ -492,10 +492,10 @@
     </row>
     <row r="12">
       <c r="A12" s="0">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>24</v>
+        <v>31</v>
       </c>
       <c r="C12" s="0" t="s">
         <v>8</v>
@@ -509,10 +509,10 @@
     </row>
     <row r="13">
       <c r="A13" s="0">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>31</v>
+        <v>50</v>
       </c>
       <c r="C13" s="0" t="s">
         <v>8</v>
@@ -526,10 +526,10 @@
     </row>
     <row r="14">
       <c r="A14" s="0">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="C14" s="0" t="s">
         <v>8</v>
@@ -543,10 +543,10 @@
     </row>
     <row r="15">
       <c r="A15" s="0">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="C15" s="0" t="s">
         <v>8</v>
@@ -560,10 +560,10 @@
     </row>
     <row r="16">
       <c r="A16" s="0">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="C16" s="0" t="s">
         <v>8</v>
@@ -577,10 +577,10 @@
     </row>
     <row r="17">
       <c r="A17" s="0">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C17" s="0" t="s">
         <v>8</v>
@@ -594,10 +594,10 @@
     </row>
     <row r="18">
       <c r="A18" s="0">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>48</v>
+        <v>37</v>
       </c>
       <c r="C18" s="0" t="s">
         <v>8</v>
@@ -611,10 +611,10 @@
     </row>
     <row r="19">
       <c r="A19" s="0">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="C19" s="0" t="s">
         <v>8</v>
@@ -628,10 +628,10 @@
     </row>
     <row r="20">
       <c r="A20" s="0">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="C20" s="0" t="s">
         <v>8</v>
@@ -645,10 +645,10 @@
     </row>
     <row r="21">
       <c r="A21" s="0">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C21" s="0" t="s">
         <v>8</v>
@@ -662,10 +662,10 @@
     </row>
     <row r="22">
       <c r="A22" s="0">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C22" s="0" t="s">
         <v>8</v>
@@ -679,10 +679,10 @@
     </row>
     <row r="23">
       <c r="A23" s="0">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>36</v>
+        <v>45</v>
       </c>
       <c r="C23" s="0" t="s">
         <v>8</v>
@@ -696,10 +696,10 @@
     </row>
     <row r="24">
       <c r="A24" s="0">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C24" s="0" t="s">
         <v>8</v>
@@ -713,10 +713,10 @@
     </row>
     <row r="25">
       <c r="A25" s="0">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="C25" s="0" t="s">
         <v>8</v>
@@ -725,23 +725,6 @@
         <v>9</v>
       </c>
       <c r="E25" s="0" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="26">
-      <c r="A26" s="0">
-        <v>29</v>
-      </c>
-      <c r="B26" s="0" t="s">
-        <v>49</v>
-      </c>
-      <c r="C26" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="D26" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="E26" s="0" t="s">
         <v>13</v>
       </c>
     </row>
@@ -752,7 +735,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -780,10 +763,10 @@
     </row>
     <row r="2">
       <c r="A2" s="0">
-        <v>30</v>
+        <v>3</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>51</v>
+        <v>15</v>
       </c>
       <c r="C2" s="0" t="s">
         <v>5</v>
@@ -800,10 +783,10 @@
     </row>
     <row r="3">
       <c r="A3" s="0">
-        <v>2</v>
+        <v>30</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>14</v>
+        <v>51</v>
       </c>
       <c r="C3" s="0" t="s">
         <v>5</v>
@@ -820,10 +803,10 @@
     </row>
     <row r="4">
       <c r="A4" s="0">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C4" s="0" t="s">
         <v>5</v>
@@ -835,6 +818,26 @@
         <v>13</v>
       </c>
       <c r="F4" s="0" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="0">
+        <v>1</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="D5" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="E5" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="F5" s="0" t="s">
         <v>13</v>
       </c>
     </row>

</xml_diff>

<commit_message>
v1: scroll vertical and horizontal, maintain centering during zoom
</commit_message>
<xml_diff>
--- a/paint_todo.xlsx
+++ b/paint_todo.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="53">
   <si>
     <t>Id</t>
   </si>
@@ -245,6 +245,9 @@
   </si>
   <si>
     <t>resize image to fit window as it resizes</t>
+  </si>
+  <si>
+    <t>8/10/2018</t>
   </si>
 </sst>
 </file>
@@ -296,7 +299,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:F25"/>
+  <dimension ref="A1:F24"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -339,10 +342,10 @@
     </row>
     <row r="3">
       <c r="A3" s="0">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>16</v>
+        <v>33</v>
       </c>
       <c r="C3" s="0" t="s">
         <v>8</v>
@@ -356,10 +359,10 @@
     </row>
     <row r="4">
       <c r="A4" s="0">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>33</v>
+        <v>18</v>
       </c>
       <c r="C4" s="0" t="s">
         <v>8</v>
@@ -373,10 +376,10 @@
     </row>
     <row r="5">
       <c r="A5" s="0">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C5" s="0" t="s">
         <v>8</v>
@@ -390,10 +393,10 @@
     </row>
     <row r="6">
       <c r="A6" s="0">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C6" s="0" t="s">
         <v>8</v>
@@ -407,10 +410,10 @@
     </row>
     <row r="7">
       <c r="A7" s="0">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C7" s="0" t="s">
         <v>8</v>
@@ -424,10 +427,10 @@
     </row>
     <row r="8">
       <c r="A8" s="0">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>21</v>
+        <v>28</v>
       </c>
       <c r="C8" s="0" t="s">
         <v>8</v>
@@ -441,10 +444,10 @@
     </row>
     <row r="9">
       <c r="A9" s="0">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="C9" s="0" t="s">
         <v>8</v>
@@ -458,10 +461,10 @@
     </row>
     <row r="10">
       <c r="A10" s="0">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C10" s="0" t="s">
         <v>8</v>
@@ -475,10 +478,10 @@
     </row>
     <row r="11">
       <c r="A11" s="0">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>24</v>
+        <v>31</v>
       </c>
       <c r="C11" s="0" t="s">
         <v>8</v>
@@ -492,10 +495,10 @@
     </row>
     <row r="12">
       <c r="A12" s="0">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>31</v>
+        <v>50</v>
       </c>
       <c r="C12" s="0" t="s">
         <v>8</v>
@@ -509,10 +512,10 @@
     </row>
     <row r="13">
       <c r="A13" s="0">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="C13" s="0" t="s">
         <v>8</v>
@@ -526,10 +529,10 @@
     </row>
     <row r="14">
       <c r="A14" s="0">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="C14" s="0" t="s">
         <v>8</v>
@@ -543,10 +546,10 @@
     </row>
     <row r="15">
       <c r="A15" s="0">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="C15" s="0" t="s">
         <v>8</v>
@@ -560,10 +563,10 @@
     </row>
     <row r="16">
       <c r="A16" s="0">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C16" s="0" t="s">
         <v>8</v>
@@ -577,10 +580,10 @@
     </row>
     <row r="17">
       <c r="A17" s="0">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>48</v>
+        <v>37</v>
       </c>
       <c r="C17" s="0" t="s">
         <v>8</v>
@@ -594,10 +597,10 @@
     </row>
     <row r="18">
       <c r="A18" s="0">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="C18" s="0" t="s">
         <v>8</v>
@@ -611,10 +614,10 @@
     </row>
     <row r="19">
       <c r="A19" s="0">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="C19" s="0" t="s">
         <v>8</v>
@@ -628,10 +631,10 @@
     </row>
     <row r="20">
       <c r="A20" s="0">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C20" s="0" t="s">
         <v>8</v>
@@ -645,10 +648,10 @@
     </row>
     <row r="21">
       <c r="A21" s="0">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C21" s="0" t="s">
         <v>8</v>
@@ -662,10 +665,10 @@
     </row>
     <row r="22">
       <c r="A22" s="0">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>36</v>
+        <v>45</v>
       </c>
       <c r="C22" s="0" t="s">
         <v>8</v>
@@ -679,10 +682,10 @@
     </row>
     <row r="23">
       <c r="A23" s="0">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C23" s="0" t="s">
         <v>8</v>
@@ -696,10 +699,10 @@
     </row>
     <row r="24">
       <c r="A24" s="0">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="C24" s="0" t="s">
         <v>8</v>
@@ -708,23 +711,6 @@
         <v>9</v>
       </c>
       <c r="E24" s="0" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="25">
-      <c r="A25" s="0">
-        <v>29</v>
-      </c>
-      <c r="B25" s="0" t="s">
-        <v>49</v>
-      </c>
-      <c r="C25" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="D25" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="E25" s="0" t="s">
         <v>13</v>
       </c>
     </row>
@@ -735,7 +721,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -763,10 +749,10 @@
     </row>
     <row r="2">
       <c r="A2" s="0">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C2" s="0" t="s">
         <v>5</v>
@@ -778,15 +764,15 @@
         <v>13</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>13</v>
+        <v>52</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="0">
-        <v>30</v>
+        <v>3</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>51</v>
+        <v>15</v>
       </c>
       <c r="C3" s="0" t="s">
         <v>5</v>
@@ -803,10 +789,10 @@
     </row>
     <row r="4">
       <c r="A4" s="0">
-        <v>2</v>
+        <v>30</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>14</v>
+        <v>51</v>
       </c>
       <c r="C4" s="0" t="s">
         <v>5</v>
@@ -823,10 +809,10 @@
     </row>
     <row r="5">
       <c r="A5" s="0">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C5" s="0" t="s">
         <v>5</v>
@@ -838,6 +824,26 @@
         <v>13</v>
       </c>
       <c r="F5" s="0" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="0">
+        <v>1</v>
+      </c>
+      <c r="B6" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="D6" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="E6" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="F6" s="0" t="s">
         <v>13</v>
       </c>
     </row>

</xml_diff>

<commit_message>
v1: change palette display width
</commit_message>
<xml_diff>
--- a/paint_todo.xlsx
+++ b/paint_todo.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="42">
   <si>
     <t>Id</t>
   </si>
@@ -31,13 +31,9 @@
     <t>Created</t>
   </si>
   <si>
-    <t>Done</t>
-  </si>
-  <si>
-    <t>Active</t>
-  </si>
-  <si>
-    <t>Max Id</t>
+    <t xml:space="preserve">what do these lines do?
+Application.EnableVisualStyles();
+Application.SetCompatibleTextRenderingDefault(false);</t>
   </si>
   <si>
     <t>Todo</t>
@@ -46,46 +42,22 @@
     <t>Task</t>
   </si>
   <si>
-    <t>Inactive</t>
-  </si>
-  <si>
-    <t>Bug</t>
-  </si>
-  <si>
-    <t xml:space="preserve">new window's console app
-- version 0 until minimum viable is complete</t>
-  </si>
-  <si>
     <t>8/9/2018</t>
   </si>
   <si>
-    <t>open an image and display it in a window at default size</t>
-  </si>
-  <si>
-    <t>zoom in and out of image</t>
-  </si>
-  <si>
-    <t>scroll horizontal and vertical when zoomed in</t>
-  </si>
-  <si>
-    <t>click on a pixel in the image, and change its color to red</t>
-  </si>
-  <si>
-    <t xml:space="preserve">when image is opened, auto-detect all black bordered regions
-and color each one a different shade of red</t>
+    <t>when image is opened, auto-detect all black bordered regions</t>
   </si>
   <si>
     <t>if a region contains no white, should i set the lightest pixel to white and reference for the pure color?</t>
-  </si>
-  <si>
-    <t>build 1 to 3 default palettes</t>
   </si>
   <si>
     <t xml:space="preserve">display a default palette along the side of the window
 - give it a vertical scroll when needed</t>
   </si>
   <si>
-    <t>select a palette color and apply to a region of the image</t>
+    <t xml:space="preserve">select a palette color and apply to a region of the image
+- fill mode
+- undo, redo</t>
   </si>
   <si>
     <t xml:space="preserve">save changes to image
@@ -95,52 +67,6 @@
   </si>
   <si>
     <t>make sure auto-detect of regions works even when image is already colored in</t>
-  </si>
-  <si>
-    <t xml:space="preserve">open edit palette mode
-- add swatches
-- remove swatches
-- change color of swatch
-- reorder swatches
-- save changes before leaving pane</t>
-  </si>
-  <si>
-    <t xml:space="preserve">open edit palette mode
-- add swatches
-- remove swatches
-- change color of swatch
-- reorder swatches
-- save changes before leaving pane
-(no duplicate colors allowed)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">click on a pixel in the image, and change its color to red
-- pixel mode</t>
-  </si>
-  <si>
-    <t xml:space="preserve">select a palette color and apply to a region of the image
-- fill mode
-- undo, redo</t>
-  </si>
-  <si>
-    <t xml:space="preserve">open edit palette mode
-- add swatches
-- remove swatches
-- change color of swatch
-- reorder swatches
-- undo, redo until pane is closed
-- save changes before leaving pane
-(no duplicate colors allowed)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">open edit palette mode
-- add swatches
-- remove swatches
-- change color of swatch
-- reorder swatches
-- undo, redo until pane is closed
-- save changes before leaving pane (save as text file)
-(no duplicate colors allowed)</t>
   </si>
   <si>
     <t xml:space="preserve">open edit palette mode
@@ -154,89 +80,6 @@
 (no duplicate colors allowed)</t>
   </si>
   <si>
-    <t xml:space="preserve">open edit palette mode
-- add swatches
-- remove swatches
-- change color of swatch
-- reorder swatches
-- undo, redo until pane is closed
-- save changes before leaving pane 
-(save as text file - or, what do other programs use?)
-(no duplicate colors allowed)
-- set how many swatches wide you want it displayed</t>
-  </si>
-  <si>
-    <t xml:space="preserve">click on a pixel in the image, and change its color to red
-- temp just to test locator</t>
-  </si>
-  <si>
-    <t xml:space="preserve">that should be it for minimum viable
-save as Version 1</t>
-  </si>
-  <si>
-    <t>build installer for Version 1 and save it in a separate folder to keep</t>
-  </si>
-  <si>
-    <t>update website with project, landing page, and links</t>
-  </si>
-  <si>
-    <t xml:space="preserve">design an icon
-apply to windows, desktop icon, and uninstall icon</t>
-  </si>
-  <si>
-    <t xml:space="preserve">program preference setting: how wide the palette area is
-- let user drag and drop divider to change palette width
-- minimum is 3 swatches, max is maybe 12</t>
-  </si>
-  <si>
-    <t xml:space="preserve">program preference setting: how wide the palette area is
-- let user drag and drop divider to change palette width
-- minimum is 3 swatches, max is maybe 12
-- save setting and reuse on next progam open</t>
-  </si>
-  <si>
-    <t xml:space="preserve">when resizing windows, default behavior is to keep the same section of image in the viewing pane
-- so expanding window would in effect zoom in</t>
-  </si>
-  <si>
-    <t>check through the program Properties &gt;&gt; Assembly Info again, make sure all is accurate</t>
-  </si>
-  <si>
-    <t xml:space="preserve">what do these lines do?
-Application.EnableVisualStyles();
-Application.SetCompatibleTextRenderingDefault(false);</t>
-  </si>
-  <si>
-    <t xml:space="preserve">remember windows size from last closing
-- full screen vs not
-- default not-full-screen size</t>
-  </si>
-  <si>
-    <t xml:space="preserve">remember windows size from last closing
-- full screen vs not
-- default not-full-screen size
-open with this size</t>
-  </si>
-  <si>
-    <t>EVERYTHING BELOW HERE IS VERSION 2</t>
-  </si>
-  <si>
-    <t>remember last used directory (save or open) and default to there in file dialogs</t>
-  </si>
-  <si>
-    <t xml:space="preserve">include support contact information
--wohaste email
--paint landing page on website
--github page</t>
-  </si>
-  <si>
-    <t xml:space="preserve">include donation information
--patreon</t>
-  </si>
-  <si>
-    <t>how to programs auto-update?</t>
-  </si>
-  <si>
     <t xml:space="preserve">program preference setting: how wide the palette area is
 - let user drag and drop divider to change palette width
 - minimum is 3 swatches, max is maybe 12
@@ -244,10 +87,91 @@
 (maybe instead of drag-n-drop the border, there are little &lt; &gt; arrow buttons that will expand/contract space one swatch at a time)</t>
   </si>
   <si>
+    <t xml:space="preserve">when resizing windows, default behavior is to keep the same section of image in the viewing pane
+- so expanding window would in effect zoom in</t>
+  </si>
+  <si>
+    <t xml:space="preserve">remember windows size from last closing
+- full screen vs not
+- default not-full-screen size
+open with this size</t>
+  </si>
+  <si>
+    <t xml:space="preserve">include support contact information
+-wohaste email
+-paint landing page on website
+-github page</t>
+  </si>
+  <si>
+    <t xml:space="preserve">include donation information
+-patreon</t>
+  </si>
+  <si>
+    <t xml:space="preserve">design an icon
+apply to windows, desktop icon, and uninstall icon</t>
+  </si>
+  <si>
+    <t>check through the program Properties &gt;&gt; Assembly Info again, make sure all is accurate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">that should be it for minimum viable
+save as Version 1</t>
+  </si>
+  <si>
+    <t>build installer for Version 1 and save it in a separate folder to keep</t>
+  </si>
+  <si>
+    <t>update website with project, landing page, and links</t>
+  </si>
+  <si>
+    <t>EVERYTHING BELOW HERE IS VERSION 2</t>
+  </si>
+  <si>
+    <t>remember last used directory (save or open) and default to there in file dialogs</t>
+  </si>
+  <si>
+    <t>how to programs auto-update?</t>
+  </si>
+  <si>
+    <t>Done</t>
+  </si>
+  <si>
+    <t xml:space="preserve">build 1 to 3 default palettes
+- downloaded some Photoshop palettes</t>
+  </si>
+  <si>
+    <t>8/11/2018</t>
+  </si>
+  <si>
+    <t>scroll horizontal and vertical when zoomed in</t>
+  </si>
+  <si>
+    <t>8/10/2018</t>
+  </si>
+  <si>
+    <t>zoom in and out of image</t>
+  </si>
+  <si>
     <t>resize image to fit window as it resizes</t>
   </si>
   <si>
-    <t>8/10/2018</t>
+    <t>open an image and display it in a window at default size</t>
+  </si>
+  <si>
+    <t xml:space="preserve">new window's console app
+- version 0 until minimum viable is complete</t>
+  </si>
+  <si>
+    <t>Active</t>
+  </si>
+  <si>
+    <t>Max Id</t>
+  </si>
+  <si>
+    <t>Inactive</t>
+  </si>
+  <si>
+    <t>Bug</t>
   </si>
 </sst>
 </file>
@@ -286,8 +210,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" applyNumberFormat="1" fontId="0" applyFont="1" xfId="0"/>
+    <xf numFmtId="0" applyNumberFormat="1" fontId="1" applyFont="1" xfId="0"/>
     <xf numFmtId="0" applyNumberFormat="1" fontId="1" applyFont="1" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
@@ -299,7 +224,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:F24"/>
+  <dimension ref="A1:F21"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -328,33 +253,33 @@
         <v>23</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>42</v>
+        <v>5</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="0">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>33</v>
+        <v>16</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4">
@@ -362,16 +287,16 @@
         <v>6</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>18</v>
+        <v>9</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
     </row>
     <row r="5">
@@ -379,339 +304,288 @@
         <v>7</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="0">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="0">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="0">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>28</v>
+        <v>14</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="0">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="E9" s="0" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="0">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="E10" s="0" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="0">
-        <v>13</v>
+        <v>24</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>31</v>
+        <v>18</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="E11" s="0" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="0">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>50</v>
+        <v>19</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="E12" s="0" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="0">
-        <v>21</v>
+        <v>28</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>40</v>
+        <v>20</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D13" s="0" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="E13" s="0" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="0">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>44</v>
+        <v>21</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D14" s="0" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="E14" s="0" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="0">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>47</v>
+        <v>22</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D15" s="0" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="E15" s="0" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="0">
-        <v>28</v>
+        <v>16</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>48</v>
+        <v>23</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D16" s="0" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="E16" s="0" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="0">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>37</v>
+        <v>24</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D17" s="0" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="E17" s="0" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="0">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>41</v>
+        <v>25</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D18" s="0" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="E18" s="0" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="0">
-        <v>16</v>
+        <v>25</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D19" s="0" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="E19" s="0" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="0">
-        <v>17</v>
+        <v>26</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
       <c r="C20" s="0" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D20" s="0" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="E20" s="0" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="0">
-        <v>18</v>
+        <v>29</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="C21" s="0" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D21" s="0" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="E21" s="0" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" s="0">
-        <v>25</v>
-      </c>
-      <c r="B22" s="0" t="s">
-        <v>45</v>
-      </c>
-      <c r="C22" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="D22" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="E22" s="0" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" s="0">
-        <v>26</v>
-      </c>
-      <c r="B23" s="0" t="s">
-        <v>46</v>
-      </c>
-      <c r="C23" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="D23" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="E23" s="0" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" s="0">
-        <v>29</v>
-      </c>
-      <c r="B24" s="0" t="s">
-        <v>49</v>
-      </c>
-      <c r="C24" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="D24" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="E24" s="0" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
     </row>
   </sheetData>
@@ -721,7 +595,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -744,107 +618,147 @@
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>5</v>
+        <v>29</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="0">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>5</v>
+        <v>29</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>52</v>
+        <v>31</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="0">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>15</v>
+        <v>30</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>5</v>
+        <v>29</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="F3" s="0" t="s">
-        <v>13</v>
+        <v>31</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="0">
-        <v>30</v>
+        <v>4</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>51</v>
+        <v>32</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>5</v>
+        <v>29</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="F4" s="0" t="s">
-        <v>13</v>
+        <v>33</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="0">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>14</v>
+        <v>34</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>5</v>
+        <v>29</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="F5" s="0" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="0">
+        <v>30</v>
+      </c>
+      <c r="B6" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="C6" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="D6" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E6" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="F6" s="0" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="0">
+        <v>2</v>
+      </c>
+      <c r="B7" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="C7" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="D7" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E7" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="F7" s="0" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="0">
         <v>1</v>
       </c>
-      <c r="B6" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="C6" s="0" t="s">
-        <v>5</v>
-      </c>
-      <c r="D6" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="E6" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="F6" s="0" t="s">
-        <v>13</v>
+      <c r="B8" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="C8" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="D8" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E8" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="F8" s="0" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>
@@ -861,30 +775,30 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1" t="s">
+      <c r="B1" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1" t="s">
-        <v>7</v>
+      <c r="E1" s="2"/>
+      <c r="F1" s="2" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="0" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>6</v>
+        <v>38</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="F2" s="0">
         <v>30</v>
@@ -892,13 +806,13 @@
     </row>
     <row r="3">
       <c r="A3" s="0" t="s">
-        <v>5</v>
+        <v>29</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>10</v>
+        <v>40</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>11</v>
+        <v>41</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
v1: save user setting for swatches-per-row
</commit_message>
<xml_diff>
--- a/paint_todo.xlsx
+++ b/paint_todo.xlsx
@@ -224,7 +224,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:F21"/>
+  <dimension ref="A1:F20"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -267,10 +267,10 @@
     </row>
     <row r="3">
       <c r="A3" s="0">
-        <v>20</v>
+        <v>6</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="C3" s="0" t="s">
         <v>6</v>
@@ -284,10 +284,10 @@
     </row>
     <row r="4">
       <c r="A4" s="0">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C4" s="0" t="s">
         <v>6</v>
@@ -301,10 +301,10 @@
     </row>
     <row r="5">
       <c r="A5" s="0">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C5" s="0" t="s">
         <v>6</v>
@@ -318,10 +318,10 @@
     </row>
     <row r="6">
       <c r="A6" s="0">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C6" s="0" t="s">
         <v>6</v>
@@ -335,10 +335,10 @@
     </row>
     <row r="7">
       <c r="A7" s="0">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C7" s="0" t="s">
         <v>6</v>
@@ -352,10 +352,10 @@
     </row>
     <row r="8">
       <c r="A8" s="0">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C8" s="0" t="s">
         <v>6</v>
@@ -369,10 +369,10 @@
     </row>
     <row r="9">
       <c r="A9" s="0">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="C9" s="0" t="s">
         <v>6</v>
@@ -386,10 +386,10 @@
     </row>
     <row r="10">
       <c r="A10" s="0">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C10" s="0" t="s">
         <v>6</v>
@@ -403,10 +403,10 @@
     </row>
     <row r="11">
       <c r="A11" s="0">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C11" s="0" t="s">
         <v>6</v>
@@ -420,10 +420,10 @@
     </row>
     <row r="12">
       <c r="A12" s="0">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C12" s="0" t="s">
         <v>6</v>
@@ -437,10 +437,10 @@
     </row>
     <row r="13">
       <c r="A13" s="0">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C13" s="0" t="s">
         <v>6</v>
@@ -454,10 +454,10 @@
     </row>
     <row r="14">
       <c r="A14" s="0">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C14" s="0" t="s">
         <v>6</v>
@@ -471,10 +471,10 @@
     </row>
     <row r="15">
       <c r="A15" s="0">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C15" s="0" t="s">
         <v>6</v>
@@ -488,10 +488,10 @@
     </row>
     <row r="16">
       <c r="A16" s="0">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C16" s="0" t="s">
         <v>6</v>
@@ -505,10 +505,10 @@
     </row>
     <row r="17">
       <c r="A17" s="0">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C17" s="0" t="s">
         <v>6</v>
@@ -522,10 +522,10 @@
     </row>
     <row r="18">
       <c r="A18" s="0">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C18" s="0" t="s">
         <v>6</v>
@@ -539,10 +539,10 @@
     </row>
     <row r="19">
       <c r="A19" s="0">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C19" s="0" t="s">
         <v>6</v>
@@ -556,10 +556,10 @@
     </row>
     <row r="20">
       <c r="A20" s="0">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C20" s="0" t="s">
         <v>6</v>
@@ -568,23 +568,6 @@
         <v>7</v>
       </c>
       <c r="E20" s="0" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" s="0">
-        <v>29</v>
-      </c>
-      <c r="B21" s="0" t="s">
-        <v>28</v>
-      </c>
-      <c r="C21" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="D21" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="E21" s="0" t="s">
         <v>8</v>
       </c>
     </row>
@@ -595,7 +578,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:F8"/>
+  <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -623,10 +606,10 @@
     </row>
     <row r="2">
       <c r="A2" s="0">
-        <v>9</v>
+        <v>20</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="C2" s="0" t="s">
         <v>29</v>
@@ -643,10 +626,10 @@
     </row>
     <row r="3">
       <c r="A3" s="0">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>30</v>
+        <v>11</v>
       </c>
       <c r="C3" s="0" t="s">
         <v>29</v>
@@ -663,10 +646,10 @@
     </row>
     <row r="4">
       <c r="A4" s="0">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C4" s="0" t="s">
         <v>29</v>
@@ -678,15 +661,15 @@
         <v>8</v>
       </c>
       <c r="F4" s="0" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="0">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C5" s="0" t="s">
         <v>29</v>
@@ -698,15 +681,15 @@
         <v>8</v>
       </c>
       <c r="F5" s="0" t="s">
-        <v>8</v>
+        <v>33</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="0">
-        <v>30</v>
+        <v>3</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C6" s="0" t="s">
         <v>29</v>
@@ -723,10 +706,10 @@
     </row>
     <row r="7">
       <c r="A7" s="0">
-        <v>2</v>
+        <v>30</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C7" s="0" t="s">
         <v>29</v>
@@ -743,21 +726,41 @@
     </row>
     <row r="8">
       <c r="A8" s="0">
+        <v>2</v>
+      </c>
+      <c r="B8" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="C8" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="D8" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E8" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="F8" s="0" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="0">
         <v>1</v>
       </c>
-      <c r="B8" s="0" t="s">
+      <c r="B9" s="0" t="s">
         <v>37</v>
       </c>
-      <c r="C8" s="0" t="s">
-        <v>29</v>
-      </c>
-      <c r="D8" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="E8" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="F8" s="0" t="s">
+      <c r="C9" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="D9" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E9" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="F9" s="0" t="s">
         <v>8</v>
       </c>
     </row>

</xml_diff>

<commit_message>
v1: select palette color
</commit_message>
<xml_diff>
--- a/paint_todo.xlsx
+++ b/paint_todo.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="45">
   <si>
     <t>Id</t>
   </si>
@@ -172,6 +172,15 @@
   </si>
   <si>
     <t>Bug</t>
+  </si>
+  <si>
+    <t>select a palette color</t>
+  </si>
+  <si>
+    <t>fill in a section of color on the image</t>
+  </si>
+  <si>
+    <t>undo, redo coloring a section on the image</t>
   </si>
 </sst>
 </file>
@@ -224,7 +233,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:F20"/>
+  <dimension ref="A1:F21"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -301,10 +310,10 @@
     </row>
     <row r="5">
       <c r="A5" s="0">
-        <v>10</v>
+        <v>32</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>12</v>
+        <v>43</v>
       </c>
       <c r="C5" s="0" t="s">
         <v>6</v>
@@ -313,15 +322,15 @@
         <v>7</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>8</v>
+        <v>31</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="0">
-        <v>11</v>
+        <v>33</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>13</v>
+        <v>44</v>
       </c>
       <c r="C6" s="0" t="s">
         <v>6</v>
@@ -330,15 +339,15 @@
         <v>7</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>8</v>
+        <v>31</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="0">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C7" s="0" t="s">
         <v>6</v>
@@ -352,10 +361,10 @@
     </row>
     <row r="8">
       <c r="A8" s="0">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C8" s="0" t="s">
         <v>6</v>
@@ -369,10 +378,10 @@
     </row>
     <row r="9">
       <c r="A9" s="0">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C9" s="0" t="s">
         <v>6</v>
@@ -386,10 +395,10 @@
     </row>
     <row r="10">
       <c r="A10" s="0">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C10" s="0" t="s">
         <v>6</v>
@@ -403,10 +412,10 @@
     </row>
     <row r="11">
       <c r="A11" s="0">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C11" s="0" t="s">
         <v>6</v>
@@ -420,10 +429,10 @@
     </row>
     <row r="12">
       <c r="A12" s="0">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C12" s="0" t="s">
         <v>6</v>
@@ -437,10 +446,10 @@
     </row>
     <row r="13">
       <c r="A13" s="0">
-        <v>19</v>
+        <v>28</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C13" s="0" t="s">
         <v>6</v>
@@ -454,10 +463,10 @@
     </row>
     <row r="14">
       <c r="A14" s="0">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C14" s="0" t="s">
         <v>6</v>
@@ -471,10 +480,10 @@
     </row>
     <row r="15">
       <c r="A15" s="0">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C15" s="0" t="s">
         <v>6</v>
@@ -488,10 +497,10 @@
     </row>
     <row r="16">
       <c r="A16" s="0">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C16" s="0" t="s">
         <v>6</v>
@@ -505,10 +514,10 @@
     </row>
     <row r="17">
       <c r="A17" s="0">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C17" s="0" t="s">
         <v>6</v>
@@ -522,10 +531,10 @@
     </row>
     <row r="18">
       <c r="A18" s="0">
+        <v>18</v>
+      </c>
+      <c r="B18" s="0" t="s">
         <v>25</v>
-      </c>
-      <c r="B18" s="0" t="s">
-        <v>26</v>
       </c>
       <c r="C18" s="0" t="s">
         <v>6</v>
@@ -539,10 +548,10 @@
     </row>
     <row r="19">
       <c r="A19" s="0">
+        <v>25</v>
+      </c>
+      <c r="B19" s="0" t="s">
         <v>26</v>
-      </c>
-      <c r="B19" s="0" t="s">
-        <v>27</v>
       </c>
       <c r="C19" s="0" t="s">
         <v>6</v>
@@ -556,18 +565,35 @@
     </row>
     <row r="20">
       <c r="A20" s="0">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B20" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="C20" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D20" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E20" s="0" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="0">
+        <v>29</v>
+      </c>
+      <c r="B21" s="0" t="s">
         <v>28</v>
       </c>
-      <c r="C20" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="D20" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="E20" s="0" t="s">
+      <c r="C21" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D21" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E21" s="0" t="s">
         <v>8</v>
       </c>
     </row>
@@ -578,7 +604,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:F9"/>
+  <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -606,10 +632,10 @@
     </row>
     <row r="2">
       <c r="A2" s="0">
-        <v>20</v>
+        <v>31</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>16</v>
+        <v>42</v>
       </c>
       <c r="C2" s="0" t="s">
         <v>29</v>
@@ -618,7 +644,7 @@
         <v>7</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>8</v>
+        <v>31</v>
       </c>
       <c r="F2" s="0" t="s">
         <v>31</v>
@@ -626,10 +652,10 @@
     </row>
     <row r="3">
       <c r="A3" s="0">
-        <v>9</v>
+        <v>20</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="C3" s="0" t="s">
         <v>29</v>
@@ -646,10 +672,10 @@
     </row>
     <row r="4">
       <c r="A4" s="0">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>30</v>
+        <v>11</v>
       </c>
       <c r="C4" s="0" t="s">
         <v>29</v>
@@ -666,10 +692,10 @@
     </row>
     <row r="5">
       <c r="A5" s="0">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C5" s="0" t="s">
         <v>29</v>
@@ -681,15 +707,15 @@
         <v>8</v>
       </c>
       <c r="F5" s="0" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="0">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C6" s="0" t="s">
         <v>29</v>
@@ -701,15 +727,15 @@
         <v>8</v>
       </c>
       <c r="F6" s="0" t="s">
-        <v>8</v>
+        <v>33</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="0">
-        <v>30</v>
+        <v>3</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C7" s="0" t="s">
         <v>29</v>
@@ -726,10 +752,10 @@
     </row>
     <row r="8">
       <c r="A8" s="0">
-        <v>2</v>
+        <v>30</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C8" s="0" t="s">
         <v>29</v>
@@ -746,21 +772,41 @@
     </row>
     <row r="9">
       <c r="A9" s="0">
+        <v>2</v>
+      </c>
+      <c r="B9" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="C9" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="D9" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E9" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="F9" s="0" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="0">
         <v>1</v>
       </c>
-      <c r="B9" s="0" t="s">
+      <c r="B10" s="0" t="s">
         <v>37</v>
       </c>
-      <c r="C9" s="0" t="s">
-        <v>29</v>
-      </c>
-      <c r="D9" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="E9" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="F9" s="0" t="s">
+      <c r="C10" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="D10" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E10" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="F10" s="0" t="s">
         <v>8</v>
       </c>
     </row>
@@ -804,7 +850,7 @@
         <v>7</v>
       </c>
       <c r="F2" s="0">
-        <v>30</v>
+        <v>33</v>
       </c>
     </row>
     <row r="3">

</xml_diff>

<commit_message>
v1: basic apply color
</commit_message>
<xml_diff>
--- a/paint_todo.xlsx
+++ b/paint_todo.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="46">
   <si>
     <t>Id</t>
   </si>
@@ -181,6 +181,9 @@
   </si>
   <si>
     <t>undo, redo coloring a section on the image</t>
+  </si>
+  <si>
+    <t>when zooming, if a scroll bar is all the way to min or max, keep it there</t>
   </si>
 </sst>
 </file>
@@ -233,7 +236,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:F21"/>
+  <dimension ref="A1:F22"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -395,10 +398,10 @@
     </row>
     <row r="10">
       <c r="A10" s="0">
-        <v>21</v>
+        <v>34</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>17</v>
+        <v>45</v>
       </c>
       <c r="C10" s="0" t="s">
         <v>6</v>
@@ -407,15 +410,15 @@
         <v>7</v>
       </c>
       <c r="E10" s="0" t="s">
-        <v>8</v>
+        <v>31</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="0">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C11" s="0" t="s">
         <v>6</v>
@@ -429,10 +432,10 @@
     </row>
     <row r="12">
       <c r="A12" s="0">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C12" s="0" t="s">
         <v>6</v>
@@ -446,10 +449,10 @@
     </row>
     <row r="13">
       <c r="A13" s="0">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C13" s="0" t="s">
         <v>6</v>
@@ -463,10 +466,10 @@
     </row>
     <row r="14">
       <c r="A14" s="0">
-        <v>19</v>
+        <v>28</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C14" s="0" t="s">
         <v>6</v>
@@ -480,10 +483,10 @@
     </row>
     <row r="15">
       <c r="A15" s="0">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C15" s="0" t="s">
         <v>6</v>
@@ -497,10 +500,10 @@
     </row>
     <row r="16">
       <c r="A16" s="0">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C16" s="0" t="s">
         <v>6</v>
@@ -514,10 +517,10 @@
     </row>
     <row r="17">
       <c r="A17" s="0">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C17" s="0" t="s">
         <v>6</v>
@@ -531,10 +534,10 @@
     </row>
     <row r="18">
       <c r="A18" s="0">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C18" s="0" t="s">
         <v>6</v>
@@ -548,10 +551,10 @@
     </row>
     <row r="19">
       <c r="A19" s="0">
+        <v>18</v>
+      </c>
+      <c r="B19" s="0" t="s">
         <v>25</v>
-      </c>
-      <c r="B19" s="0" t="s">
-        <v>26</v>
       </c>
       <c r="C19" s="0" t="s">
         <v>6</v>
@@ -565,10 +568,10 @@
     </row>
     <row r="20">
       <c r="A20" s="0">
+        <v>25</v>
+      </c>
+      <c r="B20" s="0" t="s">
         <v>26</v>
-      </c>
-      <c r="B20" s="0" t="s">
-        <v>27</v>
       </c>
       <c r="C20" s="0" t="s">
         <v>6</v>
@@ -582,18 +585,35 @@
     </row>
     <row r="21">
       <c r="A21" s="0">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B21" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="C21" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D21" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E21" s="0" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="0">
+        <v>29</v>
+      </c>
+      <c r="B22" s="0" t="s">
         <v>28</v>
       </c>
-      <c r="C21" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="D21" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="E21" s="0" t="s">
+      <c r="C22" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D22" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E22" s="0" t="s">
         <v>8</v>
       </c>
     </row>
@@ -850,7 +870,7 @@
         <v>7</v>
       </c>
       <c r="F2" s="0">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="3">

</xml_diff>

<commit_message>
v1: apply color to region without losing values
</commit_message>
<xml_diff>
--- a/paint_todo.xlsx
+++ b/paint_todo.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="49">
   <si>
     <t>Id</t>
   </si>
@@ -51,13 +51,13 @@
     <t>if a region contains no white, should i set the lightest pixel to white and reference for the pure color?</t>
   </si>
   <si>
-    <t xml:space="preserve">display a default palette along the side of the window
-- give it a vertical scroll when needed</t>
-  </si>
-  <si>
-    <t xml:space="preserve">select a palette color and apply to a region of the image
-- fill mode
-- undo, redo</t>
+    <t>fill in a section of color on the image</t>
+  </si>
+  <si>
+    <t>8/11/2018</t>
+  </si>
+  <si>
+    <t>undo, redo coloring a section on the image</t>
   </si>
   <si>
     <t xml:space="preserve">save changes to image
@@ -67,6 +67,14 @@
   </si>
   <si>
     <t>make sure auto-detect of regions works even when image is already colored in</t>
+  </si>
+  <si>
+    <t xml:space="preserve">set and check tolerance for "black" and "white"
+- "blacks" will be left untouched
+- "whites" will be treated as pure white, which will in effect alter then to white</t>
+  </si>
+  <si>
+    <t>8/12/2018</t>
   </si>
   <si>
     <t xml:space="preserve">open edit palette mode
@@ -80,6 +88,61 @@
 (no duplicate colors allowed)</t>
   </si>
   <si>
+    <t>when zooming, if a scroll bar is all the way to min or max, keep it there</t>
+  </si>
+  <si>
+    <t xml:space="preserve">when resizing windows, default behavior is to keep the same section of image in the viewing pane
+- so expanding window would in effect zoom in</t>
+  </si>
+  <si>
+    <t xml:space="preserve">remember windows size from last closing
+- full screen vs not
+- default not-full-screen size
+open with this size</t>
+  </si>
+  <si>
+    <t xml:space="preserve">include support contact information
+-wohaste email
+-paint landing page on website
+-github page</t>
+  </si>
+  <si>
+    <t xml:space="preserve">include donation information
+-patreon</t>
+  </si>
+  <si>
+    <t xml:space="preserve">design an icon
+apply to windows, desktop icon, and uninstall icon</t>
+  </si>
+  <si>
+    <t>check through the program Properties &gt;&gt; Assembly Info again, make sure all is accurate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">that should be it for minimum viable
+save as Version 1</t>
+  </si>
+  <si>
+    <t>build installer for Version 1 and save it in a separate folder to keep</t>
+  </si>
+  <si>
+    <t>update website with project, landing page, and links</t>
+  </si>
+  <si>
+    <t>EVERYTHING BELOW HERE IS VERSION 2</t>
+  </si>
+  <si>
+    <t>remember last used directory (save or open) and default to there in file dialogs</t>
+  </si>
+  <si>
+    <t>how to programs auto-update?</t>
+  </si>
+  <si>
+    <t>Done</t>
+  </si>
+  <si>
+    <t>select a palette color</t>
+  </si>
+  <si>
     <t xml:space="preserve">program preference setting: how wide the palette area is
 - let user drag and drop divider to change palette width
 - minimum is 3 swatches, max is maybe 12
@@ -87,62 +150,14 @@
 (maybe instead of drag-n-drop the border, there are little &lt; &gt; arrow buttons that will expand/contract space one swatch at a time)</t>
   </si>
   <si>
-    <t xml:space="preserve">when resizing windows, default behavior is to keep the same section of image in the viewing pane
-- so expanding window would in effect zoom in</t>
-  </si>
-  <si>
-    <t xml:space="preserve">remember windows size from last closing
-- full screen vs not
-- default not-full-screen size
-open with this size</t>
-  </si>
-  <si>
-    <t xml:space="preserve">include support contact information
--wohaste email
--paint landing page on website
--github page</t>
-  </si>
-  <si>
-    <t xml:space="preserve">include donation information
--patreon</t>
-  </si>
-  <si>
-    <t xml:space="preserve">design an icon
-apply to windows, desktop icon, and uninstall icon</t>
-  </si>
-  <si>
-    <t>check through the program Properties &gt;&gt; Assembly Info again, make sure all is accurate</t>
-  </si>
-  <si>
-    <t xml:space="preserve">that should be it for minimum viable
-save as Version 1</t>
-  </si>
-  <si>
-    <t>build installer for Version 1 and save it in a separate folder to keep</t>
-  </si>
-  <si>
-    <t>update website with project, landing page, and links</t>
-  </si>
-  <si>
-    <t>EVERYTHING BELOW HERE IS VERSION 2</t>
-  </si>
-  <si>
-    <t>remember last used directory (save or open) and default to there in file dialogs</t>
-  </si>
-  <si>
-    <t>how to programs auto-update?</t>
-  </si>
-  <si>
-    <t>Done</t>
+    <t xml:space="preserve">display a default palette along the side of the window
+- give it a vertical scroll when needed</t>
   </si>
   <si>
     <t xml:space="preserve">build 1 to 3 default palettes
 - downloaded some Photoshop palettes</t>
   </si>
   <si>
-    <t>8/11/2018</t>
-  </si>
-  <si>
     <t>scroll horizontal and vertical when zoomed in</t>
   </si>
   <si>
@@ -174,16 +189,10 @@
     <t>Bug</t>
   </si>
   <si>
-    <t>select a palette color</t>
-  </si>
-  <si>
-    <t>fill in a section of color on the image</t>
-  </si>
-  <si>
-    <t>undo, redo coloring a section on the image</t>
-  </si>
-  <si>
-    <t>when zooming, if a scroll bar is all the way to min or max, keep it there</t>
+    <t>what to rename ColorPalette library to so it does not conflict with object ColorPalette?</t>
+  </si>
+  <si>
+    <t>apply color over color without changing underlying values</t>
   </si>
 </sst>
 </file>
@@ -279,10 +288,10 @@
     </row>
     <row r="3">
       <c r="A3" s="0">
-        <v>6</v>
+        <v>36</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>9</v>
+        <v>47</v>
       </c>
       <c r="C3" s="0" t="s">
         <v>6</v>
@@ -291,15 +300,15 @@
         <v>7</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="0">
-        <v>7</v>
+        <v>33</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="C4" s="0" t="s">
         <v>6</v>
@@ -308,15 +317,15 @@
         <v>7</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="0">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="C5" s="0" t="s">
         <v>6</v>
@@ -325,15 +334,15 @@
         <v>7</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="0">
-        <v>33</v>
+        <v>11</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>44</v>
+        <v>14</v>
       </c>
       <c r="C6" s="0" t="s">
         <v>6</v>
@@ -342,15 +351,15 @@
         <v>7</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>31</v>
+        <v>8</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="0">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C7" s="0" t="s">
         <v>6</v>
@@ -364,10 +373,10 @@
     </row>
     <row r="8">
       <c r="A8" s="0">
-        <v>12</v>
+        <v>35</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C8" s="0" t="s">
         <v>6</v>
@@ -376,7 +385,7 @@
         <v>7</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
     </row>
     <row r="9">
@@ -384,7 +393,7 @@
         <v>13</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="C9" s="0" t="s">
         <v>6</v>
@@ -401,7 +410,7 @@
         <v>34</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>45</v>
+        <v>19</v>
       </c>
       <c r="C10" s="0" t="s">
         <v>6</v>
@@ -410,7 +419,7 @@
         <v>7</v>
       </c>
       <c r="E10" s="0" t="s">
-        <v>31</v>
+        <v>12</v>
       </c>
     </row>
     <row r="11">
@@ -418,7 +427,7 @@
         <v>21</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="C11" s="0" t="s">
         <v>6</v>
@@ -435,7 +444,7 @@
         <v>24</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="C12" s="0" t="s">
         <v>6</v>
@@ -452,7 +461,7 @@
         <v>27</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="C13" s="0" t="s">
         <v>6</v>
@@ -469,7 +478,7 @@
         <v>28</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="C14" s="0" t="s">
         <v>6</v>
@@ -486,7 +495,7 @@
         <v>19</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="C15" s="0" t="s">
         <v>6</v>
@@ -503,7 +512,7 @@
         <v>22</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="C16" s="0" t="s">
         <v>6</v>
@@ -520,7 +529,7 @@
         <v>16</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="C17" s="0" t="s">
         <v>6</v>
@@ -537,7 +546,7 @@
         <v>17</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="C18" s="0" t="s">
         <v>6</v>
@@ -554,7 +563,7 @@
         <v>18</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="C19" s="0" t="s">
         <v>6</v>
@@ -571,7 +580,7 @@
         <v>25</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="C20" s="0" t="s">
         <v>6</v>
@@ -588,7 +597,7 @@
         <v>26</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="C21" s="0" t="s">
         <v>6</v>
@@ -605,7 +614,7 @@
         <v>29</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="C22" s="0" t="s">
         <v>6</v>
@@ -624,7 +633,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:F10"/>
+  <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -647,58 +656,58 @@
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="0">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>42</v>
+        <v>11</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="D2" s="0" t="s">
         <v>7</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>31</v>
+        <v>12</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="0">
-        <v>20</v>
+        <v>31</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>16</v>
+        <v>33</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="D3" s="0" t="s">
         <v>7</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="F3" s="0" t="s">
-        <v>31</v>
+        <v>12</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="0">
-        <v>9</v>
+        <v>20</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>11</v>
+        <v>34</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="D4" s="0" t="s">
         <v>7</v>
@@ -707,18 +716,18 @@
         <v>8</v>
       </c>
       <c r="F4" s="0" t="s">
-        <v>31</v>
+        <v>12</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="0">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="D5" s="0" t="s">
         <v>7</v>
@@ -727,18 +736,18 @@
         <v>8</v>
       </c>
       <c r="F5" s="0" t="s">
-        <v>31</v>
+        <v>12</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="0">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="D6" s="0" t="s">
         <v>7</v>
@@ -747,18 +756,18 @@
         <v>8</v>
       </c>
       <c r="F6" s="0" t="s">
-        <v>33</v>
+        <v>12</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="0">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="D7" s="0" t="s">
         <v>7</v>
@@ -767,18 +776,18 @@
         <v>8</v>
       </c>
       <c r="F7" s="0" t="s">
-        <v>8</v>
+        <v>38</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="0">
-        <v>30</v>
+        <v>3</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="D8" s="0" t="s">
         <v>7</v>
@@ -792,13 +801,13 @@
     </row>
     <row r="9">
       <c r="A9" s="0">
-        <v>2</v>
+        <v>30</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="D9" s="0" t="s">
         <v>7</v>
@@ -812,21 +821,41 @@
     </row>
     <row r="10">
       <c r="A10" s="0">
+        <v>2</v>
+      </c>
+      <c r="B10" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="C10" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="D10" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E10" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="F10" s="0" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="0">
         <v>1</v>
       </c>
-      <c r="B10" s="0" t="s">
-        <v>37</v>
-      </c>
-      <c r="C10" s="0" t="s">
-        <v>29</v>
-      </c>
-      <c r="D10" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="E10" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="F10" s="0" t="s">
+      <c r="B11" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="C11" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="D11" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E11" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="F11" s="0" t="s">
         <v>8</v>
       </c>
     </row>
@@ -848,7 +877,7 @@
         <v>2</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="C1" s="2"/>
       <c r="D1" s="2" t="s">
@@ -856,7 +885,7 @@
       </c>
       <c r="E1" s="2"/>
       <c r="F1" s="2" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
     </row>
     <row r="2">
@@ -864,24 +893,24 @@
         <v>6</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="D2" s="0" t="s">
         <v>7</v>
       </c>
       <c r="F2" s="0">
-        <v>34</v>
+        <v>37</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="0" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
v1: treat partial transparency like gray
</commit_message>
<xml_diff>
--- a/paint_todo.xlsx
+++ b/paint_todo.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="52">
   <si>
     <t>Id</t>
   </si>
@@ -193,6 +193,17 @@
   </si>
   <si>
     <t>apply color over color without changing underlying values</t>
+  </si>
+  <si>
+    <t xml:space="preserve">set and check tolerance for "black" and "white"
+- "blacks" will be left untouched
+- "whites" will be treated as pure white, which will in effect alter them to white</t>
+  </si>
+  <si>
+    <t>support applying color while zoomed in or out</t>
+  </si>
+  <si>
+    <t>bug: it isn't actually keeping the grayscale</t>
   </si>
 </sst>
 </file>
@@ -245,7 +256,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:F22"/>
+  <dimension ref="A1:F23"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -305,10 +316,10 @@
     </row>
     <row r="4">
       <c r="A4" s="0">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>13</v>
+        <v>51</v>
       </c>
       <c r="C4" s="0" t="s">
         <v>6</v>
@@ -317,15 +328,15 @@
         <v>7</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="0">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="C5" s="0" t="s">
         <v>6</v>
@@ -339,10 +350,10 @@
     </row>
     <row r="6">
       <c r="A6" s="0">
-        <v>11</v>
+        <v>33</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C6" s="0" t="s">
         <v>6</v>
@@ -351,15 +362,15 @@
         <v>7</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="0">
-        <v>12</v>
+        <v>37</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>15</v>
+        <v>48</v>
       </c>
       <c r="C7" s="0" t="s">
         <v>6</v>
@@ -368,15 +379,15 @@
         <v>7</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="0">
-        <v>35</v>
+        <v>11</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C8" s="0" t="s">
         <v>6</v>
@@ -385,15 +396,15 @@
         <v>7</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>17</v>
+        <v>8</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="0">
-        <v>13</v>
+        <v>35</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>18</v>
+        <v>49</v>
       </c>
       <c r="C9" s="0" t="s">
         <v>6</v>
@@ -402,15 +413,15 @@
         <v>7</v>
       </c>
       <c r="E9" s="0" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="0">
-        <v>34</v>
+        <v>13</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C10" s="0" t="s">
         <v>6</v>
@@ -419,15 +430,15 @@
         <v>7</v>
       </c>
       <c r="E10" s="0" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="0">
-        <v>21</v>
+        <v>34</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C11" s="0" t="s">
         <v>6</v>
@@ -436,15 +447,15 @@
         <v>7</v>
       </c>
       <c r="E11" s="0" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="0">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C12" s="0" t="s">
         <v>6</v>
@@ -458,10 +469,10 @@
     </row>
     <row r="13">
       <c r="A13" s="0">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C13" s="0" t="s">
         <v>6</v>
@@ -475,10 +486,10 @@
     </row>
     <row r="14">
       <c r="A14" s="0">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C14" s="0" t="s">
         <v>6</v>
@@ -492,10 +503,10 @@
     </row>
     <row r="15">
       <c r="A15" s="0">
-        <v>19</v>
+        <v>28</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C15" s="0" t="s">
         <v>6</v>
@@ -509,10 +520,10 @@
     </row>
     <row r="16">
       <c r="A16" s="0">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C16" s="0" t="s">
         <v>6</v>
@@ -526,10 +537,10 @@
     </row>
     <row r="17">
       <c r="A17" s="0">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C17" s="0" t="s">
         <v>6</v>
@@ -543,10 +554,10 @@
     </row>
     <row r="18">
       <c r="A18" s="0">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C18" s="0" t="s">
         <v>6</v>
@@ -560,10 +571,10 @@
     </row>
     <row r="19">
       <c r="A19" s="0">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C19" s="0" t="s">
         <v>6</v>
@@ -577,10 +588,10 @@
     </row>
     <row r="20">
       <c r="A20" s="0">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C20" s="0" t="s">
         <v>6</v>
@@ -594,10 +605,10 @@
     </row>
     <row r="21">
       <c r="A21" s="0">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C21" s="0" t="s">
         <v>6</v>
@@ -611,18 +622,35 @@
     </row>
     <row r="22">
       <c r="A22" s="0">
+        <v>26</v>
+      </c>
+      <c r="B22" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="C22" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D22" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E22" s="0" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="0">
         <v>29</v>
       </c>
-      <c r="B22" s="0" t="s">
+      <c r="B23" s="0" t="s">
         <v>31</v>
       </c>
-      <c r="C22" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="D22" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="E22" s="0" t="s">
+      <c r="C23" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D23" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E23" s="0" t="s">
         <v>8</v>
       </c>
     </row>
@@ -899,7 +927,7 @@
         <v>7</v>
       </c>
       <c r="F2" s="0">
-        <v>37</v>
+        <v>39</v>
       </c>
     </row>
     <row r="3">

</xml_diff>

<commit_message>
v1: simple apply color working
</commit_message>
<xml_diff>
--- a/paint_todo.xlsx
+++ b/paint_todo.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="51">
   <si>
     <t>Id</t>
   </si>
@@ -45,19 +45,28 @@
     <t>8/9/2018</t>
   </si>
   <si>
-    <t>when image is opened, auto-detect all black bordered regions</t>
-  </si>
-  <si>
-    <t>if a region contains no white, should i set the lightest pixel to white and reference for the pure color?</t>
-  </si>
-  <si>
-    <t>fill in a section of color on the image</t>
+    <t>what to rename ColorPalette library to so it does not conflict with object ColorPalette?</t>
+  </si>
+  <si>
+    <t>8/12/2018</t>
+  </si>
+  <si>
+    <t>zoom in needs to keep pixels clear instead of letting it blur together</t>
+  </si>
+  <si>
+    <t>8/13/2018</t>
+  </si>
+  <si>
+    <t>support applying color while zoomed in or out</t>
+  </si>
+  <si>
+    <t>undo, redo coloring a section on the image</t>
   </si>
   <si>
     <t>8/11/2018</t>
   </si>
   <si>
-    <t>undo, redo coloring a section on the image</t>
+    <t>apply color over color without changing underlying values</t>
   </si>
   <si>
     <t xml:space="preserve">save changes to image
@@ -66,15 +75,9 @@
 - jpg</t>
   </si>
   <si>
-    <t>make sure auto-detect of regions works even when image is already colored in</t>
-  </si>
-  <si>
     <t xml:space="preserve">set and check tolerance for "black" and "white"
 - "blacks" will be left untouched
-- "whites" will be treated as pure white, which will in effect alter then to white</t>
-  </si>
-  <si>
-    <t>8/12/2018</t>
+- "whites" will be treated as pure white, which will in effect alter them to white</t>
   </si>
   <si>
     <t xml:space="preserve">open edit palette mode
@@ -140,6 +143,16 @@
     <t>Done</t>
   </si>
   <si>
+    <t xml:space="preserve">bug: it isn't actually keeping the grayscale
+- wow, spent days debugging and it was just a test-line outside the area I was looking at</t>
+  </si>
+  <si>
+    <t>8/15/2018</t>
+  </si>
+  <si>
+    <t>fill in a section of color on the image</t>
+  </si>
+  <si>
     <t>select a palette color</t>
   </si>
   <si>
@@ -187,23 +200,6 @@
   </si>
   <si>
     <t>Bug</t>
-  </si>
-  <si>
-    <t>what to rename ColorPalette library to so it does not conflict with object ColorPalette?</t>
-  </si>
-  <si>
-    <t>apply color over color without changing underlying values</t>
-  </si>
-  <si>
-    <t xml:space="preserve">set and check tolerance for "black" and "white"
-- "blacks" will be left untouched
-- "whites" will be treated as pure white, which will in effect alter them to white</t>
-  </si>
-  <si>
-    <t>support applying color while zoomed in or out</t>
-  </si>
-  <si>
-    <t>bug: it isn't actually keeping the grayscale</t>
   </si>
 </sst>
 </file>
@@ -302,7 +298,7 @@
         <v>36</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>47</v>
+        <v>9</v>
       </c>
       <c r="C3" s="0" t="s">
         <v>6</v>
@@ -311,15 +307,15 @@
         <v>7</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="0">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>51</v>
+        <v>11</v>
       </c>
       <c r="C4" s="0" t="s">
         <v>6</v>
@@ -328,7 +324,7 @@
         <v>7</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
     </row>
     <row r="5">
@@ -336,7 +332,7 @@
         <v>38</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>50</v>
+        <v>13</v>
       </c>
       <c r="C5" s="0" t="s">
         <v>6</v>
@@ -345,7 +341,7 @@
         <v>7</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
     </row>
     <row r="6">
@@ -353,7 +349,7 @@
         <v>33</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C6" s="0" t="s">
         <v>6</v>
@@ -362,7 +358,7 @@
         <v>7</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
     </row>
     <row r="7">
@@ -370,7 +366,7 @@
         <v>37</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>48</v>
+        <v>16</v>
       </c>
       <c r="C7" s="0" t="s">
         <v>6</v>
@@ -379,7 +375,7 @@
         <v>7</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
     </row>
     <row r="8">
@@ -387,7 +383,7 @@
         <v>11</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="C8" s="0" t="s">
         <v>6</v>
@@ -404,7 +400,7 @@
         <v>35</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>49</v>
+        <v>18</v>
       </c>
       <c r="C9" s="0" t="s">
         <v>6</v>
@@ -413,7 +409,7 @@
         <v>7</v>
       </c>
       <c r="E9" s="0" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
     </row>
     <row r="10">
@@ -421,7 +417,7 @@
         <v>13</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C10" s="0" t="s">
         <v>6</v>
@@ -438,7 +434,7 @@
         <v>34</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C11" s="0" t="s">
         <v>6</v>
@@ -447,7 +443,7 @@
         <v>7</v>
       </c>
       <c r="E11" s="0" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
     </row>
     <row r="12">
@@ -455,7 +451,7 @@
         <v>21</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C12" s="0" t="s">
         <v>6</v>
@@ -472,7 +468,7 @@
         <v>24</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C13" s="0" t="s">
         <v>6</v>
@@ -489,7 +485,7 @@
         <v>27</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C14" s="0" t="s">
         <v>6</v>
@@ -506,7 +502,7 @@
         <v>28</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C15" s="0" t="s">
         <v>6</v>
@@ -523,7 +519,7 @@
         <v>19</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C16" s="0" t="s">
         <v>6</v>
@@ -540,7 +536,7 @@
         <v>22</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C17" s="0" t="s">
         <v>6</v>
@@ -557,7 +553,7 @@
         <v>16</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C18" s="0" t="s">
         <v>6</v>
@@ -574,7 +570,7 @@
         <v>17</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C19" s="0" t="s">
         <v>6</v>
@@ -591,7 +587,7 @@
         <v>18</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C20" s="0" t="s">
         <v>6</v>
@@ -608,7 +604,7 @@
         <v>25</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C21" s="0" t="s">
         <v>6</v>
@@ -625,7 +621,7 @@
         <v>26</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C22" s="0" t="s">
         <v>6</v>
@@ -642,7 +638,7 @@
         <v>29</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C23" s="0" t="s">
         <v>6</v>
@@ -661,7 +657,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:F11"/>
+  <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -684,78 +680,78 @@
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="0">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>11</v>
+        <v>34</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D2" s="0" t="s">
         <v>7</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>17</v>
+        <v>35</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="0">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D3" s="0" t="s">
         <v>7</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="F3" s="0" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="0">
-        <v>20</v>
+        <v>31</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D4" s="0" t="s">
         <v>7</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="F4" s="0" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="0">
-        <v>9</v>
+        <v>20</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D5" s="0" t="s">
         <v>7</v>
@@ -764,18 +760,18 @@
         <v>8</v>
       </c>
       <c r="F5" s="0" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="0">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D6" s="0" t="s">
         <v>7</v>
@@ -784,18 +780,18 @@
         <v>8</v>
       </c>
       <c r="F6" s="0" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="0">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D7" s="0" t="s">
         <v>7</v>
@@ -804,18 +800,18 @@
         <v>8</v>
       </c>
       <c r="F7" s="0" t="s">
-        <v>38</v>
+        <v>15</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="0">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D8" s="0" t="s">
         <v>7</v>
@@ -824,18 +820,18 @@
         <v>8</v>
       </c>
       <c r="F8" s="0" t="s">
-        <v>8</v>
+        <v>42</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="0">
-        <v>30</v>
+        <v>3</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D9" s="0" t="s">
         <v>7</v>
@@ -849,13 +845,13 @@
     </row>
     <row r="10">
       <c r="A10" s="0">
-        <v>2</v>
+        <v>30</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D10" s="0" t="s">
         <v>7</v>
@@ -869,21 +865,41 @@
     </row>
     <row r="11">
       <c r="A11" s="0">
+        <v>2</v>
+      </c>
+      <c r="B11" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="C11" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="D11" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E11" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="F11" s="0" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="0">
         <v>1</v>
       </c>
-      <c r="B11" s="0" t="s">
-        <v>42</v>
-      </c>
-      <c r="C11" s="0" t="s">
-        <v>32</v>
-      </c>
-      <c r="D11" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="E11" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="F11" s="0" t="s">
+      <c r="B12" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="C12" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="D12" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E12" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="F12" s="0" t="s">
         <v>8</v>
       </c>
     </row>
@@ -905,7 +921,7 @@
         <v>2</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="C1" s="2"/>
       <c r="D1" s="2" t="s">
@@ -913,7 +929,7 @@
       </c>
       <c r="E1" s="2"/>
       <c r="F1" s="2" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
     </row>
     <row r="2">
@@ -921,24 +937,24 @@
         <v>6</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="D2" s="0" t="s">
         <v>7</v>
       </c>
       <c r="F2" s="0">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="0" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
v1: pixelate images when zooming in
</commit_message>
<xml_diff>
--- a/paint_todo.xlsx
+++ b/paint_todo.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="52">
   <si>
     <t>Id</t>
   </si>
@@ -200,6 +200,9 @@
   </si>
   <si>
     <t>Bug</t>
+  </si>
+  <si>
+    <t>bug: on some colors (oranges esp.) adjusting the saturation gives a too bright color - keep it in the gray range</t>
   </si>
 </sst>
 </file>
@@ -312,10 +315,10 @@
     </row>
     <row r="4">
       <c r="A4" s="0">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>11</v>
+        <v>51</v>
       </c>
       <c r="C4" s="0" t="s">
         <v>6</v>
@@ -324,7 +327,7 @@
         <v>7</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>12</v>
+        <v>35</v>
       </c>
     </row>
     <row r="5">
@@ -657,7 +660,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:F12"/>
+  <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -685,10 +688,10 @@
     </row>
     <row r="2">
       <c r="A2" s="0">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>34</v>
+        <v>11</v>
       </c>
       <c r="C2" s="0" t="s">
         <v>33</v>
@@ -697,7 +700,7 @@
         <v>7</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="F2" s="0" t="s">
         <v>35</v>
@@ -705,10 +708,10 @@
     </row>
     <row r="3">
       <c r="A3" s="0">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C3" s="0" t="s">
         <v>33</v>
@@ -717,18 +720,18 @@
         <v>7</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="F3" s="0" t="s">
-        <v>10</v>
+        <v>35</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="0">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C4" s="0" t="s">
         <v>33</v>
@@ -740,15 +743,15 @@
         <v>15</v>
       </c>
       <c r="F4" s="0" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="0">
-        <v>20</v>
+        <v>31</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C5" s="0" t="s">
         <v>33</v>
@@ -757,7 +760,7 @@
         <v>7</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="F5" s="0" t="s">
         <v>15</v>
@@ -765,10 +768,10 @@
     </row>
     <row r="6">
       <c r="A6" s="0">
-        <v>9</v>
+        <v>20</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C6" s="0" t="s">
         <v>33</v>
@@ -785,10 +788,10 @@
     </row>
     <row r="7">
       <c r="A7" s="0">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C7" s="0" t="s">
         <v>33</v>
@@ -805,10 +808,10 @@
     </row>
     <row r="8">
       <c r="A8" s="0">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C8" s="0" t="s">
         <v>33</v>
@@ -820,15 +823,15 @@
         <v>8</v>
       </c>
       <c r="F8" s="0" t="s">
-        <v>42</v>
+        <v>15</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="0">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C9" s="0" t="s">
         <v>33</v>
@@ -840,15 +843,15 @@
         <v>8</v>
       </c>
       <c r="F9" s="0" t="s">
-        <v>8</v>
+        <v>42</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="0">
-        <v>30</v>
+        <v>3</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C10" s="0" t="s">
         <v>33</v>
@@ -865,10 +868,10 @@
     </row>
     <row r="11">
       <c r="A11" s="0">
-        <v>2</v>
+        <v>30</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C11" s="0" t="s">
         <v>33</v>
@@ -885,21 +888,41 @@
     </row>
     <row r="12">
       <c r="A12" s="0">
+        <v>2</v>
+      </c>
+      <c r="B12" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="C12" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="D12" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E12" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="F12" s="0" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="0">
         <v>1</v>
       </c>
-      <c r="B12" s="0" t="s">
+      <c r="B13" s="0" t="s">
         <v>46</v>
       </c>
-      <c r="C12" s="0" t="s">
-        <v>33</v>
-      </c>
-      <c r="D12" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="E12" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="F12" s="0" t="s">
+      <c r="C13" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="D13" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E13" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="F13" s="0" t="s">
         <v>8</v>
       </c>
     </row>
@@ -943,7 +966,7 @@
         <v>7</v>
       </c>
       <c r="F2" s="0">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="3">

</xml_diff>

<commit_message>
refactor: update to match renamed library ColorPalette to Colors
</commit_message>
<xml_diff>
--- a/paint_todo.xlsx
+++ b/paint_todo.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="58">
   <si>
     <t>Id</t>
   </si>
@@ -203,6 +203,30 @@
   </si>
   <si>
     <t>bug: on some colors (oranges esp.) adjusting the saturation gives a too bright color - keep it in the gray range</t>
+  </si>
+  <si>
+    <t xml:space="preserve">apply color over color without changing underlying values
+- change section back to grayscale
+- then to the new color</t>
+  </si>
+  <si>
+    <t>bug: expanded palette covers part of picturebox</t>
+  </si>
+  <si>
+    <t xml:space="preserve">on deep zoom, when image is getting too big, switch to zooming on just a segment of the masterImage
+- this will complicate scrollbars and color placement</t>
+  </si>
+  <si>
+    <t xml:space="preserve">move coloring operations into another thread
+- queue incoming commands
+- handle one at a time in another thread, updating display between each one</t>
+  </si>
+  <si>
+    <t>display closable modal "Please Wait" while coloring image</t>
+  </si>
+  <si>
+    <t xml:space="preserve">display closable modal "Please Wait" while coloring image
+- with "Cancel Color" option that will stop the thread and cancel the changes</t>
   </si>
 </sst>
 </file>
@@ -255,7 +279,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:F23"/>
+  <dimension ref="A1:F26"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -369,7 +393,7 @@
         <v>37</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>16</v>
+        <v>52</v>
       </c>
       <c r="C7" s="0" t="s">
         <v>6</v>
@@ -383,10 +407,10 @@
     </row>
     <row r="8">
       <c r="A8" s="0">
-        <v>11</v>
+        <v>44</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>17</v>
+        <v>55</v>
       </c>
       <c r="C8" s="0" t="s">
         <v>6</v>
@@ -395,32 +419,32 @@
         <v>7</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>8</v>
+        <v>35</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="0">
+        <v>45</v>
+      </c>
+      <c r="B9" s="0" t="s">
+        <v>57</v>
+      </c>
+      <c r="C9" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D9" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E9" s="0" t="s">
         <v>35</v>
-      </c>
-      <c r="B9" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="C9" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="D9" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="E9" s="0" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="0">
-        <v>13</v>
+        <v>42</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>19</v>
+        <v>53</v>
       </c>
       <c r="C10" s="0" t="s">
         <v>6</v>
@@ -429,15 +453,15 @@
         <v>7</v>
       </c>
       <c r="E10" s="0" t="s">
-        <v>8</v>
+        <v>35</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="0">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C11" s="0" t="s">
         <v>6</v>
@@ -446,15 +470,15 @@
         <v>7</v>
       </c>
       <c r="E11" s="0" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="0">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C12" s="0" t="s">
         <v>6</v>
@@ -468,10 +492,10 @@
     </row>
     <row r="13">
       <c r="A13" s="0">
-        <v>24</v>
+        <v>34</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C13" s="0" t="s">
         <v>6</v>
@@ -480,15 +504,15 @@
         <v>7</v>
       </c>
       <c r="E13" s="0" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="0">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C14" s="0" t="s">
         <v>6</v>
@@ -502,10 +526,10 @@
     </row>
     <row r="15">
       <c r="A15" s="0">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C15" s="0" t="s">
         <v>6</v>
@@ -519,10 +543,10 @@
     </row>
     <row r="16">
       <c r="A16" s="0">
-        <v>19</v>
+        <v>27</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C16" s="0" t="s">
         <v>6</v>
@@ -536,10 +560,10 @@
     </row>
     <row r="17">
       <c r="A17" s="0">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C17" s="0" t="s">
         <v>6</v>
@@ -553,10 +577,10 @@
     </row>
     <row r="18">
       <c r="A18" s="0">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C18" s="0" t="s">
         <v>6</v>
@@ -570,10 +594,10 @@
     </row>
     <row r="19">
       <c r="A19" s="0">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C19" s="0" t="s">
         <v>6</v>
@@ -587,10 +611,10 @@
     </row>
     <row r="20">
       <c r="A20" s="0">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C20" s="0" t="s">
         <v>6</v>
@@ -604,10 +628,10 @@
     </row>
     <row r="21">
       <c r="A21" s="0">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C21" s="0" t="s">
         <v>6</v>
@@ -621,10 +645,10 @@
     </row>
     <row r="22">
       <c r="A22" s="0">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C22" s="0" t="s">
         <v>6</v>
@@ -638,18 +662,69 @@
     </row>
     <row r="23">
       <c r="A23" s="0">
+        <v>25</v>
+      </c>
+      <c r="B23" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="C23" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D23" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E23" s="0" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="0">
+        <v>26</v>
+      </c>
+      <c r="B24" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="C24" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D24" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E24" s="0" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="0">
+        <v>43</v>
+      </c>
+      <c r="B25" s="0" t="s">
+        <v>54</v>
+      </c>
+      <c r="C25" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D25" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E25" s="0" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="0">
         <v>29</v>
       </c>
-      <c r="B23" s="0" t="s">
+      <c r="B26" s="0" t="s">
         <v>32</v>
       </c>
-      <c r="C23" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="D23" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="E23" s="0" t="s">
+      <c r="C26" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D26" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E26" s="0" t="s">
         <v>8</v>
       </c>
     </row>
@@ -660,7 +735,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:F13"/>
+  <dimension ref="A1:F14"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -688,10 +763,10 @@
     </row>
     <row r="2">
       <c r="A2" s="0">
-        <v>40</v>
+        <v>11</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="C2" s="0" t="s">
         <v>33</v>
@@ -700,7 +775,7 @@
         <v>7</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="F2" s="0" t="s">
         <v>35</v>
@@ -708,10 +783,10 @@
     </row>
     <row r="3">
       <c r="A3" s="0">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>34</v>
+        <v>11</v>
       </c>
       <c r="C3" s="0" t="s">
         <v>33</v>
@@ -720,7 +795,7 @@
         <v>7</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="F3" s="0" t="s">
         <v>35</v>
@@ -728,10 +803,10 @@
     </row>
     <row r="4">
       <c r="A4" s="0">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C4" s="0" t="s">
         <v>33</v>
@@ -740,18 +815,18 @@
         <v>7</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="F4" s="0" t="s">
-        <v>10</v>
+        <v>35</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="0">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C5" s="0" t="s">
         <v>33</v>
@@ -763,15 +838,15 @@
         <v>15</v>
       </c>
       <c r="F5" s="0" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="0">
-        <v>20</v>
+        <v>31</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C6" s="0" t="s">
         <v>33</v>
@@ -780,7 +855,7 @@
         <v>7</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="F6" s="0" t="s">
         <v>15</v>
@@ -788,10 +863,10 @@
     </row>
     <row r="7">
       <c r="A7" s="0">
-        <v>9</v>
+        <v>20</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C7" s="0" t="s">
         <v>33</v>
@@ -808,10 +883,10 @@
     </row>
     <row r="8">
       <c r="A8" s="0">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C8" s="0" t="s">
         <v>33</v>
@@ -828,10 +903,10 @@
     </row>
     <row r="9">
       <c r="A9" s="0">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C9" s="0" t="s">
         <v>33</v>
@@ -843,15 +918,15 @@
         <v>8</v>
       </c>
       <c r="F9" s="0" t="s">
-        <v>42</v>
+        <v>15</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="0">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C10" s="0" t="s">
         <v>33</v>
@@ -863,15 +938,15 @@
         <v>8</v>
       </c>
       <c r="F10" s="0" t="s">
-        <v>8</v>
+        <v>42</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="0">
-        <v>30</v>
+        <v>3</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C11" s="0" t="s">
         <v>33</v>
@@ -888,10 +963,10 @@
     </row>
     <row r="12">
       <c r="A12" s="0">
-        <v>2</v>
+        <v>30</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C12" s="0" t="s">
         <v>33</v>
@@ -908,21 +983,41 @@
     </row>
     <row r="13">
       <c r="A13" s="0">
+        <v>2</v>
+      </c>
+      <c r="B13" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="C13" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="D13" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E13" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="F13" s="0" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="0">
         <v>1</v>
       </c>
-      <c r="B13" s="0" t="s">
+      <c r="B14" s="0" t="s">
         <v>46</v>
       </c>
-      <c r="C13" s="0" t="s">
-        <v>33</v>
-      </c>
-      <c r="D13" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="E13" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="F13" s="0" t="s">
+      <c r="C14" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="D14" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E14" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="F14" s="0" t="s">
         <v>8</v>
       </c>
     </row>
@@ -966,7 +1061,7 @@
         <v>7</v>
       </c>
       <c r="F2" s="0">
-        <v>41</v>
+        <v>45</v>
       </c>
     </row>
     <row r="3">

</xml_diff>

<commit_message>
v1: adjust grayed-colors to avoid bright-saturation range
</commit_message>
<xml_diff>
--- a/paint_todo.xlsx
+++ b/paint_todo.xlsx
@@ -45,34 +45,45 @@
     <t>8/9/2018</t>
   </si>
   <si>
-    <t>what to rename ColorPalette library to so it does not conflict with object ColorPalette?</t>
+    <t>bug: on some colors (oranges esp.) adjusting the saturation gives a too bright color - keep it in the gray range</t>
+  </si>
+  <si>
+    <t>8/15/2018</t>
+  </si>
+  <si>
+    <t>support applying color while zoomed in or out</t>
   </si>
   <si>
     <t>8/12/2018</t>
   </si>
   <si>
-    <t>zoom in needs to keep pixels clear instead of letting it blur together</t>
-  </si>
-  <si>
-    <t>8/13/2018</t>
-  </si>
-  <si>
-    <t>support applying color while zoomed in or out</t>
-  </si>
-  <si>
     <t>undo, redo coloring a section on the image</t>
   </si>
   <si>
     <t>8/11/2018</t>
   </si>
   <si>
-    <t>apply color over color without changing underlying values</t>
-  </si>
-  <si>
-    <t xml:space="preserve">save changes to image
-- bitmap
-- png
-- jpg</t>
+    <t xml:space="preserve">apply color over color without changing underlying values
+- change section back to grayscale
+- then to the new color</t>
+  </si>
+  <si>
+    <t xml:space="preserve">move coloring operations into another thread
+- queue incoming commands
+- handle one at a time in another thread, updating display between each one</t>
+  </si>
+  <si>
+    <t xml:space="preserve">display closable modal "Please Wait" while coloring image
+- with "Cancel Color" option that will stop the thread and cancel the changes</t>
+  </si>
+  <si>
+    <t>bug: expanded palette covers part of picturebox</t>
+  </si>
+  <si>
+    <t>add "100%" size button</t>
+  </si>
+  <si>
+    <t>8/16/2018</t>
   </si>
   <si>
     <t xml:space="preserve">set and check tolerance for "black" and "white"
@@ -137,17 +148,33 @@
     <t>remember last used directory (save or open) and default to there in file dialogs</t>
   </si>
   <si>
+    <t xml:space="preserve">on deep zoom, when image is getting too big, switch to zooming on just a segment of the masterImage
+- this will complicate scrollbars and color placement</t>
+  </si>
+  <si>
     <t>how to programs auto-update?</t>
   </si>
   <si>
     <t>Done</t>
+  </si>
+  <si>
+    <t>what to rename ColorPalette library to so it does not conflict with object ColorPalette?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">save changes to image
+- bitmap
+- png
+- jpg</t>
+  </si>
+  <si>
+    <t>zoom in needs to keep pixels clear instead of letting it blur together</t>
+  </si>
+  <si>
+    <t>8/13/2018</t>
   </si>
   <si>
     <t xml:space="preserve">bug: it isn't actually keeping the grayscale
 - wow, spent days debugging and it was just a test-line outside the area I was looking at</t>
-  </si>
-  <si>
-    <t>8/15/2018</t>
   </si>
   <si>
     <t>fill in a section of color on the image</t>
@@ -200,33 +227,6 @@
   </si>
   <si>
     <t>Bug</t>
-  </si>
-  <si>
-    <t>bug: on some colors (oranges esp.) adjusting the saturation gives a too bright color - keep it in the gray range</t>
-  </si>
-  <si>
-    <t xml:space="preserve">apply color over color without changing underlying values
-- change section back to grayscale
-- then to the new color</t>
-  </si>
-  <si>
-    <t>bug: expanded palette covers part of picturebox</t>
-  </si>
-  <si>
-    <t xml:space="preserve">on deep zoom, when image is getting too big, switch to zooming on just a segment of the masterImage
-- this will complicate scrollbars and color placement</t>
-  </si>
-  <si>
-    <t xml:space="preserve">move coloring operations into another thread
-- queue incoming commands
-- handle one at a time in another thread, updating display between each one</t>
-  </si>
-  <si>
-    <t>display closable modal "Please Wait" while coloring image</t>
-  </si>
-  <si>
-    <t xml:space="preserve">display closable modal "Please Wait" while coloring image
-- with "Cancel Color" option that will stop the thread and cancel the changes</t>
   </si>
 </sst>
 </file>
@@ -279,7 +279,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:F26"/>
+  <dimension ref="A1:F25"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -322,10 +322,10 @@
     </row>
     <row r="3">
       <c r="A3" s="0">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C3" s="0" t="s">
         <v>6</v>
@@ -334,15 +334,15 @@
         <v>7</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="0">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>51</v>
+        <v>13</v>
       </c>
       <c r="C4" s="0" t="s">
         <v>6</v>
@@ -351,15 +351,15 @@
         <v>7</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>35</v>
+        <v>14</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="0">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C5" s="0" t="s">
         <v>6</v>
@@ -368,15 +368,15 @@
         <v>7</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="0">
-        <v>33</v>
+        <v>44</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C6" s="0" t="s">
         <v>6</v>
@@ -385,15 +385,15 @@
         <v>7</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="0">
-        <v>37</v>
+        <v>45</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>52</v>
+        <v>17</v>
       </c>
       <c r="C7" s="0" t="s">
         <v>6</v>
@@ -407,10 +407,10 @@
     </row>
     <row r="8">
       <c r="A8" s="0">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>55</v>
+        <v>18</v>
       </c>
       <c r="C8" s="0" t="s">
         <v>6</v>
@@ -419,15 +419,15 @@
         <v>7</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>35</v>
+        <v>10</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="0">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>57</v>
+        <v>19</v>
       </c>
       <c r="C9" s="0" t="s">
         <v>6</v>
@@ -436,15 +436,15 @@
         <v>7</v>
       </c>
       <c r="E9" s="0" t="s">
-        <v>35</v>
+        <v>20</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="0">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>53</v>
+        <v>21</v>
       </c>
       <c r="C10" s="0" t="s">
         <v>6</v>
@@ -453,15 +453,15 @@
         <v>7</v>
       </c>
       <c r="E10" s="0" t="s">
-        <v>35</v>
+        <v>12</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="0">
-        <v>35</v>
+        <v>13</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="C11" s="0" t="s">
         <v>6</v>
@@ -470,15 +470,15 @@
         <v>7</v>
       </c>
       <c r="E11" s="0" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="0">
-        <v>13</v>
+        <v>34</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="C12" s="0" t="s">
         <v>6</v>
@@ -487,15 +487,15 @@
         <v>7</v>
       </c>
       <c r="E12" s="0" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="0">
-        <v>34</v>
+        <v>21</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="C13" s="0" t="s">
         <v>6</v>
@@ -504,15 +504,15 @@
         <v>7</v>
       </c>
       <c r="E13" s="0" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="0">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="C14" s="0" t="s">
         <v>6</v>
@@ -526,10 +526,10 @@
     </row>
     <row r="15">
       <c r="A15" s="0">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="C15" s="0" t="s">
         <v>6</v>
@@ -543,10 +543,10 @@
     </row>
     <row r="16">
       <c r="A16" s="0">
+        <v>28</v>
+      </c>
+      <c r="B16" s="0" t="s">
         <v>27</v>
-      </c>
-      <c r="B16" s="0" t="s">
-        <v>23</v>
       </c>
       <c r="C16" s="0" t="s">
         <v>6</v>
@@ -560,10 +560,10 @@
     </row>
     <row r="17">
       <c r="A17" s="0">
+        <v>19</v>
+      </c>
+      <c r="B17" s="0" t="s">
         <v>28</v>
-      </c>
-      <c r="B17" s="0" t="s">
-        <v>24</v>
       </c>
       <c r="C17" s="0" t="s">
         <v>6</v>
@@ -577,10 +577,10 @@
     </row>
     <row r="18">
       <c r="A18" s="0">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="C18" s="0" t="s">
         <v>6</v>
@@ -594,10 +594,10 @@
     </row>
     <row r="19">
       <c r="A19" s="0">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="C19" s="0" t="s">
         <v>6</v>
@@ -611,10 +611,10 @@
     </row>
     <row r="20">
       <c r="A20" s="0">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="C20" s="0" t="s">
         <v>6</v>
@@ -628,10 +628,10 @@
     </row>
     <row r="21">
       <c r="A21" s="0">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="C21" s="0" t="s">
         <v>6</v>
@@ -645,10 +645,10 @@
     </row>
     <row r="22">
       <c r="A22" s="0">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="C22" s="0" t="s">
         <v>6</v>
@@ -662,10 +662,10 @@
     </row>
     <row r="23">
       <c r="A23" s="0">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="C23" s="0" t="s">
         <v>6</v>
@@ -679,10 +679,10 @@
     </row>
     <row r="24">
       <c r="A24" s="0">
-        <v>26</v>
+        <v>43</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="C24" s="0" t="s">
         <v>6</v>
@@ -691,15 +691,15 @@
         <v>7</v>
       </c>
       <c r="E24" s="0" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="0">
-        <v>43</v>
+        <v>29</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>54</v>
+        <v>36</v>
       </c>
       <c r="C25" s="0" t="s">
         <v>6</v>
@@ -708,23 +708,6 @@
         <v>7</v>
       </c>
       <c r="E25" s="0" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="26">
-      <c r="A26" s="0">
-        <v>29</v>
-      </c>
-      <c r="B26" s="0" t="s">
-        <v>32</v>
-      </c>
-      <c r="C26" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="D26" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="E26" s="0" t="s">
         <v>8</v>
       </c>
     </row>
@@ -735,7 +718,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:F14"/>
+  <dimension ref="A1:F16"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -758,38 +741,38 @@
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="0">
-        <v>11</v>
+        <v>41</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="D2" s="0" t="s">
         <v>7</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>35</v>
+        <v>20</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="0">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>11</v>
+        <v>38</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="D3" s="0" t="s">
         <v>7</v>
@@ -798,44 +781,44 @@
         <v>12</v>
       </c>
       <c r="F3" s="0" t="s">
-        <v>35</v>
+        <v>20</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="0">
+        <v>11</v>
+      </c>
+      <c r="B4" s="0" t="s">
         <v>39</v>
       </c>
-      <c r="B4" s="0" t="s">
-        <v>34</v>
-      </c>
       <c r="C4" s="0" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="D4" s="0" t="s">
         <v>7</v>
       </c>
       <c r="E4" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="F4" s="0" t="s">
         <v>10</v>
-      </c>
-      <c r="F4" s="0" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="0">
-        <v>32</v>
+        <v>40</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="D5" s="0" t="s">
         <v>7</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>15</v>
+        <v>41</v>
       </c>
       <c r="F5" s="0" t="s">
         <v>10</v>
@@ -843,73 +826,73 @@
     </row>
     <row r="6">
       <c r="A6" s="0">
-        <v>31</v>
+        <v>39</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>37</v>
+        <v>42</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="D6" s="0" t="s">
         <v>7</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="F6" s="0" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="0">
-        <v>20</v>
+        <v>32</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="D7" s="0" t="s">
         <v>7</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="F7" s="0" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="0">
-        <v>9</v>
+        <v>31</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="D8" s="0" t="s">
         <v>7</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="F8" s="0" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="0">
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="D9" s="0" t="s">
         <v>7</v>
@@ -918,18 +901,18 @@
         <v>8</v>
       </c>
       <c r="F9" s="0" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="0">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="D10" s="0" t="s">
         <v>7</v>
@@ -938,18 +921,18 @@
         <v>8</v>
       </c>
       <c r="F10" s="0" t="s">
-        <v>42</v>
+        <v>14</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="0">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="D11" s="0" t="s">
         <v>7</v>
@@ -958,18 +941,18 @@
         <v>8</v>
       </c>
       <c r="F11" s="0" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="0">
-        <v>30</v>
+        <v>4</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="D12" s="0" t="s">
         <v>7</v>
@@ -978,18 +961,18 @@
         <v>8</v>
       </c>
       <c r="F12" s="0" t="s">
-        <v>8</v>
+        <v>49</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="0">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="D13" s="0" t="s">
         <v>7</v>
@@ -1003,21 +986,61 @@
     </row>
     <row r="14">
       <c r="A14" s="0">
+        <v>30</v>
+      </c>
+      <c r="B14" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="C14" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="D14" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E14" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="F14" s="0" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="0">
+        <v>2</v>
+      </c>
+      <c r="B15" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="C15" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="D15" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E15" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="F15" s="0" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="0">
         <v>1</v>
       </c>
-      <c r="B14" s="0" t="s">
-        <v>46</v>
-      </c>
-      <c r="C14" s="0" t="s">
-        <v>33</v>
-      </c>
-      <c r="D14" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="E14" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="F14" s="0" t="s">
+      <c r="B16" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="C16" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="D16" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E16" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="F16" s="0" t="s">
         <v>8</v>
       </c>
     </row>
@@ -1039,7 +1062,7 @@
         <v>2</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>47</v>
+        <v>54</v>
       </c>
       <c r="C1" s="2"/>
       <c r="D1" s="2" t="s">
@@ -1047,7 +1070,7 @@
       </c>
       <c r="E1" s="2"/>
       <c r="F1" s="2" t="s">
-        <v>48</v>
+        <v>55</v>
       </c>
     </row>
     <row r="2">
@@ -1055,24 +1078,24 @@
         <v>6</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>47</v>
+        <v>54</v>
       </c>
       <c r="D2" s="0" t="s">
         <v>7</v>
       </c>
       <c r="F2" s="0">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="0" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>49</v>
+        <v>56</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>50</v>
+        <v>57</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
v1: fixed bugs in multi-threaded bitmaps; use status bar instead of wait popup
</commit_message>
<xml_diff>
--- a/paint_todo.xlsx
+++ b/paint_todo.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="61">
   <si>
     <t>Id</t>
   </si>
@@ -45,12 +45,6 @@
     <t>8/9/2018</t>
   </si>
   <si>
-    <t>bug: on some colors (oranges esp.) adjusting the saturation gives a too bright color - keep it in the gray range</t>
-  </si>
-  <si>
-    <t>8/15/2018</t>
-  </si>
-  <si>
     <t>support applying color while zoomed in or out</t>
   </si>
   <si>
@@ -71,6 +65,9 @@
     <t xml:space="preserve">move coloring operations into another thread
 - queue incoming commands
 - handle one at a time in another thread, updating display between each one</t>
+  </si>
+  <si>
+    <t>8/15/2018</t>
   </si>
   <si>
     <t xml:space="preserve">display closable modal "Please Wait" while coloring image
@@ -155,7 +152,17 @@
     <t>how to programs auto-update?</t>
   </si>
   <si>
+    <t xml:space="preserve">read about faster bitmap operations:
+https://www.codeproject.com/Tips/240428/Work-with-Bitmaps-Faster-in-Csharp-3</t>
+  </si>
+  <si>
+    <t>8/21/2018</t>
+  </si>
+  <si>
     <t>Done</t>
+  </si>
+  <si>
+    <t>bug: on some colors (oranges esp.) adjusting the saturation gives a too bright color - keep it in the gray range</t>
   </si>
   <si>
     <t>what to rename ColorPalette library to so it does not conflict with object ColorPalette?</t>
@@ -227,6 +234,11 @@
   </si>
   <si>
     <t>Bug</t>
+  </si>
+  <si>
+    <t xml:space="preserve">display closable modal "Please Wait" while coloring image
+- with "Cancel Color" option that will stop the thread and cancel the changes
+UPDATED: show status bar message</t>
   </si>
 </sst>
 </file>
@@ -279,7 +291,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:F25"/>
+  <dimension ref="A1:F24"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -325,7 +337,7 @@
         <v>38</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C3" s="0" t="s">
         <v>6</v>
@@ -334,7 +346,7 @@
         <v>7</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4">
@@ -342,7 +354,7 @@
         <v>33</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C4" s="0" t="s">
         <v>6</v>
@@ -351,7 +363,7 @@
         <v>7</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="5">
@@ -359,7 +371,7 @@
         <v>37</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C5" s="0" t="s">
         <v>6</v>
@@ -368,15 +380,15 @@
         <v>7</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="0">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C6" s="0" t="s">
         <v>6</v>
@@ -385,15 +397,15 @@
         <v>7</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="0">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C7" s="0" t="s">
         <v>6</v>
@@ -402,15 +414,15 @@
         <v>7</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="0">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C8" s="0" t="s">
         <v>6</v>
@@ -424,10 +436,10 @@
     </row>
     <row r="9">
       <c r="A9" s="0">
-        <v>46</v>
+        <v>13</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C9" s="0" t="s">
         <v>6</v>
@@ -436,15 +448,15 @@
         <v>7</v>
       </c>
       <c r="E9" s="0" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="0">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C10" s="0" t="s">
         <v>6</v>
@@ -458,10 +470,10 @@
     </row>
     <row r="11">
       <c r="A11" s="0">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C11" s="0" t="s">
         <v>6</v>
@@ -475,10 +487,10 @@
     </row>
     <row r="12">
       <c r="A12" s="0">
-        <v>34</v>
+        <v>24</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C12" s="0" t="s">
         <v>6</v>
@@ -487,15 +499,15 @@
         <v>7</v>
       </c>
       <c r="E12" s="0" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="0">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C13" s="0" t="s">
         <v>6</v>
@@ -509,10 +521,10 @@
     </row>
     <row r="14">
       <c r="A14" s="0">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C14" s="0" t="s">
         <v>6</v>
@@ -526,10 +538,10 @@
     </row>
     <row r="15">
       <c r="A15" s="0">
+        <v>19</v>
+      </c>
+      <c r="B15" s="0" t="s">
         <v>27</v>
-      </c>
-      <c r="B15" s="0" t="s">
-        <v>26</v>
       </c>
       <c r="C15" s="0" t="s">
         <v>6</v>
@@ -543,10 +555,10 @@
     </row>
     <row r="16">
       <c r="A16" s="0">
+        <v>22</v>
+      </c>
+      <c r="B16" s="0" t="s">
         <v>28</v>
-      </c>
-      <c r="B16" s="0" t="s">
-        <v>27</v>
       </c>
       <c r="C16" s="0" t="s">
         <v>6</v>
@@ -560,10 +572,10 @@
     </row>
     <row r="17">
       <c r="A17" s="0">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C17" s="0" t="s">
         <v>6</v>
@@ -577,10 +589,10 @@
     </row>
     <row r="18">
       <c r="A18" s="0">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C18" s="0" t="s">
         <v>6</v>
@@ -594,10 +606,10 @@
     </row>
     <row r="19">
       <c r="A19" s="0">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C19" s="0" t="s">
         <v>6</v>
@@ -611,10 +623,10 @@
     </row>
     <row r="20">
       <c r="A20" s="0">
-        <v>17</v>
+        <v>25</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C20" s="0" t="s">
         <v>6</v>
@@ -628,10 +640,10 @@
     </row>
     <row r="21">
       <c r="A21" s="0">
-        <v>18</v>
+        <v>26</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C21" s="0" t="s">
         <v>6</v>
@@ -645,10 +657,10 @@
     </row>
     <row r="22">
       <c r="A22" s="0">
-        <v>25</v>
+        <v>43</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C22" s="0" t="s">
         <v>6</v>
@@ -657,15 +669,15 @@
         <v>7</v>
       </c>
       <c r="E22" s="0" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="0">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C23" s="0" t="s">
         <v>6</v>
@@ -679,10 +691,10 @@
     </row>
     <row r="24">
       <c r="A24" s="0">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C24" s="0" t="s">
         <v>6</v>
@@ -691,24 +703,7 @@
         <v>7</v>
       </c>
       <c r="E24" s="0" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="25">
-      <c r="A25" s="0">
-        <v>29</v>
-      </c>
-      <c r="B25" s="0" t="s">
-        <v>36</v>
-      </c>
-      <c r="C25" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="D25" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="E25" s="0" t="s">
-        <v>8</v>
+        <v>37</v>
       </c>
     </row>
   </sheetData>
@@ -718,7 +713,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:F16"/>
+  <dimension ref="A1:F18"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -741,198 +736,198 @@
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="0">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>9</v>
+        <v>60</v>
       </c>
       <c r="C2" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="D2" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2" s="0" t="s">
         <v>37</v>
-      </c>
-      <c r="D2" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="E2" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="F2" s="0" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="0">
-        <v>36</v>
+        <v>44</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>38</v>
+        <v>14</v>
       </c>
       <c r="C3" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="D3" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E3" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3" s="0" t="s">
         <v>37</v>
-      </c>
-      <c r="D3" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="E3" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="F3" s="0" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="0">
-        <v>11</v>
+        <v>41</v>
       </c>
       <c r="B4" s="0" t="s">
         <v>39</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D4" s="0" t="s">
         <v>7</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="F4" s="0" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="0">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="B5" s="0" t="s">
         <v>40</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D5" s="0" t="s">
         <v>7</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>41</v>
+        <v>10</v>
       </c>
       <c r="F5" s="0" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="0">
-        <v>39</v>
+        <v>11</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D6" s="0" t="s">
         <v>7</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="F6" s="0" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="0">
-        <v>32</v>
+        <v>40</v>
       </c>
       <c r="B7" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="C7" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="D7" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E7" s="0" t="s">
         <v>43</v>
       </c>
-      <c r="C7" s="0" t="s">
-        <v>37</v>
-      </c>
-      <c r="D7" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="E7" s="0" t="s">
-        <v>14</v>
-      </c>
       <c r="F7" s="0" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="0">
-        <v>31</v>
+        <v>39</v>
       </c>
       <c r="B8" s="0" t="s">
         <v>44</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D8" s="0" t="s">
         <v>7</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="F8" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="0">
-        <v>20</v>
+        <v>32</v>
       </c>
       <c r="B9" s="0" t="s">
         <v>45</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D9" s="0" t="s">
         <v>7</v>
       </c>
       <c r="E9" s="0" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="F9" s="0" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="0">
-        <v>9</v>
+        <v>31</v>
       </c>
       <c r="B10" s="0" t="s">
         <v>46</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D10" s="0" t="s">
         <v>7</v>
       </c>
       <c r="E10" s="0" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="F10" s="0" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="0">
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="B11" s="0" t="s">
         <v>47</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D11" s="0" t="s">
         <v>7</v>
@@ -941,18 +936,18 @@
         <v>8</v>
       </c>
       <c r="F11" s="0" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="0">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="B12" s="0" t="s">
         <v>48</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D12" s="0" t="s">
         <v>7</v>
@@ -961,18 +956,18 @@
         <v>8</v>
       </c>
       <c r="F12" s="0" t="s">
-        <v>49</v>
+        <v>12</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="0">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D13" s="0" t="s">
         <v>7</v>
@@ -981,38 +976,38 @@
         <v>8</v>
       </c>
       <c r="F13" s="0" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="0">
-        <v>30</v>
+        <v>4</v>
       </c>
       <c r="B14" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="C14" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="D14" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E14" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="F14" s="0" t="s">
         <v>51</v>
-      </c>
-      <c r="C14" s="0" t="s">
-        <v>37</v>
-      </c>
-      <c r="D14" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="E14" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="F14" s="0" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="0">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B15" s="0" t="s">
         <v>52</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D15" s="0" t="s">
         <v>7</v>
@@ -1026,13 +1021,13 @@
     </row>
     <row r="16">
       <c r="A16" s="0">
-        <v>1</v>
+        <v>30</v>
       </c>
       <c r="B16" s="0" t="s">
         <v>53</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D16" s="0" t="s">
         <v>7</v>
@@ -1041,6 +1036,46 @@
         <v>8</v>
       </c>
       <c r="F16" s="0" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="0">
+        <v>2</v>
+      </c>
+      <c r="B17" s="0" t="s">
+        <v>54</v>
+      </c>
+      <c r="C17" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="D17" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E17" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="F17" s="0" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="0">
+        <v>1</v>
+      </c>
+      <c r="B18" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="C18" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="D18" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E18" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="F18" s="0" t="s">
         <v>8</v>
       </c>
     </row>
@@ -1062,7 +1097,7 @@
         <v>2</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="C1" s="2"/>
       <c r="D1" s="2" t="s">
@@ -1070,7 +1105,7 @@
       </c>
       <c r="E1" s="2"/>
       <c r="F1" s="2" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
     </row>
     <row r="2">
@@ -1078,24 +1113,24 @@
         <v>6</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="D2" s="0" t="s">
         <v>7</v>
       </c>
       <c r="F2" s="0">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="0" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
v1: 100% zoom option
</commit_message>
<xml_diff>
--- a/paint_todo.xlsx
+++ b/paint_todo.xlsx
@@ -291,7 +291,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:F24"/>
+  <dimension ref="A1:F23"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -402,10 +402,10 @@
     </row>
     <row r="7">
       <c r="A7" s="0">
-        <v>46</v>
+        <v>35</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C7" s="0" t="s">
         <v>6</v>
@@ -414,15 +414,15 @@
         <v>7</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="0">
-        <v>35</v>
+        <v>13</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C8" s="0" t="s">
         <v>6</v>
@@ -431,15 +431,15 @@
         <v>7</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="0">
-        <v>13</v>
+        <v>34</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C9" s="0" t="s">
         <v>6</v>
@@ -448,15 +448,15 @@
         <v>7</v>
       </c>
       <c r="E9" s="0" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="0">
-        <v>34</v>
+        <v>21</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C10" s="0" t="s">
         <v>6</v>
@@ -465,15 +465,15 @@
         <v>7</v>
       </c>
       <c r="E10" s="0" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="0">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C11" s="0" t="s">
         <v>6</v>
@@ -487,10 +487,10 @@
     </row>
     <row r="12">
       <c r="A12" s="0">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C12" s="0" t="s">
         <v>6</v>
@@ -504,10 +504,10 @@
     </row>
     <row r="13">
       <c r="A13" s="0">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C13" s="0" t="s">
         <v>6</v>
@@ -521,10 +521,10 @@
     </row>
     <row r="14">
       <c r="A14" s="0">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C14" s="0" t="s">
         <v>6</v>
@@ -538,10 +538,10 @@
     </row>
     <row r="15">
       <c r="A15" s="0">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C15" s="0" t="s">
         <v>6</v>
@@ -555,10 +555,10 @@
     </row>
     <row r="16">
       <c r="A16" s="0">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C16" s="0" t="s">
         <v>6</v>
@@ -572,10 +572,10 @@
     </row>
     <row r="17">
       <c r="A17" s="0">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C17" s="0" t="s">
         <v>6</v>
@@ -589,10 +589,10 @@
     </row>
     <row r="18">
       <c r="A18" s="0">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C18" s="0" t="s">
         <v>6</v>
@@ -606,10 +606,10 @@
     </row>
     <row r="19">
       <c r="A19" s="0">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C19" s="0" t="s">
         <v>6</v>
@@ -623,10 +623,10 @@
     </row>
     <row r="20">
       <c r="A20" s="0">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C20" s="0" t="s">
         <v>6</v>
@@ -640,10 +640,10 @@
     </row>
     <row r="21">
       <c r="A21" s="0">
-        <v>26</v>
+        <v>43</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C21" s="0" t="s">
         <v>6</v>
@@ -652,15 +652,15 @@
         <v>7</v>
       </c>
       <c r="E21" s="0" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="0">
-        <v>43</v>
+        <v>29</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C22" s="0" t="s">
         <v>6</v>
@@ -669,15 +669,15 @@
         <v>7</v>
       </c>
       <c r="E22" s="0" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="0">
-        <v>29</v>
+        <v>47</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C23" s="0" t="s">
         <v>6</v>
@@ -686,23 +686,6 @@
         <v>7</v>
       </c>
       <c r="E23" s="0" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" s="0">
-        <v>47</v>
-      </c>
-      <c r="B24" s="0" t="s">
-        <v>36</v>
-      </c>
-      <c r="C24" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="D24" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="E24" s="0" t="s">
         <v>37</v>
       </c>
     </row>
@@ -713,7 +696,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:F18"/>
+  <dimension ref="A1:F19"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -741,10 +724,10 @@
     </row>
     <row r="2">
       <c r="A2" s="0">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>60</v>
+        <v>18</v>
       </c>
       <c r="C2" s="0" t="s">
         <v>38</v>
@@ -753,7 +736,7 @@
         <v>7</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="F2" s="0" t="s">
         <v>37</v>
@@ -761,10 +744,10 @@
     </row>
     <row r="3">
       <c r="A3" s="0">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>14</v>
+        <v>60</v>
       </c>
       <c r="C3" s="0" t="s">
         <v>38</v>
@@ -781,10 +764,10 @@
     </row>
     <row r="4">
       <c r="A4" s="0">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>39</v>
+        <v>14</v>
       </c>
       <c r="C4" s="0" t="s">
         <v>38</v>
@@ -796,15 +779,15 @@
         <v>15</v>
       </c>
       <c r="F4" s="0" t="s">
-        <v>19</v>
+        <v>37</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="0">
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C5" s="0" t="s">
         <v>38</v>
@@ -813,7 +796,7 @@
         <v>7</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="F5" s="0" t="s">
         <v>19</v>
@@ -821,10 +804,10 @@
     </row>
     <row r="6">
       <c r="A6" s="0">
-        <v>11</v>
+        <v>36</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C6" s="0" t="s">
         <v>38</v>
@@ -833,18 +816,18 @@
         <v>7</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="F6" s="0" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="0">
-        <v>40</v>
+        <v>11</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C7" s="0" t="s">
         <v>38</v>
@@ -853,7 +836,7 @@
         <v>7</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>43</v>
+        <v>8</v>
       </c>
       <c r="F7" s="0" t="s">
         <v>15</v>
@@ -861,10 +844,10 @@
     </row>
     <row r="8">
       <c r="A8" s="0">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C8" s="0" t="s">
         <v>38</v>
@@ -873,7 +856,7 @@
         <v>7</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>10</v>
+        <v>43</v>
       </c>
       <c r="F8" s="0" t="s">
         <v>15</v>
@@ -881,10 +864,10 @@
     </row>
     <row r="9">
       <c r="A9" s="0">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C9" s="0" t="s">
         <v>38</v>
@@ -893,18 +876,18 @@
         <v>7</v>
       </c>
       <c r="E9" s="0" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="F9" s="0" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="0">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C10" s="0" t="s">
         <v>38</v>
@@ -916,15 +899,15 @@
         <v>12</v>
       </c>
       <c r="F10" s="0" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="0">
-        <v>20</v>
+        <v>31</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C11" s="0" t="s">
         <v>38</v>
@@ -933,7 +916,7 @@
         <v>7</v>
       </c>
       <c r="E11" s="0" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="F11" s="0" t="s">
         <v>12</v>
@@ -941,10 +924,10 @@
     </row>
     <row r="12">
       <c r="A12" s="0">
-        <v>9</v>
+        <v>20</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C12" s="0" t="s">
         <v>38</v>
@@ -961,10 +944,10 @@
     </row>
     <row r="13">
       <c r="A13" s="0">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C13" s="0" t="s">
         <v>38</v>
@@ -981,10 +964,10 @@
     </row>
     <row r="14">
       <c r="A14" s="0">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C14" s="0" t="s">
         <v>38</v>
@@ -996,15 +979,15 @@
         <v>8</v>
       </c>
       <c r="F14" s="0" t="s">
-        <v>51</v>
+        <v>12</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="0">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C15" s="0" t="s">
         <v>38</v>
@@ -1016,15 +999,15 @@
         <v>8</v>
       </c>
       <c r="F15" s="0" t="s">
-        <v>8</v>
+        <v>51</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="0">
-        <v>30</v>
+        <v>3</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C16" s="0" t="s">
         <v>38</v>
@@ -1041,10 +1024,10 @@
     </row>
     <row r="17">
       <c r="A17" s="0">
-        <v>2</v>
+        <v>30</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C17" s="0" t="s">
         <v>38</v>
@@ -1061,21 +1044,41 @@
     </row>
     <row r="18">
       <c r="A18" s="0">
+        <v>2</v>
+      </c>
+      <c r="B18" s="0" t="s">
+        <v>54</v>
+      </c>
+      <c r="C18" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="D18" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E18" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="F18" s="0" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="0">
         <v>1</v>
       </c>
-      <c r="B18" s="0" t="s">
+      <c r="B19" s="0" t="s">
         <v>55</v>
       </c>
-      <c r="C18" s="0" t="s">
-        <v>38</v>
-      </c>
-      <c r="D18" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="E18" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="F18" s="0" t="s">
+      <c r="C19" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="D19" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E19" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="F19" s="0" t="s">
         <v>8</v>
       </c>
     </row>

</xml_diff>

<commit_message>
v1: color image when zoomed in/out
</commit_message>
<xml_diff>
--- a/paint_todo.xlsx
+++ b/paint_todo.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="62">
   <si>
     <t>Id</t>
   </si>
@@ -239,6 +239,9 @@
     <t xml:space="preserve">display closable modal "Please Wait" while coloring image
 - with "Cancel Color" option that will stop the thread and cancel the changes
 UPDATED: show status bar message</t>
+  </si>
+  <si>
+    <t>bug: expanded palette covers part of picturebox and statuspanel</t>
   </si>
 </sst>
 </file>
@@ -291,7 +294,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:F23"/>
+  <dimension ref="A1:F22"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -334,10 +337,10 @@
     </row>
     <row r="3">
       <c r="A3" s="0">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C3" s="0" t="s">
         <v>6</v>
@@ -346,15 +349,15 @@
         <v>7</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="0">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C4" s="0" t="s">
         <v>6</v>
@@ -363,15 +366,15 @@
         <v>7</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="0">
-        <v>37</v>
+        <v>42</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>13</v>
+        <v>61</v>
       </c>
       <c r="C5" s="0" t="s">
         <v>6</v>
@@ -380,15 +383,15 @@
         <v>7</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="0">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="C6" s="0" t="s">
         <v>6</v>
@@ -397,15 +400,15 @@
         <v>7</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="0">
-        <v>35</v>
+        <v>13</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C7" s="0" t="s">
         <v>6</v>
@@ -414,15 +417,15 @@
         <v>7</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="0">
-        <v>13</v>
+        <v>34</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C8" s="0" t="s">
         <v>6</v>
@@ -431,15 +434,15 @@
         <v>7</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="0">
-        <v>34</v>
+        <v>21</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C9" s="0" t="s">
         <v>6</v>
@@ -448,15 +451,15 @@
         <v>7</v>
       </c>
       <c r="E9" s="0" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="0">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C10" s="0" t="s">
         <v>6</v>
@@ -470,10 +473,10 @@
     </row>
     <row r="11">
       <c r="A11" s="0">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C11" s="0" t="s">
         <v>6</v>
@@ -487,10 +490,10 @@
     </row>
     <row r="12">
       <c r="A12" s="0">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C12" s="0" t="s">
         <v>6</v>
@@ -504,10 +507,10 @@
     </row>
     <row r="13">
       <c r="A13" s="0">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C13" s="0" t="s">
         <v>6</v>
@@ -521,10 +524,10 @@
     </row>
     <row r="14">
       <c r="A14" s="0">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C14" s="0" t="s">
         <v>6</v>
@@ -538,10 +541,10 @@
     </row>
     <row r="15">
       <c r="A15" s="0">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C15" s="0" t="s">
         <v>6</v>
@@ -555,10 +558,10 @@
     </row>
     <row r="16">
       <c r="A16" s="0">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C16" s="0" t="s">
         <v>6</v>
@@ -572,10 +575,10 @@
     </row>
     <row r="17">
       <c r="A17" s="0">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C17" s="0" t="s">
         <v>6</v>
@@ -589,10 +592,10 @@
     </row>
     <row r="18">
       <c r="A18" s="0">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C18" s="0" t="s">
         <v>6</v>
@@ -606,10 +609,10 @@
     </row>
     <row r="19">
       <c r="A19" s="0">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C19" s="0" t="s">
         <v>6</v>
@@ -623,10 +626,10 @@
     </row>
     <row r="20">
       <c r="A20" s="0">
-        <v>26</v>
+        <v>43</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C20" s="0" t="s">
         <v>6</v>
@@ -635,15 +638,15 @@
         <v>7</v>
       </c>
       <c r="E20" s="0" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="0">
-        <v>43</v>
+        <v>29</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C21" s="0" t="s">
         <v>6</v>
@@ -652,15 +655,15 @@
         <v>7</v>
       </c>
       <c r="E21" s="0" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="0">
-        <v>29</v>
+        <v>47</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C22" s="0" t="s">
         <v>6</v>
@@ -669,23 +672,6 @@
         <v>7</v>
       </c>
       <c r="E22" s="0" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" s="0">
-        <v>47</v>
-      </c>
-      <c r="B23" s="0" t="s">
-        <v>36</v>
-      </c>
-      <c r="C23" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="D23" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="E23" s="0" t="s">
         <v>37</v>
       </c>
     </row>
@@ -696,7 +682,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:F19"/>
+  <dimension ref="A1:F20"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -724,10 +710,10 @@
     </row>
     <row r="2">
       <c r="A2" s="0">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>18</v>
+        <v>9</v>
       </c>
       <c r="C2" s="0" t="s">
         <v>38</v>
@@ -736,7 +722,7 @@
         <v>7</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="F2" s="0" t="s">
         <v>37</v>
@@ -744,10 +730,10 @@
     </row>
     <row r="3">
       <c r="A3" s="0">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>60</v>
+        <v>18</v>
       </c>
       <c r="C3" s="0" t="s">
         <v>38</v>
@@ -756,7 +742,7 @@
         <v>7</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="F3" s="0" t="s">
         <v>37</v>
@@ -764,10 +750,10 @@
     </row>
     <row r="4">
       <c r="A4" s="0">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>14</v>
+        <v>60</v>
       </c>
       <c r="C4" s="0" t="s">
         <v>38</v>
@@ -784,10 +770,10 @@
     </row>
     <row r="5">
       <c r="A5" s="0">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>39</v>
+        <v>14</v>
       </c>
       <c r="C5" s="0" t="s">
         <v>38</v>
@@ -799,15 +785,15 @@
         <v>15</v>
       </c>
       <c r="F5" s="0" t="s">
-        <v>19</v>
+        <v>37</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="0">
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C6" s="0" t="s">
         <v>38</v>
@@ -816,7 +802,7 @@
         <v>7</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="F6" s="0" t="s">
         <v>19</v>
@@ -824,10 +810,10 @@
     </row>
     <row r="7">
       <c r="A7" s="0">
-        <v>11</v>
+        <v>36</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C7" s="0" t="s">
         <v>38</v>
@@ -836,18 +822,18 @@
         <v>7</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="F7" s="0" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="0">
-        <v>40</v>
+        <v>11</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C8" s="0" t="s">
         <v>38</v>
@@ -856,7 +842,7 @@
         <v>7</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>43</v>
+        <v>8</v>
       </c>
       <c r="F8" s="0" t="s">
         <v>15</v>
@@ -864,10 +850,10 @@
     </row>
     <row r="9">
       <c r="A9" s="0">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C9" s="0" t="s">
         <v>38</v>
@@ -876,7 +862,7 @@
         <v>7</v>
       </c>
       <c r="E9" s="0" t="s">
-        <v>10</v>
+        <v>43</v>
       </c>
       <c r="F9" s="0" t="s">
         <v>15</v>
@@ -884,10 +870,10 @@
     </row>
     <row r="10">
       <c r="A10" s="0">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C10" s="0" t="s">
         <v>38</v>
@@ -896,18 +882,18 @@
         <v>7</v>
       </c>
       <c r="E10" s="0" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="F10" s="0" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="0">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C11" s="0" t="s">
         <v>38</v>
@@ -919,15 +905,15 @@
         <v>12</v>
       </c>
       <c r="F11" s="0" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="0">
-        <v>20</v>
+        <v>31</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C12" s="0" t="s">
         <v>38</v>
@@ -936,7 +922,7 @@
         <v>7</v>
       </c>
       <c r="E12" s="0" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="F12" s="0" t="s">
         <v>12</v>
@@ -944,10 +930,10 @@
     </row>
     <row r="13">
       <c r="A13" s="0">
-        <v>9</v>
+        <v>20</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C13" s="0" t="s">
         <v>38</v>
@@ -964,10 +950,10 @@
     </row>
     <row r="14">
       <c r="A14" s="0">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C14" s="0" t="s">
         <v>38</v>
@@ -984,10 +970,10 @@
     </row>
     <row r="15">
       <c r="A15" s="0">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C15" s="0" t="s">
         <v>38</v>
@@ -999,15 +985,15 @@
         <v>8</v>
       </c>
       <c r="F15" s="0" t="s">
-        <v>51</v>
+        <v>12</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="0">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C16" s="0" t="s">
         <v>38</v>
@@ -1019,15 +1005,15 @@
         <v>8</v>
       </c>
       <c r="F16" s="0" t="s">
-        <v>8</v>
+        <v>51</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="0">
-        <v>30</v>
+        <v>3</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C17" s="0" t="s">
         <v>38</v>
@@ -1044,10 +1030,10 @@
     </row>
     <row r="18">
       <c r="A18" s="0">
-        <v>2</v>
+        <v>30</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C18" s="0" t="s">
         <v>38</v>
@@ -1064,21 +1050,41 @@
     </row>
     <row r="19">
       <c r="A19" s="0">
+        <v>2</v>
+      </c>
+      <c r="B19" s="0" t="s">
+        <v>54</v>
+      </c>
+      <c r="C19" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="D19" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E19" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="F19" s="0" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="0">
         <v>1</v>
       </c>
-      <c r="B19" s="0" t="s">
+      <c r="B20" s="0" t="s">
         <v>55</v>
       </c>
-      <c r="C19" s="0" t="s">
-        <v>38</v>
-      </c>
-      <c r="D19" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="E19" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="F19" s="0" t="s">
+      <c r="C20" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="D20" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E20" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="F20" s="0" t="s">
         <v>8</v>
       </c>
     </row>

</xml_diff>

<commit_message>
replace color with another color
</commit_message>
<xml_diff>
--- a/paint_todo.xlsx
+++ b/paint_todo.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="63">
   <si>
     <t>Id</t>
   </si>
@@ -45,12 +45,6 @@
     <t>8/9/2018</t>
   </si>
   <si>
-    <t>support applying color while zoomed in or out</t>
-  </si>
-  <si>
-    <t>8/12/2018</t>
-  </si>
-  <si>
     <t>undo, redo coloring a section on the image</t>
   </si>
   <si>
@@ -62,25 +56,13 @@
 - then to the new color</t>
   </si>
   <si>
-    <t xml:space="preserve">move coloring operations into another thread
-- queue incoming commands
-- handle one at a time in another thread, updating display between each one</t>
+    <t>8/12/2018</t>
+  </si>
+  <si>
+    <t>bug: expanded palette covers part of picturebox and statuspanel</t>
   </si>
   <si>
     <t>8/15/2018</t>
-  </si>
-  <si>
-    <t xml:space="preserve">display closable modal "Please Wait" while coloring image
-- with "Cancel Color" option that will stop the thread and cancel the changes</t>
-  </si>
-  <si>
-    <t>bug: expanded palette covers part of picturebox</t>
-  </si>
-  <si>
-    <t>add "100%" size button</t>
-  </si>
-  <si>
-    <t>8/16/2018</t>
   </si>
   <si>
     <t xml:space="preserve">set and check tolerance for "black" and "white"
@@ -122,6 +104,13 @@
 -patreon</t>
   </si>
   <si>
+    <t xml:space="preserve">on error popup:
+display all nested errors</t>
+  </si>
+  <si>
+    <t>8/22/2018</t>
+  </si>
+  <si>
     <t xml:space="preserve">design an icon
 apply to windows, desktop icon, and uninstall icon</t>
   </si>
@@ -160,6 +149,25 @@
   </si>
   <si>
     <t>Done</t>
+  </si>
+  <si>
+    <t>support applying color while zoomed in or out</t>
+  </si>
+  <si>
+    <t>add "100%" size button</t>
+  </si>
+  <si>
+    <t>8/16/2018</t>
+  </si>
+  <si>
+    <t xml:space="preserve">display closable modal "Please Wait" while coloring image
+- with "Cancel Color" option that will stop the thread and cancel the changes
+UPDATED: show status bar message</t>
+  </si>
+  <si>
+    <t xml:space="preserve">move coloring operations into another thread
+- queue incoming commands
+- handle one at a time in another thread, updating display between each one</t>
   </si>
   <si>
     <t>bug: on some colors (oranges esp.) adjusting the saturation gives a too bright color - keep it in the gray range</t>
@@ -236,12 +244,8 @@
     <t>Bug</t>
   </si>
   <si>
-    <t xml:space="preserve">display closable modal "Please Wait" while coloring image
-- with "Cancel Color" option that will stop the thread and cancel the changes
-UPDATED: show status bar message</t>
-  </si>
-  <si>
-    <t>bug: expanded palette covers part of picturebox and statuspanel</t>
+    <t xml:space="preserve">applying color is pretty fast even on large image
+but removing the color is really slow</t>
   </si>
 </sst>
 </file>
@@ -294,7 +298,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:F22"/>
+  <dimension ref="A1:F23"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -340,7 +344,7 @@
         <v>33</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C3" s="0" t="s">
         <v>6</v>
@@ -349,15 +353,15 @@
         <v>7</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="0">
-        <v>37</v>
+        <v>48</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>13</v>
+        <v>22</v>
       </c>
       <c r="C4" s="0" t="s">
         <v>6</v>
@@ -366,7 +370,7 @@
         <v>7</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>10</v>
+        <v>23</v>
       </c>
     </row>
     <row r="5">
@@ -374,7 +378,7 @@
         <v>42</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>61</v>
+        <v>13</v>
       </c>
       <c r="C5" s="0" t="s">
         <v>6</v>
@@ -383,7 +387,7 @@
         <v>7</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="6">
@@ -391,7 +395,7 @@
         <v>35</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="C6" s="0" t="s">
         <v>6</v>
@@ -400,7 +404,7 @@
         <v>7</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
     </row>
     <row r="7">
@@ -408,7 +412,7 @@
         <v>13</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="C7" s="0" t="s">
         <v>6</v>
@@ -425,7 +429,7 @@
         <v>34</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="C8" s="0" t="s">
         <v>6</v>
@@ -434,32 +438,32 @@
         <v>7</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="0">
-        <v>21</v>
+        <v>49</v>
       </c>
       <c r="B9" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="C9" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D9" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E9" s="0" t="s">
         <v>23</v>
-      </c>
-      <c r="C9" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="D9" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="E9" s="0" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="0">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="C10" s="0" t="s">
         <v>6</v>
@@ -473,10 +477,10 @@
     </row>
     <row r="11">
       <c r="A11" s="0">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="C11" s="0" t="s">
         <v>6</v>
@@ -490,10 +494,10 @@
     </row>
     <row r="12">
       <c r="A12" s="0">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="C12" s="0" t="s">
         <v>6</v>
@@ -507,10 +511,10 @@
     </row>
     <row r="13">
       <c r="A13" s="0">
-        <v>19</v>
+        <v>28</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="C13" s="0" t="s">
         <v>6</v>
@@ -524,10 +528,10 @@
     </row>
     <row r="14">
       <c r="A14" s="0">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="C14" s="0" t="s">
         <v>6</v>
@@ -541,10 +545,10 @@
     </row>
     <row r="15">
       <c r="A15" s="0">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="C15" s="0" t="s">
         <v>6</v>
@@ -558,10 +562,10 @@
     </row>
     <row r="16">
       <c r="A16" s="0">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C16" s="0" t="s">
         <v>6</v>
@@ -575,10 +579,10 @@
     </row>
     <row r="17">
       <c r="A17" s="0">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C17" s="0" t="s">
         <v>6</v>
@@ -592,10 +596,10 @@
     </row>
     <row r="18">
       <c r="A18" s="0">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="C18" s="0" t="s">
         <v>6</v>
@@ -609,10 +613,10 @@
     </row>
     <row r="19">
       <c r="A19" s="0">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="C19" s="0" t="s">
         <v>6</v>
@@ -626,10 +630,10 @@
     </row>
     <row r="20">
       <c r="A20" s="0">
-        <v>43</v>
+        <v>26</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="C20" s="0" t="s">
         <v>6</v>
@@ -638,15 +642,15 @@
         <v>7</v>
       </c>
       <c r="E20" s="0" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="0">
-        <v>29</v>
+        <v>43</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="C21" s="0" t="s">
         <v>6</v>
@@ -655,24 +659,41 @@
         <v>7</v>
       </c>
       <c r="E21" s="0" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="0">
+        <v>29</v>
+      </c>
+      <c r="B22" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="C22" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D22" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E22" s="0" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="0">
         <v>47</v>
       </c>
-      <c r="B22" s="0" t="s">
-        <v>36</v>
-      </c>
-      <c r="C22" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="D22" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="E22" s="0" t="s">
-        <v>37</v>
+      <c r="B23" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="C23" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D23" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E23" s="0" t="s">
+        <v>34</v>
       </c>
     </row>
   </sheetData>
@@ -682,7 +703,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:F20"/>
+  <dimension ref="A1:F21"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -705,198 +726,198 @@
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="0">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="D2" s="0" t="s">
         <v>7</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>37</v>
+        <v>23</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="0">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>18</v>
+        <v>36</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="D3" s="0" t="s">
         <v>7</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="F3" s="0" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="0">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>60</v>
+        <v>37</v>
       </c>
       <c r="C4" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="D4" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E4" s="0" t="s">
         <v>38</v>
       </c>
-      <c r="D4" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="E4" s="0" t="s">
-        <v>15</v>
-      </c>
       <c r="F4" s="0" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="0">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B5" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="C5" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="D5" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E5" s="0" t="s">
         <v>14</v>
       </c>
-      <c r="C5" s="0" t="s">
-        <v>38</v>
-      </c>
-      <c r="D5" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="E5" s="0" t="s">
-        <v>15</v>
-      </c>
       <c r="F5" s="0" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="0">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="D6" s="0" t="s">
         <v>7</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F6" s="0" t="s">
-        <v>19</v>
+        <v>34</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="0">
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C7" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="D7" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E7" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="F7" s="0" t="s">
         <v>38</v>
-      </c>
-      <c r="D7" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="E7" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="F7" s="0" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="0">
-        <v>11</v>
+        <v>36</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C8" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="D8" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E8" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="F8" s="0" t="s">
         <v>38</v>
-      </c>
-      <c r="D8" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="E8" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="F8" s="0" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="0">
-        <v>40</v>
+        <v>11</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="D9" s="0" t="s">
         <v>7</v>
       </c>
       <c r="E9" s="0" t="s">
-        <v>43</v>
+        <v>8</v>
       </c>
       <c r="F9" s="0" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="0">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B10" s="0" t="s">
         <v>44</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="D10" s="0" t="s">
         <v>7</v>
       </c>
       <c r="E10" s="0" t="s">
-        <v>10</v>
+        <v>45</v>
       </c>
       <c r="F10" s="0" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="0">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="D11" s="0" t="s">
         <v>7</v>
@@ -905,24 +926,24 @@
         <v>12</v>
       </c>
       <c r="F11" s="0" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="0">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="D12" s="0" t="s">
         <v>7</v>
       </c>
       <c r="E12" s="0" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="F12" s="0" t="s">
         <v>12</v>
@@ -930,33 +951,33 @@
     </row>
     <row r="13">
       <c r="A13" s="0">
-        <v>20</v>
+        <v>31</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="D13" s="0" t="s">
         <v>7</v>
       </c>
       <c r="E13" s="0" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="F13" s="0" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="0">
-        <v>9</v>
+        <v>20</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="D14" s="0" t="s">
         <v>7</v>
@@ -965,18 +986,18 @@
         <v>8</v>
       </c>
       <c r="F14" s="0" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="0">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="D15" s="0" t="s">
         <v>7</v>
@@ -985,18 +1006,18 @@
         <v>8</v>
       </c>
       <c r="F15" s="0" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="0">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="D16" s="0" t="s">
         <v>7</v>
@@ -1005,18 +1026,18 @@
         <v>8</v>
       </c>
       <c r="F16" s="0" t="s">
-        <v>51</v>
+        <v>10</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="0">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B17" s="0" t="s">
         <v>52</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="D17" s="0" t="s">
         <v>7</v>
@@ -1025,18 +1046,18 @@
         <v>8</v>
       </c>
       <c r="F17" s="0" t="s">
-        <v>8</v>
+        <v>53</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="0">
-        <v>30</v>
+        <v>3</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="D18" s="0" t="s">
         <v>7</v>
@@ -1050,13 +1071,13 @@
     </row>
     <row r="19">
       <c r="A19" s="0">
-        <v>2</v>
+        <v>30</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="D19" s="0" t="s">
         <v>7</v>
@@ -1070,21 +1091,41 @@
     </row>
     <row r="20">
       <c r="A20" s="0">
+        <v>2</v>
+      </c>
+      <c r="B20" s="0" t="s">
+        <v>56</v>
+      </c>
+      <c r="C20" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="D20" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E20" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="F20" s="0" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="0">
         <v>1</v>
       </c>
-      <c r="B20" s="0" t="s">
-        <v>55</v>
-      </c>
-      <c r="C20" s="0" t="s">
-        <v>38</v>
-      </c>
-      <c r="D20" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="E20" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="F20" s="0" t="s">
+      <c r="B21" s="0" t="s">
+        <v>57</v>
+      </c>
+      <c r="C21" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="D21" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E21" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="F21" s="0" t="s">
         <v>8</v>
       </c>
     </row>
@@ -1106,7 +1147,7 @@
         <v>2</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="C1" s="2"/>
       <c r="D1" s="2" t="s">
@@ -1114,7 +1155,7 @@
       </c>
       <c r="E1" s="2"/>
       <c r="F1" s="2" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
     </row>
     <row r="2">
@@ -1122,24 +1163,24 @@
         <v>6</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="D2" s="0" t="s">
         <v>7</v>
       </c>
       <c r="F2" s="0">
-        <v>47</v>
+        <v>49</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="0" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
bug fix: catching exceptions from worker thread
</commit_message>
<xml_diff>
--- a/paint_todo.xlsx
+++ b/paint_todo.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="65">
   <si>
     <t>Id</t>
   </si>
@@ -250,6 +250,9 @@
   <si>
     <t xml:space="preserve">design test that generates value scale for many different colors, easy to scan with the eye
 - for instance, sometimes the adjusted color gets darker than the lightest "black", leaving a paler ring around it</t>
+  </si>
+  <si>
+    <t>replace Rabbit with smaller and better divided image</t>
   </si>
 </sst>
 </file>
@@ -302,7 +305,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:F24"/>
+  <dimension ref="A1:F25"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -498,10 +501,10 @@
     </row>
     <row r="12">
       <c r="A12" s="0">
-        <v>24</v>
+        <v>51</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>19</v>
+        <v>64</v>
       </c>
       <c r="C12" s="0" t="s">
         <v>6</v>
@@ -510,15 +513,15 @@
         <v>7</v>
       </c>
       <c r="E12" s="0" t="s">
-        <v>8</v>
+        <v>23</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="0">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C13" s="0" t="s">
         <v>6</v>
@@ -532,10 +535,10 @@
     </row>
     <row r="14">
       <c r="A14" s="0">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C14" s="0" t="s">
         <v>6</v>
@@ -549,10 +552,10 @@
     </row>
     <row r="15">
       <c r="A15" s="0">
-        <v>19</v>
+        <v>28</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C15" s="0" t="s">
         <v>6</v>
@@ -566,10 +569,10 @@
     </row>
     <row r="16">
       <c r="A16" s="0">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C16" s="0" t="s">
         <v>6</v>
@@ -583,10 +586,10 @@
     </row>
     <row r="17">
       <c r="A17" s="0">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C17" s="0" t="s">
         <v>6</v>
@@ -600,10 +603,10 @@
     </row>
     <row r="18">
       <c r="A18" s="0">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C18" s="0" t="s">
         <v>6</v>
@@ -617,10 +620,10 @@
     </row>
     <row r="19">
       <c r="A19" s="0">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C19" s="0" t="s">
         <v>6</v>
@@ -634,10 +637,10 @@
     </row>
     <row r="20">
       <c r="A20" s="0">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C20" s="0" t="s">
         <v>6</v>
@@ -651,10 +654,10 @@
     </row>
     <row r="21">
       <c r="A21" s="0">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C21" s="0" t="s">
         <v>6</v>
@@ -668,10 +671,10 @@
     </row>
     <row r="22">
       <c r="A22" s="0">
-        <v>43</v>
+        <v>26</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C22" s="0" t="s">
         <v>6</v>
@@ -680,15 +683,15 @@
         <v>7</v>
       </c>
       <c r="E22" s="0" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="0">
-        <v>29</v>
+        <v>43</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C23" s="0" t="s">
         <v>6</v>
@@ -697,23 +700,40 @@
         <v>7</v>
       </c>
       <c r="E23" s="0" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="0">
+        <v>29</v>
+      </c>
+      <c r="B24" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="C24" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D24" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E24" s="0" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="0">
         <v>47</v>
       </c>
-      <c r="B24" s="0" t="s">
+      <c r="B25" s="0" t="s">
         <v>33</v>
       </c>
-      <c r="C24" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="D24" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="E24" s="0" t="s">
+      <c r="C25" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D25" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E25" s="0" t="s">
         <v>34</v>
       </c>
     </row>
@@ -1190,7 +1210,7 @@
         <v>7</v>
       </c>
       <c r="F2" s="0">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="3">

</xml_diff>

<commit_message>
show nested error messages
</commit_message>
<xml_diff>
--- a/paint_todo.xlsx
+++ b/paint_todo.xlsx
@@ -305,7 +305,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:F25"/>
+  <dimension ref="A1:F24"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -365,10 +365,10 @@
     </row>
     <row r="4">
       <c r="A4" s="0">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="C4" s="0" t="s">
         <v>6</v>
@@ -377,15 +377,15 @@
         <v>7</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>23</v>
+        <v>14</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="0">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C5" s="0" t="s">
         <v>6</v>
@@ -394,15 +394,15 @@
         <v>7</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="0">
-        <v>35</v>
+        <v>13</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C6" s="0" t="s">
         <v>6</v>
@@ -411,15 +411,15 @@
         <v>7</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="0">
-        <v>13</v>
+        <v>50</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>16</v>
+        <v>63</v>
       </c>
       <c r="C7" s="0" t="s">
         <v>6</v>
@@ -428,15 +428,15 @@
         <v>7</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>8</v>
+        <v>23</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="0">
-        <v>50</v>
+        <v>34</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>63</v>
+        <v>17</v>
       </c>
       <c r="C8" s="0" t="s">
         <v>6</v>
@@ -445,15 +445,15 @@
         <v>7</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>23</v>
+        <v>10</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="0">
-        <v>34</v>
+        <v>49</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>17</v>
+        <v>62</v>
       </c>
       <c r="C9" s="0" t="s">
         <v>6</v>
@@ -462,15 +462,15 @@
         <v>7</v>
       </c>
       <c r="E9" s="0" t="s">
-        <v>10</v>
+        <v>23</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="0">
-        <v>49</v>
+        <v>21</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>62</v>
+        <v>18</v>
       </c>
       <c r="C10" s="0" t="s">
         <v>6</v>
@@ -479,15 +479,15 @@
         <v>7</v>
       </c>
       <c r="E10" s="0" t="s">
-        <v>23</v>
+        <v>8</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="0">
-        <v>21</v>
+        <v>51</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>18</v>
+        <v>64</v>
       </c>
       <c r="C11" s="0" t="s">
         <v>6</v>
@@ -496,15 +496,15 @@
         <v>7</v>
       </c>
       <c r="E11" s="0" t="s">
-        <v>8</v>
+        <v>23</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="0">
-        <v>51</v>
+        <v>24</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>64</v>
+        <v>19</v>
       </c>
       <c r="C12" s="0" t="s">
         <v>6</v>
@@ -513,15 +513,15 @@
         <v>7</v>
       </c>
       <c r="E12" s="0" t="s">
-        <v>23</v>
+        <v>8</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="0">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C13" s="0" t="s">
         <v>6</v>
@@ -535,10 +535,10 @@
     </row>
     <row r="14">
       <c r="A14" s="0">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C14" s="0" t="s">
         <v>6</v>
@@ -552,10 +552,10 @@
     </row>
     <row r="15">
       <c r="A15" s="0">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="C15" s="0" t="s">
         <v>6</v>
@@ -569,10 +569,10 @@
     </row>
     <row r="16">
       <c r="A16" s="0">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C16" s="0" t="s">
         <v>6</v>
@@ -586,10 +586,10 @@
     </row>
     <row r="17">
       <c r="A17" s="0">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C17" s="0" t="s">
         <v>6</v>
@@ -603,10 +603,10 @@
     </row>
     <row r="18">
       <c r="A18" s="0">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C18" s="0" t="s">
         <v>6</v>
@@ -620,10 +620,10 @@
     </row>
     <row r="19">
       <c r="A19" s="0">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C19" s="0" t="s">
         <v>6</v>
@@ -637,10 +637,10 @@
     </row>
     <row r="20">
       <c r="A20" s="0">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C20" s="0" t="s">
         <v>6</v>
@@ -654,10 +654,10 @@
     </row>
     <row r="21">
       <c r="A21" s="0">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C21" s="0" t="s">
         <v>6</v>
@@ -671,10 +671,10 @@
     </row>
     <row r="22">
       <c r="A22" s="0">
-        <v>26</v>
+        <v>43</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C22" s="0" t="s">
         <v>6</v>
@@ -683,15 +683,15 @@
         <v>7</v>
       </c>
       <c r="E22" s="0" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="0">
-        <v>43</v>
+        <v>29</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C23" s="0" t="s">
         <v>6</v>
@@ -700,15 +700,15 @@
         <v>7</v>
       </c>
       <c r="E23" s="0" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="0">
-        <v>29</v>
+        <v>47</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C24" s="0" t="s">
         <v>6</v>
@@ -717,23 +717,6 @@
         <v>7</v>
       </c>
       <c r="E24" s="0" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="25">
-      <c r="A25" s="0">
-        <v>47</v>
-      </c>
-      <c r="B25" s="0" t="s">
-        <v>33</v>
-      </c>
-      <c r="C25" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="D25" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="E25" s="0" t="s">
         <v>34</v>
       </c>
     </row>
@@ -744,7 +727,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:F21"/>
+  <dimension ref="A1:F22"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -772,10 +755,10 @@
     </row>
     <row r="2">
       <c r="A2" s="0">
-        <v>37</v>
+        <v>48</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>11</v>
+        <v>22</v>
       </c>
       <c r="C2" s="0" t="s">
         <v>35</v>
@@ -784,7 +767,7 @@
         <v>7</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="F2" s="0" t="s">
         <v>23</v>
@@ -792,10 +775,10 @@
     </row>
     <row r="3">
       <c r="A3" s="0">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>36</v>
+        <v>11</v>
       </c>
       <c r="C3" s="0" t="s">
         <v>35</v>
@@ -807,15 +790,15 @@
         <v>12</v>
       </c>
       <c r="F3" s="0" t="s">
-        <v>34</v>
+        <v>23</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="0">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C4" s="0" t="s">
         <v>35</v>
@@ -824,7 +807,7 @@
         <v>7</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>38</v>
+        <v>12</v>
       </c>
       <c r="F4" s="0" t="s">
         <v>34</v>
@@ -832,10 +815,10 @@
     </row>
     <row r="5">
       <c r="A5" s="0">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C5" s="0" t="s">
         <v>35</v>
@@ -844,7 +827,7 @@
         <v>7</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>14</v>
+        <v>38</v>
       </c>
       <c r="F5" s="0" t="s">
         <v>34</v>
@@ -852,10 +835,10 @@
     </row>
     <row r="6">
       <c r="A6" s="0">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C6" s="0" t="s">
         <v>35</v>
@@ -872,10 +855,10 @@
     </row>
     <row r="7">
       <c r="A7" s="0">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C7" s="0" t="s">
         <v>35</v>
@@ -887,15 +870,15 @@
         <v>14</v>
       </c>
       <c r="F7" s="0" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="0">
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C8" s="0" t="s">
         <v>35</v>
@@ -904,7 +887,7 @@
         <v>7</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="F8" s="0" t="s">
         <v>38</v>
@@ -912,10 +895,10 @@
     </row>
     <row r="9">
       <c r="A9" s="0">
-        <v>11</v>
+        <v>36</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C9" s="0" t="s">
         <v>35</v>
@@ -924,18 +907,18 @@
         <v>7</v>
       </c>
       <c r="E9" s="0" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="F9" s="0" t="s">
-        <v>14</v>
+        <v>38</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="0">
-        <v>40</v>
+        <v>11</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C10" s="0" t="s">
         <v>35</v>
@@ -944,7 +927,7 @@
         <v>7</v>
       </c>
       <c r="E10" s="0" t="s">
-        <v>45</v>
+        <v>8</v>
       </c>
       <c r="F10" s="0" t="s">
         <v>14</v>
@@ -952,10 +935,10 @@
     </row>
     <row r="11">
       <c r="A11" s="0">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C11" s="0" t="s">
         <v>35</v>
@@ -964,7 +947,7 @@
         <v>7</v>
       </c>
       <c r="E11" s="0" t="s">
-        <v>12</v>
+        <v>45</v>
       </c>
       <c r="F11" s="0" t="s">
         <v>14</v>
@@ -972,10 +955,10 @@
     </row>
     <row r="12">
       <c r="A12" s="0">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C12" s="0" t="s">
         <v>35</v>
@@ -984,18 +967,18 @@
         <v>7</v>
       </c>
       <c r="E12" s="0" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="F12" s="0" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="0">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C13" s="0" t="s">
         <v>35</v>
@@ -1007,15 +990,15 @@
         <v>10</v>
       </c>
       <c r="F13" s="0" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="0">
-        <v>20</v>
+        <v>31</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C14" s="0" t="s">
         <v>35</v>
@@ -1024,7 +1007,7 @@
         <v>7</v>
       </c>
       <c r="E14" s="0" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="F14" s="0" t="s">
         <v>10</v>
@@ -1032,10 +1015,10 @@
     </row>
     <row r="15">
       <c r="A15" s="0">
-        <v>9</v>
+        <v>20</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C15" s="0" t="s">
         <v>35</v>
@@ -1052,10 +1035,10 @@
     </row>
     <row r="16">
       <c r="A16" s="0">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C16" s="0" t="s">
         <v>35</v>
@@ -1072,10 +1055,10 @@
     </row>
     <row r="17">
       <c r="A17" s="0">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C17" s="0" t="s">
         <v>35</v>
@@ -1087,15 +1070,15 @@
         <v>8</v>
       </c>
       <c r="F17" s="0" t="s">
-        <v>53</v>
+        <v>10</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="0">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C18" s="0" t="s">
         <v>35</v>
@@ -1107,15 +1090,15 @@
         <v>8</v>
       </c>
       <c r="F18" s="0" t="s">
-        <v>8</v>
+        <v>53</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="0">
-        <v>30</v>
+        <v>3</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C19" s="0" t="s">
         <v>35</v>
@@ -1132,10 +1115,10 @@
     </row>
     <row r="20">
       <c r="A20" s="0">
-        <v>2</v>
+        <v>30</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C20" s="0" t="s">
         <v>35</v>
@@ -1152,21 +1135,41 @@
     </row>
     <row r="21">
       <c r="A21" s="0">
+        <v>2</v>
+      </c>
+      <c r="B21" s="0" t="s">
+        <v>56</v>
+      </c>
+      <c r="C21" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="D21" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E21" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="F21" s="0" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="0">
         <v>1</v>
       </c>
-      <c r="B21" s="0" t="s">
+      <c r="B22" s="0" t="s">
         <v>57</v>
       </c>
-      <c r="C21" s="0" t="s">
-        <v>35</v>
-      </c>
-      <c r="D21" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="E21" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="F21" s="0" t="s">
+      <c r="C22" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="D22" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E22" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="F22" s="0" t="s">
         <v>8</v>
       </c>
     </row>

</xml_diff>

<commit_message>
v1: undo/redo apply color
</commit_message>
<xml_diff>
--- a/paint_todo.xlsx
+++ b/paint_todo.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="68">
   <si>
     <t>Id</t>
   </si>
@@ -51,14 +51,6 @@
     <t>8/11/2018</t>
   </si>
   <si>
-    <t xml:space="preserve">apply color over color without changing underlying values
-- change section back to grayscale
-- then to the new color</t>
-  </si>
-  <si>
-    <t>8/12/2018</t>
-  </si>
-  <si>
     <t>bug: expanded palette covers part of picturebox and statuspanel</t>
   </si>
   <si>
@@ -68,6 +60,9 @@
     <t xml:space="preserve">set and check tolerance for "black" and "white"
 - "blacks" will be left untouched
 - "whites" will be treated as pure white, which will in effect alter them to white</t>
+  </si>
+  <si>
+    <t>8/12/2018</t>
   </si>
   <si>
     <t xml:space="preserve">open edit palette mode
@@ -81,11 +76,33 @@
 (no duplicate colors allowed)</t>
   </si>
   <si>
+    <t xml:space="preserve">design test that generates value scale for many different colors, easy to scan with the eye
+- for instance, sometimes the adjusted color gets darker than the lightest "black", leaving a paler ring around it</t>
+  </si>
+  <si>
+    <t>8/22/2018</t>
+  </si>
+  <si>
     <t>when zooming, if a scroll bar is all the way to min or max, keep it there</t>
+  </si>
+  <si>
+    <t xml:space="preserve">applying color is pretty fast even on large image
+but removing the color is really slow</t>
   </si>
   <si>
     <t xml:space="preserve">when resizing windows, default behavior is to keep the same section of image in the viewing pane
 - so expanding window would in effect zoom in</t>
+  </si>
+  <si>
+    <t xml:space="preserve">prompt to save if image has changed since last save
+- on closing program
+- on opening new image</t>
+  </si>
+  <si>
+    <t>8/23/2018</t>
+  </si>
+  <si>
+    <t>replace Rabbit with smaller and better divided image</t>
   </si>
   <si>
     <t xml:space="preserve">remember windows size from last closing
@@ -94,6 +111,11 @@
 open with this size</t>
   </si>
   <si>
+    <t xml:space="preserve">in documentation
+recommend user keeps an original b/w copy to go back to
+if conversion errors build up with lots of editing</t>
+  </si>
+  <si>
     <t xml:space="preserve">include support contact information
 -wohaste email
 -paint landing page on website
@@ -104,51 +126,53 @@
 -patreon</t>
   </si>
   <si>
+    <t xml:space="preserve">design an icon
+apply to windows, desktop icon, and uninstall icon</t>
+  </si>
+  <si>
+    <t>check through the program Properties &gt;&gt; Assembly Info again, make sure all is accurate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">that should be it for minimum viable
+save as Version 1</t>
+  </si>
+  <si>
+    <t>build installer for Version 1 and save it in a separate folder to keep</t>
+  </si>
+  <si>
+    <t>update website with project, landing page, and links</t>
+  </si>
+  <si>
+    <t>EVERYTHING BELOW HERE IS VERSION 2</t>
+  </si>
+  <si>
+    <t>remember last used directory (save or open) and default to there in file dialogs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">on deep zoom, when image is getting too big, switch to zooming on just a segment of the masterImage
+- this will complicate scrollbars and color placement</t>
+  </si>
+  <si>
+    <t>how to programs auto-update?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">read about faster bitmap operations:
+https://www.codeproject.com/Tips/240428/Work-with-Bitmaps-Faster-in-Csharp-3</t>
+  </si>
+  <si>
+    <t>8/21/2018</t>
+  </si>
+  <si>
+    <t>Done</t>
+  </si>
+  <si>
     <t xml:space="preserve">on error popup:
 display all nested errors</t>
   </si>
   <si>
-    <t>8/22/2018</t>
-  </si>
-  <si>
-    <t xml:space="preserve">design an icon
-apply to windows, desktop icon, and uninstall icon</t>
-  </si>
-  <si>
-    <t>check through the program Properties &gt;&gt; Assembly Info again, make sure all is accurate</t>
-  </si>
-  <si>
-    <t xml:space="preserve">that should be it for minimum viable
-save as Version 1</t>
-  </si>
-  <si>
-    <t>build installer for Version 1 and save it in a separate folder to keep</t>
-  </si>
-  <si>
-    <t>update website with project, landing page, and links</t>
-  </si>
-  <si>
-    <t>EVERYTHING BELOW HERE IS VERSION 2</t>
-  </si>
-  <si>
-    <t>remember last used directory (save or open) and default to there in file dialogs</t>
-  </si>
-  <si>
-    <t xml:space="preserve">on deep zoom, when image is getting too big, switch to zooming on just a segment of the masterImage
-- this will complicate scrollbars and color placement</t>
-  </si>
-  <si>
-    <t>how to programs auto-update?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">read about faster bitmap operations:
-https://www.codeproject.com/Tips/240428/Work-with-Bitmaps-Faster-in-Csharp-3</t>
-  </si>
-  <si>
-    <t>8/21/2018</t>
-  </si>
-  <si>
-    <t>Done</t>
+    <t xml:space="preserve">apply color over color without changing underlying values
+- change section back to grayscale
+- then to the new color</t>
   </si>
   <si>
     <t>support applying color while zoomed in or out</t>
@@ -242,17 +266,6 @@
   </si>
   <si>
     <t>Bug</t>
-  </si>
-  <si>
-    <t xml:space="preserve">applying color is pretty fast even on large image
-but removing the color is really slow</t>
-  </si>
-  <si>
-    <t xml:space="preserve">design test that generates value scale for many different colors, easy to scan with the eye
-- for instance, sometimes the adjusted color gets darker than the lightest "black", leaving a paler ring around it</t>
-  </si>
-  <si>
-    <t>replace Rabbit with smaller and better divided image</t>
   </si>
 </sst>
 </file>
@@ -305,7 +318,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:F24"/>
+  <dimension ref="A1:F25"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -348,10 +361,10 @@
     </row>
     <row r="3">
       <c r="A3" s="0">
-        <v>33</v>
+        <v>42</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C3" s="0" t="s">
         <v>6</v>
@@ -360,12 +373,12 @@
         <v>7</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="0">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="B4" s="0" t="s">
         <v>13</v>
@@ -382,7 +395,7 @@
     </row>
     <row r="5">
       <c r="A5" s="0">
-        <v>35</v>
+        <v>13</v>
       </c>
       <c r="B5" s="0" t="s">
         <v>15</v>
@@ -394,12 +407,12 @@
         <v>7</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="0">
-        <v>13</v>
+        <v>50</v>
       </c>
       <c r="B6" s="0" t="s">
         <v>16</v>
@@ -411,15 +424,15 @@
         <v>7</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="0">
-        <v>50</v>
+        <v>34</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>63</v>
+        <v>18</v>
       </c>
       <c r="C7" s="0" t="s">
         <v>6</v>
@@ -428,32 +441,32 @@
         <v>7</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>23</v>
+        <v>10</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="0">
-        <v>34</v>
+        <v>49</v>
       </c>
       <c r="B8" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="C8" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D8" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E8" s="0" t="s">
         <v>17</v>
-      </c>
-      <c r="C8" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="D8" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="E8" s="0" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="0">
-        <v>49</v>
+        <v>21</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>62</v>
+        <v>20</v>
       </c>
       <c r="C9" s="0" t="s">
         <v>6</v>
@@ -462,16 +475,16 @@
         <v>7</v>
       </c>
       <c r="E9" s="0" t="s">
-        <v>23</v>
+        <v>8</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="0">
+        <v>53</v>
+      </c>
+      <c r="B10" s="0" t="s">
         <v>21</v>
       </c>
-      <c r="B10" s="0" t="s">
-        <v>18</v>
-      </c>
       <c r="C10" s="0" t="s">
         <v>6</v>
       </c>
@@ -479,7 +492,7 @@
         <v>7</v>
       </c>
       <c r="E10" s="0" t="s">
-        <v>8</v>
+        <v>22</v>
       </c>
     </row>
     <row r="11">
@@ -487,7 +500,7 @@
         <v>51</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>64</v>
+        <v>23</v>
       </c>
       <c r="C11" s="0" t="s">
         <v>6</v>
@@ -496,7 +509,7 @@
         <v>7</v>
       </c>
       <c r="E11" s="0" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
     </row>
     <row r="12">
@@ -504,7 +517,7 @@
         <v>24</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="C12" s="0" t="s">
         <v>6</v>
@@ -518,10 +531,10 @@
     </row>
     <row r="13">
       <c r="A13" s="0">
-        <v>27</v>
+        <v>52</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="C13" s="0" t="s">
         <v>6</v>
@@ -530,15 +543,15 @@
         <v>7</v>
       </c>
       <c r="E13" s="0" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="0">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="C14" s="0" t="s">
         <v>6</v>
@@ -552,10 +565,10 @@
     </row>
     <row r="15">
       <c r="A15" s="0">
-        <v>19</v>
+        <v>28</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="C15" s="0" t="s">
         <v>6</v>
@@ -569,10 +582,10 @@
     </row>
     <row r="16">
       <c r="A16" s="0">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="C16" s="0" t="s">
         <v>6</v>
@@ -586,10 +599,10 @@
     </row>
     <row r="17">
       <c r="A17" s="0">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="C17" s="0" t="s">
         <v>6</v>
@@ -603,10 +616,10 @@
     </row>
     <row r="18">
       <c r="A18" s="0">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="C18" s="0" t="s">
         <v>6</v>
@@ -620,10 +633,10 @@
     </row>
     <row r="19">
       <c r="A19" s="0">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="C19" s="0" t="s">
         <v>6</v>
@@ -637,10 +650,10 @@
     </row>
     <row r="20">
       <c r="A20" s="0">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="C20" s="0" t="s">
         <v>6</v>
@@ -654,10 +667,10 @@
     </row>
     <row r="21">
       <c r="A21" s="0">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="C21" s="0" t="s">
         <v>6</v>
@@ -671,10 +684,10 @@
     </row>
     <row r="22">
       <c r="A22" s="0">
-        <v>43</v>
+        <v>26</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="C22" s="0" t="s">
         <v>6</v>
@@ -683,15 +696,15 @@
         <v>7</v>
       </c>
       <c r="E22" s="0" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="0">
-        <v>29</v>
+        <v>43</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="C23" s="0" t="s">
         <v>6</v>
@@ -700,24 +713,41 @@
         <v>7</v>
       </c>
       <c r="E23" s="0" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="0">
+        <v>29</v>
+      </c>
+      <c r="B24" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="C24" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D24" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E24" s="0" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="0">
         <v>47</v>
       </c>
-      <c r="B24" s="0" t="s">
-        <v>33</v>
-      </c>
-      <c r="C24" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="D24" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="E24" s="0" t="s">
-        <v>34</v>
+      <c r="B25" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="C25" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D25" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E25" s="0" t="s">
+        <v>38</v>
       </c>
     </row>
   </sheetData>
@@ -727,7 +757,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:F22"/>
+  <dimension ref="A1:F23"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -750,144 +780,144 @@
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="0">
-        <v>48</v>
+        <v>33</v>
       </c>
       <c r="B2" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="D2" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2" s="0" t="s">
         <v>22</v>
-      </c>
-      <c r="C2" s="0" t="s">
-        <v>35</v>
-      </c>
-      <c r="D2" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="E2" s="0" t="s">
-        <v>23</v>
-      </c>
-      <c r="F2" s="0" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="0">
-        <v>37</v>
+        <v>48</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>11</v>
+        <v>40</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="D3" s="0" t="s">
         <v>7</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="F3" s="0" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="0">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="D4" s="0" t="s">
         <v>7</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="F4" s="0" t="s">
-        <v>34</v>
+        <v>17</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="0">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>37</v>
+        <v>42</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="D5" s="0" t="s">
         <v>7</v>
       </c>
       <c r="E5" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="F5" s="0" t="s">
         <v>38</v>
-      </c>
-      <c r="F5" s="0" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="0">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="D6" s="0" t="s">
         <v>7</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>14</v>
+        <v>44</v>
       </c>
       <c r="F6" s="0" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="0">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="D7" s="0" t="s">
         <v>7</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="F7" s="0" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="0">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="D8" s="0" t="s">
         <v>7</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="F8" s="0" t="s">
         <v>38</v>
@@ -895,13 +925,13 @@
     </row>
     <row r="9">
       <c r="A9" s="0">
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="D9" s="0" t="s">
         <v>7</v>
@@ -910,84 +940,84 @@
         <v>12</v>
       </c>
       <c r="F9" s="0" t="s">
-        <v>38</v>
+        <v>44</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="0">
-        <v>11</v>
+        <v>36</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="D10" s="0" t="s">
         <v>7</v>
       </c>
       <c r="E10" s="0" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="F10" s="0" t="s">
-        <v>14</v>
+        <v>44</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="0">
-        <v>40</v>
+        <v>11</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>44</v>
+        <v>49</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="D11" s="0" t="s">
         <v>7</v>
       </c>
       <c r="E11" s="0" t="s">
-        <v>45</v>
+        <v>8</v>
       </c>
       <c r="F11" s="0" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="0">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="D12" s="0" t="s">
         <v>7</v>
       </c>
       <c r="E12" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="F12" s="0" t="s">
         <v>12</v>
-      </c>
-      <c r="F12" s="0" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="0">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>47</v>
+        <v>52</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="D13" s="0" t="s">
         <v>7</v>
       </c>
       <c r="E13" s="0" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="F13" s="0" t="s">
         <v>12</v>
@@ -995,13 +1025,13 @@
     </row>
     <row r="14">
       <c r="A14" s="0">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="D14" s="0" t="s">
         <v>7</v>
@@ -1010,24 +1040,24 @@
         <v>10</v>
       </c>
       <c r="F14" s="0" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="0">
-        <v>20</v>
+        <v>31</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>49</v>
+        <v>54</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="D15" s="0" t="s">
         <v>7</v>
       </c>
       <c r="E15" s="0" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="F15" s="0" t="s">
         <v>10</v>
@@ -1035,13 +1065,13 @@
     </row>
     <row r="16">
       <c r="A16" s="0">
-        <v>9</v>
+        <v>20</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>50</v>
+        <v>55</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="D16" s="0" t="s">
         <v>7</v>
@@ -1055,13 +1085,13 @@
     </row>
     <row r="17">
       <c r="A17" s="0">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>51</v>
+        <v>56</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="D17" s="0" t="s">
         <v>7</v>
@@ -1075,13 +1105,13 @@
     </row>
     <row r="18">
       <c r="A18" s="0">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="D18" s="0" t="s">
         <v>7</v>
@@ -1090,18 +1120,18 @@
         <v>8</v>
       </c>
       <c r="F18" s="0" t="s">
-        <v>53</v>
+        <v>10</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="0">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="D19" s="0" t="s">
         <v>7</v>
@@ -1110,18 +1140,18 @@
         <v>8</v>
       </c>
       <c r="F19" s="0" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="0">
-        <v>30</v>
+        <v>3</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="C20" s="0" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="D20" s="0" t="s">
         <v>7</v>
@@ -1135,13 +1165,13 @@
     </row>
     <row r="21">
       <c r="A21" s="0">
-        <v>2</v>
+        <v>30</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
       <c r="C21" s="0" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="D21" s="0" t="s">
         <v>7</v>
@@ -1155,21 +1185,41 @@
     </row>
     <row r="22">
       <c r="A22" s="0">
+        <v>2</v>
+      </c>
+      <c r="B22" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="C22" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="D22" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E22" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="F22" s="0" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="0">
         <v>1</v>
       </c>
-      <c r="B22" s="0" t="s">
-        <v>57</v>
-      </c>
-      <c r="C22" s="0" t="s">
-        <v>35</v>
-      </c>
-      <c r="D22" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="E22" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="F22" s="0" t="s">
+      <c r="B23" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="C23" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="D23" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E23" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="F23" s="0" t="s">
         <v>8</v>
       </c>
     </row>
@@ -1191,7 +1241,7 @@
         <v>2</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>58</v>
+        <v>64</v>
       </c>
       <c r="C1" s="2"/>
       <c r="D1" s="2" t="s">
@@ -1199,7 +1249,7 @@
       </c>
       <c r="E1" s="2"/>
       <c r="F1" s="2" t="s">
-        <v>59</v>
+        <v>65</v>
       </c>
     </row>
     <row r="2">
@@ -1207,24 +1257,24 @@
         <v>6</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>58</v>
+        <v>64</v>
       </c>
       <c r="D2" s="0" t="s">
         <v>7</v>
       </c>
       <c r="F2" s="0">
-        <v>51</v>
+        <v>53</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="0" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>60</v>
+        <v>66</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>61</v>
+        <v>67</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
bug fix: palette panel overlapping image and status panel
</commit_message>
<xml_diff>
--- a/paint_todo.xlsx
+++ b/paint_todo.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="69">
   <si>
     <t>Id</t>
   </si>
@@ -266,6 +266,11 @@
   </si>
   <si>
     <t>Bug</t>
+  </si>
+  <si>
+    <t xml:space="preserve">make a MasterImage class
+that one-time figures out all the regions in a background thread
+and provides that data to the color worker</t>
   </si>
 </sst>
 </file>
@@ -361,10 +366,10 @@
     </row>
     <row r="3">
       <c r="A3" s="0">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C3" s="0" t="s">
         <v>6</v>
@@ -373,15 +378,15 @@
         <v>7</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="0">
-        <v>35</v>
+        <v>13</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C4" s="0" t="s">
         <v>6</v>
@@ -390,15 +395,15 @@
         <v>7</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="0">
-        <v>13</v>
+        <v>50</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C5" s="0" t="s">
         <v>6</v>
@@ -407,15 +412,15 @@
         <v>7</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="0">
-        <v>50</v>
+        <v>34</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C6" s="0" t="s">
         <v>6</v>
@@ -424,15 +429,15 @@
         <v>7</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="0">
-        <v>34</v>
+        <v>49</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C7" s="0" t="s">
         <v>6</v>
@@ -441,15 +446,15 @@
         <v>7</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="0">
-        <v>49</v>
+        <v>21</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C8" s="0" t="s">
         <v>6</v>
@@ -458,15 +463,15 @@
         <v>7</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>17</v>
+        <v>8</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="0">
-        <v>21</v>
+        <v>54</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>20</v>
+        <v>68</v>
       </c>
       <c r="C9" s="0" t="s">
         <v>6</v>
@@ -475,7 +480,7 @@
         <v>7</v>
       </c>
       <c r="E9" s="0" t="s">
-        <v>8</v>
+        <v>22</v>
       </c>
     </row>
     <row r="10">
@@ -757,7 +762,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:F23"/>
+  <dimension ref="A1:F24"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -785,10 +790,10 @@
     </row>
     <row r="2">
       <c r="A2" s="0">
-        <v>33</v>
+        <v>42</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C2" s="0" t="s">
         <v>39</v>
@@ -797,7 +802,7 @@
         <v>7</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="F2" s="0" t="s">
         <v>22</v>
@@ -805,10 +810,10 @@
     </row>
     <row r="3">
       <c r="A3" s="0">
-        <v>48</v>
+        <v>33</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>40</v>
+        <v>9</v>
       </c>
       <c r="C3" s="0" t="s">
         <v>39</v>
@@ -817,18 +822,18 @@
         <v>7</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="F3" s="0" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="0">
-        <v>37</v>
+        <v>48</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C4" s="0" t="s">
         <v>39</v>
@@ -837,7 +842,7 @@
         <v>7</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="F4" s="0" t="s">
         <v>17</v>
@@ -845,10 +850,10 @@
     </row>
     <row r="5">
       <c r="A5" s="0">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C5" s="0" t="s">
         <v>39</v>
@@ -860,15 +865,15 @@
         <v>14</v>
       </c>
       <c r="F5" s="0" t="s">
-        <v>38</v>
+        <v>17</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="0">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C6" s="0" t="s">
         <v>39</v>
@@ -877,7 +882,7 @@
         <v>7</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>44</v>
+        <v>14</v>
       </c>
       <c r="F6" s="0" t="s">
         <v>38</v>
@@ -885,10 +890,10 @@
     </row>
     <row r="7">
       <c r="A7" s="0">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C7" s="0" t="s">
         <v>39</v>
@@ -897,7 +902,7 @@
         <v>7</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>12</v>
+        <v>44</v>
       </c>
       <c r="F7" s="0" t="s">
         <v>38</v>
@@ -905,10 +910,10 @@
     </row>
     <row r="8">
       <c r="A8" s="0">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C8" s="0" t="s">
         <v>39</v>
@@ -925,10 +930,10 @@
     </row>
     <row r="9">
       <c r="A9" s="0">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C9" s="0" t="s">
         <v>39</v>
@@ -940,15 +945,15 @@
         <v>12</v>
       </c>
       <c r="F9" s="0" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="0">
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C10" s="0" t="s">
         <v>39</v>
@@ -957,7 +962,7 @@
         <v>7</v>
       </c>
       <c r="E10" s="0" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="F10" s="0" t="s">
         <v>44</v>
@@ -965,10 +970,10 @@
     </row>
     <row r="11">
       <c r="A11" s="0">
-        <v>11</v>
+        <v>36</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C11" s="0" t="s">
         <v>39</v>
@@ -977,18 +982,18 @@
         <v>7</v>
       </c>
       <c r="E11" s="0" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="F11" s="0" t="s">
-        <v>12</v>
+        <v>44</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="0">
-        <v>40</v>
+        <v>11</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C12" s="0" t="s">
         <v>39</v>
@@ -997,7 +1002,7 @@
         <v>7</v>
       </c>
       <c r="E12" s="0" t="s">
-        <v>51</v>
+        <v>8</v>
       </c>
       <c r="F12" s="0" t="s">
         <v>12</v>
@@ -1005,10 +1010,10 @@
     </row>
     <row r="13">
       <c r="A13" s="0">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C13" s="0" t="s">
         <v>39</v>
@@ -1017,7 +1022,7 @@
         <v>7</v>
       </c>
       <c r="E13" s="0" t="s">
-        <v>14</v>
+        <v>51</v>
       </c>
       <c r="F13" s="0" t="s">
         <v>12</v>
@@ -1025,10 +1030,10 @@
     </row>
     <row r="14">
       <c r="A14" s="0">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C14" s="0" t="s">
         <v>39</v>
@@ -1037,18 +1042,18 @@
         <v>7</v>
       </c>
       <c r="E14" s="0" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="F14" s="0" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="0">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C15" s="0" t="s">
         <v>39</v>
@@ -1060,15 +1065,15 @@
         <v>10</v>
       </c>
       <c r="F15" s="0" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="0">
-        <v>20</v>
+        <v>31</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C16" s="0" t="s">
         <v>39</v>
@@ -1077,7 +1082,7 @@
         <v>7</v>
       </c>
       <c r="E16" s="0" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="F16" s="0" t="s">
         <v>10</v>
@@ -1085,10 +1090,10 @@
     </row>
     <row r="17">
       <c r="A17" s="0">
-        <v>9</v>
+        <v>20</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C17" s="0" t="s">
         <v>39</v>
@@ -1105,10 +1110,10 @@
     </row>
     <row r="18">
       <c r="A18" s="0">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C18" s="0" t="s">
         <v>39</v>
@@ -1125,10 +1130,10 @@
     </row>
     <row r="19">
       <c r="A19" s="0">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C19" s="0" t="s">
         <v>39</v>
@@ -1140,15 +1145,15 @@
         <v>8</v>
       </c>
       <c r="F19" s="0" t="s">
-        <v>59</v>
+        <v>10</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="0">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C20" s="0" t="s">
         <v>39</v>
@@ -1160,15 +1165,15 @@
         <v>8</v>
       </c>
       <c r="F20" s="0" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="0">
-        <v>30</v>
+        <v>3</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C21" s="0" t="s">
         <v>39</v>
@@ -1185,10 +1190,10 @@
     </row>
     <row r="22">
       <c r="A22" s="0">
-        <v>2</v>
+        <v>30</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C22" s="0" t="s">
         <v>39</v>
@@ -1205,21 +1210,41 @@
     </row>
     <row r="23">
       <c r="A23" s="0">
+        <v>2</v>
+      </c>
+      <c r="B23" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="C23" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="D23" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E23" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="F23" s="0" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="0">
         <v>1</v>
       </c>
-      <c r="B23" s="0" t="s">
+      <c r="B24" s="0" t="s">
         <v>63</v>
       </c>
-      <c r="C23" s="0" t="s">
-        <v>39</v>
-      </c>
-      <c r="D23" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="E23" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="F23" s="0" t="s">
+      <c r="C24" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="D24" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E24" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="F24" s="0" t="s">
         <v>8</v>
       </c>
     </row>
@@ -1263,7 +1288,7 @@
         <v>7</v>
       </c>
       <c r="F2" s="0">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row r="3">

</xml_diff>

<commit_message>
add color to palette
</commit_message>
<xml_diff>
--- a/paint_todo.xlsx
+++ b/paint_todo.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="86">
   <si>
     <t>Id</t>
   </si>
@@ -302,6 +302,36 @@
   <si>
     <t xml:space="preserve">New Color Dialog
 - have Saturation/Value trackbars both start in upper-left at black</t>
+  </si>
+  <si>
+    <t xml:space="preserve">edit palette: save changes
+see updates in main form
+- save or lose changes on close</t>
+  </si>
+  <si>
+    <t>edit palette: remove color</t>
+  </si>
+  <si>
+    <t>edit palette: edit color in place</t>
+  </si>
+  <si>
+    <t>edit palette: reorder</t>
+  </si>
+  <si>
+    <t>edit palette: undo/redo all changes</t>
+  </si>
+  <si>
+    <t>new color: enter an rgb value</t>
+  </si>
+  <si>
+    <t>new color: enter a hexadecimal value</t>
+  </si>
+  <si>
+    <t>new color: enter an hsv value</t>
+  </si>
+  <si>
+    <t xml:space="preserve">open edit palette mode
+- add swatches</t>
   </si>
 </sst>
 </file>
@@ -354,7 +384,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:F32"/>
+  <dimension ref="A1:F39"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -414,10 +444,10 @@
     </row>
     <row r="4">
       <c r="A4" s="0">
-        <v>13</v>
+        <v>62</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>15</v>
+        <v>77</v>
       </c>
       <c r="C4" s="0" t="s">
         <v>6</v>
@@ -426,15 +456,15 @@
         <v>7</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>8</v>
+        <v>72</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="0">
-        <v>55</v>
+        <v>63</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>69</v>
+        <v>78</v>
       </c>
       <c r="C5" s="0" t="s">
         <v>6</v>
@@ -443,15 +473,15 @@
         <v>7</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>22</v>
+        <v>72</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="0">
-        <v>50</v>
+        <v>64</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>16</v>
+        <v>79</v>
       </c>
       <c r="C6" s="0" t="s">
         <v>6</v>
@@ -460,15 +490,15 @@
         <v>7</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>17</v>
+        <v>72</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="0">
-        <v>34</v>
+        <v>65</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>18</v>
+        <v>80</v>
       </c>
       <c r="C7" s="0" t="s">
         <v>6</v>
@@ -477,15 +507,15 @@
         <v>7</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>10</v>
+        <v>72</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="0">
-        <v>59</v>
+        <v>66</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>74</v>
+        <v>81</v>
       </c>
       <c r="C8" s="0" t="s">
         <v>6</v>
@@ -499,10 +529,10 @@
     </row>
     <row r="9">
       <c r="A9" s="0">
-        <v>49</v>
+        <v>67</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>19</v>
+        <v>82</v>
       </c>
       <c r="C9" s="0" t="s">
         <v>6</v>
@@ -511,15 +541,15 @@
         <v>7</v>
       </c>
       <c r="E9" s="0" t="s">
-        <v>17</v>
+        <v>72</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="0">
-        <v>56</v>
+        <v>68</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>70</v>
+        <v>83</v>
       </c>
       <c r="C10" s="0" t="s">
         <v>6</v>
@@ -528,15 +558,15 @@
         <v>7</v>
       </c>
       <c r="E10" s="0" t="s">
-        <v>22</v>
+        <v>72</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="0">
-        <v>21</v>
+        <v>69</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>20</v>
+        <v>84</v>
       </c>
       <c r="C11" s="0" t="s">
         <v>6</v>
@@ -545,15 +575,15 @@
         <v>7</v>
       </c>
       <c r="E11" s="0" t="s">
-        <v>8</v>
+        <v>72</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="0">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="C12" s="0" t="s">
         <v>6</v>
@@ -567,10 +597,10 @@
     </row>
     <row r="13">
       <c r="A13" s="0">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="C13" s="0" t="s">
         <v>6</v>
@@ -579,15 +609,15 @@
         <v>7</v>
       </c>
       <c r="E13" s="0" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="0">
-        <v>51</v>
+        <v>34</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="C14" s="0" t="s">
         <v>6</v>
@@ -596,15 +626,15 @@
         <v>7</v>
       </c>
       <c r="E14" s="0" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="0">
-        <v>24</v>
+        <v>59</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>24</v>
+        <v>74</v>
       </c>
       <c r="C15" s="0" t="s">
         <v>6</v>
@@ -613,15 +643,15 @@
         <v>7</v>
       </c>
       <c r="E15" s="0" t="s">
-        <v>8</v>
+        <v>72</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="0">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="C16" s="0" t="s">
         <v>6</v>
@@ -635,10 +665,10 @@
     </row>
     <row r="17">
       <c r="A17" s="0">
-        <v>27</v>
+        <v>56</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>26</v>
+        <v>70</v>
       </c>
       <c r="C17" s="0" t="s">
         <v>6</v>
@@ -647,15 +677,15 @@
         <v>7</v>
       </c>
       <c r="E17" s="0" t="s">
-        <v>8</v>
+        <v>22</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="0">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="C18" s="0" t="s">
         <v>6</v>
@@ -669,10 +699,10 @@
     </row>
     <row r="19">
       <c r="A19" s="0">
-        <v>19</v>
+        <v>54</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>28</v>
+        <v>68</v>
       </c>
       <c r="C19" s="0" t="s">
         <v>6</v>
@@ -681,32 +711,32 @@
         <v>7</v>
       </c>
       <c r="E19" s="0" t="s">
-        <v>8</v>
+        <v>22</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="0">
+        <v>53</v>
+      </c>
+      <c r="B20" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="C20" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D20" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E20" s="0" t="s">
         <v>22</v>
-      </c>
-      <c r="B20" s="0" t="s">
-        <v>29</v>
-      </c>
-      <c r="C20" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="D20" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="E20" s="0" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="0">
-        <v>16</v>
+        <v>51</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="C21" s="0" t="s">
         <v>6</v>
@@ -715,15 +745,15 @@
         <v>7</v>
       </c>
       <c r="E21" s="0" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="0">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="C22" s="0" t="s">
         <v>6</v>
@@ -737,10 +767,10 @@
     </row>
     <row r="23">
       <c r="A23" s="0">
-        <v>18</v>
+        <v>52</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="C23" s="0" t="s">
         <v>6</v>
@@ -749,15 +779,15 @@
         <v>7</v>
       </c>
       <c r="E23" s="0" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="0">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="C24" s="0" t="s">
         <v>6</v>
@@ -771,10 +801,10 @@
     </row>
     <row r="25">
       <c r="A25" s="0">
-        <v>57</v>
+        <v>28</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>71</v>
+        <v>27</v>
       </c>
       <c r="C25" s="0" t="s">
         <v>6</v>
@@ -783,15 +813,15 @@
         <v>7</v>
       </c>
       <c r="E25" s="0" t="s">
-        <v>72</v>
+        <v>8</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="0">
-        <v>58</v>
+        <v>19</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>73</v>
+        <v>28</v>
       </c>
       <c r="C26" s="0" t="s">
         <v>6</v>
@@ -800,15 +830,15 @@
         <v>7</v>
       </c>
       <c r="E26" s="0" t="s">
-        <v>72</v>
+        <v>8</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="0">
-        <v>61</v>
+        <v>22</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>76</v>
+        <v>29</v>
       </c>
       <c r="C27" s="0" t="s">
         <v>6</v>
@@ -817,15 +847,15 @@
         <v>7</v>
       </c>
       <c r="E27" s="0" t="s">
-        <v>72</v>
+        <v>8</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="0">
-        <v>26</v>
+        <v>16</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="C28" s="0" t="s">
         <v>6</v>
@@ -839,10 +869,10 @@
     </row>
     <row r="29">
       <c r="A29" s="0">
-        <v>43</v>
+        <v>17</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="C29" s="0" t="s">
         <v>6</v>
@@ -851,15 +881,15 @@
         <v>7</v>
       </c>
       <c r="E29" s="0" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="0">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="B30" s="0" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="C30" s="0" t="s">
         <v>6</v>
@@ -873,10 +903,10 @@
     </row>
     <row r="31">
       <c r="A31" s="0">
-        <v>47</v>
+        <v>25</v>
       </c>
       <c r="B31" s="0" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="C31" s="0" t="s">
         <v>6</v>
@@ -885,23 +915,142 @@
         <v>7</v>
       </c>
       <c r="E31" s="0" t="s">
-        <v>38</v>
+        <v>8</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="0">
+        <v>57</v>
+      </c>
+      <c r="B32" s="0" t="s">
+        <v>71</v>
+      </c>
+      <c r="C32" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D32" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E32" s="0" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="0">
+        <v>58</v>
+      </c>
+      <c r="B33" s="0" t="s">
+        <v>73</v>
+      </c>
+      <c r="C33" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D33" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E33" s="0" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="0">
+        <v>61</v>
+      </c>
+      <c r="B34" s="0" t="s">
+        <v>76</v>
+      </c>
+      <c r="C34" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D34" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E34" s="0" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="0">
+        <v>26</v>
+      </c>
+      <c r="B35" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="C35" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D35" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E35" s="0" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="0">
+        <v>43</v>
+      </c>
+      <c r="B36" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="C36" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D36" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E36" s="0" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" s="0">
+        <v>29</v>
+      </c>
+      <c r="B37" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="C37" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D37" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E37" s="0" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" s="0">
+        <v>47</v>
+      </c>
+      <c r="B38" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="C38" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D38" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E38" s="0" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" s="0">
         <v>60</v>
       </c>
-      <c r="B32" s="0" t="s">
+      <c r="B39" s="0" t="s">
         <v>75</v>
       </c>
-      <c r="C32" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="D32" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="E32" s="0" t="s">
+      <c r="C39" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D39" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E39" s="0" t="s">
         <v>72</v>
       </c>
     </row>
@@ -912,7 +1061,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:F24"/>
+  <dimension ref="A1:F25"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -940,10 +1089,10 @@
     </row>
     <row r="2">
       <c r="A2" s="0">
-        <v>42</v>
+        <v>13</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>11</v>
+        <v>85</v>
       </c>
       <c r="C2" s="0" t="s">
         <v>39</v>
@@ -952,18 +1101,18 @@
         <v>7</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>22</v>
+        <v>72</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="0">
-        <v>33</v>
+        <v>42</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C3" s="0" t="s">
         <v>39</v>
@@ -972,7 +1121,7 @@
         <v>7</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="F3" s="0" t="s">
         <v>22</v>
@@ -980,10 +1129,10 @@
     </row>
     <row r="4">
       <c r="A4" s="0">
-        <v>48</v>
+        <v>33</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>40</v>
+        <v>9</v>
       </c>
       <c r="C4" s="0" t="s">
         <v>39</v>
@@ -992,18 +1141,18 @@
         <v>7</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="F4" s="0" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="0">
-        <v>37</v>
+        <v>48</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C5" s="0" t="s">
         <v>39</v>
@@ -1012,7 +1161,7 @@
         <v>7</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="F5" s="0" t="s">
         <v>17</v>
@@ -1020,10 +1169,10 @@
     </row>
     <row r="6">
       <c r="A6" s="0">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C6" s="0" t="s">
         <v>39</v>
@@ -1035,15 +1184,15 @@
         <v>14</v>
       </c>
       <c r="F6" s="0" t="s">
-        <v>38</v>
+        <v>17</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="0">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C7" s="0" t="s">
         <v>39</v>
@@ -1052,7 +1201,7 @@
         <v>7</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>44</v>
+        <v>14</v>
       </c>
       <c r="F7" s="0" t="s">
         <v>38</v>
@@ -1060,10 +1209,10 @@
     </row>
     <row r="8">
       <c r="A8" s="0">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C8" s="0" t="s">
         <v>39</v>
@@ -1072,7 +1221,7 @@
         <v>7</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>12</v>
+        <v>44</v>
       </c>
       <c r="F8" s="0" t="s">
         <v>38</v>
@@ -1080,10 +1229,10 @@
     </row>
     <row r="9">
       <c r="A9" s="0">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C9" s="0" t="s">
         <v>39</v>
@@ -1100,10 +1249,10 @@
     </row>
     <row r="10">
       <c r="A10" s="0">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C10" s="0" t="s">
         <v>39</v>
@@ -1115,15 +1264,15 @@
         <v>12</v>
       </c>
       <c r="F10" s="0" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="0">
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C11" s="0" t="s">
         <v>39</v>
@@ -1132,7 +1281,7 @@
         <v>7</v>
       </c>
       <c r="E11" s="0" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="F11" s="0" t="s">
         <v>44</v>
@@ -1140,10 +1289,10 @@
     </row>
     <row r="12">
       <c r="A12" s="0">
-        <v>11</v>
+        <v>36</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C12" s="0" t="s">
         <v>39</v>
@@ -1152,18 +1301,18 @@
         <v>7</v>
       </c>
       <c r="E12" s="0" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="F12" s="0" t="s">
-        <v>12</v>
+        <v>44</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="0">
-        <v>40</v>
+        <v>11</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C13" s="0" t="s">
         <v>39</v>
@@ -1172,7 +1321,7 @@
         <v>7</v>
       </c>
       <c r="E13" s="0" t="s">
-        <v>51</v>
+        <v>8</v>
       </c>
       <c r="F13" s="0" t="s">
         <v>12</v>
@@ -1180,10 +1329,10 @@
     </row>
     <row r="14">
       <c r="A14" s="0">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C14" s="0" t="s">
         <v>39</v>
@@ -1192,7 +1341,7 @@
         <v>7</v>
       </c>
       <c r="E14" s="0" t="s">
-        <v>14</v>
+        <v>51</v>
       </c>
       <c r="F14" s="0" t="s">
         <v>12</v>
@@ -1200,10 +1349,10 @@
     </row>
     <row r="15">
       <c r="A15" s="0">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C15" s="0" t="s">
         <v>39</v>
@@ -1212,18 +1361,18 @@
         <v>7</v>
       </c>
       <c r="E15" s="0" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="F15" s="0" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="0">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C16" s="0" t="s">
         <v>39</v>
@@ -1235,15 +1384,15 @@
         <v>10</v>
       </c>
       <c r="F16" s="0" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="0">
-        <v>20</v>
+        <v>31</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C17" s="0" t="s">
         <v>39</v>
@@ -1252,7 +1401,7 @@
         <v>7</v>
       </c>
       <c r="E17" s="0" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="F17" s="0" t="s">
         <v>10</v>
@@ -1260,10 +1409,10 @@
     </row>
     <row r="18">
       <c r="A18" s="0">
-        <v>9</v>
+        <v>20</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C18" s="0" t="s">
         <v>39</v>
@@ -1280,10 +1429,10 @@
     </row>
     <row r="19">
       <c r="A19" s="0">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C19" s="0" t="s">
         <v>39</v>
@@ -1300,10 +1449,10 @@
     </row>
     <row r="20">
       <c r="A20" s="0">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C20" s="0" t="s">
         <v>39</v>
@@ -1315,15 +1464,15 @@
         <v>8</v>
       </c>
       <c r="F20" s="0" t="s">
-        <v>59</v>
+        <v>10</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="0">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C21" s="0" t="s">
         <v>39</v>
@@ -1335,15 +1484,15 @@
         <v>8</v>
       </c>
       <c r="F21" s="0" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="0">
-        <v>30</v>
+        <v>3</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C22" s="0" t="s">
         <v>39</v>
@@ -1360,10 +1509,10 @@
     </row>
     <row r="23">
       <c r="A23" s="0">
-        <v>2</v>
+        <v>30</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C23" s="0" t="s">
         <v>39</v>
@@ -1380,21 +1529,41 @@
     </row>
     <row r="24">
       <c r="A24" s="0">
+        <v>2</v>
+      </c>
+      <c r="B24" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="C24" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="D24" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E24" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="F24" s="0" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="0">
         <v>1</v>
       </c>
-      <c r="B24" s="0" t="s">
+      <c r="B25" s="0" t="s">
         <v>63</v>
       </c>
-      <c r="C24" s="0" t="s">
-        <v>39</v>
-      </c>
-      <c r="D24" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="E24" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="F24" s="0" t="s">
+      <c r="C25" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="D25" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E25" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="F25" s="0" t="s">
         <v>8</v>
       </c>
     </row>
@@ -1438,7 +1607,7 @@
         <v>7</v>
       </c>
       <c r="F2" s="0">
-        <v>61</v>
+        <v>69</v>
       </c>
     </row>
     <row r="3">

</xml_diff>

<commit_message>
color palette: remove color
</commit_message>
<xml_diff>
--- a/paint_todo.xlsx
+++ b/paint_todo.xlsx
@@ -384,7 +384,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:F39"/>
+  <dimension ref="A1:F38"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -461,10 +461,10 @@
     </row>
     <row r="5">
       <c r="A5" s="0">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="C5" s="0" t="s">
         <v>6</v>
@@ -478,10 +478,10 @@
     </row>
     <row r="6">
       <c r="A6" s="0">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C6" s="0" t="s">
         <v>6</v>
@@ -495,10 +495,10 @@
     </row>
     <row r="7">
       <c r="A7" s="0">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="C7" s="0" t="s">
         <v>6</v>
@@ -512,10 +512,10 @@
     </row>
     <row r="8">
       <c r="A8" s="0">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="C8" s="0" t="s">
         <v>6</v>
@@ -529,10 +529,10 @@
     </row>
     <row r="9">
       <c r="A9" s="0">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="C9" s="0" t="s">
         <v>6</v>
@@ -546,10 +546,10 @@
     </row>
     <row r="10">
       <c r="A10" s="0">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C10" s="0" t="s">
         <v>6</v>
@@ -563,11 +563,11 @@
     </row>
     <row r="11">
       <c r="A11" s="0">
+        <v>55</v>
+      </c>
+      <c r="B11" s="0" t="s">
         <v>69</v>
       </c>
-      <c r="B11" s="0" t="s">
-        <v>84</v>
-      </c>
       <c r="C11" s="0" t="s">
         <v>6</v>
       </c>
@@ -575,15 +575,15 @@
         <v>7</v>
       </c>
       <c r="E11" s="0" t="s">
-        <v>72</v>
+        <v>22</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="0">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>69</v>
+        <v>16</v>
       </c>
       <c r="C12" s="0" t="s">
         <v>6</v>
@@ -592,15 +592,15 @@
         <v>7</v>
       </c>
       <c r="E12" s="0" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="0">
-        <v>50</v>
+        <v>34</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C13" s="0" t="s">
         <v>6</v>
@@ -609,15 +609,15 @@
         <v>7</v>
       </c>
       <c r="E13" s="0" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="0">
-        <v>34</v>
+        <v>59</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>18</v>
+        <v>74</v>
       </c>
       <c r="C14" s="0" t="s">
         <v>6</v>
@@ -626,15 +626,15 @@
         <v>7</v>
       </c>
       <c r="E14" s="0" t="s">
-        <v>10</v>
+        <v>72</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="0">
-        <v>59</v>
+        <v>49</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>74</v>
+        <v>19</v>
       </c>
       <c r="C15" s="0" t="s">
         <v>6</v>
@@ -643,15 +643,15 @@
         <v>7</v>
       </c>
       <c r="E15" s="0" t="s">
-        <v>72</v>
+        <v>17</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="0">
-        <v>49</v>
+        <v>56</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>19</v>
+        <v>70</v>
       </c>
       <c r="C16" s="0" t="s">
         <v>6</v>
@@ -660,15 +660,15 @@
         <v>7</v>
       </c>
       <c r="E16" s="0" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="0">
-        <v>56</v>
+        <v>21</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>70</v>
+        <v>20</v>
       </c>
       <c r="C17" s="0" t="s">
         <v>6</v>
@@ -677,15 +677,15 @@
         <v>7</v>
       </c>
       <c r="E17" s="0" t="s">
-        <v>22</v>
+        <v>8</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="0">
-        <v>21</v>
+        <v>54</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>20</v>
+        <v>68</v>
       </c>
       <c r="C18" s="0" t="s">
         <v>6</v>
@@ -694,15 +694,15 @@
         <v>7</v>
       </c>
       <c r="E18" s="0" t="s">
-        <v>8</v>
+        <v>22</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="0">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>68</v>
+        <v>21</v>
       </c>
       <c r="C19" s="0" t="s">
         <v>6</v>
@@ -716,10 +716,10 @@
     </row>
     <row r="20">
       <c r="A20" s="0">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="C20" s="0" t="s">
         <v>6</v>
@@ -728,15 +728,15 @@
         <v>7</v>
       </c>
       <c r="E20" s="0" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="0">
-        <v>51</v>
+        <v>24</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C21" s="0" t="s">
         <v>6</v>
@@ -745,15 +745,15 @@
         <v>7</v>
       </c>
       <c r="E21" s="0" t="s">
-        <v>17</v>
+        <v>8</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="0">
-        <v>24</v>
+        <v>52</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C22" s="0" t="s">
         <v>6</v>
@@ -762,15 +762,15 @@
         <v>7</v>
       </c>
       <c r="E22" s="0" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="0">
-        <v>52</v>
+        <v>27</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C23" s="0" t="s">
         <v>6</v>
@@ -779,15 +779,15 @@
         <v>7</v>
       </c>
       <c r="E23" s="0" t="s">
-        <v>17</v>
+        <v>8</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="0">
+        <v>28</v>
+      </c>
+      <c r="B24" s="0" t="s">
         <v>27</v>
-      </c>
-      <c r="B24" s="0" t="s">
-        <v>26</v>
       </c>
       <c r="C24" s="0" t="s">
         <v>6</v>
@@ -801,10 +801,10 @@
     </row>
     <row r="25">
       <c r="A25" s="0">
+        <v>19</v>
+      </c>
+      <c r="B25" s="0" t="s">
         <v>28</v>
-      </c>
-      <c r="B25" s="0" t="s">
-        <v>27</v>
       </c>
       <c r="C25" s="0" t="s">
         <v>6</v>
@@ -818,10 +818,10 @@
     </row>
     <row r="26">
       <c r="A26" s="0">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C26" s="0" t="s">
         <v>6</v>
@@ -835,10 +835,10 @@
     </row>
     <row r="27">
       <c r="A27" s="0">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C27" s="0" t="s">
         <v>6</v>
@@ -852,10 +852,10 @@
     </row>
     <row r="28">
       <c r="A28" s="0">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C28" s="0" t="s">
         <v>6</v>
@@ -869,10 +869,10 @@
     </row>
     <row r="29">
       <c r="A29" s="0">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C29" s="0" t="s">
         <v>6</v>
@@ -886,10 +886,10 @@
     </row>
     <row r="30">
       <c r="A30" s="0">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="B30" s="0" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C30" s="0" t="s">
         <v>6</v>
@@ -903,10 +903,10 @@
     </row>
     <row r="31">
       <c r="A31" s="0">
-        <v>25</v>
+        <v>57</v>
       </c>
       <c r="B31" s="0" t="s">
-        <v>33</v>
+        <v>71</v>
       </c>
       <c r="C31" s="0" t="s">
         <v>6</v>
@@ -915,15 +915,15 @@
         <v>7</v>
       </c>
       <c r="E31" s="0" t="s">
-        <v>8</v>
+        <v>72</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="0">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B32" s="0" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="C32" s="0" t="s">
         <v>6</v>
@@ -937,10 +937,10 @@
     </row>
     <row r="33">
       <c r="A33" s="0">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="B33" s="0" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="C33" s="0" t="s">
         <v>6</v>
@@ -954,10 +954,10 @@
     </row>
     <row r="34">
       <c r="A34" s="0">
-        <v>61</v>
+        <v>26</v>
       </c>
       <c r="B34" s="0" t="s">
-        <v>76</v>
+        <v>34</v>
       </c>
       <c r="C34" s="0" t="s">
         <v>6</v>
@@ -966,15 +966,15 @@
         <v>7</v>
       </c>
       <c r="E34" s="0" t="s">
-        <v>72</v>
+        <v>8</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="0">
-        <v>26</v>
+        <v>43</v>
       </c>
       <c r="B35" s="0" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C35" s="0" t="s">
         <v>6</v>
@@ -983,15 +983,15 @@
         <v>7</v>
       </c>
       <c r="E35" s="0" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="0">
-        <v>43</v>
+        <v>29</v>
       </c>
       <c r="B36" s="0" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C36" s="0" t="s">
         <v>6</v>
@@ -1000,15 +1000,15 @@
         <v>7</v>
       </c>
       <c r="E36" s="0" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="0">
-        <v>29</v>
+        <v>47</v>
       </c>
       <c r="B37" s="0" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C37" s="0" t="s">
         <v>6</v>
@@ -1017,15 +1017,15 @@
         <v>7</v>
       </c>
       <c r="E37" s="0" t="s">
-        <v>8</v>
+        <v>38</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="0">
-        <v>47</v>
+        <v>60</v>
       </c>
       <c r="B38" s="0" t="s">
-        <v>37</v>
+        <v>75</v>
       </c>
       <c r="C38" s="0" t="s">
         <v>6</v>
@@ -1034,23 +1034,6 @@
         <v>7</v>
       </c>
       <c r="E38" s="0" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="39">
-      <c r="A39" s="0">
-        <v>60</v>
-      </c>
-      <c r="B39" s="0" t="s">
-        <v>75</v>
-      </c>
-      <c r="C39" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="D39" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="E39" s="0" t="s">
         <v>72</v>
       </c>
     </row>
@@ -1061,7 +1044,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:F25"/>
+  <dimension ref="A1:F26"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1089,10 +1072,10 @@
     </row>
     <row r="2">
       <c r="A2" s="0">
-        <v>13</v>
+        <v>63</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
       <c r="C2" s="0" t="s">
         <v>39</v>
@@ -1101,7 +1084,7 @@
         <v>7</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>8</v>
+        <v>72</v>
       </c>
       <c r="F2" s="0" t="s">
         <v>72</v>
@@ -1109,10 +1092,10 @@
     </row>
     <row r="3">
       <c r="A3" s="0">
-        <v>42</v>
+        <v>13</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>11</v>
+        <v>85</v>
       </c>
       <c r="C3" s="0" t="s">
         <v>39</v>
@@ -1121,18 +1104,18 @@
         <v>7</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="F3" s="0" t="s">
-        <v>22</v>
+        <v>72</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="0">
-        <v>33</v>
+        <v>42</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C4" s="0" t="s">
         <v>39</v>
@@ -1141,7 +1124,7 @@
         <v>7</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="F4" s="0" t="s">
         <v>22</v>
@@ -1149,10 +1132,10 @@
     </row>
     <row r="5">
       <c r="A5" s="0">
-        <v>48</v>
+        <v>33</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>40</v>
+        <v>9</v>
       </c>
       <c r="C5" s="0" t="s">
         <v>39</v>
@@ -1161,18 +1144,18 @@
         <v>7</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="F5" s="0" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="0">
-        <v>37</v>
+        <v>48</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C6" s="0" t="s">
         <v>39</v>
@@ -1181,7 +1164,7 @@
         <v>7</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="F6" s="0" t="s">
         <v>17</v>
@@ -1189,10 +1172,10 @@
     </row>
     <row r="7">
       <c r="A7" s="0">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C7" s="0" t="s">
         <v>39</v>
@@ -1204,15 +1187,15 @@
         <v>14</v>
       </c>
       <c r="F7" s="0" t="s">
-        <v>38</v>
+        <v>17</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="0">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C8" s="0" t="s">
         <v>39</v>
@@ -1221,7 +1204,7 @@
         <v>7</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>44</v>
+        <v>14</v>
       </c>
       <c r="F8" s="0" t="s">
         <v>38</v>
@@ -1229,10 +1212,10 @@
     </row>
     <row r="9">
       <c r="A9" s="0">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C9" s="0" t="s">
         <v>39</v>
@@ -1241,7 +1224,7 @@
         <v>7</v>
       </c>
       <c r="E9" s="0" t="s">
-        <v>12</v>
+        <v>44</v>
       </c>
       <c r="F9" s="0" t="s">
         <v>38</v>
@@ -1249,10 +1232,10 @@
     </row>
     <row r="10">
       <c r="A10" s="0">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C10" s="0" t="s">
         <v>39</v>
@@ -1269,10 +1252,10 @@
     </row>
     <row r="11">
       <c r="A11" s="0">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C11" s="0" t="s">
         <v>39</v>
@@ -1284,15 +1267,15 @@
         <v>12</v>
       </c>
       <c r="F11" s="0" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="0">
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C12" s="0" t="s">
         <v>39</v>
@@ -1301,7 +1284,7 @@
         <v>7</v>
       </c>
       <c r="E12" s="0" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="F12" s="0" t="s">
         <v>44</v>
@@ -1309,10 +1292,10 @@
     </row>
     <row r="13">
       <c r="A13" s="0">
-        <v>11</v>
+        <v>36</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C13" s="0" t="s">
         <v>39</v>
@@ -1321,18 +1304,18 @@
         <v>7</v>
       </c>
       <c r="E13" s="0" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="F13" s="0" t="s">
-        <v>12</v>
+        <v>44</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="0">
-        <v>40</v>
+        <v>11</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C14" s="0" t="s">
         <v>39</v>
@@ -1341,7 +1324,7 @@
         <v>7</v>
       </c>
       <c r="E14" s="0" t="s">
-        <v>51</v>
+        <v>8</v>
       </c>
       <c r="F14" s="0" t="s">
         <v>12</v>
@@ -1349,10 +1332,10 @@
     </row>
     <row r="15">
       <c r="A15" s="0">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C15" s="0" t="s">
         <v>39</v>
@@ -1361,7 +1344,7 @@
         <v>7</v>
       </c>
       <c r="E15" s="0" t="s">
-        <v>14</v>
+        <v>51</v>
       </c>
       <c r="F15" s="0" t="s">
         <v>12</v>
@@ -1369,10 +1352,10 @@
     </row>
     <row r="16">
       <c r="A16" s="0">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C16" s="0" t="s">
         <v>39</v>
@@ -1381,18 +1364,18 @@
         <v>7</v>
       </c>
       <c r="E16" s="0" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="F16" s="0" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="0">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C17" s="0" t="s">
         <v>39</v>
@@ -1404,15 +1387,15 @@
         <v>10</v>
       </c>
       <c r="F17" s="0" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="0">
-        <v>20</v>
+        <v>31</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C18" s="0" t="s">
         <v>39</v>
@@ -1421,7 +1404,7 @@
         <v>7</v>
       </c>
       <c r="E18" s="0" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="F18" s="0" t="s">
         <v>10</v>
@@ -1429,10 +1412,10 @@
     </row>
     <row r="19">
       <c r="A19" s="0">
-        <v>9</v>
+        <v>20</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C19" s="0" t="s">
         <v>39</v>
@@ -1449,10 +1432,10 @@
     </row>
     <row r="20">
       <c r="A20" s="0">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C20" s="0" t="s">
         <v>39</v>
@@ -1469,10 +1452,10 @@
     </row>
     <row r="21">
       <c r="A21" s="0">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C21" s="0" t="s">
         <v>39</v>
@@ -1484,15 +1467,15 @@
         <v>8</v>
       </c>
       <c r="F21" s="0" t="s">
-        <v>59</v>
+        <v>10</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="0">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C22" s="0" t="s">
         <v>39</v>
@@ -1504,15 +1487,15 @@
         <v>8</v>
       </c>
       <c r="F22" s="0" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="0">
-        <v>30</v>
+        <v>3</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C23" s="0" t="s">
         <v>39</v>
@@ -1529,10 +1512,10 @@
     </row>
     <row r="24">
       <c r="A24" s="0">
-        <v>2</v>
+        <v>30</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C24" s="0" t="s">
         <v>39</v>
@@ -1549,21 +1532,41 @@
     </row>
     <row r="25">
       <c r="A25" s="0">
+        <v>2</v>
+      </c>
+      <c r="B25" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="C25" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="D25" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E25" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="F25" s="0" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="0">
         <v>1</v>
       </c>
-      <c r="B25" s="0" t="s">
+      <c r="B26" s="0" t="s">
         <v>63</v>
       </c>
-      <c r="C25" s="0" t="s">
-        <v>39</v>
-      </c>
-      <c r="D25" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="E25" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="F25" s="0" t="s">
+      <c r="C26" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="D26" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E26" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="F26" s="0" t="s">
         <v>8</v>
       </c>
     </row>

</xml_diff>

<commit_message>
color palette: replace color
</commit_message>
<xml_diff>
--- a/paint_todo.xlsx
+++ b/paint_todo.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="87">
   <si>
     <t>Id</t>
   </si>
@@ -332,6 +332,9 @@
   <si>
     <t xml:space="preserve">open edit palette mode
 - add swatches</t>
+  </si>
+  <si>
+    <t>edit palette: add new color, but start from existing color</t>
   </si>
 </sst>
 </file>
@@ -461,10 +464,10 @@
     </row>
     <row r="5">
       <c r="A5" s="0">
-        <v>64</v>
+        <v>70</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>79</v>
+        <v>86</v>
       </c>
       <c r="C5" s="0" t="s">
         <v>6</v>
@@ -1044,7 +1047,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:F26"/>
+  <dimension ref="A1:F27"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1072,10 +1075,10 @@
     </row>
     <row r="2">
       <c r="A2" s="0">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="C2" s="0" t="s">
         <v>39</v>
@@ -1092,10 +1095,10 @@
     </row>
     <row r="3">
       <c r="A3" s="0">
-        <v>13</v>
+        <v>63</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
       <c r="C3" s="0" t="s">
         <v>39</v>
@@ -1104,7 +1107,7 @@
         <v>7</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>8</v>
+        <v>72</v>
       </c>
       <c r="F3" s="0" t="s">
         <v>72</v>
@@ -1112,10 +1115,10 @@
     </row>
     <row r="4">
       <c r="A4" s="0">
-        <v>42</v>
+        <v>13</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>11</v>
+        <v>85</v>
       </c>
       <c r="C4" s="0" t="s">
         <v>39</v>
@@ -1124,18 +1127,18 @@
         <v>7</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="F4" s="0" t="s">
-        <v>22</v>
+        <v>72</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="0">
-        <v>33</v>
+        <v>42</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C5" s="0" t="s">
         <v>39</v>
@@ -1144,7 +1147,7 @@
         <v>7</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="F5" s="0" t="s">
         <v>22</v>
@@ -1152,10 +1155,10 @@
     </row>
     <row r="6">
       <c r="A6" s="0">
-        <v>48</v>
+        <v>33</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>40</v>
+        <v>9</v>
       </c>
       <c r="C6" s="0" t="s">
         <v>39</v>
@@ -1164,18 +1167,18 @@
         <v>7</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="F6" s="0" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="0">
-        <v>37</v>
+        <v>48</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C7" s="0" t="s">
         <v>39</v>
@@ -1184,7 +1187,7 @@
         <v>7</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="F7" s="0" t="s">
         <v>17</v>
@@ -1192,10 +1195,10 @@
     </row>
     <row r="8">
       <c r="A8" s="0">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C8" s="0" t="s">
         <v>39</v>
@@ -1207,15 +1210,15 @@
         <v>14</v>
       </c>
       <c r="F8" s="0" t="s">
-        <v>38</v>
+        <v>17</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="0">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C9" s="0" t="s">
         <v>39</v>
@@ -1224,7 +1227,7 @@
         <v>7</v>
       </c>
       <c r="E9" s="0" t="s">
-        <v>44</v>
+        <v>14</v>
       </c>
       <c r="F9" s="0" t="s">
         <v>38</v>
@@ -1232,10 +1235,10 @@
     </row>
     <row r="10">
       <c r="A10" s="0">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C10" s="0" t="s">
         <v>39</v>
@@ -1244,7 +1247,7 @@
         <v>7</v>
       </c>
       <c r="E10" s="0" t="s">
-        <v>12</v>
+        <v>44</v>
       </c>
       <c r="F10" s="0" t="s">
         <v>38</v>
@@ -1252,10 +1255,10 @@
     </row>
     <row r="11">
       <c r="A11" s="0">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C11" s="0" t="s">
         <v>39</v>
@@ -1272,10 +1275,10 @@
     </row>
     <row r="12">
       <c r="A12" s="0">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C12" s="0" t="s">
         <v>39</v>
@@ -1287,15 +1290,15 @@
         <v>12</v>
       </c>
       <c r="F12" s="0" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="0">
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C13" s="0" t="s">
         <v>39</v>
@@ -1304,7 +1307,7 @@
         <v>7</v>
       </c>
       <c r="E13" s="0" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="F13" s="0" t="s">
         <v>44</v>
@@ -1312,10 +1315,10 @@
     </row>
     <row r="14">
       <c r="A14" s="0">
-        <v>11</v>
+        <v>36</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C14" s="0" t="s">
         <v>39</v>
@@ -1324,18 +1327,18 @@
         <v>7</v>
       </c>
       <c r="E14" s="0" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="F14" s="0" t="s">
-        <v>12</v>
+        <v>44</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="0">
-        <v>40</v>
+        <v>11</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C15" s="0" t="s">
         <v>39</v>
@@ -1344,7 +1347,7 @@
         <v>7</v>
       </c>
       <c r="E15" s="0" t="s">
-        <v>51</v>
+        <v>8</v>
       </c>
       <c r="F15" s="0" t="s">
         <v>12</v>
@@ -1352,10 +1355,10 @@
     </row>
     <row r="16">
       <c r="A16" s="0">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C16" s="0" t="s">
         <v>39</v>
@@ -1364,7 +1367,7 @@
         <v>7</v>
       </c>
       <c r="E16" s="0" t="s">
-        <v>14</v>
+        <v>51</v>
       </c>
       <c r="F16" s="0" t="s">
         <v>12</v>
@@ -1372,10 +1375,10 @@
     </row>
     <row r="17">
       <c r="A17" s="0">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C17" s="0" t="s">
         <v>39</v>
@@ -1384,18 +1387,18 @@
         <v>7</v>
       </c>
       <c r="E17" s="0" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="F17" s="0" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="0">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C18" s="0" t="s">
         <v>39</v>
@@ -1407,15 +1410,15 @@
         <v>10</v>
       </c>
       <c r="F18" s="0" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="0">
-        <v>20</v>
+        <v>31</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C19" s="0" t="s">
         <v>39</v>
@@ -1424,7 +1427,7 @@
         <v>7</v>
       </c>
       <c r="E19" s="0" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="F19" s="0" t="s">
         <v>10</v>
@@ -1432,10 +1435,10 @@
     </row>
     <row r="20">
       <c r="A20" s="0">
-        <v>9</v>
+        <v>20</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C20" s="0" t="s">
         <v>39</v>
@@ -1452,10 +1455,10 @@
     </row>
     <row r="21">
       <c r="A21" s="0">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C21" s="0" t="s">
         <v>39</v>
@@ -1472,10 +1475,10 @@
     </row>
     <row r="22">
       <c r="A22" s="0">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C22" s="0" t="s">
         <v>39</v>
@@ -1487,15 +1490,15 @@
         <v>8</v>
       </c>
       <c r="F22" s="0" t="s">
-        <v>59</v>
+        <v>10</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="0">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C23" s="0" t="s">
         <v>39</v>
@@ -1507,15 +1510,15 @@
         <v>8</v>
       </c>
       <c r="F23" s="0" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="0">
-        <v>30</v>
+        <v>3</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C24" s="0" t="s">
         <v>39</v>
@@ -1532,10 +1535,10 @@
     </row>
     <row r="25">
       <c r="A25" s="0">
-        <v>2</v>
+        <v>30</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C25" s="0" t="s">
         <v>39</v>
@@ -1552,21 +1555,41 @@
     </row>
     <row r="26">
       <c r="A26" s="0">
+        <v>2</v>
+      </c>
+      <c r="B26" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="C26" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="D26" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E26" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="F26" s="0" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="0">
         <v>1</v>
       </c>
-      <c r="B26" s="0" t="s">
+      <c r="B27" s="0" t="s">
         <v>63</v>
       </c>
-      <c r="C26" s="0" t="s">
-        <v>39</v>
-      </c>
-      <c r="D26" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="E26" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="F26" s="0" t="s">
+      <c r="C27" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="D27" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E27" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="F27" s="0" t="s">
         <v>8</v>
       </c>
     </row>
@@ -1610,7 +1633,7 @@
         <v>7</v>
       </c>
       <c r="F2" s="0">
-        <v>69</v>
+        <v>70</v>
       </c>
     </row>
     <row r="3">

</xml_diff>

<commit_message>
color palette: add new based on existing
</commit_message>
<xml_diff>
--- a/paint_todo.xlsx
+++ b/paint_todo.xlsx
@@ -387,7 +387,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:F38"/>
+  <dimension ref="A1:F37"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -464,10 +464,10 @@
     </row>
     <row r="5">
       <c r="A5" s="0">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="C5" s="0" t="s">
         <v>6</v>
@@ -481,10 +481,10 @@
     </row>
     <row r="6">
       <c r="A6" s="0">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="C6" s="0" t="s">
         <v>6</v>
@@ -498,10 +498,10 @@
     </row>
     <row r="7">
       <c r="A7" s="0">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="C7" s="0" t="s">
         <v>6</v>
@@ -515,10 +515,10 @@
     </row>
     <row r="8">
       <c r="A8" s="0">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="C8" s="0" t="s">
         <v>6</v>
@@ -532,10 +532,10 @@
     </row>
     <row r="9">
       <c r="A9" s="0">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C9" s="0" t="s">
         <v>6</v>
@@ -549,11 +549,11 @@
     </row>
     <row r="10">
       <c r="A10" s="0">
+        <v>55</v>
+      </c>
+      <c r="B10" s="0" t="s">
         <v>69</v>
       </c>
-      <c r="B10" s="0" t="s">
-        <v>84</v>
-      </c>
       <c r="C10" s="0" t="s">
         <v>6</v>
       </c>
@@ -561,15 +561,15 @@
         <v>7</v>
       </c>
       <c r="E10" s="0" t="s">
-        <v>72</v>
+        <v>22</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="0">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>69</v>
+        <v>16</v>
       </c>
       <c r="C11" s="0" t="s">
         <v>6</v>
@@ -578,15 +578,15 @@
         <v>7</v>
       </c>
       <c r="E11" s="0" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="0">
-        <v>50</v>
+        <v>34</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C12" s="0" t="s">
         <v>6</v>
@@ -595,15 +595,15 @@
         <v>7</v>
       </c>
       <c r="E12" s="0" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="0">
-        <v>34</v>
+        <v>59</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>18</v>
+        <v>74</v>
       </c>
       <c r="C13" s="0" t="s">
         <v>6</v>
@@ -612,15 +612,15 @@
         <v>7</v>
       </c>
       <c r="E13" s="0" t="s">
-        <v>10</v>
+        <v>72</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="0">
-        <v>59</v>
+        <v>49</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>74</v>
+        <v>19</v>
       </c>
       <c r="C14" s="0" t="s">
         <v>6</v>
@@ -629,15 +629,15 @@
         <v>7</v>
       </c>
       <c r="E14" s="0" t="s">
-        <v>72</v>
+        <v>17</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="0">
-        <v>49</v>
+        <v>56</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>19</v>
+        <v>70</v>
       </c>
       <c r="C15" s="0" t="s">
         <v>6</v>
@@ -646,15 +646,15 @@
         <v>7</v>
       </c>
       <c r="E15" s="0" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="0">
-        <v>56</v>
+        <v>21</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>70</v>
+        <v>20</v>
       </c>
       <c r="C16" s="0" t="s">
         <v>6</v>
@@ -663,15 +663,15 @@
         <v>7</v>
       </c>
       <c r="E16" s="0" t="s">
-        <v>22</v>
+        <v>8</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="0">
-        <v>21</v>
+        <v>54</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>20</v>
+        <v>68</v>
       </c>
       <c r="C17" s="0" t="s">
         <v>6</v>
@@ -680,15 +680,15 @@
         <v>7</v>
       </c>
       <c r="E17" s="0" t="s">
-        <v>8</v>
+        <v>22</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="0">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>68</v>
+        <v>21</v>
       </c>
       <c r="C18" s="0" t="s">
         <v>6</v>
@@ -702,10 +702,10 @@
     </row>
     <row r="19">
       <c r="A19" s="0">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="C19" s="0" t="s">
         <v>6</v>
@@ -714,15 +714,15 @@
         <v>7</v>
       </c>
       <c r="E19" s="0" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="0">
-        <v>51</v>
+        <v>24</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C20" s="0" t="s">
         <v>6</v>
@@ -731,15 +731,15 @@
         <v>7</v>
       </c>
       <c r="E20" s="0" t="s">
-        <v>17</v>
+        <v>8</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="0">
-        <v>24</v>
+        <v>52</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C21" s="0" t="s">
         <v>6</v>
@@ -748,15 +748,15 @@
         <v>7</v>
       </c>
       <c r="E21" s="0" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="0">
-        <v>52</v>
+        <v>27</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C22" s="0" t="s">
         <v>6</v>
@@ -765,15 +765,15 @@
         <v>7</v>
       </c>
       <c r="E22" s="0" t="s">
-        <v>17</v>
+        <v>8</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="0">
+        <v>28</v>
+      </c>
+      <c r="B23" s="0" t="s">
         <v>27</v>
-      </c>
-      <c r="B23" s="0" t="s">
-        <v>26</v>
       </c>
       <c r="C23" s="0" t="s">
         <v>6</v>
@@ -787,10 +787,10 @@
     </row>
     <row r="24">
       <c r="A24" s="0">
+        <v>19</v>
+      </c>
+      <c r="B24" s="0" t="s">
         <v>28</v>
-      </c>
-      <c r="B24" s="0" t="s">
-        <v>27</v>
       </c>
       <c r="C24" s="0" t="s">
         <v>6</v>
@@ -804,10 +804,10 @@
     </row>
     <row r="25">
       <c r="A25" s="0">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C25" s="0" t="s">
         <v>6</v>
@@ -821,10 +821,10 @@
     </row>
     <row r="26">
       <c r="A26" s="0">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C26" s="0" t="s">
         <v>6</v>
@@ -838,10 +838,10 @@
     </row>
     <row r="27">
       <c r="A27" s="0">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C27" s="0" t="s">
         <v>6</v>
@@ -855,10 +855,10 @@
     </row>
     <row r="28">
       <c r="A28" s="0">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C28" s="0" t="s">
         <v>6</v>
@@ -872,10 +872,10 @@
     </row>
     <row r="29">
       <c r="A29" s="0">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C29" s="0" t="s">
         <v>6</v>
@@ -889,10 +889,10 @@
     </row>
     <row r="30">
       <c r="A30" s="0">
-        <v>25</v>
+        <v>57</v>
       </c>
       <c r="B30" s="0" t="s">
-        <v>33</v>
+        <v>71</v>
       </c>
       <c r="C30" s="0" t="s">
         <v>6</v>
@@ -901,15 +901,15 @@
         <v>7</v>
       </c>
       <c r="E30" s="0" t="s">
-        <v>8</v>
+        <v>72</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="0">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B31" s="0" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="C31" s="0" t="s">
         <v>6</v>
@@ -923,10 +923,10 @@
     </row>
     <row r="32">
       <c r="A32" s="0">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="B32" s="0" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="C32" s="0" t="s">
         <v>6</v>
@@ -940,10 +940,10 @@
     </row>
     <row r="33">
       <c r="A33" s="0">
-        <v>61</v>
+        <v>26</v>
       </c>
       <c r="B33" s="0" t="s">
-        <v>76</v>
+        <v>34</v>
       </c>
       <c r="C33" s="0" t="s">
         <v>6</v>
@@ -952,15 +952,15 @@
         <v>7</v>
       </c>
       <c r="E33" s="0" t="s">
-        <v>72</v>
+        <v>8</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="0">
-        <v>26</v>
+        <v>43</v>
       </c>
       <c r="B34" s="0" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C34" s="0" t="s">
         <v>6</v>
@@ -969,15 +969,15 @@
         <v>7</v>
       </c>
       <c r="E34" s="0" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="0">
-        <v>43</v>
+        <v>29</v>
       </c>
       <c r="B35" s="0" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C35" s="0" t="s">
         <v>6</v>
@@ -986,15 +986,15 @@
         <v>7</v>
       </c>
       <c r="E35" s="0" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="0">
-        <v>29</v>
+        <v>47</v>
       </c>
       <c r="B36" s="0" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C36" s="0" t="s">
         <v>6</v>
@@ -1003,15 +1003,15 @@
         <v>7</v>
       </c>
       <c r="E36" s="0" t="s">
-        <v>8</v>
+        <v>38</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="0">
-        <v>47</v>
+        <v>60</v>
       </c>
       <c r="B37" s="0" t="s">
-        <v>37</v>
+        <v>75</v>
       </c>
       <c r="C37" s="0" t="s">
         <v>6</v>
@@ -1020,23 +1020,6 @@
         <v>7</v>
       </c>
       <c r="E37" s="0" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="38">
-      <c r="A38" s="0">
-        <v>60</v>
-      </c>
-      <c r="B38" s="0" t="s">
-        <v>75</v>
-      </c>
-      <c r="C38" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="D38" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="E38" s="0" t="s">
         <v>72</v>
       </c>
     </row>
@@ -1047,7 +1030,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:F27"/>
+  <dimension ref="A1:F28"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1075,10 +1058,10 @@
     </row>
     <row r="2">
       <c r="A2" s="0">
-        <v>64</v>
+        <v>70</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>79</v>
+        <v>86</v>
       </c>
       <c r="C2" s="0" t="s">
         <v>39</v>
@@ -1095,10 +1078,10 @@
     </row>
     <row r="3">
       <c r="A3" s="0">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="C3" s="0" t="s">
         <v>39</v>
@@ -1115,10 +1098,10 @@
     </row>
     <row r="4">
       <c r="A4" s="0">
-        <v>13</v>
+        <v>63</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
       <c r="C4" s="0" t="s">
         <v>39</v>
@@ -1127,7 +1110,7 @@
         <v>7</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>8</v>
+        <v>72</v>
       </c>
       <c r="F4" s="0" t="s">
         <v>72</v>
@@ -1135,10 +1118,10 @@
     </row>
     <row r="5">
       <c r="A5" s="0">
-        <v>42</v>
+        <v>13</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>11</v>
+        <v>85</v>
       </c>
       <c r="C5" s="0" t="s">
         <v>39</v>
@@ -1147,18 +1130,18 @@
         <v>7</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="F5" s="0" t="s">
-        <v>22</v>
+        <v>72</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="0">
-        <v>33</v>
+        <v>42</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C6" s="0" t="s">
         <v>39</v>
@@ -1167,7 +1150,7 @@
         <v>7</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="F6" s="0" t="s">
         <v>22</v>
@@ -1175,10 +1158,10 @@
     </row>
     <row r="7">
       <c r="A7" s="0">
-        <v>48</v>
+        <v>33</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>40</v>
+        <v>9</v>
       </c>
       <c r="C7" s="0" t="s">
         <v>39</v>
@@ -1187,18 +1170,18 @@
         <v>7</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="F7" s="0" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="0">
-        <v>37</v>
+        <v>48</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C8" s="0" t="s">
         <v>39</v>
@@ -1207,7 +1190,7 @@
         <v>7</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="F8" s="0" t="s">
         <v>17</v>
@@ -1215,10 +1198,10 @@
     </row>
     <row r="9">
       <c r="A9" s="0">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C9" s="0" t="s">
         <v>39</v>
@@ -1230,15 +1213,15 @@
         <v>14</v>
       </c>
       <c r="F9" s="0" t="s">
-        <v>38</v>
+        <v>17</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="0">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C10" s="0" t="s">
         <v>39</v>
@@ -1247,7 +1230,7 @@
         <v>7</v>
       </c>
       <c r="E10" s="0" t="s">
-        <v>44</v>
+        <v>14</v>
       </c>
       <c r="F10" s="0" t="s">
         <v>38</v>
@@ -1255,10 +1238,10 @@
     </row>
     <row r="11">
       <c r="A11" s="0">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C11" s="0" t="s">
         <v>39</v>
@@ -1267,7 +1250,7 @@
         <v>7</v>
       </c>
       <c r="E11" s="0" t="s">
-        <v>12</v>
+        <v>44</v>
       </c>
       <c r="F11" s="0" t="s">
         <v>38</v>
@@ -1275,10 +1258,10 @@
     </row>
     <row r="12">
       <c r="A12" s="0">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C12" s="0" t="s">
         <v>39</v>
@@ -1295,10 +1278,10 @@
     </row>
     <row r="13">
       <c r="A13" s="0">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C13" s="0" t="s">
         <v>39</v>
@@ -1310,15 +1293,15 @@
         <v>12</v>
       </c>
       <c r="F13" s="0" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="0">
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C14" s="0" t="s">
         <v>39</v>
@@ -1327,7 +1310,7 @@
         <v>7</v>
       </c>
       <c r="E14" s="0" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="F14" s="0" t="s">
         <v>44</v>
@@ -1335,10 +1318,10 @@
     </row>
     <row r="15">
       <c r="A15" s="0">
-        <v>11</v>
+        <v>36</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C15" s="0" t="s">
         <v>39</v>
@@ -1347,18 +1330,18 @@
         <v>7</v>
       </c>
       <c r="E15" s="0" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="F15" s="0" t="s">
-        <v>12</v>
+        <v>44</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="0">
-        <v>40</v>
+        <v>11</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C16" s="0" t="s">
         <v>39</v>
@@ -1367,7 +1350,7 @@
         <v>7</v>
       </c>
       <c r="E16" s="0" t="s">
-        <v>51</v>
+        <v>8</v>
       </c>
       <c r="F16" s="0" t="s">
         <v>12</v>
@@ -1375,10 +1358,10 @@
     </row>
     <row r="17">
       <c r="A17" s="0">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C17" s="0" t="s">
         <v>39</v>
@@ -1387,7 +1370,7 @@
         <v>7</v>
       </c>
       <c r="E17" s="0" t="s">
-        <v>14</v>
+        <v>51</v>
       </c>
       <c r="F17" s="0" t="s">
         <v>12</v>
@@ -1395,10 +1378,10 @@
     </row>
     <row r="18">
       <c r="A18" s="0">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C18" s="0" t="s">
         <v>39</v>
@@ -1407,18 +1390,18 @@
         <v>7</v>
       </c>
       <c r="E18" s="0" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="F18" s="0" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="0">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C19" s="0" t="s">
         <v>39</v>
@@ -1430,15 +1413,15 @@
         <v>10</v>
       </c>
       <c r="F19" s="0" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="0">
-        <v>20</v>
+        <v>31</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C20" s="0" t="s">
         <v>39</v>
@@ -1447,7 +1430,7 @@
         <v>7</v>
       </c>
       <c r="E20" s="0" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="F20" s="0" t="s">
         <v>10</v>
@@ -1455,10 +1438,10 @@
     </row>
     <row r="21">
       <c r="A21" s="0">
-        <v>9</v>
+        <v>20</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C21" s="0" t="s">
         <v>39</v>
@@ -1475,10 +1458,10 @@
     </row>
     <row r="22">
       <c r="A22" s="0">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C22" s="0" t="s">
         <v>39</v>
@@ -1495,10 +1478,10 @@
     </row>
     <row r="23">
       <c r="A23" s="0">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C23" s="0" t="s">
         <v>39</v>
@@ -1510,15 +1493,15 @@
         <v>8</v>
       </c>
       <c r="F23" s="0" t="s">
-        <v>59</v>
+        <v>10</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="0">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C24" s="0" t="s">
         <v>39</v>
@@ -1530,15 +1513,15 @@
         <v>8</v>
       </c>
       <c r="F24" s="0" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="0">
-        <v>30</v>
+        <v>3</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C25" s="0" t="s">
         <v>39</v>
@@ -1555,10 +1538,10 @@
     </row>
     <row r="26">
       <c r="A26" s="0">
-        <v>2</v>
+        <v>30</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C26" s="0" t="s">
         <v>39</v>
@@ -1575,21 +1558,41 @@
     </row>
     <row r="27">
       <c r="A27" s="0">
+        <v>2</v>
+      </c>
+      <c r="B27" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="C27" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="D27" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E27" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="F27" s="0" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="0">
         <v>1</v>
       </c>
-      <c r="B27" s="0" t="s">
+      <c r="B28" s="0" t="s">
         <v>63</v>
       </c>
-      <c r="C27" s="0" t="s">
-        <v>39</v>
-      </c>
-      <c r="D27" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="E27" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="F27" s="0" t="s">
+      <c r="C28" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="D28" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E28" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="F28" s="0" t="s">
         <v>8</v>
       </c>
     </row>

</xml_diff>

<commit_message>
save palette changes, refresh main form, option to discard unsaved changes
</commit_message>
<xml_diff>
--- a/paint_todo.xlsx
+++ b/paint_todo.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="91">
   <si>
     <t>Id</t>
   </si>
@@ -338,6 +338,15 @@
   </si>
   <si>
     <t>edit palette: display rgb/hexdecimal/hsv values of selected color</t>
+  </si>
+  <si>
+    <t>entirely new palette</t>
+  </si>
+  <si>
+    <t>edit palette: on close, refresh main form palette based on what was just saved</t>
+  </si>
+  <si>
+    <t>edit palette: possibly replace "add color" button with a default extra swatch at the end of the list with a "plus sign" on it</t>
   </si>
 </sst>
 </file>
@@ -390,7 +399,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:F38"/>
+  <dimension ref="A1:F39"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -450,10 +459,10 @@
     </row>
     <row r="4">
       <c r="A4" s="0">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="C4" s="0" t="s">
         <v>6</v>
@@ -467,10 +476,10 @@
     </row>
     <row r="5">
       <c r="A5" s="0">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="C5" s="0" t="s">
         <v>6</v>
@@ -484,10 +493,10 @@
     </row>
     <row r="6">
       <c r="A6" s="0">
-        <v>66</v>
+        <v>71</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>81</v>
+        <v>87</v>
       </c>
       <c r="C6" s="0" t="s">
         <v>6</v>
@@ -501,10 +510,10 @@
     </row>
     <row r="7">
       <c r="A7" s="0">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="C7" s="0" t="s">
         <v>6</v>
@@ -518,10 +527,10 @@
     </row>
     <row r="8">
       <c r="A8" s="0">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="C8" s="0" t="s">
         <v>6</v>
@@ -535,10 +544,10 @@
     </row>
     <row r="9">
       <c r="A9" s="0">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C9" s="0" t="s">
         <v>6</v>
@@ -552,10 +561,10 @@
     </row>
     <row r="10">
       <c r="A10" s="0">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
       <c r="C10" s="0" t="s">
         <v>6</v>
@@ -994,10 +1003,10 @@
     </row>
     <row r="36">
       <c r="A36" s="0">
-        <v>29</v>
+        <v>74</v>
       </c>
       <c r="B36" s="0" t="s">
-        <v>36</v>
+        <v>90</v>
       </c>
       <c r="C36" s="0" t="s">
         <v>6</v>
@@ -1006,15 +1015,15 @@
         <v>7</v>
       </c>
       <c r="E36" s="0" t="s">
-        <v>8</v>
+        <v>72</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="0">
-        <v>47</v>
+        <v>29</v>
       </c>
       <c r="B37" s="0" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C37" s="0" t="s">
         <v>6</v>
@@ -1023,23 +1032,40 @@
         <v>7</v>
       </c>
       <c r="E37" s="0" t="s">
-        <v>38</v>
+        <v>8</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="0">
+        <v>47</v>
+      </c>
+      <c r="B38" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="C38" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D38" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E38" s="0" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" s="0">
         <v>60</v>
       </c>
-      <c r="B38" s="0" t="s">
+      <c r="B39" s="0" t="s">
         <v>75</v>
       </c>
-      <c r="C38" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="D38" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="E38" s="0" t="s">
+      <c r="C39" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D39" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E39" s="0" t="s">
         <v>72</v>
       </c>
     </row>
@@ -1050,7 +1076,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:F28"/>
+  <dimension ref="A1:F29"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1078,10 +1104,10 @@
     </row>
     <row r="2">
       <c r="A2" s="0">
-        <v>70</v>
+        <v>62</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>86</v>
+        <v>77</v>
       </c>
       <c r="C2" s="0" t="s">
         <v>39</v>
@@ -1098,10 +1124,10 @@
     </row>
     <row r="3">
       <c r="A3" s="0">
-        <v>64</v>
+        <v>70</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>79</v>
+        <v>86</v>
       </c>
       <c r="C3" s="0" t="s">
         <v>39</v>
@@ -1118,10 +1144,10 @@
     </row>
     <row r="4">
       <c r="A4" s="0">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="C4" s="0" t="s">
         <v>39</v>
@@ -1138,10 +1164,10 @@
     </row>
     <row r="5">
       <c r="A5" s="0">
-        <v>13</v>
+        <v>63</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
       <c r="C5" s="0" t="s">
         <v>39</v>
@@ -1150,7 +1176,7 @@
         <v>7</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>8</v>
+        <v>72</v>
       </c>
       <c r="F5" s="0" t="s">
         <v>72</v>
@@ -1158,10 +1184,10 @@
     </row>
     <row r="6">
       <c r="A6" s="0">
-        <v>42</v>
+        <v>13</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>11</v>
+        <v>85</v>
       </c>
       <c r="C6" s="0" t="s">
         <v>39</v>
@@ -1170,18 +1196,18 @@
         <v>7</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="F6" s="0" t="s">
-        <v>22</v>
+        <v>72</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="0">
-        <v>33</v>
+        <v>42</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C7" s="0" t="s">
         <v>39</v>
@@ -1190,7 +1216,7 @@
         <v>7</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="F7" s="0" t="s">
         <v>22</v>
@@ -1198,10 +1224,10 @@
     </row>
     <row r="8">
       <c r="A8" s="0">
-        <v>48</v>
+        <v>33</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>40</v>
+        <v>9</v>
       </c>
       <c r="C8" s="0" t="s">
         <v>39</v>
@@ -1210,18 +1236,18 @@
         <v>7</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="F8" s="0" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="0">
-        <v>37</v>
+        <v>48</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C9" s="0" t="s">
         <v>39</v>
@@ -1230,7 +1256,7 @@
         <v>7</v>
       </c>
       <c r="E9" s="0" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="F9" s="0" t="s">
         <v>17</v>
@@ -1238,10 +1264,10 @@
     </row>
     <row r="10">
       <c r="A10" s="0">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C10" s="0" t="s">
         <v>39</v>
@@ -1253,15 +1279,15 @@
         <v>14</v>
       </c>
       <c r="F10" s="0" t="s">
-        <v>38</v>
+        <v>17</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="0">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C11" s="0" t="s">
         <v>39</v>
@@ -1270,7 +1296,7 @@
         <v>7</v>
       </c>
       <c r="E11" s="0" t="s">
-        <v>44</v>
+        <v>14</v>
       </c>
       <c r="F11" s="0" t="s">
         <v>38</v>
@@ -1278,10 +1304,10 @@
     </row>
     <row r="12">
       <c r="A12" s="0">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C12" s="0" t="s">
         <v>39</v>
@@ -1290,7 +1316,7 @@
         <v>7</v>
       </c>
       <c r="E12" s="0" t="s">
-        <v>12</v>
+        <v>44</v>
       </c>
       <c r="F12" s="0" t="s">
         <v>38</v>
@@ -1298,10 +1324,10 @@
     </row>
     <row r="13">
       <c r="A13" s="0">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C13" s="0" t="s">
         <v>39</v>
@@ -1318,10 +1344,10 @@
     </row>
     <row r="14">
       <c r="A14" s="0">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C14" s="0" t="s">
         <v>39</v>
@@ -1333,15 +1359,15 @@
         <v>12</v>
       </c>
       <c r="F14" s="0" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="0">
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C15" s="0" t="s">
         <v>39</v>
@@ -1350,7 +1376,7 @@
         <v>7</v>
       </c>
       <c r="E15" s="0" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="F15" s="0" t="s">
         <v>44</v>
@@ -1358,10 +1384,10 @@
     </row>
     <row r="16">
       <c r="A16" s="0">
-        <v>11</v>
+        <v>36</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C16" s="0" t="s">
         <v>39</v>
@@ -1370,18 +1396,18 @@
         <v>7</v>
       </c>
       <c r="E16" s="0" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="F16" s="0" t="s">
-        <v>12</v>
+        <v>44</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="0">
-        <v>40</v>
+        <v>11</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C17" s="0" t="s">
         <v>39</v>
@@ -1390,7 +1416,7 @@
         <v>7</v>
       </c>
       <c r="E17" s="0" t="s">
-        <v>51</v>
+        <v>8</v>
       </c>
       <c r="F17" s="0" t="s">
         <v>12</v>
@@ -1398,10 +1424,10 @@
     </row>
     <row r="18">
       <c r="A18" s="0">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C18" s="0" t="s">
         <v>39</v>
@@ -1410,7 +1436,7 @@
         <v>7</v>
       </c>
       <c r="E18" s="0" t="s">
-        <v>14</v>
+        <v>51</v>
       </c>
       <c r="F18" s="0" t="s">
         <v>12</v>
@@ -1418,10 +1444,10 @@
     </row>
     <row r="19">
       <c r="A19" s="0">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C19" s="0" t="s">
         <v>39</v>
@@ -1430,18 +1456,18 @@
         <v>7</v>
       </c>
       <c r="E19" s="0" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="F19" s="0" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="0">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C20" s="0" t="s">
         <v>39</v>
@@ -1453,15 +1479,15 @@
         <v>10</v>
       </c>
       <c r="F20" s="0" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="0">
-        <v>20</v>
+        <v>31</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C21" s="0" t="s">
         <v>39</v>
@@ -1470,7 +1496,7 @@
         <v>7</v>
       </c>
       <c r="E21" s="0" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="F21" s="0" t="s">
         <v>10</v>
@@ -1478,10 +1504,10 @@
     </row>
     <row r="22">
       <c r="A22" s="0">
-        <v>9</v>
+        <v>20</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C22" s="0" t="s">
         <v>39</v>
@@ -1498,10 +1524,10 @@
     </row>
     <row r="23">
       <c r="A23" s="0">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C23" s="0" t="s">
         <v>39</v>
@@ -1518,10 +1544,10 @@
     </row>
     <row r="24">
       <c r="A24" s="0">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C24" s="0" t="s">
         <v>39</v>
@@ -1533,15 +1559,15 @@
         <v>8</v>
       </c>
       <c r="F24" s="0" t="s">
-        <v>59</v>
+        <v>10</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="0">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C25" s="0" t="s">
         <v>39</v>
@@ -1553,15 +1579,15 @@
         <v>8</v>
       </c>
       <c r="F25" s="0" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="0">
-        <v>30</v>
+        <v>3</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C26" s="0" t="s">
         <v>39</v>
@@ -1578,10 +1604,10 @@
     </row>
     <row r="27">
       <c r="A27" s="0">
-        <v>2</v>
+        <v>30</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C27" s="0" t="s">
         <v>39</v>
@@ -1598,21 +1624,41 @@
     </row>
     <row r="28">
       <c r="A28" s="0">
+        <v>2</v>
+      </c>
+      <c r="B28" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="C28" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="D28" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E28" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="F28" s="0" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="0">
         <v>1</v>
       </c>
-      <c r="B28" s="0" t="s">
+      <c r="B29" s="0" t="s">
         <v>63</v>
       </c>
-      <c r="C28" s="0" t="s">
-        <v>39</v>
-      </c>
-      <c r="D28" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="E28" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="F28" s="0" t="s">
+      <c r="C29" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="D29" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E29" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="F29" s="0" t="s">
         <v>8</v>
       </c>
     </row>
@@ -1656,7 +1702,7 @@
         <v>7</v>
       </c>
       <c r="F2" s="0">
-        <v>71</v>
+        <v>74</v>
       </c>
     </row>
     <row r="3">

</xml_diff>

<commit_message>
edit palette: undo, redo
</commit_message>
<xml_diff>
--- a/paint_todo.xlsx
+++ b/paint_todo.xlsx
@@ -399,7 +399,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:F39"/>
+  <dimension ref="A1:F38"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -459,10 +459,10 @@
     </row>
     <row r="4">
       <c r="A4" s="0">
-        <v>65</v>
+        <v>71</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>80</v>
+        <v>87</v>
       </c>
       <c r="C4" s="0" t="s">
         <v>6</v>
@@ -476,10 +476,10 @@
     </row>
     <row r="5">
       <c r="A5" s="0">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="C5" s="0" t="s">
         <v>6</v>
@@ -493,10 +493,10 @@
     </row>
     <row r="6">
       <c r="A6" s="0">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="C6" s="0" t="s">
         <v>6</v>
@@ -510,10 +510,10 @@
     </row>
     <row r="7">
       <c r="A7" s="0">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="C7" s="0" t="s">
         <v>6</v>
@@ -527,10 +527,10 @@
     </row>
     <row r="8">
       <c r="A8" s="0">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>83</v>
+        <v>88</v>
       </c>
       <c r="C8" s="0" t="s">
         <v>6</v>
@@ -544,11 +544,11 @@
     </row>
     <row r="9">
       <c r="A9" s="0">
+        <v>55</v>
+      </c>
+      <c r="B9" s="0" t="s">
         <v>69</v>
       </c>
-      <c r="B9" s="0" t="s">
-        <v>84</v>
-      </c>
       <c r="C9" s="0" t="s">
         <v>6</v>
       </c>
@@ -556,15 +556,15 @@
         <v>7</v>
       </c>
       <c r="E9" s="0" t="s">
-        <v>72</v>
+        <v>22</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="0">
-        <v>72</v>
+        <v>50</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>88</v>
+        <v>16</v>
       </c>
       <c r="C10" s="0" t="s">
         <v>6</v>
@@ -573,15 +573,15 @@
         <v>7</v>
       </c>
       <c r="E10" s="0" t="s">
-        <v>72</v>
+        <v>17</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="0">
-        <v>55</v>
+        <v>34</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>69</v>
+        <v>18</v>
       </c>
       <c r="C11" s="0" t="s">
         <v>6</v>
@@ -590,15 +590,15 @@
         <v>7</v>
       </c>
       <c r="E11" s="0" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="0">
-        <v>50</v>
+        <v>59</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>16</v>
+        <v>74</v>
       </c>
       <c r="C12" s="0" t="s">
         <v>6</v>
@@ -607,15 +607,15 @@
         <v>7</v>
       </c>
       <c r="E12" s="0" t="s">
-        <v>17</v>
+        <v>72</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="0">
-        <v>34</v>
+        <v>49</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C13" s="0" t="s">
         <v>6</v>
@@ -624,15 +624,15 @@
         <v>7</v>
       </c>
       <c r="E13" s="0" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="0">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="C14" s="0" t="s">
         <v>6</v>
@@ -641,15 +641,15 @@
         <v>7</v>
       </c>
       <c r="E14" s="0" t="s">
-        <v>72</v>
+        <v>22</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="0">
-        <v>49</v>
+        <v>21</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C15" s="0" t="s">
         <v>6</v>
@@ -658,15 +658,15 @@
         <v>7</v>
       </c>
       <c r="E15" s="0" t="s">
-        <v>17</v>
+        <v>8</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="0">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C16" s="0" t="s">
         <v>6</v>
@@ -680,11 +680,11 @@
     </row>
     <row r="17">
       <c r="A17" s="0">
+        <v>53</v>
+      </c>
+      <c r="B17" s="0" t="s">
         <v>21</v>
       </c>
-      <c r="B17" s="0" t="s">
-        <v>20</v>
-      </c>
       <c r="C17" s="0" t="s">
         <v>6</v>
       </c>
@@ -692,15 +692,15 @@
         <v>7</v>
       </c>
       <c r="E17" s="0" t="s">
-        <v>8</v>
+        <v>22</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="0">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>68</v>
+        <v>23</v>
       </c>
       <c r="C18" s="0" t="s">
         <v>6</v>
@@ -709,15 +709,15 @@
         <v>7</v>
       </c>
       <c r="E18" s="0" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="0">
-        <v>53</v>
+        <v>24</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="C19" s="0" t="s">
         <v>6</v>
@@ -726,15 +726,15 @@
         <v>7</v>
       </c>
       <c r="E19" s="0" t="s">
-        <v>22</v>
+        <v>8</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="0">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="C20" s="0" t="s">
         <v>6</v>
@@ -748,10 +748,10 @@
     </row>
     <row r="21">
       <c r="A21" s="0">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="C21" s="0" t="s">
         <v>6</v>
@@ -765,10 +765,10 @@
     </row>
     <row r="22">
       <c r="A22" s="0">
-        <v>52</v>
+        <v>28</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="C22" s="0" t="s">
         <v>6</v>
@@ -777,15 +777,15 @@
         <v>7</v>
       </c>
       <c r="E22" s="0" t="s">
-        <v>17</v>
+        <v>8</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="0">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="C23" s="0" t="s">
         <v>6</v>
@@ -799,10 +799,10 @@
     </row>
     <row r="24">
       <c r="A24" s="0">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C24" s="0" t="s">
         <v>6</v>
@@ -816,10 +816,10 @@
     </row>
     <row r="25">
       <c r="A25" s="0">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="C25" s="0" t="s">
         <v>6</v>
@@ -833,10 +833,10 @@
     </row>
     <row r="26">
       <c r="A26" s="0">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="C26" s="0" t="s">
         <v>6</v>
@@ -850,10 +850,10 @@
     </row>
     <row r="27">
       <c r="A27" s="0">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="C27" s="0" t="s">
         <v>6</v>
@@ -867,10 +867,10 @@
     </row>
     <row r="28">
       <c r="A28" s="0">
-        <v>17</v>
+        <v>25</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="C28" s="0" t="s">
         <v>6</v>
@@ -884,10 +884,10 @@
     </row>
     <row r="29">
       <c r="A29" s="0">
-        <v>18</v>
+        <v>57</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>32</v>
+        <v>71</v>
       </c>
       <c r="C29" s="0" t="s">
         <v>6</v>
@@ -896,15 +896,15 @@
         <v>7</v>
       </c>
       <c r="E29" s="0" t="s">
-        <v>8</v>
+        <v>72</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="0">
-        <v>25</v>
+        <v>65</v>
       </c>
       <c r="B30" s="0" t="s">
-        <v>33</v>
+        <v>80</v>
       </c>
       <c r="C30" s="0" t="s">
         <v>6</v>
@@ -913,15 +913,15 @@
         <v>7</v>
       </c>
       <c r="E30" s="0" t="s">
-        <v>8</v>
+        <v>72</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="0">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B31" s="0" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="C31" s="0" t="s">
         <v>6</v>
@@ -935,10 +935,10 @@
     </row>
     <row r="32">
       <c r="A32" s="0">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="B32" s="0" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="C32" s="0" t="s">
         <v>6</v>
@@ -952,10 +952,10 @@
     </row>
     <row r="33">
       <c r="A33" s="0">
-        <v>61</v>
+        <v>26</v>
       </c>
       <c r="B33" s="0" t="s">
-        <v>76</v>
+        <v>34</v>
       </c>
       <c r="C33" s="0" t="s">
         <v>6</v>
@@ -964,15 +964,15 @@
         <v>7</v>
       </c>
       <c r="E33" s="0" t="s">
-        <v>72</v>
+        <v>8</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="0">
-        <v>26</v>
+        <v>43</v>
       </c>
       <c r="B34" s="0" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C34" s="0" t="s">
         <v>6</v>
@@ -981,15 +981,15 @@
         <v>7</v>
       </c>
       <c r="E34" s="0" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="0">
-        <v>43</v>
+        <v>74</v>
       </c>
       <c r="B35" s="0" t="s">
-        <v>35</v>
+        <v>90</v>
       </c>
       <c r="C35" s="0" t="s">
         <v>6</v>
@@ -998,15 +998,15 @@
         <v>7</v>
       </c>
       <c r="E35" s="0" t="s">
-        <v>12</v>
+        <v>72</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="0">
-        <v>74</v>
+        <v>29</v>
       </c>
       <c r="B36" s="0" t="s">
-        <v>90</v>
+        <v>36</v>
       </c>
       <c r="C36" s="0" t="s">
         <v>6</v>
@@ -1015,15 +1015,15 @@
         <v>7</v>
       </c>
       <c r="E36" s="0" t="s">
-        <v>72</v>
+        <v>8</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="0">
-        <v>29</v>
+        <v>47</v>
       </c>
       <c r="B37" s="0" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C37" s="0" t="s">
         <v>6</v>
@@ -1032,15 +1032,15 @@
         <v>7</v>
       </c>
       <c r="E37" s="0" t="s">
-        <v>8</v>
+        <v>38</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="0">
-        <v>47</v>
+        <v>60</v>
       </c>
       <c r="B38" s="0" t="s">
-        <v>37</v>
+        <v>75</v>
       </c>
       <c r="C38" s="0" t="s">
         <v>6</v>
@@ -1049,23 +1049,6 @@
         <v>7</v>
       </c>
       <c r="E38" s="0" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="39">
-      <c r="A39" s="0">
-        <v>60</v>
-      </c>
-      <c r="B39" s="0" t="s">
-        <v>75</v>
-      </c>
-      <c r="C39" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="D39" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="E39" s="0" t="s">
         <v>72</v>
       </c>
     </row>
@@ -1076,7 +1059,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:F29"/>
+  <dimension ref="A1:F30"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1104,10 +1087,10 @@
     </row>
     <row r="2">
       <c r="A2" s="0">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="C2" s="0" t="s">
         <v>39</v>
@@ -1124,10 +1107,10 @@
     </row>
     <row r="3">
       <c r="A3" s="0">
-        <v>70</v>
+        <v>62</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>86</v>
+        <v>77</v>
       </c>
       <c r="C3" s="0" t="s">
         <v>39</v>
@@ -1144,10 +1127,10 @@
     </row>
     <row r="4">
       <c r="A4" s="0">
-        <v>64</v>
+        <v>70</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>79</v>
+        <v>86</v>
       </c>
       <c r="C4" s="0" t="s">
         <v>39</v>
@@ -1164,10 +1147,10 @@
     </row>
     <row r="5">
       <c r="A5" s="0">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="C5" s="0" t="s">
         <v>39</v>
@@ -1184,10 +1167,10 @@
     </row>
     <row r="6">
       <c r="A6" s="0">
-        <v>13</v>
+        <v>63</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
       <c r="C6" s="0" t="s">
         <v>39</v>
@@ -1196,7 +1179,7 @@
         <v>7</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>8</v>
+        <v>72</v>
       </c>
       <c r="F6" s="0" t="s">
         <v>72</v>
@@ -1204,10 +1187,10 @@
     </row>
     <row r="7">
       <c r="A7" s="0">
-        <v>42</v>
+        <v>13</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>11</v>
+        <v>85</v>
       </c>
       <c r="C7" s="0" t="s">
         <v>39</v>
@@ -1216,18 +1199,18 @@
         <v>7</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="F7" s="0" t="s">
-        <v>22</v>
+        <v>72</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="0">
-        <v>33</v>
+        <v>42</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C8" s="0" t="s">
         <v>39</v>
@@ -1236,7 +1219,7 @@
         <v>7</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="F8" s="0" t="s">
         <v>22</v>
@@ -1244,10 +1227,10 @@
     </row>
     <row r="9">
       <c r="A9" s="0">
-        <v>48</v>
+        <v>33</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>40</v>
+        <v>9</v>
       </c>
       <c r="C9" s="0" t="s">
         <v>39</v>
@@ -1256,18 +1239,18 @@
         <v>7</v>
       </c>
       <c r="E9" s="0" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="F9" s="0" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="0">
-        <v>37</v>
+        <v>48</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C10" s="0" t="s">
         <v>39</v>
@@ -1276,7 +1259,7 @@
         <v>7</v>
       </c>
       <c r="E10" s="0" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="F10" s="0" t="s">
         <v>17</v>
@@ -1284,10 +1267,10 @@
     </row>
     <row r="11">
       <c r="A11" s="0">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C11" s="0" t="s">
         <v>39</v>
@@ -1299,15 +1282,15 @@
         <v>14</v>
       </c>
       <c r="F11" s="0" t="s">
-        <v>38</v>
+        <v>17</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="0">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C12" s="0" t="s">
         <v>39</v>
@@ -1316,7 +1299,7 @@
         <v>7</v>
       </c>
       <c r="E12" s="0" t="s">
-        <v>44</v>
+        <v>14</v>
       </c>
       <c r="F12" s="0" t="s">
         <v>38</v>
@@ -1324,10 +1307,10 @@
     </row>
     <row r="13">
       <c r="A13" s="0">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C13" s="0" t="s">
         <v>39</v>
@@ -1336,7 +1319,7 @@
         <v>7</v>
       </c>
       <c r="E13" s="0" t="s">
-        <v>12</v>
+        <v>44</v>
       </c>
       <c r="F13" s="0" t="s">
         <v>38</v>
@@ -1344,10 +1327,10 @@
     </row>
     <row r="14">
       <c r="A14" s="0">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C14" s="0" t="s">
         <v>39</v>
@@ -1364,10 +1347,10 @@
     </row>
     <row r="15">
       <c r="A15" s="0">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C15" s="0" t="s">
         <v>39</v>
@@ -1379,15 +1362,15 @@
         <v>12</v>
       </c>
       <c r="F15" s="0" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="0">
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C16" s="0" t="s">
         <v>39</v>
@@ -1396,7 +1379,7 @@
         <v>7</v>
       </c>
       <c r="E16" s="0" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="F16" s="0" t="s">
         <v>44</v>
@@ -1404,10 +1387,10 @@
     </row>
     <row r="17">
       <c r="A17" s="0">
-        <v>11</v>
+        <v>36</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C17" s="0" t="s">
         <v>39</v>
@@ -1416,18 +1399,18 @@
         <v>7</v>
       </c>
       <c r="E17" s="0" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="F17" s="0" t="s">
-        <v>12</v>
+        <v>44</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="0">
-        <v>40</v>
+        <v>11</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C18" s="0" t="s">
         <v>39</v>
@@ -1436,7 +1419,7 @@
         <v>7</v>
       </c>
       <c r="E18" s="0" t="s">
-        <v>51</v>
+        <v>8</v>
       </c>
       <c r="F18" s="0" t="s">
         <v>12</v>
@@ -1444,10 +1427,10 @@
     </row>
     <row r="19">
       <c r="A19" s="0">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C19" s="0" t="s">
         <v>39</v>
@@ -1456,7 +1439,7 @@
         <v>7</v>
       </c>
       <c r="E19" s="0" t="s">
-        <v>14</v>
+        <v>51</v>
       </c>
       <c r="F19" s="0" t="s">
         <v>12</v>
@@ -1464,10 +1447,10 @@
     </row>
     <row r="20">
       <c r="A20" s="0">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C20" s="0" t="s">
         <v>39</v>
@@ -1476,18 +1459,18 @@
         <v>7</v>
       </c>
       <c r="E20" s="0" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="F20" s="0" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="0">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C21" s="0" t="s">
         <v>39</v>
@@ -1499,15 +1482,15 @@
         <v>10</v>
       </c>
       <c r="F21" s="0" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="0">
-        <v>20</v>
+        <v>31</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C22" s="0" t="s">
         <v>39</v>
@@ -1516,7 +1499,7 @@
         <v>7</v>
       </c>
       <c r="E22" s="0" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="F22" s="0" t="s">
         <v>10</v>
@@ -1524,10 +1507,10 @@
     </row>
     <row r="23">
       <c r="A23" s="0">
-        <v>9</v>
+        <v>20</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C23" s="0" t="s">
         <v>39</v>
@@ -1544,10 +1527,10 @@
     </row>
     <row r="24">
       <c r="A24" s="0">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C24" s="0" t="s">
         <v>39</v>
@@ -1564,10 +1547,10 @@
     </row>
     <row r="25">
       <c r="A25" s="0">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C25" s="0" t="s">
         <v>39</v>
@@ -1579,15 +1562,15 @@
         <v>8</v>
       </c>
       <c r="F25" s="0" t="s">
-        <v>59</v>
+        <v>10</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="0">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C26" s="0" t="s">
         <v>39</v>
@@ -1599,15 +1582,15 @@
         <v>8</v>
       </c>
       <c r="F26" s="0" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="0">
-        <v>30</v>
+        <v>3</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C27" s="0" t="s">
         <v>39</v>
@@ -1624,10 +1607,10 @@
     </row>
     <row r="28">
       <c r="A28" s="0">
-        <v>2</v>
+        <v>30</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C28" s="0" t="s">
         <v>39</v>
@@ -1644,21 +1627,41 @@
     </row>
     <row r="29">
       <c r="A29" s="0">
+        <v>2</v>
+      </c>
+      <c r="B29" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="C29" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="D29" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E29" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="F29" s="0" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="0">
         <v>1</v>
       </c>
-      <c r="B29" s="0" t="s">
+      <c r="B30" s="0" t="s">
         <v>63</v>
       </c>
-      <c r="C29" s="0" t="s">
-        <v>39</v>
-      </c>
-      <c r="D29" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="E29" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="F29" s="0" t="s">
+      <c r="C30" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="D30" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E30" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="F30" s="0" t="s">
         <v>8</v>
       </c>
     </row>

</xml_diff>

<commit_message>
refactor: consistently name Dialogs and put in same folder
</commit_message>
<xml_diff>
--- a/paint_todo.xlsx
+++ b/paint_todo.xlsx
@@ -399,7 +399,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:F37"/>
+  <dimension ref="A1:F36"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -612,10 +612,10 @@
     </row>
     <row r="13">
       <c r="A13" s="0">
-        <v>56</v>
+        <v>21</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>70</v>
+        <v>20</v>
       </c>
       <c r="C13" s="0" t="s">
         <v>6</v>
@@ -624,15 +624,15 @@
         <v>7</v>
       </c>
       <c r="E13" s="0" t="s">
-        <v>22</v>
+        <v>8</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="0">
-        <v>21</v>
+        <v>54</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>20</v>
+        <v>68</v>
       </c>
       <c r="C14" s="0" t="s">
         <v>6</v>
@@ -641,15 +641,15 @@
         <v>7</v>
       </c>
       <c r="E14" s="0" t="s">
-        <v>8</v>
+        <v>22</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="0">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>68</v>
+        <v>21</v>
       </c>
       <c r="C15" s="0" t="s">
         <v>6</v>
@@ -663,10 +663,10 @@
     </row>
     <row r="16">
       <c r="A16" s="0">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="C16" s="0" t="s">
         <v>6</v>
@@ -675,15 +675,15 @@
         <v>7</v>
       </c>
       <c r="E16" s="0" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="0">
-        <v>51</v>
+        <v>24</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C17" s="0" t="s">
         <v>6</v>
@@ -692,15 +692,15 @@
         <v>7</v>
       </c>
       <c r="E17" s="0" t="s">
-        <v>17</v>
+        <v>8</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="0">
-        <v>24</v>
+        <v>52</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C18" s="0" t="s">
         <v>6</v>
@@ -709,15 +709,15 @@
         <v>7</v>
       </c>
       <c r="E18" s="0" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="0">
-        <v>52</v>
+        <v>27</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C19" s="0" t="s">
         <v>6</v>
@@ -726,15 +726,15 @@
         <v>7</v>
       </c>
       <c r="E19" s="0" t="s">
-        <v>17</v>
+        <v>8</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="0">
+        <v>28</v>
+      </c>
+      <c r="B20" s="0" t="s">
         <v>27</v>
-      </c>
-      <c r="B20" s="0" t="s">
-        <v>26</v>
       </c>
       <c r="C20" s="0" t="s">
         <v>6</v>
@@ -748,10 +748,10 @@
     </row>
     <row r="21">
       <c r="A21" s="0">
+        <v>19</v>
+      </c>
+      <c r="B21" s="0" t="s">
         <v>28</v>
-      </c>
-      <c r="B21" s="0" t="s">
-        <v>27</v>
       </c>
       <c r="C21" s="0" t="s">
         <v>6</v>
@@ -765,10 +765,10 @@
     </row>
     <row r="22">
       <c r="A22" s="0">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C22" s="0" t="s">
         <v>6</v>
@@ -782,10 +782,10 @@
     </row>
     <row r="23">
       <c r="A23" s="0">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C23" s="0" t="s">
         <v>6</v>
@@ -799,10 +799,10 @@
     </row>
     <row r="24">
       <c r="A24" s="0">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C24" s="0" t="s">
         <v>6</v>
@@ -816,10 +816,10 @@
     </row>
     <row r="25">
       <c r="A25" s="0">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C25" s="0" t="s">
         <v>6</v>
@@ -833,10 +833,10 @@
     </row>
     <row r="26">
       <c r="A26" s="0">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C26" s="0" t="s">
         <v>6</v>
@@ -850,10 +850,10 @@
     </row>
     <row r="27">
       <c r="A27" s="0">
-        <v>25</v>
+        <v>57</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>33</v>
+        <v>71</v>
       </c>
       <c r="C27" s="0" t="s">
         <v>6</v>
@@ -862,15 +862,15 @@
         <v>7</v>
       </c>
       <c r="E27" s="0" t="s">
-        <v>8</v>
+        <v>72</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="0">
-        <v>57</v>
+        <v>65</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>71</v>
+        <v>80</v>
       </c>
       <c r="C28" s="0" t="s">
         <v>6</v>
@@ -884,10 +884,10 @@
     </row>
     <row r="29">
       <c r="A29" s="0">
-        <v>65</v>
+        <v>58</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="C29" s="0" t="s">
         <v>6</v>
@@ -901,10 +901,10 @@
     </row>
     <row r="30">
       <c r="A30" s="0">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="B30" s="0" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="C30" s="0" t="s">
         <v>6</v>
@@ -918,10 +918,10 @@
     </row>
     <row r="31">
       <c r="A31" s="0">
-        <v>61</v>
+        <v>26</v>
       </c>
       <c r="B31" s="0" t="s">
-        <v>76</v>
+        <v>34</v>
       </c>
       <c r="C31" s="0" t="s">
         <v>6</v>
@@ -930,15 +930,15 @@
         <v>7</v>
       </c>
       <c r="E31" s="0" t="s">
-        <v>72</v>
+        <v>8</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="0">
-        <v>26</v>
+        <v>43</v>
       </c>
       <c r="B32" s="0" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C32" s="0" t="s">
         <v>6</v>
@@ -947,15 +947,15 @@
         <v>7</v>
       </c>
       <c r="E32" s="0" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="0">
-        <v>43</v>
+        <v>74</v>
       </c>
       <c r="B33" s="0" t="s">
-        <v>35</v>
+        <v>90</v>
       </c>
       <c r="C33" s="0" t="s">
         <v>6</v>
@@ -964,15 +964,15 @@
         <v>7</v>
       </c>
       <c r="E33" s="0" t="s">
-        <v>12</v>
+        <v>72</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="0">
-        <v>74</v>
+        <v>29</v>
       </c>
       <c r="B34" s="0" t="s">
-        <v>90</v>
+        <v>36</v>
       </c>
       <c r="C34" s="0" t="s">
         <v>6</v>
@@ -981,15 +981,15 @@
         <v>7</v>
       </c>
       <c r="E34" s="0" t="s">
-        <v>72</v>
+        <v>8</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="0">
-        <v>29</v>
+        <v>47</v>
       </c>
       <c r="B35" s="0" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C35" s="0" t="s">
         <v>6</v>
@@ -998,15 +998,15 @@
         <v>7</v>
       </c>
       <c r="E35" s="0" t="s">
-        <v>8</v>
+        <v>38</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="0">
-        <v>47</v>
+        <v>60</v>
       </c>
       <c r="B36" s="0" t="s">
-        <v>37</v>
+        <v>75</v>
       </c>
       <c r="C36" s="0" t="s">
         <v>6</v>
@@ -1015,23 +1015,6 @@
         <v>7</v>
       </c>
       <c r="E36" s="0" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="37">
-      <c r="A37" s="0">
-        <v>60</v>
-      </c>
-      <c r="B37" s="0" t="s">
-        <v>75</v>
-      </c>
-      <c r="C37" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="D37" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="E37" s="0" t="s">
         <v>72</v>
       </c>
     </row>
@@ -1042,7 +1025,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:F31"/>
+  <dimension ref="A1:F32"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1070,10 +1053,10 @@
     </row>
     <row r="2">
       <c r="A2" s="0">
-        <v>72</v>
+        <v>56</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>88</v>
+        <v>70</v>
       </c>
       <c r="C2" s="0" t="s">
         <v>39</v>
@@ -1082,7 +1065,7 @@
         <v>7</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>72</v>
+        <v>22</v>
       </c>
       <c r="F2" s="0" t="s">
         <v>72</v>
@@ -1090,10 +1073,10 @@
     </row>
     <row r="3">
       <c r="A3" s="0">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>81</v>
+        <v>88</v>
       </c>
       <c r="C3" s="0" t="s">
         <v>39</v>
@@ -1110,10 +1093,10 @@
     </row>
     <row r="4">
       <c r="A4" s="0">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="C4" s="0" t="s">
         <v>39</v>
@@ -1130,10 +1113,10 @@
     </row>
     <row r="5">
       <c r="A5" s="0">
-        <v>70</v>
+        <v>62</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>86</v>
+        <v>77</v>
       </c>
       <c r="C5" s="0" t="s">
         <v>39</v>
@@ -1150,10 +1133,10 @@
     </row>
     <row r="6">
       <c r="A6" s="0">
-        <v>64</v>
+        <v>70</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>79</v>
+        <v>86</v>
       </c>
       <c r="C6" s="0" t="s">
         <v>39</v>
@@ -1170,10 +1153,10 @@
     </row>
     <row r="7">
       <c r="A7" s="0">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="C7" s="0" t="s">
         <v>39</v>
@@ -1190,10 +1173,10 @@
     </row>
     <row r="8">
       <c r="A8" s="0">
-        <v>13</v>
+        <v>63</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
       <c r="C8" s="0" t="s">
         <v>39</v>
@@ -1202,7 +1185,7 @@
         <v>7</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>8</v>
+        <v>72</v>
       </c>
       <c r="F8" s="0" t="s">
         <v>72</v>
@@ -1210,10 +1193,10 @@
     </row>
     <row r="9">
       <c r="A9" s="0">
-        <v>42</v>
+        <v>13</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>11</v>
+        <v>85</v>
       </c>
       <c r="C9" s="0" t="s">
         <v>39</v>
@@ -1222,18 +1205,18 @@
         <v>7</v>
       </c>
       <c r="E9" s="0" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="F9" s="0" t="s">
-        <v>22</v>
+        <v>72</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="0">
-        <v>33</v>
+        <v>42</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C10" s="0" t="s">
         <v>39</v>
@@ -1242,7 +1225,7 @@
         <v>7</v>
       </c>
       <c r="E10" s="0" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="F10" s="0" t="s">
         <v>22</v>
@@ -1250,10 +1233,10 @@
     </row>
     <row r="11">
       <c r="A11" s="0">
-        <v>48</v>
+        <v>33</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>40</v>
+        <v>9</v>
       </c>
       <c r="C11" s="0" t="s">
         <v>39</v>
@@ -1262,18 +1245,18 @@
         <v>7</v>
       </c>
       <c r="E11" s="0" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="F11" s="0" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="0">
-        <v>37</v>
+        <v>48</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C12" s="0" t="s">
         <v>39</v>
@@ -1282,7 +1265,7 @@
         <v>7</v>
       </c>
       <c r="E12" s="0" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="F12" s="0" t="s">
         <v>17</v>
@@ -1290,10 +1273,10 @@
     </row>
     <row r="13">
       <c r="A13" s="0">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C13" s="0" t="s">
         <v>39</v>
@@ -1305,15 +1288,15 @@
         <v>14</v>
       </c>
       <c r="F13" s="0" t="s">
-        <v>38</v>
+        <v>17</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="0">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C14" s="0" t="s">
         <v>39</v>
@@ -1322,7 +1305,7 @@
         <v>7</v>
       </c>
       <c r="E14" s="0" t="s">
-        <v>44</v>
+        <v>14</v>
       </c>
       <c r="F14" s="0" t="s">
         <v>38</v>
@@ -1330,10 +1313,10 @@
     </row>
     <row r="15">
       <c r="A15" s="0">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C15" s="0" t="s">
         <v>39</v>
@@ -1342,7 +1325,7 @@
         <v>7</v>
       </c>
       <c r="E15" s="0" t="s">
-        <v>12</v>
+        <v>44</v>
       </c>
       <c r="F15" s="0" t="s">
         <v>38</v>
@@ -1350,10 +1333,10 @@
     </row>
     <row r="16">
       <c r="A16" s="0">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C16" s="0" t="s">
         <v>39</v>
@@ -1370,10 +1353,10 @@
     </row>
     <row r="17">
       <c r="A17" s="0">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C17" s="0" t="s">
         <v>39</v>
@@ -1385,15 +1368,15 @@
         <v>12</v>
       </c>
       <c r="F17" s="0" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="0">
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C18" s="0" t="s">
         <v>39</v>
@@ -1402,7 +1385,7 @@
         <v>7</v>
       </c>
       <c r="E18" s="0" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="F18" s="0" t="s">
         <v>44</v>
@@ -1410,10 +1393,10 @@
     </row>
     <row r="19">
       <c r="A19" s="0">
-        <v>11</v>
+        <v>36</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C19" s="0" t="s">
         <v>39</v>
@@ -1422,18 +1405,18 @@
         <v>7</v>
       </c>
       <c r="E19" s="0" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="F19" s="0" t="s">
-        <v>12</v>
+        <v>44</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="0">
-        <v>40</v>
+        <v>11</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C20" s="0" t="s">
         <v>39</v>
@@ -1442,7 +1425,7 @@
         <v>7</v>
       </c>
       <c r="E20" s="0" t="s">
-        <v>51</v>
+        <v>8</v>
       </c>
       <c r="F20" s="0" t="s">
         <v>12</v>
@@ -1450,10 +1433,10 @@
     </row>
     <row r="21">
       <c r="A21" s="0">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C21" s="0" t="s">
         <v>39</v>
@@ -1462,7 +1445,7 @@
         <v>7</v>
       </c>
       <c r="E21" s="0" t="s">
-        <v>14</v>
+        <v>51</v>
       </c>
       <c r="F21" s="0" t="s">
         <v>12</v>
@@ -1470,10 +1453,10 @@
     </row>
     <row r="22">
       <c r="A22" s="0">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C22" s="0" t="s">
         <v>39</v>
@@ -1482,18 +1465,18 @@
         <v>7</v>
       </c>
       <c r="E22" s="0" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="F22" s="0" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="0">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C23" s="0" t="s">
         <v>39</v>
@@ -1505,15 +1488,15 @@
         <v>10</v>
       </c>
       <c r="F23" s="0" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="0">
-        <v>20</v>
+        <v>31</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C24" s="0" t="s">
         <v>39</v>
@@ -1522,7 +1505,7 @@
         <v>7</v>
       </c>
       <c r="E24" s="0" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="F24" s="0" t="s">
         <v>10</v>
@@ -1530,10 +1513,10 @@
     </row>
     <row r="25">
       <c r="A25" s="0">
-        <v>9</v>
+        <v>20</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C25" s="0" t="s">
         <v>39</v>
@@ -1550,10 +1533,10 @@
     </row>
     <row r="26">
       <c r="A26" s="0">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C26" s="0" t="s">
         <v>39</v>
@@ -1570,10 +1553,10 @@
     </row>
     <row r="27">
       <c r="A27" s="0">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C27" s="0" t="s">
         <v>39</v>
@@ -1585,15 +1568,15 @@
         <v>8</v>
       </c>
       <c r="F27" s="0" t="s">
-        <v>59</v>
+        <v>10</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="0">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C28" s="0" t="s">
         <v>39</v>
@@ -1605,15 +1588,15 @@
         <v>8</v>
       </c>
       <c r="F28" s="0" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="0">
-        <v>30</v>
+        <v>3</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C29" s="0" t="s">
         <v>39</v>
@@ -1630,10 +1613,10 @@
     </row>
     <row r="30">
       <c r="A30" s="0">
-        <v>2</v>
+        <v>30</v>
       </c>
       <c r="B30" s="0" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C30" s="0" t="s">
         <v>39</v>
@@ -1650,21 +1633,41 @@
     </row>
     <row r="31">
       <c r="A31" s="0">
+        <v>2</v>
+      </c>
+      <c r="B31" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="C31" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="D31" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E31" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="F31" s="0" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="0">
         <v>1</v>
       </c>
-      <c r="B31" s="0" t="s">
+      <c r="B32" s="0" t="s">
         <v>63</v>
       </c>
-      <c r="C31" s="0" t="s">
-        <v>39</v>
-      </c>
-      <c r="D31" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="E31" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="F31" s="0" t="s">
+      <c r="C32" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="D32" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E32" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="F32" s="0" t="s">
         <v>8</v>
       </c>
     </row>

</xml_diff>

<commit_message>
refactor: use SwatchPanel on main form
</commit_message>
<xml_diff>
--- a/paint_todo.xlsx
+++ b/paint_todo.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="92">
   <si>
     <t>Id</t>
   </si>
@@ -347,6 +347,9 @@
   </si>
   <si>
     <t>edit palette: possibly replace "add color" button with a default extra swatch at the end of the list with a "plus sign" on it</t>
+  </si>
+  <si>
+    <t>remember last open palette and reopen it next time program starts</t>
   </si>
 </sst>
 </file>
@@ -459,10 +462,10 @@
     </row>
     <row r="4">
       <c r="A4" s="0">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>87</v>
+        <v>91</v>
       </c>
       <c r="C4" s="0" t="s">
         <v>6</v>
@@ -476,10 +479,10 @@
     </row>
     <row r="5">
       <c r="A5" s="0">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
       <c r="C5" s="0" t="s">
         <v>6</v>
@@ -493,10 +496,10 @@
     </row>
     <row r="6">
       <c r="A6" s="0">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C6" s="0" t="s">
         <v>6</v>
@@ -510,10 +513,10 @@
     </row>
     <row r="7">
       <c r="A7" s="0">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C7" s="0" t="s">
         <v>6</v>
@@ -527,10 +530,10 @@
     </row>
     <row r="8">
       <c r="A8" s="0">
-        <v>55</v>
+        <v>69</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>69</v>
+        <v>84</v>
       </c>
       <c r="C8" s="0" t="s">
         <v>6</v>
@@ -539,7 +542,7 @@
         <v>7</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>22</v>
+        <v>72</v>
       </c>
     </row>
     <row r="9">
@@ -1025,7 +1028,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:F32"/>
+  <dimension ref="A1:F33"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1053,10 +1056,10 @@
     </row>
     <row r="2">
       <c r="A2" s="0">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C2" s="0" t="s">
         <v>39</v>
@@ -1073,10 +1076,10 @@
     </row>
     <row r="3">
       <c r="A3" s="0">
-        <v>72</v>
+        <v>56</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>88</v>
+        <v>70</v>
       </c>
       <c r="C3" s="0" t="s">
         <v>39</v>
@@ -1085,7 +1088,7 @@
         <v>7</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>72</v>
+        <v>22</v>
       </c>
       <c r="F3" s="0" t="s">
         <v>72</v>
@@ -1093,10 +1096,10 @@
     </row>
     <row r="4">
       <c r="A4" s="0">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>81</v>
+        <v>88</v>
       </c>
       <c r="C4" s="0" t="s">
         <v>39</v>
@@ -1113,10 +1116,10 @@
     </row>
     <row r="5">
       <c r="A5" s="0">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="C5" s="0" t="s">
         <v>39</v>
@@ -1133,10 +1136,10 @@
     </row>
     <row r="6">
       <c r="A6" s="0">
-        <v>70</v>
+        <v>62</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>86</v>
+        <v>77</v>
       </c>
       <c r="C6" s="0" t="s">
         <v>39</v>
@@ -1153,10 +1156,10 @@
     </row>
     <row r="7">
       <c r="A7" s="0">
-        <v>64</v>
+        <v>70</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>79</v>
+        <v>86</v>
       </c>
       <c r="C7" s="0" t="s">
         <v>39</v>
@@ -1173,10 +1176,10 @@
     </row>
     <row r="8">
       <c r="A8" s="0">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="C8" s="0" t="s">
         <v>39</v>
@@ -1193,10 +1196,10 @@
     </row>
     <row r="9">
       <c r="A9" s="0">
-        <v>13</v>
+        <v>63</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
       <c r="C9" s="0" t="s">
         <v>39</v>
@@ -1205,7 +1208,7 @@
         <v>7</v>
       </c>
       <c r="E9" s="0" t="s">
-        <v>8</v>
+        <v>72</v>
       </c>
       <c r="F9" s="0" t="s">
         <v>72</v>
@@ -1213,10 +1216,10 @@
     </row>
     <row r="10">
       <c r="A10" s="0">
-        <v>42</v>
+        <v>13</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>11</v>
+        <v>85</v>
       </c>
       <c r="C10" s="0" t="s">
         <v>39</v>
@@ -1225,18 +1228,18 @@
         <v>7</v>
       </c>
       <c r="E10" s="0" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="F10" s="0" t="s">
-        <v>22</v>
+        <v>72</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="0">
-        <v>33</v>
+        <v>42</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C11" s="0" t="s">
         <v>39</v>
@@ -1245,7 +1248,7 @@
         <v>7</v>
       </c>
       <c r="E11" s="0" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="F11" s="0" t="s">
         <v>22</v>
@@ -1253,10 +1256,10 @@
     </row>
     <row r="12">
       <c r="A12" s="0">
-        <v>48</v>
+        <v>33</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>40</v>
+        <v>9</v>
       </c>
       <c r="C12" s="0" t="s">
         <v>39</v>
@@ -1265,18 +1268,18 @@
         <v>7</v>
       </c>
       <c r="E12" s="0" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="F12" s="0" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="0">
-        <v>37</v>
+        <v>48</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C13" s="0" t="s">
         <v>39</v>
@@ -1285,7 +1288,7 @@
         <v>7</v>
       </c>
       <c r="E13" s="0" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="F13" s="0" t="s">
         <v>17</v>
@@ -1293,10 +1296,10 @@
     </row>
     <row r="14">
       <c r="A14" s="0">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C14" s="0" t="s">
         <v>39</v>
@@ -1308,15 +1311,15 @@
         <v>14</v>
       </c>
       <c r="F14" s="0" t="s">
-        <v>38</v>
+        <v>17</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="0">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C15" s="0" t="s">
         <v>39</v>
@@ -1325,7 +1328,7 @@
         <v>7</v>
       </c>
       <c r="E15" s="0" t="s">
-        <v>44</v>
+        <v>14</v>
       </c>
       <c r="F15" s="0" t="s">
         <v>38</v>
@@ -1333,10 +1336,10 @@
     </row>
     <row r="16">
       <c r="A16" s="0">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C16" s="0" t="s">
         <v>39</v>
@@ -1345,7 +1348,7 @@
         <v>7</v>
       </c>
       <c r="E16" s="0" t="s">
-        <v>12</v>
+        <v>44</v>
       </c>
       <c r="F16" s="0" t="s">
         <v>38</v>
@@ -1353,10 +1356,10 @@
     </row>
     <row r="17">
       <c r="A17" s="0">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C17" s="0" t="s">
         <v>39</v>
@@ -1373,10 +1376,10 @@
     </row>
     <row r="18">
       <c r="A18" s="0">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C18" s="0" t="s">
         <v>39</v>
@@ -1388,15 +1391,15 @@
         <v>12</v>
       </c>
       <c r="F18" s="0" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="0">
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C19" s="0" t="s">
         <v>39</v>
@@ -1405,7 +1408,7 @@
         <v>7</v>
       </c>
       <c r="E19" s="0" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="F19" s="0" t="s">
         <v>44</v>
@@ -1413,10 +1416,10 @@
     </row>
     <row r="20">
       <c r="A20" s="0">
-        <v>11</v>
+        <v>36</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C20" s="0" t="s">
         <v>39</v>
@@ -1425,18 +1428,18 @@
         <v>7</v>
       </c>
       <c r="E20" s="0" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="F20" s="0" t="s">
-        <v>12</v>
+        <v>44</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="0">
-        <v>40</v>
+        <v>11</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C21" s="0" t="s">
         <v>39</v>
@@ -1445,7 +1448,7 @@
         <v>7</v>
       </c>
       <c r="E21" s="0" t="s">
-        <v>51</v>
+        <v>8</v>
       </c>
       <c r="F21" s="0" t="s">
         <v>12</v>
@@ -1453,10 +1456,10 @@
     </row>
     <row r="22">
       <c r="A22" s="0">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C22" s="0" t="s">
         <v>39</v>
@@ -1465,7 +1468,7 @@
         <v>7</v>
       </c>
       <c r="E22" s="0" t="s">
-        <v>14</v>
+        <v>51</v>
       </c>
       <c r="F22" s="0" t="s">
         <v>12</v>
@@ -1473,10 +1476,10 @@
     </row>
     <row r="23">
       <c r="A23" s="0">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C23" s="0" t="s">
         <v>39</v>
@@ -1485,18 +1488,18 @@
         <v>7</v>
       </c>
       <c r="E23" s="0" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="F23" s="0" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="0">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C24" s="0" t="s">
         <v>39</v>
@@ -1508,15 +1511,15 @@
         <v>10</v>
       </c>
       <c r="F24" s="0" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="0">
-        <v>20</v>
+        <v>31</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C25" s="0" t="s">
         <v>39</v>
@@ -1525,7 +1528,7 @@
         <v>7</v>
       </c>
       <c r="E25" s="0" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="F25" s="0" t="s">
         <v>10</v>
@@ -1533,10 +1536,10 @@
     </row>
     <row r="26">
       <c r="A26" s="0">
-        <v>9</v>
+        <v>20</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C26" s="0" t="s">
         <v>39</v>
@@ -1553,10 +1556,10 @@
     </row>
     <row r="27">
       <c r="A27" s="0">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C27" s="0" t="s">
         <v>39</v>
@@ -1573,10 +1576,10 @@
     </row>
     <row r="28">
       <c r="A28" s="0">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C28" s="0" t="s">
         <v>39</v>
@@ -1588,15 +1591,15 @@
         <v>8</v>
       </c>
       <c r="F28" s="0" t="s">
-        <v>59</v>
+        <v>10</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="0">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C29" s="0" t="s">
         <v>39</v>
@@ -1608,15 +1611,15 @@
         <v>8</v>
       </c>
       <c r="F29" s="0" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="0">
-        <v>30</v>
+        <v>3</v>
       </c>
       <c r="B30" s="0" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C30" s="0" t="s">
         <v>39</v>
@@ -1633,10 +1636,10 @@
     </row>
     <row r="31">
       <c r="A31" s="0">
-        <v>2</v>
+        <v>30</v>
       </c>
       <c r="B31" s="0" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C31" s="0" t="s">
         <v>39</v>
@@ -1653,21 +1656,41 @@
     </row>
     <row r="32">
       <c r="A32" s="0">
+        <v>2</v>
+      </c>
+      <c r="B32" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="C32" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="D32" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E32" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="F32" s="0" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="0">
         <v>1</v>
       </c>
-      <c r="B32" s="0" t="s">
+      <c r="B33" s="0" t="s">
         <v>63</v>
       </c>
-      <c r="C32" s="0" t="s">
-        <v>39</v>
-      </c>
-      <c r="D32" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="E32" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="F32" s="0" t="s">
+      <c r="C33" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="D33" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E33" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="F33" s="0" t="s">
         <v>8</v>
       </c>
     </row>
@@ -1711,7 +1734,7 @@
         <v>7</v>
       </c>
       <c r="F2" s="0">
-        <v>74</v>
+        <v>75</v>
       </c>
     </row>
     <row r="3">

</xml_diff>

<commit_message>
settings: remember last open palette
</commit_message>
<xml_diff>
--- a/paint_todo.xlsx
+++ b/paint_todo.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="90">
   <si>
     <t>Id</t>
   </si>
@@ -45,18 +45,6 @@
     <t>8/9/2018</t>
   </si>
   <si>
-    <t>undo, redo coloring a section on the image</t>
-  </si>
-  <si>
-    <t>8/11/2018</t>
-  </si>
-  <si>
-    <t>bug: expanded palette covers part of picturebox and statuspanel</t>
-  </si>
-  <si>
-    <t>8/15/2018</t>
-  </si>
-  <si>
     <t xml:space="preserve">set and check tolerance for "black" and "white"
 - "blacks" will be left untouched
 - "whites" will be treated as pure white, which will in effect alter them to white</t>
@@ -65,15 +53,19 @@
     <t>8/12/2018</t>
   </si>
   <si>
-    <t xml:space="preserve">open edit palette mode
-- add swatches
-- remove swatches
-- change color of swatch
-- reorder swatches
-- undo, redo until pane is closed
-- save changes before leaving pane 
-(save as text file - or, what do other programs use?)
-(no duplicate colors allowed)</t>
+    <t>edit palette: display rgb/hexdecimal/hsv values of selected color</t>
+  </si>
+  <si>
+    <t>8/24/2018</t>
+  </si>
+  <si>
+    <t>new color: enter an rgb value</t>
+  </si>
+  <si>
+    <t>new color: enter a hexadecimal value</t>
+  </si>
+  <si>
+    <t>new color: enter an hsv value</t>
   </si>
   <si>
     <t xml:space="preserve">design test that generates value scale for many different colors, easy to scan with the eye
@@ -86,20 +78,31 @@
     <t>when zooming, if a scroll bar is all the way to min or max, keep it there</t>
   </si>
   <si>
+    <t>8/11/2018</t>
+  </si>
+  <si>
+    <t>refactor WithoutHaste.Drawing.Colors HSV to use ints instead of floats (0-360, 0-100, 0-100)</t>
+  </si>
+  <si>
     <t xml:space="preserve">applying color is pretty fast even on large image
 but removing the color is really slow</t>
   </si>
   <si>
     <t xml:space="preserve">when resizing windows, default behavior is to keep the same section of image in the viewing pane
 - so expanding window would in effect zoom in</t>
+  </si>
+  <si>
+    <t xml:space="preserve">make a MasterImage class
+that one-time figures out all the regions in a background thread
+and provides that data to the color worker</t>
+  </si>
+  <si>
+    <t>8/23/2018</t>
   </si>
   <si>
     <t xml:space="preserve">prompt to save if image has changed since last save
 - on closing program
 - on opening new image</t>
-  </si>
-  <si>
-    <t>8/23/2018</t>
   </si>
   <si>
     <t>replace Rabbit with smaller and better divided image</t>
@@ -146,6 +149,24 @@
     <t>EVERYTHING BELOW HERE IS VERSION 2</t>
   </si>
   <si>
+    <t xml:space="preserve">create custom trackbar control
+- drag and drop
+- small adjustments with arrow keys or buttons
+- shows selected color larger above pointer
+put in WithoutHaste.Windows.GUI</t>
+  </si>
+  <si>
+    <t>edit palette: reorder</t>
+  </si>
+  <si>
+    <t xml:space="preserve">possible update to New Color Dialog
+change Hue selector into quarter-circle curve and nestles around the Saturation/Value selector</t>
+  </si>
+  <si>
+    <t xml:space="preserve">New Color Dialog
+- have Saturation/Value trackbars both start in upper-left at black</t>
+  </si>
+  <si>
     <t>remember last used directory (save or open) and default to there in file dialogs</t>
   </si>
   <si>
@@ -153,6 +174,12 @@
 - this will complicate scrollbars and color placement</t>
   </si>
   <si>
+    <t>8/15/2018</t>
+  </si>
+  <si>
+    <t>edit palette: possibly replace "add color" button with a default extra swatch at the end of the list with a "plus sign" on it</t>
+  </si>
+  <si>
     <t>how to programs auto-update?</t>
   </si>
   <si>
@@ -163,7 +190,50 @@
     <t>8/21/2018</t>
   </si>
   <si>
+    <t xml:space="preserve">look into this website about color formats
+http://colorizer.org/</t>
+  </si>
+  <si>
     <t>Done</t>
+  </si>
+  <si>
+    <t>remember last open palette and reopen it next time program starts</t>
+  </si>
+  <si>
+    <t>use SwatchPanel object for main palette display</t>
+  </si>
+  <si>
+    <t>change names of dialog-only forms to XDialog</t>
+  </si>
+  <si>
+    <t>entirely new palette</t>
+  </si>
+  <si>
+    <t>edit palette: undo/redo all changes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">edit palette: save changes
+see updates in main form
+- save or lose changes on close</t>
+  </si>
+  <si>
+    <t>edit palette: add new color, but start from existing color</t>
+  </si>
+  <si>
+    <t>edit palette: edit color in place</t>
+  </si>
+  <si>
+    <t>edit palette: remove color</t>
+  </si>
+  <si>
+    <t xml:space="preserve">open edit palette mode
+- add swatches</t>
+  </si>
+  <si>
+    <t>bug: expanded palette covers part of picturebox and statuspanel</t>
+  </si>
+  <si>
+    <t>undo, redo coloring a section on the image</t>
   </si>
   <si>
     <t xml:space="preserve">on error popup:
@@ -266,90 +336,6 @@
   </si>
   <si>
     <t>Bug</t>
-  </si>
-  <si>
-    <t xml:space="preserve">make a MasterImage class
-that one-time figures out all the regions in a background thread
-and provides that data to the color worker</t>
-  </si>
-  <si>
-    <t>use SwatchPanel object for main palette display</t>
-  </si>
-  <si>
-    <t>change names of dialog-only forms to XDialog</t>
-  </si>
-  <si>
-    <t xml:space="preserve">create custom trackbar control
-- drag and drop
-- small adjustments with arrow keys or buttons
-- shows selected color larger above pointer
-put in WithoutHaste.Windows.GUI</t>
-  </si>
-  <si>
-    <t>8/24/2018</t>
-  </si>
-  <si>
-    <t xml:space="preserve">possible update to New Color Dialog
-change Hue selector into quarter-circle curve and nestles around the Saturation/Value selector</t>
-  </si>
-  <si>
-    <t>refactor WithoutHaste.Drawing.Colors HSV to use ints instead of floats (0-360, 0-100, 0-100)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">look into this website about color formats
-http://colorizer.org/</t>
-  </si>
-  <si>
-    <t xml:space="preserve">New Color Dialog
-- have Saturation/Value trackbars both start in upper-left at black</t>
-  </si>
-  <si>
-    <t xml:space="preserve">edit palette: save changes
-see updates in main form
-- save or lose changes on close</t>
-  </si>
-  <si>
-    <t>edit palette: remove color</t>
-  </si>
-  <si>
-    <t>edit palette: edit color in place</t>
-  </si>
-  <si>
-    <t>edit palette: reorder</t>
-  </si>
-  <si>
-    <t>edit palette: undo/redo all changes</t>
-  </si>
-  <si>
-    <t>new color: enter an rgb value</t>
-  </si>
-  <si>
-    <t>new color: enter a hexadecimal value</t>
-  </si>
-  <si>
-    <t>new color: enter an hsv value</t>
-  </si>
-  <si>
-    <t xml:space="preserve">open edit palette mode
-- add swatches</t>
-  </si>
-  <si>
-    <t>edit palette: add new color, but start from existing color</t>
-  </si>
-  <si>
-    <t>edit palette: display rgb/hexdecimal/hsv values of selected color</t>
-  </si>
-  <si>
-    <t>entirely new palette</t>
-  </si>
-  <si>
-    <t>edit palette: on close, refresh main form palette based on what was just saved</t>
-  </si>
-  <si>
-    <t>edit palette: possibly replace "add color" button with a default extra swatch at the end of the list with a "plus sign" on it</t>
-  </si>
-  <si>
-    <t>remember last open palette and reopen it next time program starts</t>
   </si>
 </sst>
 </file>
@@ -402,7 +388,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:F36"/>
+  <dimension ref="A1:F35"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -448,7 +434,7 @@
         <v>35</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C3" s="0" t="s">
         <v>6</v>
@@ -457,15 +443,15 @@
         <v>7</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="0">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>91</v>
+        <v>11</v>
       </c>
       <c r="C4" s="0" t="s">
         <v>6</v>
@@ -474,15 +460,15 @@
         <v>7</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>72</v>
+        <v>12</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="0">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>87</v>
+        <v>13</v>
       </c>
       <c r="C5" s="0" t="s">
         <v>6</v>
@@ -491,15 +477,15 @@
         <v>7</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>72</v>
+        <v>12</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="0">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>82</v>
+        <v>14</v>
       </c>
       <c r="C6" s="0" t="s">
         <v>6</v>
@@ -508,15 +494,15 @@
         <v>7</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>72</v>
+        <v>12</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="0">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>83</v>
+        <v>15</v>
       </c>
       <c r="C7" s="0" t="s">
         <v>6</v>
@@ -525,15 +511,15 @@
         <v>7</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>72</v>
+        <v>12</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="0">
-        <v>69</v>
+        <v>50</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>84</v>
+        <v>16</v>
       </c>
       <c r="C8" s="0" t="s">
         <v>6</v>
@@ -542,15 +528,15 @@
         <v>7</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>72</v>
+        <v>17</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="0">
-        <v>50</v>
+        <v>34</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C9" s="0" t="s">
         <v>6</v>
@@ -559,15 +545,15 @@
         <v>7</v>
       </c>
       <c r="E9" s="0" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="0">
-        <v>34</v>
+        <v>59</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C10" s="0" t="s">
         <v>6</v>
@@ -576,15 +562,15 @@
         <v>7</v>
       </c>
       <c r="E10" s="0" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="0">
-        <v>59</v>
+        <v>49</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>74</v>
+        <v>21</v>
       </c>
       <c r="C11" s="0" t="s">
         <v>6</v>
@@ -593,15 +579,15 @@
         <v>7</v>
       </c>
       <c r="E11" s="0" t="s">
-        <v>72</v>
+        <v>17</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="0">
-        <v>49</v>
+        <v>21</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="C12" s="0" t="s">
         <v>6</v>
@@ -610,15 +596,15 @@
         <v>7</v>
       </c>
       <c r="E12" s="0" t="s">
-        <v>17</v>
+        <v>8</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="0">
-        <v>21</v>
+        <v>54</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="C13" s="0" t="s">
         <v>6</v>
@@ -627,15 +613,15 @@
         <v>7</v>
       </c>
       <c r="E13" s="0" t="s">
-        <v>8</v>
+        <v>24</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="0">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>68</v>
+        <v>25</v>
       </c>
       <c r="C14" s="0" t="s">
         <v>6</v>
@@ -644,15 +630,15 @@
         <v>7</v>
       </c>
       <c r="E14" s="0" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="0">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="C15" s="0" t="s">
         <v>6</v>
@@ -661,15 +647,15 @@
         <v>7</v>
       </c>
       <c r="E15" s="0" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="0">
-        <v>51</v>
+        <v>24</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="C16" s="0" t="s">
         <v>6</v>
@@ -678,15 +664,15 @@
         <v>7</v>
       </c>
       <c r="E16" s="0" t="s">
-        <v>17</v>
+        <v>8</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="0">
-        <v>24</v>
+        <v>52</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="C17" s="0" t="s">
         <v>6</v>
@@ -695,15 +681,15 @@
         <v>7</v>
       </c>
       <c r="E17" s="0" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="0">
-        <v>52</v>
+        <v>27</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="C18" s="0" t="s">
         <v>6</v>
@@ -712,15 +698,15 @@
         <v>7</v>
       </c>
       <c r="E18" s="0" t="s">
-        <v>17</v>
+        <v>8</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="0">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="C19" s="0" t="s">
         <v>6</v>
@@ -734,10 +720,10 @@
     </row>
     <row r="20">
       <c r="A20" s="0">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="C20" s="0" t="s">
         <v>6</v>
@@ -751,10 +737,10 @@
     </row>
     <row r="21">
       <c r="A21" s="0">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="C21" s="0" t="s">
         <v>6</v>
@@ -768,10 +754,10 @@
     </row>
     <row r="22">
       <c r="A22" s="0">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="C22" s="0" t="s">
         <v>6</v>
@@ -785,10 +771,10 @@
     </row>
     <row r="23">
       <c r="A23" s="0">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="C23" s="0" t="s">
         <v>6</v>
@@ -802,10 +788,10 @@
     </row>
     <row r="24">
       <c r="A24" s="0">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="C24" s="0" t="s">
         <v>6</v>
@@ -819,10 +805,10 @@
     </row>
     <row r="25">
       <c r="A25" s="0">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="C25" s="0" t="s">
         <v>6</v>
@@ -836,10 +822,10 @@
     </row>
     <row r="26">
       <c r="A26" s="0">
-        <v>25</v>
+        <v>57</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="C26" s="0" t="s">
         <v>6</v>
@@ -848,15 +834,15 @@
         <v>7</v>
       </c>
       <c r="E26" s="0" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="0">
-        <v>57</v>
+        <v>65</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>71</v>
+        <v>38</v>
       </c>
       <c r="C27" s="0" t="s">
         <v>6</v>
@@ -865,15 +851,15 @@
         <v>7</v>
       </c>
       <c r="E27" s="0" t="s">
-        <v>72</v>
+        <v>12</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="0">
-        <v>65</v>
+        <v>58</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>80</v>
+        <v>39</v>
       </c>
       <c r="C28" s="0" t="s">
         <v>6</v>
@@ -882,15 +868,15 @@
         <v>7</v>
       </c>
       <c r="E28" s="0" t="s">
-        <v>72</v>
+        <v>12</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="0">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>73</v>
+        <v>40</v>
       </c>
       <c r="C29" s="0" t="s">
         <v>6</v>
@@ -899,15 +885,15 @@
         <v>7</v>
       </c>
       <c r="E29" s="0" t="s">
-        <v>72</v>
+        <v>12</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="0">
-        <v>61</v>
+        <v>26</v>
       </c>
       <c r="B30" s="0" t="s">
-        <v>76</v>
+        <v>41</v>
       </c>
       <c r="C30" s="0" t="s">
         <v>6</v>
@@ -916,15 +902,15 @@
         <v>7</v>
       </c>
       <c r="E30" s="0" t="s">
-        <v>72</v>
+        <v>8</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="0">
-        <v>26</v>
+        <v>43</v>
       </c>
       <c r="B31" s="0" t="s">
-        <v>34</v>
+        <v>42</v>
       </c>
       <c r="C31" s="0" t="s">
         <v>6</v>
@@ -933,15 +919,15 @@
         <v>7</v>
       </c>
       <c r="E31" s="0" t="s">
-        <v>8</v>
+        <v>43</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="0">
-        <v>43</v>
+        <v>74</v>
       </c>
       <c r="B32" s="0" t="s">
-        <v>35</v>
+        <v>44</v>
       </c>
       <c r="C32" s="0" t="s">
         <v>6</v>
@@ -955,10 +941,10 @@
     </row>
     <row r="33">
       <c r="A33" s="0">
-        <v>74</v>
+        <v>29</v>
       </c>
       <c r="B33" s="0" t="s">
-        <v>90</v>
+        <v>45</v>
       </c>
       <c r="C33" s="0" t="s">
         <v>6</v>
@@ -967,15 +953,15 @@
         <v>7</v>
       </c>
       <c r="E33" s="0" t="s">
-        <v>72</v>
+        <v>8</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="0">
-        <v>29</v>
+        <v>47</v>
       </c>
       <c r="B34" s="0" t="s">
-        <v>36</v>
+        <v>46</v>
       </c>
       <c r="C34" s="0" t="s">
         <v>6</v>
@@ -984,15 +970,15 @@
         <v>7</v>
       </c>
       <c r="E34" s="0" t="s">
-        <v>8</v>
+        <v>47</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="0">
-        <v>47</v>
+        <v>60</v>
       </c>
       <c r="B35" s="0" t="s">
-        <v>37</v>
+        <v>48</v>
       </c>
       <c r="C35" s="0" t="s">
         <v>6</v>
@@ -1001,24 +987,7 @@
         <v>7</v>
       </c>
       <c r="E35" s="0" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="36">
-      <c r="A36" s="0">
-        <v>60</v>
-      </c>
-      <c r="B36" s="0" t="s">
-        <v>75</v>
-      </c>
-      <c r="C36" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="D36" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="E36" s="0" t="s">
-        <v>72</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>
@@ -1028,7 +997,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:F33"/>
+  <dimension ref="A1:F34"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1051,264 +1020,264 @@
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>39</v>
+        <v>49</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="0">
-        <v>55</v>
+        <v>75</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>69</v>
+        <v>50</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>39</v>
+        <v>49</v>
       </c>
       <c r="D2" s="0" t="s">
         <v>7</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>22</v>
+        <v>12</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>72</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="0">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>70</v>
+        <v>51</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>39</v>
+        <v>49</v>
       </c>
       <c r="D3" s="0" t="s">
         <v>7</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="F3" s="0" t="s">
-        <v>72</v>
+        <v>12</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="0">
-        <v>72</v>
+        <v>56</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>88</v>
+        <v>52</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>39</v>
+        <v>49</v>
       </c>
       <c r="D4" s="0" t="s">
         <v>7</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>72</v>
+        <v>24</v>
       </c>
       <c r="F4" s="0" t="s">
-        <v>72</v>
+        <v>12</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="0">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>81</v>
+        <v>53</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>39</v>
+        <v>49</v>
       </c>
       <c r="D5" s="0" t="s">
         <v>7</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>72</v>
+        <v>12</v>
       </c>
       <c r="F5" s="0" t="s">
-        <v>72</v>
+        <v>12</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="0">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>77</v>
+        <v>54</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>39</v>
+        <v>49</v>
       </c>
       <c r="D6" s="0" t="s">
         <v>7</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>72</v>
+        <v>12</v>
       </c>
       <c r="F6" s="0" t="s">
-        <v>72</v>
+        <v>12</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="0">
-        <v>70</v>
+        <v>62</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>86</v>
+        <v>55</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>39</v>
+        <v>49</v>
       </c>
       <c r="D7" s="0" t="s">
         <v>7</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>72</v>
+        <v>12</v>
       </c>
       <c r="F7" s="0" t="s">
-        <v>72</v>
+        <v>12</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="0">
-        <v>64</v>
+        <v>70</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>79</v>
+        <v>56</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>39</v>
+        <v>49</v>
       </c>
       <c r="D8" s="0" t="s">
         <v>7</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>72</v>
+        <v>12</v>
       </c>
       <c r="F8" s="0" t="s">
-        <v>72</v>
+        <v>12</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="0">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>78</v>
+        <v>57</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>39</v>
+        <v>49</v>
       </c>
       <c r="D9" s="0" t="s">
         <v>7</v>
       </c>
       <c r="E9" s="0" t="s">
-        <v>72</v>
+        <v>12</v>
       </c>
       <c r="F9" s="0" t="s">
-        <v>72</v>
+        <v>12</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="0">
-        <v>13</v>
+        <v>63</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>85</v>
+        <v>58</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>39</v>
+        <v>49</v>
       </c>
       <c r="D10" s="0" t="s">
         <v>7</v>
       </c>
       <c r="E10" s="0" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="F10" s="0" t="s">
-        <v>72</v>
+        <v>12</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="0">
-        <v>42</v>
+        <v>13</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>11</v>
+        <v>59</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>39</v>
+        <v>49</v>
       </c>
       <c r="D11" s="0" t="s">
         <v>7</v>
       </c>
       <c r="E11" s="0" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="F11" s="0" t="s">
-        <v>22</v>
+        <v>12</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="0">
-        <v>33</v>
+        <v>42</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>9</v>
+        <v>60</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>39</v>
+        <v>49</v>
       </c>
       <c r="D12" s="0" t="s">
         <v>7</v>
       </c>
       <c r="E12" s="0" t="s">
-        <v>10</v>
+        <v>43</v>
       </c>
       <c r="F12" s="0" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="0">
-        <v>48</v>
+        <v>33</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>40</v>
+        <v>61</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>39</v>
+        <v>49</v>
       </c>
       <c r="D13" s="0" t="s">
         <v>7</v>
       </c>
       <c r="E13" s="0" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="F13" s="0" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="0">
-        <v>37</v>
+        <v>48</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>41</v>
+        <v>62</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>39</v>
+        <v>49</v>
       </c>
       <c r="D14" s="0" t="s">
         <v>7</v>
       </c>
       <c r="E14" s="0" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="F14" s="0" t="s">
         <v>17</v>
@@ -1316,193 +1285,193 @@
     </row>
     <row r="15">
       <c r="A15" s="0">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>42</v>
+        <v>63</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>39</v>
+        <v>49</v>
       </c>
       <c r="D15" s="0" t="s">
         <v>7</v>
       </c>
       <c r="E15" s="0" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="F15" s="0" t="s">
-        <v>38</v>
+        <v>17</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="0">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>43</v>
+        <v>64</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>39</v>
+        <v>49</v>
       </c>
       <c r="D16" s="0" t="s">
         <v>7</v>
       </c>
       <c r="E16" s="0" t="s">
-        <v>44</v>
+        <v>10</v>
       </c>
       <c r="F16" s="0" t="s">
-        <v>38</v>
+        <v>47</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="0">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>45</v>
+        <v>65</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>39</v>
+        <v>49</v>
       </c>
       <c r="D17" s="0" t="s">
         <v>7</v>
       </c>
       <c r="E17" s="0" t="s">
-        <v>12</v>
+        <v>66</v>
       </c>
       <c r="F17" s="0" t="s">
-        <v>38</v>
+        <v>47</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="0">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>46</v>
+        <v>67</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>39</v>
+        <v>49</v>
       </c>
       <c r="D18" s="0" t="s">
         <v>7</v>
       </c>
       <c r="E18" s="0" t="s">
-        <v>12</v>
+        <v>43</v>
       </c>
       <c r="F18" s="0" t="s">
-        <v>38</v>
+        <v>47</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="0">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="B19" s="0" t="s">
+        <v>68</v>
+      </c>
+      <c r="C19" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="D19" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E19" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="F19" s="0" t="s">
         <v>47</v>
-      </c>
-      <c r="C19" s="0" t="s">
-        <v>39</v>
-      </c>
-      <c r="D19" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="E19" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="F19" s="0" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="0">
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>48</v>
+        <v>69</v>
       </c>
       <c r="C20" s="0" t="s">
-        <v>39</v>
+        <v>49</v>
       </c>
       <c r="D20" s="0" t="s">
         <v>7</v>
       </c>
       <c r="E20" s="0" t="s">
-        <v>14</v>
+        <v>43</v>
       </c>
       <c r="F20" s="0" t="s">
-        <v>44</v>
+        <v>66</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="0">
-        <v>11</v>
+        <v>36</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>49</v>
+        <v>70</v>
       </c>
       <c r="C21" s="0" t="s">
-        <v>39</v>
+        <v>49</v>
       </c>
       <c r="D21" s="0" t="s">
         <v>7</v>
       </c>
       <c r="E21" s="0" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="F21" s="0" t="s">
-        <v>12</v>
+        <v>66</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="0">
-        <v>40</v>
+        <v>11</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>50</v>
+        <v>71</v>
       </c>
       <c r="C22" s="0" t="s">
-        <v>39</v>
+        <v>49</v>
       </c>
       <c r="D22" s="0" t="s">
         <v>7</v>
       </c>
       <c r="E22" s="0" t="s">
-        <v>51</v>
+        <v>8</v>
       </c>
       <c r="F22" s="0" t="s">
-        <v>12</v>
+        <v>43</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="0">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>52</v>
+        <v>72</v>
       </c>
       <c r="C23" s="0" t="s">
-        <v>39</v>
+        <v>49</v>
       </c>
       <c r="D23" s="0" t="s">
         <v>7</v>
       </c>
       <c r="E23" s="0" t="s">
-        <v>14</v>
+        <v>73</v>
       </c>
       <c r="F23" s="0" t="s">
-        <v>12</v>
+        <v>43</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="0">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>53</v>
+        <v>74</v>
       </c>
       <c r="C24" s="0" t="s">
-        <v>39</v>
+        <v>49</v>
       </c>
       <c r="D24" s="0" t="s">
         <v>7</v>
@@ -1511,24 +1480,24 @@
         <v>10</v>
       </c>
       <c r="F24" s="0" t="s">
-        <v>14</v>
+        <v>43</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="0">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>54</v>
+        <v>75</v>
       </c>
       <c r="C25" s="0" t="s">
-        <v>39</v>
+        <v>49</v>
       </c>
       <c r="D25" s="0" t="s">
         <v>7</v>
       </c>
       <c r="E25" s="0" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="F25" s="0" t="s">
         <v>10</v>
@@ -1536,33 +1505,33 @@
     </row>
     <row r="26">
       <c r="A26" s="0">
-        <v>20</v>
+        <v>31</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>55</v>
+        <v>76</v>
       </c>
       <c r="C26" s="0" t="s">
-        <v>39</v>
+        <v>49</v>
       </c>
       <c r="D26" s="0" t="s">
         <v>7</v>
       </c>
       <c r="E26" s="0" t="s">
-        <v>8</v>
+        <v>19</v>
       </c>
       <c r="F26" s="0" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="0">
-        <v>9</v>
+        <v>20</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>56</v>
+        <v>77</v>
       </c>
       <c r="C27" s="0" t="s">
-        <v>39</v>
+        <v>49</v>
       </c>
       <c r="D27" s="0" t="s">
         <v>7</v>
@@ -1571,18 +1540,18 @@
         <v>8</v>
       </c>
       <c r="F27" s="0" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="0">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>57</v>
+        <v>78</v>
       </c>
       <c r="C28" s="0" t="s">
-        <v>39</v>
+        <v>49</v>
       </c>
       <c r="D28" s="0" t="s">
         <v>7</v>
@@ -1591,18 +1560,18 @@
         <v>8</v>
       </c>
       <c r="F28" s="0" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="0">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>58</v>
+        <v>79</v>
       </c>
       <c r="C29" s="0" t="s">
-        <v>39</v>
+        <v>49</v>
       </c>
       <c r="D29" s="0" t="s">
         <v>7</v>
@@ -1611,18 +1580,18 @@
         <v>8</v>
       </c>
       <c r="F29" s="0" t="s">
-        <v>59</v>
+        <v>19</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="0">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B30" s="0" t="s">
-        <v>60</v>
+        <v>80</v>
       </c>
       <c r="C30" s="0" t="s">
-        <v>39</v>
+        <v>49</v>
       </c>
       <c r="D30" s="0" t="s">
         <v>7</v>
@@ -1631,18 +1600,18 @@
         <v>8</v>
       </c>
       <c r="F30" s="0" t="s">
-        <v>8</v>
+        <v>81</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="0">
-        <v>30</v>
+        <v>3</v>
       </c>
       <c r="B31" s="0" t="s">
-        <v>61</v>
+        <v>82</v>
       </c>
       <c r="C31" s="0" t="s">
-        <v>39</v>
+        <v>49</v>
       </c>
       <c r="D31" s="0" t="s">
         <v>7</v>
@@ -1656,13 +1625,13 @@
     </row>
     <row r="32">
       <c r="A32" s="0">
-        <v>2</v>
+        <v>30</v>
       </c>
       <c r="B32" s="0" t="s">
-        <v>62</v>
+        <v>83</v>
       </c>
       <c r="C32" s="0" t="s">
-        <v>39</v>
+        <v>49</v>
       </c>
       <c r="D32" s="0" t="s">
         <v>7</v>
@@ -1676,21 +1645,41 @@
     </row>
     <row r="33">
       <c r="A33" s="0">
+        <v>2</v>
+      </c>
+      <c r="B33" s="0" t="s">
+        <v>84</v>
+      </c>
+      <c r="C33" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="D33" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E33" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="F33" s="0" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="0">
         <v>1</v>
       </c>
-      <c r="B33" s="0" t="s">
-        <v>63</v>
-      </c>
-      <c r="C33" s="0" t="s">
-        <v>39</v>
-      </c>
-      <c r="D33" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="E33" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="F33" s="0" t="s">
+      <c r="B34" s="0" t="s">
+        <v>85</v>
+      </c>
+      <c r="C34" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="D34" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E34" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="F34" s="0" t="s">
         <v>8</v>
       </c>
     </row>
@@ -1712,7 +1701,7 @@
         <v>2</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>64</v>
+        <v>86</v>
       </c>
       <c r="C1" s="2"/>
       <c r="D1" s="2" t="s">
@@ -1720,7 +1709,7 @@
       </c>
       <c r="E1" s="2"/>
       <c r="F1" s="2" t="s">
-        <v>65</v>
+        <v>87</v>
       </c>
     </row>
     <row r="2">
@@ -1728,7 +1717,7 @@
         <v>6</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>64</v>
+        <v>86</v>
       </c>
       <c r="D2" s="0" t="s">
         <v>7</v>
@@ -1739,13 +1728,13 @@
     </row>
     <row r="3">
       <c r="A3" s="0" t="s">
-        <v>39</v>
+        <v>49</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>66</v>
+        <v>88</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>67</v>
+        <v>89</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
refactor: icon manager into fully static interface
</commit_message>
<xml_diff>
--- a/paint_todo.xlsx
+++ b/paint_todo.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="91">
   <si>
     <t>Id</t>
   </si>
@@ -336,6 +336,10 @@
   </si>
   <si>
     <t>Bug</t>
+  </si>
+  <si>
+    <t xml:space="preserve">edit palette: possibly replace "add color" button with a default extra swatch at the end of the list with a "plus sign" on it
+or a "plus" icon in the toolbar</t>
   </si>
 </sst>
 </file>
@@ -927,7 +931,7 @@
         <v>74</v>
       </c>
       <c r="B32" s="0" t="s">
-        <v>44</v>
+        <v>90</v>
       </c>
       <c r="C32" s="0" t="s">
         <v>6</v>

</xml_diff>

<commit_message>
support palette format .pal
</commit_message>
<xml_diff>
--- a/paint_todo.xlsx
+++ b/paint_todo.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="98">
   <si>
     <t>Id</t>
   </si>
@@ -340,6 +340,32 @@
   <si>
     <t xml:space="preserve">edit palette: possibly replace "add color" button with a default extra swatch at the end of the list with a "plus sign" on it
 or a "plus" icon in the toolbar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">prompt to save if image has changed since last save
+- on closing program
+- on opening new image
+Add this tracking to MasterImage class</t>
+  </si>
+  <si>
+    <t>full documentation</t>
+  </si>
+  <si>
+    <t>full documentation of Perpetual Paint</t>
+  </si>
+  <si>
+    <t>full documentation of support library Colors</t>
+  </si>
+  <si>
+    <t>full documentation of support library GUI</t>
+  </si>
+  <si>
+    <t>documentation: include request for sample palette files for the specific formats/color spaces I can't verify because I don't have a test file to load</t>
+  </si>
+  <si>
+    <t xml:space="preserve">documentation: include request for sample palette files for the specific formats/color spaces I can't verify because I don't have a test file to load
+- maybe in the actual error messages from the library, too
+- like, send me the file you are trying to read so I can add support for it</t>
   </si>
 </sst>
 </file>
@@ -392,7 +418,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:F34"/>
+  <dimension ref="A1:F38"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -625,7 +651,7 @@
         <v>53</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>25</v>
+        <v>91</v>
       </c>
       <c r="C14" s="0" t="s">
         <v>6</v>
@@ -656,10 +682,10 @@
     </row>
     <row r="16">
       <c r="A16" s="0">
-        <v>52</v>
+        <v>76</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>28</v>
+        <v>93</v>
       </c>
       <c r="C16" s="0" t="s">
         <v>6</v>
@@ -668,15 +694,15 @@
         <v>7</v>
       </c>
       <c r="E16" s="0" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="0">
-        <v>27</v>
+        <v>79</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>29</v>
+        <v>97</v>
       </c>
       <c r="C17" s="0" t="s">
         <v>6</v>
@@ -685,15 +711,15 @@
         <v>7</v>
       </c>
       <c r="E17" s="0" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="0">
-        <v>28</v>
+        <v>77</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>30</v>
+        <v>94</v>
       </c>
       <c r="C18" s="0" t="s">
         <v>6</v>
@@ -702,15 +728,15 @@
         <v>7</v>
       </c>
       <c r="E18" s="0" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="0">
-        <v>19</v>
+        <v>78</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>31</v>
+        <v>95</v>
       </c>
       <c r="C19" s="0" t="s">
         <v>6</v>
@@ -719,15 +745,15 @@
         <v>7</v>
       </c>
       <c r="E19" s="0" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="0">
-        <v>22</v>
+        <v>52</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="C20" s="0" t="s">
         <v>6</v>
@@ -736,15 +762,15 @@
         <v>7</v>
       </c>
       <c r="E20" s="0" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="0">
-        <v>16</v>
+        <v>27</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="C21" s="0" t="s">
         <v>6</v>
@@ -758,10 +784,10 @@
     </row>
     <row r="22">
       <c r="A22" s="0">
-        <v>17</v>
+        <v>28</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="C22" s="0" t="s">
         <v>6</v>
@@ -775,10 +801,10 @@
     </row>
     <row r="23">
       <c r="A23" s="0">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="C23" s="0" t="s">
         <v>6</v>
@@ -792,10 +818,10 @@
     </row>
     <row r="24">
       <c r="A24" s="0">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="C24" s="0" t="s">
         <v>6</v>
@@ -809,10 +835,10 @@
     </row>
     <row r="25">
       <c r="A25" s="0">
-        <v>57</v>
+        <v>16</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="C25" s="0" t="s">
         <v>6</v>
@@ -821,15 +847,15 @@
         <v>7</v>
       </c>
       <c r="E25" s="0" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="0">
-        <v>65</v>
+        <v>17</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="C26" s="0" t="s">
         <v>6</v>
@@ -838,15 +864,15 @@
         <v>7</v>
       </c>
       <c r="E26" s="0" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="0">
-        <v>58</v>
+        <v>18</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="C27" s="0" t="s">
         <v>6</v>
@@ -855,15 +881,15 @@
         <v>7</v>
       </c>
       <c r="E27" s="0" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="0">
-        <v>61</v>
+        <v>25</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="C28" s="0" t="s">
         <v>6</v>
@@ -872,15 +898,15 @@
         <v>7</v>
       </c>
       <c r="E28" s="0" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="0">
-        <v>26</v>
+        <v>57</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="C29" s="0" t="s">
         <v>6</v>
@@ -889,15 +915,15 @@
         <v>7</v>
       </c>
       <c r="E29" s="0" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="0">
-        <v>43</v>
+        <v>65</v>
       </c>
       <c r="B30" s="0" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="C30" s="0" t="s">
         <v>6</v>
@@ -906,15 +932,15 @@
         <v>7</v>
       </c>
       <c r="E30" s="0" t="s">
-        <v>43</v>
+        <v>12</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="0">
-        <v>74</v>
+        <v>58</v>
       </c>
       <c r="B31" s="0" t="s">
-        <v>90</v>
+        <v>39</v>
       </c>
       <c r="C31" s="0" t="s">
         <v>6</v>
@@ -928,10 +954,10 @@
     </row>
     <row r="32">
       <c r="A32" s="0">
-        <v>29</v>
+        <v>61</v>
       </c>
       <c r="B32" s="0" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="C32" s="0" t="s">
         <v>6</v>
@@ -940,15 +966,15 @@
         <v>7</v>
       </c>
       <c r="E32" s="0" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="0">
-        <v>47</v>
+        <v>26</v>
       </c>
       <c r="B33" s="0" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="C33" s="0" t="s">
         <v>6</v>
@@ -957,23 +983,91 @@
         <v>7</v>
       </c>
       <c r="E33" s="0" t="s">
-        <v>47</v>
+        <v>8</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="0">
+        <v>43</v>
+      </c>
+      <c r="B34" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="C34" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D34" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E34" s="0" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="0">
+        <v>74</v>
+      </c>
+      <c r="B35" s="0" t="s">
+        <v>90</v>
+      </c>
+      <c r="C35" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D35" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E35" s="0" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="0">
+        <v>29</v>
+      </c>
+      <c r="B36" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="C36" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D36" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E36" s="0" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" s="0">
+        <v>47</v>
+      </c>
+      <c r="B37" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="C37" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D37" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E37" s="0" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" s="0">
         <v>60</v>
       </c>
-      <c r="B34" s="0" t="s">
+      <c r="B38" s="0" t="s">
         <v>48</v>
       </c>
-      <c r="C34" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="D34" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="E34" s="0" t="s">
+      <c r="C38" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D38" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E38" s="0" t="s">
         <v>12</v>
       </c>
     </row>
@@ -1730,7 +1824,7 @@
         <v>7</v>
       </c>
       <c r="F2" s="0">
-        <v>75</v>
+        <v>79</v>
       </c>
     </row>
     <row r="3">

</xml_diff>

<commit_message>
edit palette: display different format data for selected color
</commit_message>
<xml_diff>
--- a/paint_todo.xlsx
+++ b/paint_todo.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="102">
   <si>
     <t>Id</t>
   </si>
@@ -102,16 +102,29 @@
   <si>
     <t xml:space="preserve">prompt to save if image has changed since last save
 - on closing program
-- on opening new image</t>
+- on opening new image
+Add this tracking to MasterImage class</t>
   </si>
   <si>
     <t>replace Rabbit with smaller and better divided image</t>
   </si>
   <si>
-    <t xml:space="preserve">remember windows size from last closing
-- full screen vs not
-- default not-full-screen size
-open with this size</t>
+    <t>full documentation of Perpetual Paint</t>
+  </si>
+  <si>
+    <t xml:space="preserve">documentation: include request for sample palette files for the specific formats/color spaces I can't verify because I don't have a test file to load
+- maybe in the actual error messages from the library, too
+- like, send me the file you are trying to read so I can add support for it</t>
+  </si>
+  <si>
+    <t xml:space="preserve">in Paint documenation
+describe the use-case of converting between palette formats: open file, edit palette, save as new format</t>
+  </si>
+  <si>
+    <t>full documentation of support library Colors</t>
+  </si>
+  <si>
+    <t>full documentation of support library GUI</t>
   </si>
   <si>
     <t xml:space="preserve">in documentation
@@ -144,6 +157,22 @@
   </si>
   <si>
     <t>update website with project, landing page, and links</t>
+  </si>
+  <si>
+    <t>VERSION 1.5: PROJECTS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">secondary optional form
+open multiple files
+select one to see and edit in main form</t>
+  </si>
+  <si>
+    <t xml:space="preserve">save project:
+- list of images
+- a palette</t>
+  </si>
+  <si>
+    <t>open project</t>
   </si>
   <si>
     <t>EVERYTHING BELOW HERE IS VERSION 2</t>
@@ -177,7 +206,8 @@
     <t>8/15/2018</t>
   </si>
   <si>
-    <t>edit palette: possibly replace "add color" button with a default extra swatch at the end of the list with a "plus sign" on it</t>
+    <t xml:space="preserve">edit palette: possibly replace "add color" button with a default extra swatch at the end of the list with a "plus sign" on it
+or a "plus" icon in the toolbar</t>
   </si>
   <si>
     <t>how to programs auto-update?</t>
@@ -195,6 +225,12 @@
   </si>
   <si>
     <t>Done</t>
+  </si>
+  <si>
+    <t xml:space="preserve">remember windows size from last closing
+- full screen vs not
+- default not-full-screen size
+open with this size</t>
   </si>
   <si>
     <t>remember last open palette and reopen it next time program starts</t>
@@ -338,38 +374,17 @@
     <t>Bug</t>
   </si>
   <si>
-    <t xml:space="preserve">edit palette: possibly replace "add color" button with a default extra swatch at the end of the list with a "plus sign" on it
-or a "plus" icon in the toolbar</t>
-  </si>
-  <si>
-    <t xml:space="preserve">prompt to save if image has changed since last save
-- on closing program
-- on opening new image
-Add this tracking to MasterImage class</t>
-  </si>
-  <si>
-    <t>full documentation</t>
-  </si>
-  <si>
-    <t>full documentation of Perpetual Paint</t>
-  </si>
-  <si>
-    <t>full documentation of support library Colors</t>
-  </si>
-  <si>
-    <t>full documentation of support library GUI</t>
-  </si>
-  <si>
-    <t>documentation: include request for sample palette files for the specific formats/color spaces I can't verify because I don't have a test file to load</t>
-  </si>
-  <si>
-    <t xml:space="preserve">documentation: include request for sample palette files for the specific formats/color spaces I can't verify because I don't have a test file to load
-- maybe in the actual error messages from the library, too
-- like, send me the file you are trying to read so I can add support for it</t>
-  </si>
-  <si>
-    <t xml:space="preserve">in Paint documenation
-describe the use-case of converting between palette formats: open file, edit palette, save as new format</t>
+    <t xml:space="preserve">save project:
+- list of images
+- a palette
+select a file format to use, save in plain text</t>
+  </si>
+  <si>
+    <t>put in top of documentation that program is being actively developed, so open to bug reports and feature requests</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bug: Palette &gt; New &gt; Done
+get error because no filename to open in main form</t>
   </si>
 </sst>
 </file>
@@ -422,7 +437,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:F39"/>
+  <dimension ref="A1:F43"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -448,10 +463,10 @@
     </row>
     <row r="2">
       <c r="A2" s="0">
-        <v>23</v>
+        <v>35</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="C2" s="0" t="s">
         <v>6</v>
@@ -460,15 +475,15 @@
         <v>7</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="0">
-        <v>35</v>
+        <v>67</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="C3" s="0" t="s">
         <v>6</v>
@@ -477,15 +492,15 @@
         <v>7</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="0">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="C4" s="0" t="s">
         <v>6</v>
@@ -499,10 +514,10 @@
     </row>
     <row r="5">
       <c r="A5" s="0">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C5" s="0" t="s">
         <v>6</v>
@@ -516,10 +531,10 @@
     </row>
     <row r="6">
       <c r="A6" s="0">
-        <v>68</v>
+        <v>50</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C6" s="0" t="s">
         <v>6</v>
@@ -528,15 +543,15 @@
         <v>7</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="0">
-        <v>69</v>
+        <v>34</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="C7" s="0" t="s">
         <v>6</v>
@@ -545,15 +560,15 @@
         <v>7</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="0">
-        <v>50</v>
+        <v>59</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="C8" s="0" t="s">
         <v>6</v>
@@ -562,15 +577,15 @@
         <v>7</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="0">
-        <v>34</v>
+        <v>49</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="C9" s="0" t="s">
         <v>6</v>
@@ -579,15 +594,15 @@
         <v>7</v>
       </c>
       <c r="E9" s="0" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="0">
-        <v>59</v>
+        <v>21</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="C10" s="0" t="s">
         <v>6</v>
@@ -596,15 +611,15 @@
         <v>7</v>
       </c>
       <c r="E10" s="0" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="0">
-        <v>49</v>
+        <v>86</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>21</v>
+        <v>101</v>
       </c>
       <c r="C11" s="0" t="s">
         <v>6</v>
@@ -613,15 +628,15 @@
         <v>7</v>
       </c>
       <c r="E11" s="0" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="0">
-        <v>21</v>
+        <v>54</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C12" s="0" t="s">
         <v>6</v>
@@ -630,15 +645,15 @@
         <v>7</v>
       </c>
       <c r="E12" s="0" t="s">
-        <v>8</v>
+        <v>24</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="0">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="C13" s="0" t="s">
         <v>6</v>
@@ -652,10 +667,10 @@
     </row>
     <row r="14">
       <c r="A14" s="0">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>91</v>
+        <v>26</v>
       </c>
       <c r="C14" s="0" t="s">
         <v>6</v>
@@ -664,15 +679,15 @@
         <v>7</v>
       </c>
       <c r="E14" s="0" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="0">
-        <v>51</v>
+        <v>76</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C15" s="0" t="s">
         <v>6</v>
@@ -681,15 +696,15 @@
         <v>7</v>
       </c>
       <c r="E15" s="0" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="0">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>93</v>
+        <v>28</v>
       </c>
       <c r="C16" s="0" t="s">
         <v>6</v>
@@ -703,10 +718,10 @@
     </row>
     <row r="17">
       <c r="A17" s="0">
-        <v>79</v>
+        <v>85</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="C17" s="0" t="s">
         <v>6</v>
@@ -723,7 +738,7 @@
         <v>80</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>98</v>
+        <v>29</v>
       </c>
       <c r="C18" s="0" t="s">
         <v>6</v>
@@ -740,7 +755,7 @@
         <v>77</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>94</v>
+        <v>30</v>
       </c>
       <c r="C19" s="0" t="s">
         <v>6</v>
@@ -757,7 +772,7 @@
         <v>78</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>95</v>
+        <v>31</v>
       </c>
       <c r="C20" s="0" t="s">
         <v>6</v>
@@ -774,7 +789,7 @@
         <v>52</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="C21" s="0" t="s">
         <v>6</v>
@@ -791,7 +806,7 @@
         <v>27</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="C22" s="0" t="s">
         <v>6</v>
@@ -808,7 +823,7 @@
         <v>28</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="C23" s="0" t="s">
         <v>6</v>
@@ -825,7 +840,7 @@
         <v>19</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="C24" s="0" t="s">
         <v>6</v>
@@ -842,7 +857,7 @@
         <v>22</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="C25" s="0" t="s">
         <v>6</v>
@@ -859,7 +874,7 @@
         <v>16</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="C26" s="0" t="s">
         <v>6</v>
@@ -876,7 +891,7 @@
         <v>17</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="C27" s="0" t="s">
         <v>6</v>
@@ -893,7 +908,7 @@
         <v>18</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="C28" s="0" t="s">
         <v>6</v>
@@ -907,10 +922,10 @@
     </row>
     <row r="29">
       <c r="A29" s="0">
-        <v>25</v>
+        <v>81</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="C29" s="0" t="s">
         <v>6</v>
@@ -919,15 +934,15 @@
         <v>7</v>
       </c>
       <c r="E29" s="0" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="0">
-        <v>57</v>
+        <v>82</v>
       </c>
       <c r="B30" s="0" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="C30" s="0" t="s">
         <v>6</v>
@@ -941,10 +956,10 @@
     </row>
     <row r="31">
       <c r="A31" s="0">
-        <v>65</v>
+        <v>83</v>
       </c>
       <c r="B31" s="0" t="s">
-        <v>38</v>
+        <v>99</v>
       </c>
       <c r="C31" s="0" t="s">
         <v>6</v>
@@ -958,10 +973,10 @@
     </row>
     <row r="32">
       <c r="A32" s="0">
-        <v>58</v>
+        <v>84</v>
       </c>
       <c r="B32" s="0" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="C32" s="0" t="s">
         <v>6</v>
@@ -975,10 +990,10 @@
     </row>
     <row r="33">
       <c r="A33" s="0">
-        <v>61</v>
+        <v>25</v>
       </c>
       <c r="B33" s="0" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="C33" s="0" t="s">
         <v>6</v>
@@ -987,15 +1002,15 @@
         <v>7</v>
       </c>
       <c r="E33" s="0" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="0">
-        <v>26</v>
+        <v>57</v>
       </c>
       <c r="B34" s="0" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="C34" s="0" t="s">
         <v>6</v>
@@ -1004,15 +1019,15 @@
         <v>7</v>
       </c>
       <c r="E34" s="0" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="0">
-        <v>43</v>
+        <v>65</v>
       </c>
       <c r="B35" s="0" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="C35" s="0" t="s">
         <v>6</v>
@@ -1021,15 +1036,15 @@
         <v>7</v>
       </c>
       <c r="E35" s="0" t="s">
-        <v>43</v>
+        <v>12</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="0">
-        <v>74</v>
+        <v>58</v>
       </c>
       <c r="B36" s="0" t="s">
-        <v>90</v>
+        <v>47</v>
       </c>
       <c r="C36" s="0" t="s">
         <v>6</v>
@@ -1043,10 +1058,10 @@
     </row>
     <row r="37">
       <c r="A37" s="0">
-        <v>29</v>
+        <v>61</v>
       </c>
       <c r="B37" s="0" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="C37" s="0" t="s">
         <v>6</v>
@@ -1055,15 +1070,15 @@
         <v>7</v>
       </c>
       <c r="E37" s="0" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="0">
-        <v>47</v>
+        <v>26</v>
       </c>
       <c r="B38" s="0" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="C38" s="0" t="s">
         <v>6</v>
@@ -1072,23 +1087,91 @@
         <v>7</v>
       </c>
       <c r="E38" s="0" t="s">
-        <v>47</v>
+        <v>8</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="0">
+        <v>43</v>
+      </c>
+      <c r="B39" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="C39" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D39" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E39" s="0" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" s="0">
+        <v>74</v>
+      </c>
+      <c r="B40" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="C40" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D40" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E40" s="0" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" s="0">
+        <v>29</v>
+      </c>
+      <c r="B41" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="C41" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D41" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E41" s="0" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" s="0">
+        <v>47</v>
+      </c>
+      <c r="B42" s="0" t="s">
+        <v>54</v>
+      </c>
+      <c r="C42" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D42" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E42" s="0" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" s="0">
         <v>60</v>
       </c>
-      <c r="B39" s="0" t="s">
-        <v>48</v>
-      </c>
-      <c r="C39" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="D39" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="E39" s="0" t="s">
+      <c r="B43" s="0" t="s">
+        <v>56</v>
+      </c>
+      <c r="C43" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D43" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E43" s="0" t="s">
         <v>12</v>
       </c>
     </row>
@@ -1099,7 +1182,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:F35"/>
+  <dimension ref="A1:F36"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1122,24 +1205,24 @@
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>49</v>
+        <v>57</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="0">
-        <v>24</v>
+        <v>71</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>27</v>
+        <v>11</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>49</v>
+        <v>57</v>
       </c>
       <c r="D2" s="0" t="s">
         <v>7</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="F2" s="0" t="s">
         <v>12</v>
@@ -1147,19 +1230,19 @@
     </row>
     <row r="3">
       <c r="A3" s="0">
-        <v>75</v>
+        <v>24</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>50</v>
+        <v>58</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>49</v>
+        <v>57</v>
       </c>
       <c r="D3" s="0" t="s">
         <v>7</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="F3" s="0" t="s">
         <v>12</v>
@@ -1167,19 +1250,19 @@
     </row>
     <row r="4">
       <c r="A4" s="0">
-        <v>55</v>
+        <v>75</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>51</v>
+        <v>59</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>49</v>
+        <v>57</v>
       </c>
       <c r="D4" s="0" t="s">
         <v>7</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="F4" s="0" t="s">
         <v>12</v>
@@ -1187,13 +1270,13 @@
     </row>
     <row r="5">
       <c r="A5" s="0">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>52</v>
+        <v>60</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>49</v>
+        <v>57</v>
       </c>
       <c r="D5" s="0" t="s">
         <v>7</v>
@@ -1207,19 +1290,19 @@
     </row>
     <row r="6">
       <c r="A6" s="0">
-        <v>72</v>
+        <v>56</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>53</v>
+        <v>61</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>49</v>
+        <v>57</v>
       </c>
       <c r="D6" s="0" t="s">
         <v>7</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="F6" s="0" t="s">
         <v>12</v>
@@ -1227,13 +1310,13 @@
     </row>
     <row r="7">
       <c r="A7" s="0">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>54</v>
+        <v>62</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>49</v>
+        <v>57</v>
       </c>
       <c r="D7" s="0" t="s">
         <v>7</v>
@@ -1247,13 +1330,13 @@
     </row>
     <row r="8">
       <c r="A8" s="0">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>55</v>
+        <v>63</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>49</v>
+        <v>57</v>
       </c>
       <c r="D8" s="0" t="s">
         <v>7</v>
@@ -1267,13 +1350,13 @@
     </row>
     <row r="9">
       <c r="A9" s="0">
-        <v>70</v>
+        <v>62</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>56</v>
+        <v>64</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>49</v>
+        <v>57</v>
       </c>
       <c r="D9" s="0" t="s">
         <v>7</v>
@@ -1287,13 +1370,13 @@
     </row>
     <row r="10">
       <c r="A10" s="0">
-        <v>64</v>
+        <v>70</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>57</v>
+        <v>65</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>49</v>
+        <v>57</v>
       </c>
       <c r="D10" s="0" t="s">
         <v>7</v>
@@ -1307,13 +1390,13 @@
     </row>
     <row r="11">
       <c r="A11" s="0">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>58</v>
+        <v>66</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>49</v>
+        <v>57</v>
       </c>
       <c r="D11" s="0" t="s">
         <v>7</v>
@@ -1327,19 +1410,19 @@
     </row>
     <row r="12">
       <c r="A12" s="0">
-        <v>13</v>
+        <v>63</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>59</v>
+        <v>67</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>49</v>
+        <v>57</v>
       </c>
       <c r="D12" s="0" t="s">
         <v>7</v>
       </c>
       <c r="E12" s="0" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="F12" s="0" t="s">
         <v>12</v>
@@ -1347,39 +1430,39 @@
     </row>
     <row r="13">
       <c r="A13" s="0">
-        <v>42</v>
+        <v>13</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>60</v>
+        <v>68</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>49</v>
+        <v>57</v>
       </c>
       <c r="D13" s="0" t="s">
         <v>7</v>
       </c>
       <c r="E13" s="0" t="s">
-        <v>43</v>
+        <v>8</v>
       </c>
       <c r="F13" s="0" t="s">
-        <v>24</v>
+        <v>12</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="0">
-        <v>33</v>
+        <v>42</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>61</v>
+        <v>69</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>49</v>
+        <v>57</v>
       </c>
       <c r="D14" s="0" t="s">
         <v>7</v>
       </c>
       <c r="E14" s="0" t="s">
-        <v>19</v>
+        <v>51</v>
       </c>
       <c r="F14" s="0" t="s">
         <v>24</v>
@@ -1387,39 +1470,39 @@
     </row>
     <row r="15">
       <c r="A15" s="0">
-        <v>48</v>
+        <v>33</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>62</v>
+        <v>70</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>49</v>
+        <v>57</v>
       </c>
       <c r="D15" s="0" t="s">
         <v>7</v>
       </c>
       <c r="E15" s="0" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="F15" s="0" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="0">
-        <v>37</v>
+        <v>48</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>63</v>
+        <v>71</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>49</v>
+        <v>57</v>
       </c>
       <c r="D16" s="0" t="s">
         <v>7</v>
       </c>
       <c r="E16" s="0" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="F16" s="0" t="s">
         <v>17</v>
@@ -1427,13 +1510,13 @@
     </row>
     <row r="17">
       <c r="A17" s="0">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>64</v>
+        <v>72</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>49</v>
+        <v>57</v>
       </c>
       <c r="D17" s="0" t="s">
         <v>7</v>
@@ -1442,198 +1525,198 @@
         <v>10</v>
       </c>
       <c r="F17" s="0" t="s">
-        <v>47</v>
+        <v>17</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="0">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>65</v>
+        <v>73</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>49</v>
+        <v>57</v>
       </c>
       <c r="D18" s="0" t="s">
         <v>7</v>
       </c>
       <c r="E18" s="0" t="s">
-        <v>66</v>
+        <v>10</v>
       </c>
       <c r="F18" s="0" t="s">
-        <v>47</v>
+        <v>55</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="0">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>67</v>
+        <v>74</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>49</v>
+        <v>57</v>
       </c>
       <c r="D19" s="0" t="s">
         <v>7</v>
       </c>
       <c r="E19" s="0" t="s">
-        <v>43</v>
+        <v>75</v>
       </c>
       <c r="F19" s="0" t="s">
-        <v>47</v>
+        <v>55</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="0">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>68</v>
+        <v>76</v>
       </c>
       <c r="C20" s="0" t="s">
-        <v>49</v>
+        <v>57</v>
       </c>
       <c r="D20" s="0" t="s">
         <v>7</v>
       </c>
       <c r="E20" s="0" t="s">
-        <v>43</v>
+        <v>51</v>
       </c>
       <c r="F20" s="0" t="s">
-        <v>47</v>
+        <v>55</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="0">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>69</v>
+        <v>77</v>
       </c>
       <c r="C21" s="0" t="s">
-        <v>49</v>
+        <v>57</v>
       </c>
       <c r="D21" s="0" t="s">
         <v>7</v>
       </c>
       <c r="E21" s="0" t="s">
-        <v>43</v>
+        <v>51</v>
       </c>
       <c r="F21" s="0" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="0">
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>70</v>
+        <v>78</v>
       </c>
       <c r="C22" s="0" t="s">
-        <v>49</v>
+        <v>57</v>
       </c>
       <c r="D22" s="0" t="s">
         <v>7</v>
       </c>
       <c r="E22" s="0" t="s">
-        <v>10</v>
+        <v>51</v>
       </c>
       <c r="F22" s="0" t="s">
-        <v>66</v>
+        <v>75</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="0">
-        <v>11</v>
+        <v>36</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>71</v>
+        <v>79</v>
       </c>
       <c r="C23" s="0" t="s">
-        <v>49</v>
+        <v>57</v>
       </c>
       <c r="D23" s="0" t="s">
         <v>7</v>
       </c>
       <c r="E23" s="0" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="F23" s="0" t="s">
-        <v>43</v>
+        <v>75</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="0">
-        <v>40</v>
+        <v>11</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>72</v>
+        <v>80</v>
       </c>
       <c r="C24" s="0" t="s">
-        <v>49</v>
+        <v>57</v>
       </c>
       <c r="D24" s="0" t="s">
         <v>7</v>
       </c>
       <c r="E24" s="0" t="s">
-        <v>73</v>
+        <v>8</v>
       </c>
       <c r="F24" s="0" t="s">
-        <v>43</v>
+        <v>51</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="0">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>74</v>
+        <v>81</v>
       </c>
       <c r="C25" s="0" t="s">
-        <v>49</v>
+        <v>57</v>
       </c>
       <c r="D25" s="0" t="s">
         <v>7</v>
       </c>
       <c r="E25" s="0" t="s">
-        <v>10</v>
+        <v>82</v>
       </c>
       <c r="F25" s="0" t="s">
-        <v>43</v>
+        <v>51</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="0">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>75</v>
+        <v>83</v>
       </c>
       <c r="C26" s="0" t="s">
-        <v>49</v>
+        <v>57</v>
       </c>
       <c r="D26" s="0" t="s">
         <v>7</v>
       </c>
       <c r="E26" s="0" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="F26" s="0" t="s">
-        <v>10</v>
+        <v>51</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="0">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>76</v>
+        <v>84</v>
       </c>
       <c r="C27" s="0" t="s">
-        <v>49</v>
+        <v>57</v>
       </c>
       <c r="D27" s="0" t="s">
         <v>7</v>
@@ -1642,24 +1725,24 @@
         <v>19</v>
       </c>
       <c r="F27" s="0" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="0">
-        <v>20</v>
+        <v>31</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>77</v>
+        <v>85</v>
       </c>
       <c r="C28" s="0" t="s">
-        <v>49</v>
+        <v>57</v>
       </c>
       <c r="D28" s="0" t="s">
         <v>7</v>
       </c>
       <c r="E28" s="0" t="s">
-        <v>8</v>
+        <v>19</v>
       </c>
       <c r="F28" s="0" t="s">
         <v>19</v>
@@ -1667,13 +1750,13 @@
     </row>
     <row r="29">
       <c r="A29" s="0">
-        <v>9</v>
+        <v>20</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>78</v>
+        <v>86</v>
       </c>
       <c r="C29" s="0" t="s">
-        <v>49</v>
+        <v>57</v>
       </c>
       <c r="D29" s="0" t="s">
         <v>7</v>
@@ -1687,13 +1770,13 @@
     </row>
     <row r="30">
       <c r="A30" s="0">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B30" s="0" t="s">
-        <v>79</v>
+        <v>87</v>
       </c>
       <c r="C30" s="0" t="s">
-        <v>49</v>
+        <v>57</v>
       </c>
       <c r="D30" s="0" t="s">
         <v>7</v>
@@ -1707,13 +1790,13 @@
     </row>
     <row r="31">
       <c r="A31" s="0">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="B31" s="0" t="s">
-        <v>80</v>
+        <v>88</v>
       </c>
       <c r="C31" s="0" t="s">
-        <v>49</v>
+        <v>57</v>
       </c>
       <c r="D31" s="0" t="s">
         <v>7</v>
@@ -1722,18 +1805,18 @@
         <v>8</v>
       </c>
       <c r="F31" s="0" t="s">
-        <v>81</v>
+        <v>19</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="0">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B32" s="0" t="s">
-        <v>82</v>
+        <v>89</v>
       </c>
       <c r="C32" s="0" t="s">
-        <v>49</v>
+        <v>57</v>
       </c>
       <c r="D32" s="0" t="s">
         <v>7</v>
@@ -1742,18 +1825,18 @@
         <v>8</v>
       </c>
       <c r="F32" s="0" t="s">
-        <v>8</v>
+        <v>90</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="0">
-        <v>30</v>
+        <v>3</v>
       </c>
       <c r="B33" s="0" t="s">
-        <v>83</v>
+        <v>91</v>
       </c>
       <c r="C33" s="0" t="s">
-        <v>49</v>
+        <v>57</v>
       </c>
       <c r="D33" s="0" t="s">
         <v>7</v>
@@ -1767,13 +1850,13 @@
     </row>
     <row r="34">
       <c r="A34" s="0">
-        <v>2</v>
+        <v>30</v>
       </c>
       <c r="B34" s="0" t="s">
-        <v>84</v>
+        <v>92</v>
       </c>
       <c r="C34" s="0" t="s">
-        <v>49</v>
+        <v>57</v>
       </c>
       <c r="D34" s="0" t="s">
         <v>7</v>
@@ -1787,21 +1870,41 @@
     </row>
     <row r="35">
       <c r="A35" s="0">
+        <v>2</v>
+      </c>
+      <c r="B35" s="0" t="s">
+        <v>93</v>
+      </c>
+      <c r="C35" s="0" t="s">
+        <v>57</v>
+      </c>
+      <c r="D35" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E35" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="F35" s="0" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="0">
         <v>1</v>
       </c>
-      <c r="B35" s="0" t="s">
-        <v>85</v>
-      </c>
-      <c r="C35" s="0" t="s">
-        <v>49</v>
-      </c>
-      <c r="D35" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="E35" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="F35" s="0" t="s">
+      <c r="B36" s="0" t="s">
+        <v>94</v>
+      </c>
+      <c r="C36" s="0" t="s">
+        <v>57</v>
+      </c>
+      <c r="D36" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E36" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="F36" s="0" t="s">
         <v>8</v>
       </c>
     </row>
@@ -1823,7 +1926,7 @@
         <v>2</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>86</v>
+        <v>95</v>
       </c>
       <c r="C1" s="2"/>
       <c r="D1" s="2" t="s">
@@ -1831,7 +1934,7 @@
       </c>
       <c r="E1" s="2"/>
       <c r="F1" s="2" t="s">
-        <v>87</v>
+        <v>96</v>
       </c>
     </row>
     <row r="2">
@@ -1839,24 +1942,24 @@
         <v>6</v>
       </c>
       <c r="B2" s="0" t="s">
+        <v>95</v>
+      </c>
+      <c r="D2" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="F2" s="0">
         <v>86</v>
-      </c>
-      <c r="D2" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="F2" s="0">
-        <v>80</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="0" t="s">
-        <v>49</v>
+        <v>57</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>88</v>
+        <v>97</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>89</v>
+        <v>98</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
edit palette dialog layout
</commit_message>
<xml_diff>
--- a/paint_todo.xlsx
+++ b/paint_todo.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="103">
   <si>
     <t>Id</t>
   </si>
@@ -29,20 +29,6 @@
   </si>
   <si>
     <t>Created</t>
-  </si>
-  <si>
-    <t xml:space="preserve">what do these lines do?
-Application.EnableVisualStyles();
-Application.SetCompatibleTextRenderingDefault(false);</t>
-  </si>
-  <si>
-    <t>Todo</t>
-  </si>
-  <si>
-    <t>Task</t>
-  </si>
-  <si>
-    <t>8/9/2018</t>
   </si>
   <si>
     <t xml:space="preserve">set and check tolerance for "black" and "white"
@@ -50,16 +36,19 @@
 - "whites" will be treated as pure white, which will in effect alter them to white</t>
   </si>
   <si>
+    <t>Todo</t>
+  </si>
+  <si>
+    <t>Task</t>
+  </si>
+  <si>
     <t>8/12/2018</t>
   </si>
   <si>
-    <t>edit palette: display rgb/hexdecimal/hsv values of selected color</t>
+    <t>new color: enter an rgb value</t>
   </si>
   <si>
     <t>8/24/2018</t>
-  </si>
-  <si>
-    <t>new color: enter an rgb value</t>
   </si>
   <si>
     <t>new color: enter a hexadecimal value</t>
@@ -84,12 +73,25 @@
     <t>refactor WithoutHaste.Drawing.Colors HSV to use ints instead of floats (0-360, 0-100, 0-100)</t>
   </si>
   <si>
+    <t>refactor all history actions and panels to use proper events instead of delegate properties</t>
+  </si>
+  <si>
+    <t>8/25/2018</t>
+  </si>
+  <si>
     <t xml:space="preserve">applying color is pretty fast even on large image
 but removing the color is really slow</t>
   </si>
   <si>
     <t xml:space="preserve">when resizing windows, default behavior is to keep the same section of image in the viewing pane
 - so expanding window would in effect zoom in</t>
+  </si>
+  <si>
+    <t>8/9/2018</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bug: Palette &gt; New &gt; Done
+get error because no filename to open in main form</t>
   </si>
   <si>
     <t xml:space="preserve">make a MasterImage class
@@ -117,6 +119,9 @@
 - like, send me the file you are trying to read so I can add support for it</t>
   </si>
   <si>
+    <t>put in top of documentation that program is being actively developed, so open to bug reports and feature requests</t>
+  </si>
+  <si>
     <t xml:space="preserve">in Paint documenation
 describe the use-case of converting between palette formats: open file, edit palette, save as new format</t>
   </si>
@@ -169,7 +174,8 @@
   <si>
     <t xml:space="preserve">save project:
 - list of images
-- a palette</t>
+- a palette
+select a file format to use, save in plain text</t>
   </si>
   <si>
     <t>open project</t>
@@ -227,6 +233,9 @@
     <t>Done</t>
   </si>
   <si>
+    <t>edit palette: display rgb/hexdecimal/hsv values of selected color</t>
+  </si>
+  <si>
     <t xml:space="preserve">remember windows size from last closing
 - full screen vs not
 - default not-full-screen size
@@ -374,17 +383,10 @@
     <t>Bug</t>
   </si>
   <si>
-    <t xml:space="preserve">save project:
-- list of images
-- a palette
-select a file format to use, save in plain text</t>
-  </si>
-  <si>
-    <t>put in top of documentation that program is being actively developed, so open to bug reports and feature requests</t>
-  </si>
-  <si>
-    <t xml:space="preserve">bug: Palette &gt; New &gt; Done
-get error because no filename to open in main form</t>
+    <t xml:space="preserve">to be consistent with System.Convert naming standards
+update ConvertColors
+- To&lt;Type&gt;(FromType)
+- &lt;FromType&gt;To&lt;Type&gt;(list of generic params)</t>
   </si>
 </sst>
 </file>
@@ -437,7 +439,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:F43"/>
+  <dimension ref="A1:F45"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -463,7 +465,7 @@
     </row>
     <row r="2">
       <c r="A2" s="0">
-        <v>35</v>
+        <v>67</v>
       </c>
       <c r="B2" s="0" t="s">
         <v>9</v>
@@ -480,10 +482,10 @@
     </row>
     <row r="3">
       <c r="A3" s="0">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C3" s="0" t="s">
         <v>6</v>
@@ -492,15 +494,15 @@
         <v>7</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="0">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C4" s="0" t="s">
         <v>6</v>
@@ -509,15 +511,15 @@
         <v>7</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="0">
-        <v>69</v>
+        <v>50</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C5" s="0" t="s">
         <v>6</v>
@@ -526,32 +528,32 @@
         <v>7</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="0">
-        <v>50</v>
+        <v>34</v>
       </c>
       <c r="B6" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D6" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E6" s="0" t="s">
         <v>16</v>
-      </c>
-      <c r="C6" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="D6" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="E6" s="0" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="0">
-        <v>34</v>
+        <v>59</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C7" s="0" t="s">
         <v>6</v>
@@ -560,15 +562,15 @@
         <v>7</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="0">
-        <v>59</v>
+        <v>87</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C8" s="0" t="s">
         <v>6</v>
@@ -577,7 +579,7 @@
         <v>7</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
     </row>
     <row r="9">
@@ -585,7 +587,7 @@
         <v>49</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C9" s="0" t="s">
         <v>6</v>
@@ -594,7 +596,7 @@
         <v>7</v>
       </c>
       <c r="E9" s="0" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
     </row>
     <row r="10">
@@ -602,7 +604,7 @@
         <v>21</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C10" s="0" t="s">
         <v>6</v>
@@ -611,7 +613,7 @@
         <v>7</v>
       </c>
       <c r="E10" s="0" t="s">
-        <v>8</v>
+        <v>22</v>
       </c>
     </row>
     <row r="11">
@@ -619,7 +621,7 @@
         <v>86</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>101</v>
+        <v>23</v>
       </c>
       <c r="C11" s="0" t="s">
         <v>6</v>
@@ -628,7 +630,7 @@
         <v>7</v>
       </c>
       <c r="E11" s="0" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="12">
@@ -636,7 +638,7 @@
         <v>54</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C12" s="0" t="s">
         <v>6</v>
@@ -645,15 +647,15 @@
         <v>7</v>
       </c>
       <c r="E12" s="0" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="0">
-        <v>53</v>
+        <v>88</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>25</v>
+        <v>102</v>
       </c>
       <c r="C13" s="0" t="s">
         <v>6</v>
@@ -662,12 +664,12 @@
         <v>7</v>
       </c>
       <c r="E13" s="0" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="0">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="B14" s="0" t="s">
         <v>26</v>
@@ -679,12 +681,12 @@
         <v>7</v>
       </c>
       <c r="E14" s="0" t="s">
-        <v>17</v>
+        <v>25</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="0">
-        <v>76</v>
+        <v>51</v>
       </c>
       <c r="B15" s="0" t="s">
         <v>27</v>
@@ -696,12 +698,12 @@
         <v>7</v>
       </c>
       <c r="E15" s="0" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="0">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="B16" s="0" t="s">
         <v>28</v>
@@ -713,15 +715,15 @@
         <v>7</v>
       </c>
       <c r="E16" s="0" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="0">
-        <v>85</v>
+        <v>35</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>100</v>
+        <v>5</v>
       </c>
       <c r="C17" s="0" t="s">
         <v>6</v>
@@ -730,12 +732,12 @@
         <v>7</v>
       </c>
       <c r="E17" s="0" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="0">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B18" s="0" t="s">
         <v>29</v>
@@ -747,12 +749,12 @@
         <v>7</v>
       </c>
       <c r="E18" s="0" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="0">
-        <v>77</v>
+        <v>85</v>
       </c>
       <c r="B19" s="0" t="s">
         <v>30</v>
@@ -764,12 +766,12 @@
         <v>7</v>
       </c>
       <c r="E19" s="0" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="0">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="B20" s="0" t="s">
         <v>31</v>
@@ -781,12 +783,12 @@
         <v>7</v>
       </c>
       <c r="E20" s="0" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="0">
-        <v>52</v>
+        <v>77</v>
       </c>
       <c r="B21" s="0" t="s">
         <v>32</v>
@@ -798,12 +800,12 @@
         <v>7</v>
       </c>
       <c r="E21" s="0" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="0">
-        <v>27</v>
+        <v>78</v>
       </c>
       <c r="B22" s="0" t="s">
         <v>33</v>
@@ -815,12 +817,12 @@
         <v>7</v>
       </c>
       <c r="E22" s="0" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="0">
-        <v>28</v>
+        <v>52</v>
       </c>
       <c r="B23" s="0" t="s">
         <v>34</v>
@@ -832,12 +834,12 @@
         <v>7</v>
       </c>
       <c r="E23" s="0" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="0">
-        <v>19</v>
+        <v>27</v>
       </c>
       <c r="B24" s="0" t="s">
         <v>35</v>
@@ -849,12 +851,12 @@
         <v>7</v>
       </c>
       <c r="E24" s="0" t="s">
-        <v>8</v>
+        <v>22</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="0">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="B25" s="0" t="s">
         <v>36</v>
@@ -866,12 +868,12 @@
         <v>7</v>
       </c>
       <c r="E25" s="0" t="s">
-        <v>8</v>
+        <v>22</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="0">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="B26" s="0" t="s">
         <v>37</v>
@@ -883,12 +885,12 @@
         <v>7</v>
       </c>
       <c r="E26" s="0" t="s">
-        <v>8</v>
+        <v>22</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="0">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="B27" s="0" t="s">
         <v>38</v>
@@ -900,12 +902,12 @@
         <v>7</v>
       </c>
       <c r="E27" s="0" t="s">
-        <v>8</v>
+        <v>22</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="0">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B28" s="0" t="s">
         <v>39</v>
@@ -917,12 +919,12 @@
         <v>7</v>
       </c>
       <c r="E28" s="0" t="s">
-        <v>8</v>
+        <v>22</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="0">
-        <v>81</v>
+        <v>17</v>
       </c>
       <c r="B29" s="0" t="s">
         <v>40</v>
@@ -934,12 +936,12 @@
         <v>7</v>
       </c>
       <c r="E29" s="0" t="s">
-        <v>12</v>
+        <v>22</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="0">
-        <v>82</v>
+        <v>18</v>
       </c>
       <c r="B30" s="0" t="s">
         <v>41</v>
@@ -951,15 +953,15 @@
         <v>7</v>
       </c>
       <c r="E30" s="0" t="s">
-        <v>12</v>
+        <v>22</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="0">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B31" s="0" t="s">
-        <v>99</v>
+        <v>42</v>
       </c>
       <c r="C31" s="0" t="s">
         <v>6</v>
@@ -968,12 +970,12 @@
         <v>7</v>
       </c>
       <c r="E31" s="0" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="0">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B32" s="0" t="s">
         <v>43</v>
@@ -985,12 +987,12 @@
         <v>7</v>
       </c>
       <c r="E32" s="0" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="0">
-        <v>25</v>
+        <v>83</v>
       </c>
       <c r="B33" s="0" t="s">
         <v>44</v>
@@ -1002,12 +1004,12 @@
         <v>7</v>
       </c>
       <c r="E33" s="0" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="0">
-        <v>57</v>
+        <v>84</v>
       </c>
       <c r="B34" s="0" t="s">
         <v>45</v>
@@ -1019,12 +1021,12 @@
         <v>7</v>
       </c>
       <c r="E34" s="0" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="0">
-        <v>65</v>
+        <v>25</v>
       </c>
       <c r="B35" s="0" t="s">
         <v>46</v>
@@ -1036,12 +1038,12 @@
         <v>7</v>
       </c>
       <c r="E35" s="0" t="s">
-        <v>12</v>
+        <v>22</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="0">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B36" s="0" t="s">
         <v>47</v>
@@ -1053,12 +1055,12 @@
         <v>7</v>
       </c>
       <c r="E36" s="0" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="0">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="B37" s="0" t="s">
         <v>48</v>
@@ -1070,12 +1072,12 @@
         <v>7</v>
       </c>
       <c r="E37" s="0" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="0">
-        <v>26</v>
+        <v>58</v>
       </c>
       <c r="B38" s="0" t="s">
         <v>49</v>
@@ -1087,12 +1089,12 @@
         <v>7</v>
       </c>
       <c r="E38" s="0" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="0">
-        <v>43</v>
+        <v>61</v>
       </c>
       <c r="B39" s="0" t="s">
         <v>50</v>
@@ -1104,15 +1106,15 @@
         <v>7</v>
       </c>
       <c r="E39" s="0" t="s">
-        <v>51</v>
+        <v>10</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="0">
-        <v>74</v>
+        <v>26</v>
       </c>
       <c r="B40" s="0" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C40" s="0" t="s">
         <v>6</v>
@@ -1121,29 +1123,29 @@
         <v>7</v>
       </c>
       <c r="E40" s="0" t="s">
-        <v>12</v>
+        <v>22</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="0">
-        <v>29</v>
+        <v>43</v>
       </c>
       <c r="B41" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="C41" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D41" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E41" s="0" t="s">
         <v>53</v>
-      </c>
-      <c r="C41" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="D41" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="E41" s="0" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="0">
-        <v>47</v>
+        <v>74</v>
       </c>
       <c r="B42" s="0" t="s">
         <v>54</v>
@@ -1155,24 +1157,58 @@
         <v>7</v>
       </c>
       <c r="E42" s="0" t="s">
-        <v>55</v>
+        <v>10</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" s="0">
+        <v>29</v>
+      </c>
+      <c r="B43" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="C43" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D43" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E43" s="0" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" s="0">
+        <v>47</v>
+      </c>
+      <c r="B44" s="0" t="s">
+        <v>56</v>
+      </c>
+      <c r="C44" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D44" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E44" s="0" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" s="0">
         <v>60</v>
       </c>
-      <c r="B43" s="0" t="s">
-        <v>56</v>
-      </c>
-      <c r="C43" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="D43" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="E43" s="0" t="s">
-        <v>12</v>
+      <c r="B45" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="C45" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D45" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E45" s="0" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -1205,7 +1241,7 @@
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
     </row>
     <row r="2">
@@ -1213,19 +1249,19 @@
         <v>71</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>11</v>
+        <v>60</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="D2" s="0" t="s">
         <v>7</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3">
@@ -1233,19 +1269,19 @@
         <v>24</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="D3" s="0" t="s">
         <v>7</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>8</v>
+        <v>22</v>
       </c>
       <c r="F3" s="0" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4">
@@ -1253,19 +1289,19 @@
         <v>75</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="D4" s="0" t="s">
         <v>7</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="F4" s="0" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="5">
@@ -1273,19 +1309,19 @@
         <v>55</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="D5" s="0" t="s">
         <v>7</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="F5" s="0" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="6">
@@ -1293,19 +1329,19 @@
         <v>56</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="D6" s="0" t="s">
         <v>7</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="F6" s="0" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="7">
@@ -1313,19 +1349,19 @@
         <v>72</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="D7" s="0" t="s">
         <v>7</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="F7" s="0" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="8">
@@ -1333,19 +1369,19 @@
         <v>66</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="D8" s="0" t="s">
         <v>7</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="F8" s="0" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="9">
@@ -1353,19 +1389,19 @@
         <v>62</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="D9" s="0" t="s">
         <v>7</v>
       </c>
       <c r="E9" s="0" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="F9" s="0" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="10">
@@ -1373,19 +1409,19 @@
         <v>70</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="D10" s="0" t="s">
         <v>7</v>
       </c>
       <c r="E10" s="0" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="F10" s="0" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="11">
@@ -1393,19 +1429,19 @@
         <v>64</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="D11" s="0" t="s">
         <v>7</v>
       </c>
       <c r="E11" s="0" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="F11" s="0" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="12">
@@ -1413,19 +1449,19 @@
         <v>63</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="D12" s="0" t="s">
         <v>7</v>
       </c>
       <c r="E12" s="0" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="F12" s="0" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="13">
@@ -1433,19 +1469,19 @@
         <v>13</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="D13" s="0" t="s">
         <v>7</v>
       </c>
       <c r="E13" s="0" t="s">
-        <v>8</v>
+        <v>22</v>
       </c>
       <c r="F13" s="0" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="14">
@@ -1453,19 +1489,19 @@
         <v>42</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="D14" s="0" t="s">
         <v>7</v>
       </c>
       <c r="E14" s="0" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="F14" s="0" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="15">
@@ -1473,19 +1509,19 @@
         <v>33</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="D15" s="0" t="s">
         <v>7</v>
       </c>
       <c r="E15" s="0" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="F15" s="0" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="16">
@@ -1493,19 +1529,19 @@
         <v>48</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="D16" s="0" t="s">
         <v>7</v>
       </c>
       <c r="E16" s="0" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="F16" s="0" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
     </row>
     <row r="17">
@@ -1513,19 +1549,19 @@
         <v>37</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="D17" s="0" t="s">
         <v>7</v>
       </c>
       <c r="E17" s="0" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="F17" s="0" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
     </row>
     <row r="18">
@@ -1533,19 +1569,19 @@
         <v>38</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="C18" s="0" t="s">
+        <v>59</v>
+      </c>
+      <c r="D18" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E18" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="F18" s="0" t="s">
         <v>57</v>
-      </c>
-      <c r="D18" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="E18" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="F18" s="0" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="19">
@@ -1553,19 +1589,19 @@
         <v>46</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="C19" s="0" t="s">
+        <v>59</v>
+      </c>
+      <c r="D19" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E19" s="0" t="s">
+        <v>78</v>
+      </c>
+      <c r="F19" s="0" t="s">
         <v>57</v>
-      </c>
-      <c r="D19" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="E19" s="0" t="s">
-        <v>75</v>
-      </c>
-      <c r="F19" s="0" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="20">
@@ -1573,19 +1609,19 @@
         <v>45</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="C20" s="0" t="s">
+        <v>59</v>
+      </c>
+      <c r="D20" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E20" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="F20" s="0" t="s">
         <v>57</v>
-      </c>
-      <c r="D20" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="E20" s="0" t="s">
-        <v>51</v>
-      </c>
-      <c r="F20" s="0" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="21">
@@ -1593,19 +1629,19 @@
         <v>44</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="C21" s="0" t="s">
+        <v>59</v>
+      </c>
+      <c r="D21" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E21" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="F21" s="0" t="s">
         <v>57</v>
-      </c>
-      <c r="D21" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="E21" s="0" t="s">
-        <v>51</v>
-      </c>
-      <c r="F21" s="0" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="22">
@@ -1613,19 +1649,19 @@
         <v>41</v>
       </c>
       <c r="B22" s="0" t="s">
+        <v>81</v>
+      </c>
+      <c r="C22" s="0" t="s">
+        <v>59</v>
+      </c>
+      <c r="D22" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E22" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="F22" s="0" t="s">
         <v>78</v>
-      </c>
-      <c r="C22" s="0" t="s">
-        <v>57</v>
-      </c>
-      <c r="D22" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="E22" s="0" t="s">
-        <v>51</v>
-      </c>
-      <c r="F22" s="0" t="s">
-        <v>75</v>
       </c>
     </row>
     <row r="23">
@@ -1633,19 +1669,19 @@
         <v>36</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="C23" s="0" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="D23" s="0" t="s">
         <v>7</v>
       </c>
       <c r="E23" s="0" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="F23" s="0" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
     </row>
     <row r="24">
@@ -1653,19 +1689,19 @@
         <v>11</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="C24" s="0" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="D24" s="0" t="s">
         <v>7</v>
       </c>
       <c r="E24" s="0" t="s">
-        <v>8</v>
+        <v>22</v>
       </c>
       <c r="F24" s="0" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
     </row>
     <row r="25">
@@ -1673,19 +1709,19 @@
         <v>40</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="C25" s="0" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="D25" s="0" t="s">
         <v>7</v>
       </c>
       <c r="E25" s="0" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="F25" s="0" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
     </row>
     <row r="26">
@@ -1693,19 +1729,19 @@
         <v>39</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="C26" s="0" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="D26" s="0" t="s">
         <v>7</v>
       </c>
       <c r="E26" s="0" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="F26" s="0" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
     </row>
     <row r="27">
@@ -1713,19 +1749,19 @@
         <v>32</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="C27" s="0" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="D27" s="0" t="s">
         <v>7</v>
       </c>
       <c r="E27" s="0" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="F27" s="0" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="28">
@@ -1733,19 +1769,19 @@
         <v>31</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="C28" s="0" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="D28" s="0" t="s">
         <v>7</v>
       </c>
       <c r="E28" s="0" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="F28" s="0" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
     <row r="29">
@@ -1753,19 +1789,19 @@
         <v>20</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="C29" s="0" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="D29" s="0" t="s">
         <v>7</v>
       </c>
       <c r="E29" s="0" t="s">
-        <v>8</v>
+        <v>22</v>
       </c>
       <c r="F29" s="0" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
     <row r="30">
@@ -1773,19 +1809,19 @@
         <v>9</v>
       </c>
       <c r="B30" s="0" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="C30" s="0" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="D30" s="0" t="s">
         <v>7</v>
       </c>
       <c r="E30" s="0" t="s">
-        <v>8</v>
+        <v>22</v>
       </c>
       <c r="F30" s="0" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
     <row r="31">
@@ -1793,19 +1829,19 @@
         <v>8</v>
       </c>
       <c r="B31" s="0" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="C31" s="0" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="D31" s="0" t="s">
         <v>7</v>
       </c>
       <c r="E31" s="0" t="s">
-        <v>8</v>
+        <v>22</v>
       </c>
       <c r="F31" s="0" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
     <row r="32">
@@ -1813,19 +1849,19 @@
         <v>4</v>
       </c>
       <c r="B32" s="0" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="C32" s="0" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="D32" s="0" t="s">
         <v>7</v>
       </c>
       <c r="E32" s="0" t="s">
-        <v>8</v>
+        <v>22</v>
       </c>
       <c r="F32" s="0" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
     </row>
     <row r="33">
@@ -1833,19 +1869,19 @@
         <v>3</v>
       </c>
       <c r="B33" s="0" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="C33" s="0" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="D33" s="0" t="s">
         <v>7</v>
       </c>
       <c r="E33" s="0" t="s">
-        <v>8</v>
+        <v>22</v>
       </c>
       <c r="F33" s="0" t="s">
-        <v>8</v>
+        <v>22</v>
       </c>
     </row>
     <row r="34">
@@ -1853,19 +1889,19 @@
         <v>30</v>
       </c>
       <c r="B34" s="0" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="C34" s="0" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="D34" s="0" t="s">
         <v>7</v>
       </c>
       <c r="E34" s="0" t="s">
-        <v>8</v>
+        <v>22</v>
       </c>
       <c r="F34" s="0" t="s">
-        <v>8</v>
+        <v>22</v>
       </c>
     </row>
     <row r="35">
@@ -1873,19 +1909,19 @@
         <v>2</v>
       </c>
       <c r="B35" s="0" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="C35" s="0" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="D35" s="0" t="s">
         <v>7</v>
       </c>
       <c r="E35" s="0" t="s">
-        <v>8</v>
+        <v>22</v>
       </c>
       <c r="F35" s="0" t="s">
-        <v>8</v>
+        <v>22</v>
       </c>
     </row>
     <row r="36">
@@ -1893,19 +1929,19 @@
         <v>1</v>
       </c>
       <c r="B36" s="0" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="C36" s="0" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="D36" s="0" t="s">
         <v>7</v>
       </c>
       <c r="E36" s="0" t="s">
-        <v>8</v>
+        <v>22</v>
       </c>
       <c r="F36" s="0" t="s">
-        <v>8</v>
+        <v>22</v>
       </c>
     </row>
   </sheetData>
@@ -1926,7 +1962,7 @@
         <v>2</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="C1" s="2"/>
       <c r="D1" s="2" t="s">
@@ -1934,7 +1970,7 @@
       </c>
       <c r="E1" s="2"/>
       <c r="F1" s="2" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
     </row>
     <row r="2">
@@ -1942,24 +1978,24 @@
         <v>6</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="D2" s="0" t="s">
         <v>7</v>
       </c>
       <c r="F2" s="0">
-        <v>86</v>
+        <v>88</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="0" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
edit palette: new color by hexadecimal/rgb/hsv
</commit_message>
<xml_diff>
--- a/paint_todo.xlsx
+++ b/paint_todo.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="104">
   <si>
     <t>Id</t>
   </si>
@@ -387,6 +387,10 @@
 update ConvertColors
 - To&lt;Type&gt;(FromType)
 - &lt;FromType&gt;To&lt;Type&gt;(list of generic params)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">having problems with imprecise color format conversions
+it's really important they be perfectly reversible</t>
   </si>
 </sst>
 </file>
@@ -439,7 +443,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:F45"/>
+  <dimension ref="A1:F43"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -465,10 +469,10 @@
     </row>
     <row r="2">
       <c r="A2" s="0">
-        <v>67</v>
+        <v>50</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="C2" s="0" t="s">
         <v>6</v>
@@ -477,15 +481,15 @@
         <v>7</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="0">
-        <v>68</v>
+        <v>34</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="C3" s="0" t="s">
         <v>6</v>
@@ -494,15 +498,15 @@
         <v>7</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="0">
-        <v>69</v>
+        <v>59</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="C4" s="0" t="s">
         <v>6</v>
@@ -516,10 +520,10 @@
     </row>
     <row r="5">
       <c r="A5" s="0">
-        <v>50</v>
+        <v>87</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="C5" s="0" t="s">
         <v>6</v>
@@ -528,15 +532,15 @@
         <v>7</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="0">
-        <v>34</v>
+        <v>49</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="C6" s="0" t="s">
         <v>6</v>
@@ -545,15 +549,15 @@
         <v>7</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="0">
-        <v>59</v>
+        <v>21</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="C7" s="0" t="s">
         <v>6</v>
@@ -562,15 +566,15 @@
         <v>7</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="0">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="C8" s="0" t="s">
         <v>6</v>
@@ -579,15 +583,15 @@
         <v>7</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="0">
-        <v>49</v>
+        <v>54</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="C9" s="0" t="s">
         <v>6</v>
@@ -596,15 +600,15 @@
         <v>7</v>
       </c>
       <c r="E9" s="0" t="s">
-        <v>14</v>
+        <v>25</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="0">
-        <v>21</v>
+        <v>89</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>21</v>
+        <v>103</v>
       </c>
       <c r="C10" s="0" t="s">
         <v>6</v>
@@ -613,15 +617,15 @@
         <v>7</v>
       </c>
       <c r="E10" s="0" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="0">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>23</v>
+        <v>102</v>
       </c>
       <c r="C11" s="0" t="s">
         <v>6</v>
@@ -630,15 +634,15 @@
         <v>7</v>
       </c>
       <c r="E11" s="0" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="0">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="C12" s="0" t="s">
         <v>6</v>
@@ -652,10 +656,10 @@
     </row>
     <row r="13">
       <c r="A13" s="0">
-        <v>88</v>
+        <v>51</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>102</v>
+        <v>27</v>
       </c>
       <c r="C13" s="0" t="s">
         <v>6</v>
@@ -664,15 +668,15 @@
         <v>7</v>
       </c>
       <c r="E13" s="0" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="0">
-        <v>53</v>
+        <v>76</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="C14" s="0" t="s">
         <v>6</v>
@@ -681,15 +685,15 @@
         <v>7</v>
       </c>
       <c r="E14" s="0" t="s">
-        <v>25</v>
+        <v>10</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="0">
-        <v>51</v>
+        <v>35</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>27</v>
+        <v>5</v>
       </c>
       <c r="C15" s="0" t="s">
         <v>6</v>
@@ -698,15 +702,15 @@
         <v>7</v>
       </c>
       <c r="E15" s="0" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="0">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C16" s="0" t="s">
         <v>6</v>
@@ -720,10 +724,10 @@
     </row>
     <row r="17">
       <c r="A17" s="0">
-        <v>35</v>
+        <v>85</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>5</v>
+        <v>30</v>
       </c>
       <c r="C17" s="0" t="s">
         <v>6</v>
@@ -732,15 +736,15 @@
         <v>7</v>
       </c>
       <c r="E17" s="0" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="0">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="C18" s="0" t="s">
         <v>6</v>
@@ -754,10 +758,10 @@
     </row>
     <row r="19">
       <c r="A19" s="0">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="C19" s="0" t="s">
         <v>6</v>
@@ -771,10 +775,10 @@
     </row>
     <row r="20">
       <c r="A20" s="0">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="C20" s="0" t="s">
         <v>6</v>
@@ -788,10 +792,10 @@
     </row>
     <row r="21">
       <c r="A21" s="0">
-        <v>77</v>
+        <v>52</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C21" s="0" t="s">
         <v>6</v>
@@ -800,15 +804,15 @@
         <v>7</v>
       </c>
       <c r="E21" s="0" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="0">
-        <v>78</v>
+        <v>27</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="C22" s="0" t="s">
         <v>6</v>
@@ -817,15 +821,15 @@
         <v>7</v>
       </c>
       <c r="E22" s="0" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="0">
-        <v>52</v>
+        <v>28</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="C23" s="0" t="s">
         <v>6</v>
@@ -834,15 +838,15 @@
         <v>7</v>
       </c>
       <c r="E23" s="0" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="0">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="C24" s="0" t="s">
         <v>6</v>
@@ -856,10 +860,10 @@
     </row>
     <row r="25">
       <c r="A25" s="0">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="C25" s="0" t="s">
         <v>6</v>
@@ -873,10 +877,10 @@
     </row>
     <row r="26">
       <c r="A26" s="0">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="C26" s="0" t="s">
         <v>6</v>
@@ -890,10 +894,10 @@
     </row>
     <row r="27">
       <c r="A27" s="0">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="C27" s="0" t="s">
         <v>6</v>
@@ -907,10 +911,10 @@
     </row>
     <row r="28">
       <c r="A28" s="0">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C28" s="0" t="s">
         <v>6</v>
@@ -924,10 +928,10 @@
     </row>
     <row r="29">
       <c r="A29" s="0">
-        <v>17</v>
+        <v>81</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="C29" s="0" t="s">
         <v>6</v>
@@ -936,15 +940,15 @@
         <v>7</v>
       </c>
       <c r="E29" s="0" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="0">
-        <v>18</v>
+        <v>82</v>
       </c>
       <c r="B30" s="0" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="C30" s="0" t="s">
         <v>6</v>
@@ -953,15 +957,15 @@
         <v>7</v>
       </c>
       <c r="E30" s="0" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="0">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="B31" s="0" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="C31" s="0" t="s">
         <v>6</v>
@@ -975,10 +979,10 @@
     </row>
     <row r="32">
       <c r="A32" s="0">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="B32" s="0" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="C32" s="0" t="s">
         <v>6</v>
@@ -992,10 +996,10 @@
     </row>
     <row r="33">
       <c r="A33" s="0">
-        <v>83</v>
+        <v>25</v>
       </c>
       <c r="B33" s="0" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="C33" s="0" t="s">
         <v>6</v>
@@ -1004,15 +1008,15 @@
         <v>7</v>
       </c>
       <c r="E33" s="0" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="0">
-        <v>84</v>
+        <v>57</v>
       </c>
       <c r="B34" s="0" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="C34" s="0" t="s">
         <v>6</v>
@@ -1026,10 +1030,10 @@
     </row>
     <row r="35">
       <c r="A35" s="0">
-        <v>25</v>
+        <v>65</v>
       </c>
       <c r="B35" s="0" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="C35" s="0" t="s">
         <v>6</v>
@@ -1038,15 +1042,15 @@
         <v>7</v>
       </c>
       <c r="E35" s="0" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="0">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B36" s="0" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="C36" s="0" t="s">
         <v>6</v>
@@ -1060,10 +1064,10 @@
     </row>
     <row r="37">
       <c r="A37" s="0">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="B37" s="0" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="C37" s="0" t="s">
         <v>6</v>
@@ -1077,10 +1081,10 @@
     </row>
     <row r="38">
       <c r="A38" s="0">
-        <v>58</v>
+        <v>26</v>
       </c>
       <c r="B38" s="0" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="C38" s="0" t="s">
         <v>6</v>
@@ -1089,15 +1093,15 @@
         <v>7</v>
       </c>
       <c r="E38" s="0" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="0">
-        <v>61</v>
+        <v>43</v>
       </c>
       <c r="B39" s="0" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="C39" s="0" t="s">
         <v>6</v>
@@ -1106,15 +1110,15 @@
         <v>7</v>
       </c>
       <c r="E39" s="0" t="s">
-        <v>10</v>
+        <v>53</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="0">
-        <v>26</v>
+        <v>74</v>
       </c>
       <c r="B40" s="0" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="C40" s="0" t="s">
         <v>6</v>
@@ -1123,15 +1127,15 @@
         <v>7</v>
       </c>
       <c r="E40" s="0" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="0">
-        <v>43</v>
+        <v>29</v>
       </c>
       <c r="B41" s="0" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="C41" s="0" t="s">
         <v>6</v>
@@ -1140,15 +1144,15 @@
         <v>7</v>
       </c>
       <c r="E41" s="0" t="s">
-        <v>53</v>
+        <v>22</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="0">
-        <v>74</v>
+        <v>47</v>
       </c>
       <c r="B42" s="0" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="C42" s="0" t="s">
         <v>6</v>
@@ -1157,15 +1161,15 @@
         <v>7</v>
       </c>
       <c r="E42" s="0" t="s">
-        <v>10</v>
+        <v>57</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" s="0">
-        <v>29</v>
+        <v>60</v>
       </c>
       <c r="B43" s="0" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="C43" s="0" t="s">
         <v>6</v>
@@ -1174,40 +1178,6 @@
         <v>7</v>
       </c>
       <c r="E43" s="0" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="44">
-      <c r="A44" s="0">
-        <v>47</v>
-      </c>
-      <c r="B44" s="0" t="s">
-        <v>56</v>
-      </c>
-      <c r="C44" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="D44" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="E44" s="0" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="45">
-      <c r="A45" s="0">
-        <v>60</v>
-      </c>
-      <c r="B45" s="0" t="s">
-        <v>58</v>
-      </c>
-      <c r="C45" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="D45" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="E45" s="0" t="s">
         <v>10</v>
       </c>
     </row>
@@ -1218,7 +1188,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:F36"/>
+  <dimension ref="A1:F39"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1246,10 +1216,10 @@
     </row>
     <row r="2">
       <c r="A2" s="0">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>60</v>
+        <v>12</v>
       </c>
       <c r="C2" s="0" t="s">
         <v>59</v>
@@ -1261,15 +1231,15 @@
         <v>10</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="0">
-        <v>24</v>
+        <v>68</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>61</v>
+        <v>11</v>
       </c>
       <c r="C3" s="0" t="s">
         <v>59</v>
@@ -1278,18 +1248,18 @@
         <v>7</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="F3" s="0" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="0">
-        <v>75</v>
+        <v>67</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>62</v>
+        <v>9</v>
       </c>
       <c r="C4" s="0" t="s">
         <v>59</v>
@@ -1301,15 +1271,15 @@
         <v>10</v>
       </c>
       <c r="F4" s="0" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="0">
-        <v>55</v>
+        <v>71</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="C5" s="0" t="s">
         <v>59</v>
@@ -1318,7 +1288,7 @@
         <v>7</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>25</v>
+        <v>10</v>
       </c>
       <c r="F5" s="0" t="s">
         <v>10</v>
@@ -1326,10 +1296,10 @@
     </row>
     <row r="6">
       <c r="A6" s="0">
-        <v>56</v>
+        <v>24</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="C6" s="0" t="s">
         <v>59</v>
@@ -1338,7 +1308,7 @@
         <v>7</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="F6" s="0" t="s">
         <v>10</v>
@@ -1346,10 +1316,10 @@
     </row>
     <row r="7">
       <c r="A7" s="0">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="C7" s="0" t="s">
         <v>59</v>
@@ -1366,10 +1336,10 @@
     </row>
     <row r="8">
       <c r="A8" s="0">
-        <v>66</v>
+        <v>55</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="C8" s="0" t="s">
         <v>59</v>
@@ -1378,7 +1348,7 @@
         <v>7</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>10</v>
+        <v>25</v>
       </c>
       <c r="F8" s="0" t="s">
         <v>10</v>
@@ -1386,10 +1356,10 @@
     </row>
     <row r="9">
       <c r="A9" s="0">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="C9" s="0" t="s">
         <v>59</v>
@@ -1398,7 +1368,7 @@
         <v>7</v>
       </c>
       <c r="E9" s="0" t="s">
-        <v>10</v>
+        <v>25</v>
       </c>
       <c r="F9" s="0" t="s">
         <v>10</v>
@@ -1406,10 +1376,10 @@
     </row>
     <row r="10">
       <c r="A10" s="0">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="C10" s="0" t="s">
         <v>59</v>
@@ -1426,10 +1396,10 @@
     </row>
     <row r="11">
       <c r="A11" s="0">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="C11" s="0" t="s">
         <v>59</v>
@@ -1446,10 +1416,10 @@
     </row>
     <row r="12">
       <c r="A12" s="0">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="C12" s="0" t="s">
         <v>59</v>
@@ -1466,10 +1436,10 @@
     </row>
     <row r="13">
       <c r="A13" s="0">
-        <v>13</v>
+        <v>70</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="C13" s="0" t="s">
         <v>59</v>
@@ -1478,7 +1448,7 @@
         <v>7</v>
       </c>
       <c r="E13" s="0" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="F13" s="0" t="s">
         <v>10</v>
@@ -1486,10 +1456,10 @@
     </row>
     <row r="14">
       <c r="A14" s="0">
-        <v>42</v>
+        <v>64</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="C14" s="0" t="s">
         <v>59</v>
@@ -1498,18 +1468,18 @@
         <v>7</v>
       </c>
       <c r="E14" s="0" t="s">
-        <v>53</v>
+        <v>10</v>
       </c>
       <c r="F14" s="0" t="s">
-        <v>25</v>
+        <v>10</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="0">
-        <v>33</v>
+        <v>63</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="C15" s="0" t="s">
         <v>59</v>
@@ -1518,18 +1488,18 @@
         <v>7</v>
       </c>
       <c r="E15" s="0" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="F15" s="0" t="s">
-        <v>25</v>
+        <v>10</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="0">
-        <v>48</v>
+        <v>13</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="C16" s="0" t="s">
         <v>59</v>
@@ -1538,18 +1508,18 @@
         <v>7</v>
       </c>
       <c r="E16" s="0" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="F16" s="0" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="0">
-        <v>37</v>
+        <v>42</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="C17" s="0" t="s">
         <v>59</v>
@@ -1558,18 +1528,18 @@
         <v>7</v>
       </c>
       <c r="E17" s="0" t="s">
-        <v>8</v>
+        <v>53</v>
       </c>
       <c r="F17" s="0" t="s">
-        <v>14</v>
+        <v>25</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="0">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="C18" s="0" t="s">
         <v>59</v>
@@ -1578,18 +1548,18 @@
         <v>7</v>
       </c>
       <c r="E18" s="0" t="s">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="F18" s="0" t="s">
-        <v>57</v>
+        <v>25</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="0">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="C19" s="0" t="s">
         <v>59</v>
@@ -1598,18 +1568,18 @@
         <v>7</v>
       </c>
       <c r="E19" s="0" t="s">
-        <v>78</v>
+        <v>14</v>
       </c>
       <c r="F19" s="0" t="s">
-        <v>57</v>
+        <v>14</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="0">
-        <v>45</v>
+        <v>37</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="C20" s="0" t="s">
         <v>59</v>
@@ -1618,18 +1588,18 @@
         <v>7</v>
       </c>
       <c r="E20" s="0" t="s">
-        <v>53</v>
+        <v>8</v>
       </c>
       <c r="F20" s="0" t="s">
-        <v>57</v>
+        <v>14</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="0">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="C21" s="0" t="s">
         <v>59</v>
@@ -1638,7 +1608,7 @@
         <v>7</v>
       </c>
       <c r="E21" s="0" t="s">
-        <v>53</v>
+        <v>8</v>
       </c>
       <c r="F21" s="0" t="s">
         <v>57</v>
@@ -1646,10 +1616,10 @@
     </row>
     <row r="22">
       <c r="A22" s="0">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="C22" s="0" t="s">
         <v>59</v>
@@ -1658,18 +1628,18 @@
         <v>7</v>
       </c>
       <c r="E22" s="0" t="s">
-        <v>53</v>
+        <v>78</v>
       </c>
       <c r="F22" s="0" t="s">
-        <v>78</v>
+        <v>57</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="0">
-        <v>36</v>
+        <v>45</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="C23" s="0" t="s">
         <v>59</v>
@@ -1678,18 +1648,18 @@
         <v>7</v>
       </c>
       <c r="E23" s="0" t="s">
-        <v>8</v>
+        <v>53</v>
       </c>
       <c r="F23" s="0" t="s">
-        <v>78</v>
+        <v>57</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="0">
-        <v>11</v>
+        <v>44</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="C24" s="0" t="s">
         <v>59</v>
@@ -1698,18 +1668,18 @@
         <v>7</v>
       </c>
       <c r="E24" s="0" t="s">
-        <v>22</v>
+        <v>53</v>
       </c>
       <c r="F24" s="0" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="0">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="C25" s="0" t="s">
         <v>59</v>
@@ -1718,18 +1688,18 @@
         <v>7</v>
       </c>
       <c r="E25" s="0" t="s">
-        <v>85</v>
+        <v>53</v>
       </c>
       <c r="F25" s="0" t="s">
-        <v>53</v>
+        <v>78</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="0">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="C26" s="0" t="s">
         <v>59</v>
@@ -1741,15 +1711,15 @@
         <v>8</v>
       </c>
       <c r="F26" s="0" t="s">
-        <v>53</v>
+        <v>78</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="0">
-        <v>32</v>
+        <v>11</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="C27" s="0" t="s">
         <v>59</v>
@@ -1758,18 +1728,18 @@
         <v>7</v>
       </c>
       <c r="E27" s="0" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="F27" s="0" t="s">
-        <v>8</v>
+        <v>53</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="0">
-        <v>31</v>
+        <v>40</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="C28" s="0" t="s">
         <v>59</v>
@@ -1778,18 +1748,18 @@
         <v>7</v>
       </c>
       <c r="E28" s="0" t="s">
-        <v>16</v>
+        <v>85</v>
       </c>
       <c r="F28" s="0" t="s">
-        <v>16</v>
+        <v>53</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="0">
-        <v>20</v>
+        <v>39</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="C29" s="0" t="s">
         <v>59</v>
@@ -1798,18 +1768,18 @@
         <v>7</v>
       </c>
       <c r="E29" s="0" t="s">
-        <v>22</v>
+        <v>8</v>
       </c>
       <c r="F29" s="0" t="s">
-        <v>16</v>
+        <v>53</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="0">
-        <v>9</v>
+        <v>32</v>
       </c>
       <c r="B30" s="0" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="C30" s="0" t="s">
         <v>59</v>
@@ -1818,18 +1788,18 @@
         <v>7</v>
       </c>
       <c r="E30" s="0" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="F30" s="0" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="0">
-        <v>8</v>
+        <v>31</v>
       </c>
       <c r="B31" s="0" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="C31" s="0" t="s">
         <v>59</v>
@@ -1838,7 +1808,7 @@
         <v>7</v>
       </c>
       <c r="E31" s="0" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="F31" s="0" t="s">
         <v>16</v>
@@ -1846,10 +1816,10 @@
     </row>
     <row r="32">
       <c r="A32" s="0">
-        <v>4</v>
+        <v>20</v>
       </c>
       <c r="B32" s="0" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="C32" s="0" t="s">
         <v>59</v>
@@ -1861,15 +1831,15 @@
         <v>22</v>
       </c>
       <c r="F32" s="0" t="s">
-        <v>93</v>
+        <v>16</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="0">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="B33" s="0" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="C33" s="0" t="s">
         <v>59</v>
@@ -1881,15 +1851,15 @@
         <v>22</v>
       </c>
       <c r="F33" s="0" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="0">
-        <v>30</v>
+        <v>8</v>
       </c>
       <c r="B34" s="0" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="C34" s="0" t="s">
         <v>59</v>
@@ -1901,15 +1871,15 @@
         <v>22</v>
       </c>
       <c r="F34" s="0" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="0">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B35" s="0" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="C35" s="0" t="s">
         <v>59</v>
@@ -1921,26 +1891,86 @@
         <v>22</v>
       </c>
       <c r="F35" s="0" t="s">
-        <v>22</v>
+        <v>93</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="0">
+        <v>3</v>
+      </c>
+      <c r="B36" s="0" t="s">
+        <v>94</v>
+      </c>
+      <c r="C36" s="0" t="s">
+        <v>59</v>
+      </c>
+      <c r="D36" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E36" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="F36" s="0" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" s="0">
+        <v>30</v>
+      </c>
+      <c r="B37" s="0" t="s">
+        <v>95</v>
+      </c>
+      <c r="C37" s="0" t="s">
+        <v>59</v>
+      </c>
+      <c r="D37" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E37" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="F37" s="0" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" s="0">
+        <v>2</v>
+      </c>
+      <c r="B38" s="0" t="s">
+        <v>96</v>
+      </c>
+      <c r="C38" s="0" t="s">
+        <v>59</v>
+      </c>
+      <c r="D38" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E38" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="F38" s="0" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" s="0">
         <v>1</v>
       </c>
-      <c r="B36" s="0" t="s">
+      <c r="B39" s="0" t="s">
         <v>97</v>
       </c>
-      <c r="C36" s="0" t="s">
-        <v>59</v>
-      </c>
-      <c r="D36" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="E36" s="0" t="s">
-        <v>22</v>
-      </c>
-      <c r="F36" s="0" t="s">
+      <c r="C39" s="0" t="s">
+        <v>59</v>
+      </c>
+      <c r="D39" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E39" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="F39" s="0" t="s">
         <v>22</v>
       </c>
     </row>
@@ -1984,7 +2014,7 @@
         <v>7</v>
       </c>
       <c r="F2" s="0">
-        <v>88</v>
+        <v>89</v>
       </c>
     </row>
     <row r="3">

</xml_diff>

<commit_message>
bug fix: loop back of color change events in New Color Dialog
</commit_message>
<xml_diff>
--- a/paint_todo.xlsx
+++ b/paint_todo.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="105">
   <si>
     <t>Id</t>
   </si>
@@ -391,6 +391,11 @@
   <si>
     <t xml:space="preserve">having problems with imprecise color format conversions
 it's really important they be perfectly reversible</t>
+  </si>
+  <si>
+    <t xml:space="preserve">refactor WithoutHaste.Drawing.Colors HSV to use ints instead of floats (0-360, 0-100, 0-100)
+CANCELLED
+more research online shows that float is proper for HSV</t>
   </si>
 </sst>
 </file>
@@ -443,7 +448,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:F43"/>
+  <dimension ref="A1:F41"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -503,10 +508,10 @@
     </row>
     <row r="4">
       <c r="A4" s="0">
-        <v>59</v>
+        <v>87</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C4" s="0" t="s">
         <v>6</v>
@@ -515,15 +520,15 @@
         <v>7</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="0">
-        <v>87</v>
+        <v>49</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C5" s="0" t="s">
         <v>6</v>
@@ -532,15 +537,15 @@
         <v>7</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="0">
-        <v>49</v>
+        <v>21</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C6" s="0" t="s">
         <v>6</v>
@@ -549,15 +554,15 @@
         <v>7</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="0">
-        <v>21</v>
+        <v>86</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="C7" s="0" t="s">
         <v>6</v>
@@ -566,15 +571,15 @@
         <v>7</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="0">
-        <v>86</v>
+        <v>54</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C8" s="0" t="s">
         <v>6</v>
@@ -583,15 +588,15 @@
         <v>7</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>10</v>
+        <v>25</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="0">
-        <v>54</v>
+        <v>88</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>24</v>
+        <v>102</v>
       </c>
       <c r="C9" s="0" t="s">
         <v>6</v>
@@ -600,15 +605,15 @@
         <v>7</v>
       </c>
       <c r="E9" s="0" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="0">
-        <v>89</v>
+        <v>53</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>103</v>
+        <v>26</v>
       </c>
       <c r="C10" s="0" t="s">
         <v>6</v>
@@ -617,15 +622,15 @@
         <v>7</v>
       </c>
       <c r="E10" s="0" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="0">
-        <v>88</v>
+        <v>51</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>102</v>
+        <v>27</v>
       </c>
       <c r="C11" s="0" t="s">
         <v>6</v>
@@ -634,15 +639,15 @@
         <v>7</v>
       </c>
       <c r="E11" s="0" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="0">
-        <v>53</v>
+        <v>76</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="C12" s="0" t="s">
         <v>6</v>
@@ -651,15 +656,15 @@
         <v>7</v>
       </c>
       <c r="E12" s="0" t="s">
-        <v>25</v>
+        <v>10</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="0">
-        <v>51</v>
+        <v>35</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>27</v>
+        <v>5</v>
       </c>
       <c r="C13" s="0" t="s">
         <v>6</v>
@@ -668,15 +673,15 @@
         <v>7</v>
       </c>
       <c r="E13" s="0" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="0">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C14" s="0" t="s">
         <v>6</v>
@@ -690,10 +695,10 @@
     </row>
     <row r="15">
       <c r="A15" s="0">
-        <v>35</v>
+        <v>85</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>5</v>
+        <v>30</v>
       </c>
       <c r="C15" s="0" t="s">
         <v>6</v>
@@ -702,15 +707,15 @@
         <v>7</v>
       </c>
       <c r="E15" s="0" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="0">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="C16" s="0" t="s">
         <v>6</v>
@@ -724,10 +729,10 @@
     </row>
     <row r="17">
       <c r="A17" s="0">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="C17" s="0" t="s">
         <v>6</v>
@@ -741,10 +746,10 @@
     </row>
     <row r="18">
       <c r="A18" s="0">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="C18" s="0" t="s">
         <v>6</v>
@@ -758,10 +763,10 @@
     </row>
     <row r="19">
       <c r="A19" s="0">
-        <v>77</v>
+        <v>52</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C19" s="0" t="s">
         <v>6</v>
@@ -770,15 +775,15 @@
         <v>7</v>
       </c>
       <c r="E19" s="0" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="0">
-        <v>78</v>
+        <v>27</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="C20" s="0" t="s">
         <v>6</v>
@@ -787,15 +792,15 @@
         <v>7</v>
       </c>
       <c r="E20" s="0" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="0">
-        <v>52</v>
+        <v>28</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="C21" s="0" t="s">
         <v>6</v>
@@ -804,15 +809,15 @@
         <v>7</v>
       </c>
       <c r="E21" s="0" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="0">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="C22" s="0" t="s">
         <v>6</v>
@@ -826,10 +831,10 @@
     </row>
     <row r="23">
       <c r="A23" s="0">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="C23" s="0" t="s">
         <v>6</v>
@@ -843,10 +848,10 @@
     </row>
     <row r="24">
       <c r="A24" s="0">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="C24" s="0" t="s">
         <v>6</v>
@@ -860,10 +865,10 @@
     </row>
     <row r="25">
       <c r="A25" s="0">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="C25" s="0" t="s">
         <v>6</v>
@@ -877,10 +882,10 @@
     </row>
     <row r="26">
       <c r="A26" s="0">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C26" s="0" t="s">
         <v>6</v>
@@ -894,10 +899,10 @@
     </row>
     <row r="27">
       <c r="A27" s="0">
-        <v>17</v>
+        <v>81</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="C27" s="0" t="s">
         <v>6</v>
@@ -906,15 +911,15 @@
         <v>7</v>
       </c>
       <c r="E27" s="0" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="0">
-        <v>18</v>
+        <v>82</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="C28" s="0" t="s">
         <v>6</v>
@@ -923,15 +928,15 @@
         <v>7</v>
       </c>
       <c r="E28" s="0" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="0">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="C29" s="0" t="s">
         <v>6</v>
@@ -945,10 +950,10 @@
     </row>
     <row r="30">
       <c r="A30" s="0">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="B30" s="0" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="C30" s="0" t="s">
         <v>6</v>
@@ -962,10 +967,10 @@
     </row>
     <row r="31">
       <c r="A31" s="0">
-        <v>83</v>
+        <v>25</v>
       </c>
       <c r="B31" s="0" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="C31" s="0" t="s">
         <v>6</v>
@@ -974,15 +979,15 @@
         <v>7</v>
       </c>
       <c r="E31" s="0" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="0">
-        <v>84</v>
+        <v>57</v>
       </c>
       <c r="B32" s="0" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="C32" s="0" t="s">
         <v>6</v>
@@ -996,10 +1001,10 @@
     </row>
     <row r="33">
       <c r="A33" s="0">
-        <v>25</v>
+        <v>65</v>
       </c>
       <c r="B33" s="0" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="C33" s="0" t="s">
         <v>6</v>
@@ -1008,15 +1013,15 @@
         <v>7</v>
       </c>
       <c r="E33" s="0" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="0">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B34" s="0" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="C34" s="0" t="s">
         <v>6</v>
@@ -1030,10 +1035,10 @@
     </row>
     <row r="35">
       <c r="A35" s="0">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="B35" s="0" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="C35" s="0" t="s">
         <v>6</v>
@@ -1047,10 +1052,10 @@
     </row>
     <row r="36">
       <c r="A36" s="0">
-        <v>58</v>
+        <v>26</v>
       </c>
       <c r="B36" s="0" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="C36" s="0" t="s">
         <v>6</v>
@@ -1059,15 +1064,15 @@
         <v>7</v>
       </c>
       <c r="E36" s="0" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="0">
-        <v>61</v>
+        <v>43</v>
       </c>
       <c r="B37" s="0" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="C37" s="0" t="s">
         <v>6</v>
@@ -1076,15 +1081,15 @@
         <v>7</v>
       </c>
       <c r="E37" s="0" t="s">
-        <v>10</v>
+        <v>53</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="0">
-        <v>26</v>
+        <v>74</v>
       </c>
       <c r="B38" s="0" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="C38" s="0" t="s">
         <v>6</v>
@@ -1093,15 +1098,15 @@
         <v>7</v>
       </c>
       <c r="E38" s="0" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="0">
-        <v>43</v>
+        <v>29</v>
       </c>
       <c r="B39" s="0" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="C39" s="0" t="s">
         <v>6</v>
@@ -1110,15 +1115,15 @@
         <v>7</v>
       </c>
       <c r="E39" s="0" t="s">
-        <v>53</v>
+        <v>22</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="0">
-        <v>74</v>
+        <v>47</v>
       </c>
       <c r="B40" s="0" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="C40" s="0" t="s">
         <v>6</v>
@@ -1127,15 +1132,15 @@
         <v>7</v>
       </c>
       <c r="E40" s="0" t="s">
-        <v>10</v>
+        <v>57</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="0">
-        <v>29</v>
+        <v>60</v>
       </c>
       <c r="B41" s="0" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="C41" s="0" t="s">
         <v>6</v>
@@ -1144,40 +1149,6 @@
         <v>7</v>
       </c>
       <c r="E41" s="0" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="42">
-      <c r="A42" s="0">
-        <v>47</v>
-      </c>
-      <c r="B42" s="0" t="s">
-        <v>56</v>
-      </c>
-      <c r="C42" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="D42" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="E42" s="0" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="43">
-      <c r="A43" s="0">
-        <v>60</v>
-      </c>
-      <c r="B43" s="0" t="s">
-        <v>58</v>
-      </c>
-      <c r="C43" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="D43" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="E43" s="0" t="s">
         <v>10</v>
       </c>
     </row>
@@ -1188,7 +1159,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:F39"/>
+  <dimension ref="A1:F41"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1216,10 +1187,10 @@
     </row>
     <row r="2">
       <c r="A2" s="0">
-        <v>69</v>
+        <v>89</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>12</v>
+        <v>103</v>
       </c>
       <c r="C2" s="0" t="s">
         <v>59</v>
@@ -1228,7 +1199,7 @@
         <v>7</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="F2" s="0" t="s">
         <v>19</v>
@@ -1236,10 +1207,10 @@
     </row>
     <row r="3">
       <c r="A3" s="0">
-        <v>68</v>
+        <v>59</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>11</v>
+        <v>104</v>
       </c>
       <c r="C3" s="0" t="s">
         <v>59</v>
@@ -1256,10 +1227,10 @@
     </row>
     <row r="4">
       <c r="A4" s="0">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="C4" s="0" t="s">
         <v>59</v>
@@ -1276,10 +1247,10 @@
     </row>
     <row r="5">
       <c r="A5" s="0">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>60</v>
+        <v>11</v>
       </c>
       <c r="C5" s="0" t="s">
         <v>59</v>
@@ -1291,15 +1262,15 @@
         <v>10</v>
       </c>
       <c r="F5" s="0" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="0">
-        <v>24</v>
+        <v>67</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>61</v>
+        <v>9</v>
       </c>
       <c r="C6" s="0" t="s">
         <v>59</v>
@@ -1308,18 +1279,18 @@
         <v>7</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="F6" s="0" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="0">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C7" s="0" t="s">
         <v>59</v>
@@ -1336,10 +1307,10 @@
     </row>
     <row r="8">
       <c r="A8" s="0">
-        <v>55</v>
+        <v>24</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C8" s="0" t="s">
         <v>59</v>
@@ -1348,7 +1319,7 @@
         <v>7</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="F8" s="0" t="s">
         <v>10</v>
@@ -1356,10 +1327,10 @@
     </row>
     <row r="9">
       <c r="A9" s="0">
-        <v>56</v>
+        <v>75</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C9" s="0" t="s">
         <v>59</v>
@@ -1368,7 +1339,7 @@
         <v>7</v>
       </c>
       <c r="E9" s="0" t="s">
-        <v>25</v>
+        <v>10</v>
       </c>
       <c r="F9" s="0" t="s">
         <v>10</v>
@@ -1376,10 +1347,10 @@
     </row>
     <row r="10">
       <c r="A10" s="0">
-        <v>72</v>
+        <v>55</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C10" s="0" t="s">
         <v>59</v>
@@ -1388,7 +1359,7 @@
         <v>7</v>
       </c>
       <c r="E10" s="0" t="s">
-        <v>10</v>
+        <v>25</v>
       </c>
       <c r="F10" s="0" t="s">
         <v>10</v>
@@ -1396,10 +1367,10 @@
     </row>
     <row r="11">
       <c r="A11" s="0">
-        <v>66</v>
+        <v>56</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C11" s="0" t="s">
         <v>59</v>
@@ -1408,7 +1379,7 @@
         <v>7</v>
       </c>
       <c r="E11" s="0" t="s">
-        <v>10</v>
+        <v>25</v>
       </c>
       <c r="F11" s="0" t="s">
         <v>10</v>
@@ -1416,10 +1387,10 @@
     </row>
     <row r="12">
       <c r="A12" s="0">
-        <v>62</v>
+        <v>72</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C12" s="0" t="s">
         <v>59</v>
@@ -1436,10 +1407,10 @@
     </row>
     <row r="13">
       <c r="A13" s="0">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C13" s="0" t="s">
         <v>59</v>
@@ -1456,10 +1427,10 @@
     </row>
     <row r="14">
       <c r="A14" s="0">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C14" s="0" t="s">
         <v>59</v>
@@ -1476,10 +1447,10 @@
     </row>
     <row r="15">
       <c r="A15" s="0">
-        <v>63</v>
+        <v>70</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C15" s="0" t="s">
         <v>59</v>
@@ -1496,10 +1467,10 @@
     </row>
     <row r="16">
       <c r="A16" s="0">
-        <v>13</v>
+        <v>64</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C16" s="0" t="s">
         <v>59</v>
@@ -1508,7 +1479,7 @@
         <v>7</v>
       </c>
       <c r="E16" s="0" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="F16" s="0" t="s">
         <v>10</v>
@@ -1516,10 +1487,10 @@
     </row>
     <row r="17">
       <c r="A17" s="0">
-        <v>42</v>
+        <v>63</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C17" s="0" t="s">
         <v>59</v>
@@ -1528,18 +1499,18 @@
         <v>7</v>
       </c>
       <c r="E17" s="0" t="s">
-        <v>53</v>
+        <v>10</v>
       </c>
       <c r="F17" s="0" t="s">
-        <v>25</v>
+        <v>10</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="0">
-        <v>33</v>
+        <v>13</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C18" s="0" t="s">
         <v>59</v>
@@ -1548,18 +1519,18 @@
         <v>7</v>
       </c>
       <c r="E18" s="0" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="F18" s="0" t="s">
-        <v>25</v>
+        <v>10</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="0">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C19" s="0" t="s">
         <v>59</v>
@@ -1568,18 +1539,18 @@
         <v>7</v>
       </c>
       <c r="E19" s="0" t="s">
-        <v>14</v>
+        <v>53</v>
       </c>
       <c r="F19" s="0" t="s">
-        <v>14</v>
+        <v>25</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="0">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C20" s="0" t="s">
         <v>59</v>
@@ -1588,18 +1559,18 @@
         <v>7</v>
       </c>
       <c r="E20" s="0" t="s">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="F20" s="0" t="s">
-        <v>14</v>
+        <v>25</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="0">
-        <v>38</v>
+        <v>48</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C21" s="0" t="s">
         <v>59</v>
@@ -1608,18 +1579,18 @@
         <v>7</v>
       </c>
       <c r="E21" s="0" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="F21" s="0" t="s">
-        <v>57</v>
+        <v>14</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="0">
-        <v>46</v>
+        <v>37</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C22" s="0" t="s">
         <v>59</v>
@@ -1628,18 +1599,18 @@
         <v>7</v>
       </c>
       <c r="E22" s="0" t="s">
-        <v>78</v>
+        <v>8</v>
       </c>
       <c r="F22" s="0" t="s">
-        <v>57</v>
+        <v>14</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="0">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="C23" s="0" t="s">
         <v>59</v>
@@ -1648,7 +1619,7 @@
         <v>7</v>
       </c>
       <c r="E23" s="0" t="s">
-        <v>53</v>
+        <v>8</v>
       </c>
       <c r="F23" s="0" t="s">
         <v>57</v>
@@ -1656,10 +1627,10 @@
     </row>
     <row r="24">
       <c r="A24" s="0">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="C24" s="0" t="s">
         <v>59</v>
@@ -1668,7 +1639,7 @@
         <v>7</v>
       </c>
       <c r="E24" s="0" t="s">
-        <v>53</v>
+        <v>78</v>
       </c>
       <c r="F24" s="0" t="s">
         <v>57</v>
@@ -1676,10 +1647,10 @@
     </row>
     <row r="25">
       <c r="A25" s="0">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C25" s="0" t="s">
         <v>59</v>
@@ -1691,15 +1662,15 @@
         <v>53</v>
       </c>
       <c r="F25" s="0" t="s">
-        <v>78</v>
+        <v>57</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="0">
-        <v>36</v>
+        <v>44</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C26" s="0" t="s">
         <v>59</v>
@@ -1708,18 +1679,18 @@
         <v>7</v>
       </c>
       <c r="E26" s="0" t="s">
-        <v>8</v>
+        <v>53</v>
       </c>
       <c r="F26" s="0" t="s">
-        <v>78</v>
+        <v>57</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="0">
-        <v>11</v>
+        <v>41</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C27" s="0" t="s">
         <v>59</v>
@@ -1728,18 +1699,18 @@
         <v>7</v>
       </c>
       <c r="E27" s="0" t="s">
-        <v>22</v>
+        <v>53</v>
       </c>
       <c r="F27" s="0" t="s">
-        <v>53</v>
+        <v>78</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="0">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C28" s="0" t="s">
         <v>59</v>
@@ -1748,18 +1719,18 @@
         <v>7</v>
       </c>
       <c r="E28" s="0" t="s">
-        <v>85</v>
+        <v>8</v>
       </c>
       <c r="F28" s="0" t="s">
-        <v>53</v>
+        <v>78</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="0">
-        <v>39</v>
+        <v>11</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="C29" s="0" t="s">
         <v>59</v>
@@ -1768,7 +1739,7 @@
         <v>7</v>
       </c>
       <c r="E29" s="0" t="s">
-        <v>8</v>
+        <v>22</v>
       </c>
       <c r="F29" s="0" t="s">
         <v>53</v>
@@ -1776,10 +1747,10 @@
     </row>
     <row r="30">
       <c r="A30" s="0">
-        <v>32</v>
+        <v>40</v>
       </c>
       <c r="B30" s="0" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="C30" s="0" t="s">
         <v>59</v>
@@ -1788,18 +1759,18 @@
         <v>7</v>
       </c>
       <c r="E30" s="0" t="s">
-        <v>16</v>
+        <v>85</v>
       </c>
       <c r="F30" s="0" t="s">
-        <v>8</v>
+        <v>53</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="0">
-        <v>31</v>
+        <v>39</v>
       </c>
       <c r="B31" s="0" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C31" s="0" t="s">
         <v>59</v>
@@ -1808,18 +1779,18 @@
         <v>7</v>
       </c>
       <c r="E31" s="0" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="F31" s="0" t="s">
-        <v>16</v>
+        <v>53</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="0">
-        <v>20</v>
+        <v>32</v>
       </c>
       <c r="B32" s="0" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C32" s="0" t="s">
         <v>59</v>
@@ -1828,18 +1799,18 @@
         <v>7</v>
       </c>
       <c r="E32" s="0" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="F32" s="0" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="0">
-        <v>9</v>
+        <v>31</v>
       </c>
       <c r="B33" s="0" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C33" s="0" t="s">
         <v>59</v>
@@ -1848,7 +1819,7 @@
         <v>7</v>
       </c>
       <c r="E33" s="0" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="F33" s="0" t="s">
         <v>16</v>
@@ -1856,10 +1827,10 @@
     </row>
     <row r="34">
       <c r="A34" s="0">
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="B34" s="0" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C34" s="0" t="s">
         <v>59</v>
@@ -1876,10 +1847,10 @@
     </row>
     <row r="35">
       <c r="A35" s="0">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="B35" s="0" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C35" s="0" t="s">
         <v>59</v>
@@ -1891,15 +1862,15 @@
         <v>22</v>
       </c>
       <c r="F35" s="0" t="s">
-        <v>93</v>
+        <v>16</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="0">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="B36" s="0" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="C36" s="0" t="s">
         <v>59</v>
@@ -1911,15 +1882,15 @@
         <v>22</v>
       </c>
       <c r="F36" s="0" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="0">
-        <v>30</v>
+        <v>4</v>
       </c>
       <c r="B37" s="0" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="C37" s="0" t="s">
         <v>59</v>
@@ -1931,15 +1902,15 @@
         <v>22</v>
       </c>
       <c r="F37" s="0" t="s">
-        <v>22</v>
+        <v>93</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="0">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B38" s="0" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C38" s="0" t="s">
         <v>59</v>
@@ -1956,21 +1927,61 @@
     </row>
     <row r="39">
       <c r="A39" s="0">
+        <v>30</v>
+      </c>
+      <c r="B39" s="0" t="s">
+        <v>95</v>
+      </c>
+      <c r="C39" s="0" t="s">
+        <v>59</v>
+      </c>
+      <c r="D39" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E39" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="F39" s="0" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" s="0">
+        <v>2</v>
+      </c>
+      <c r="B40" s="0" t="s">
+        <v>96</v>
+      </c>
+      <c r="C40" s="0" t="s">
+        <v>59</v>
+      </c>
+      <c r="D40" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E40" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="F40" s="0" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" s="0">
         <v>1</v>
       </c>
-      <c r="B39" s="0" t="s">
+      <c r="B41" s="0" t="s">
         <v>97</v>
       </c>
-      <c r="C39" s="0" t="s">
-        <v>59</v>
-      </c>
-      <c r="D39" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="E39" s="0" t="s">
-        <v>22</v>
-      </c>
-      <c r="F39" s="0" t="s">
+      <c r="C41" s="0" t="s">
+        <v>59</v>
+      </c>
+      <c r="D41" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E41" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="F41" s="0" t="s">
         <v>22</v>
       </c>
     </row>

</xml_diff>

<commit_message>
setup of color test cases
</commit_message>
<xml_diff>
--- a/paint_todo.xlsx
+++ b/paint_todo.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="106">
   <si>
     <t>Id</t>
   </si>
@@ -396,6 +396,9 @@
     <t xml:space="preserve">refactor WithoutHaste.Drawing.Colors HSV to use ints instead of floats (0-360, 0-100, 0-100)
 CANCELLED
 more research online shows that float is proper for HSV</t>
+  </si>
+  <si>
+    <t>name all Settings properties in OneImageForm with prefix "Setting" for consistency</t>
   </si>
 </sst>
 </file>
@@ -448,7 +451,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:F41"/>
+  <dimension ref="A1:F42"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -610,10 +613,10 @@
     </row>
     <row r="10">
       <c r="A10" s="0">
-        <v>53</v>
+        <v>90</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>26</v>
+        <v>105</v>
       </c>
       <c r="C10" s="0" t="s">
         <v>6</v>
@@ -622,15 +625,15 @@
         <v>7</v>
       </c>
       <c r="E10" s="0" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="0">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C11" s="0" t="s">
         <v>6</v>
@@ -639,15 +642,15 @@
         <v>7</v>
       </c>
       <c r="E11" s="0" t="s">
-        <v>14</v>
+        <v>25</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="0">
-        <v>76</v>
+        <v>51</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C12" s="0" t="s">
         <v>6</v>
@@ -656,15 +659,15 @@
         <v>7</v>
       </c>
       <c r="E12" s="0" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="0">
-        <v>35</v>
+        <v>76</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>5</v>
+        <v>28</v>
       </c>
       <c r="C13" s="0" t="s">
         <v>6</v>
@@ -673,15 +676,15 @@
         <v>7</v>
       </c>
       <c r="E13" s="0" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="0">
-        <v>79</v>
+        <v>35</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>29</v>
+        <v>5</v>
       </c>
       <c r="C14" s="0" t="s">
         <v>6</v>
@@ -690,15 +693,15 @@
         <v>7</v>
       </c>
       <c r="E14" s="0" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="0">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C15" s="0" t="s">
         <v>6</v>
@@ -712,10 +715,10 @@
     </row>
     <row r="16">
       <c r="A16" s="0">
-        <v>80</v>
+        <v>85</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C16" s="0" t="s">
         <v>6</v>
@@ -729,10 +732,10 @@
     </row>
     <row r="17">
       <c r="A17" s="0">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C17" s="0" t="s">
         <v>6</v>
@@ -746,10 +749,10 @@
     </row>
     <row r="18">
       <c r="A18" s="0">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C18" s="0" t="s">
         <v>6</v>
@@ -763,10 +766,10 @@
     </row>
     <row r="19">
       <c r="A19" s="0">
-        <v>52</v>
+        <v>78</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C19" s="0" t="s">
         <v>6</v>
@@ -775,15 +778,15 @@
         <v>7</v>
       </c>
       <c r="E19" s="0" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="0">
-        <v>27</v>
+        <v>52</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C20" s="0" t="s">
         <v>6</v>
@@ -792,15 +795,15 @@
         <v>7</v>
       </c>
       <c r="E20" s="0" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="0">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C21" s="0" t="s">
         <v>6</v>
@@ -814,10 +817,10 @@
     </row>
     <row r="22">
       <c r="A22" s="0">
-        <v>19</v>
+        <v>28</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C22" s="0" t="s">
         <v>6</v>
@@ -831,10 +834,10 @@
     </row>
     <row r="23">
       <c r="A23" s="0">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C23" s="0" t="s">
         <v>6</v>
@@ -848,10 +851,10 @@
     </row>
     <row r="24">
       <c r="A24" s="0">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C24" s="0" t="s">
         <v>6</v>
@@ -865,10 +868,10 @@
     </row>
     <row r="25">
       <c r="A25" s="0">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C25" s="0" t="s">
         <v>6</v>
@@ -882,10 +885,10 @@
     </row>
     <row r="26">
       <c r="A26" s="0">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C26" s="0" t="s">
         <v>6</v>
@@ -899,10 +902,10 @@
     </row>
     <row r="27">
       <c r="A27" s="0">
-        <v>81</v>
+        <v>18</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C27" s="0" t="s">
         <v>6</v>
@@ -911,15 +914,15 @@
         <v>7</v>
       </c>
       <c r="E27" s="0" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="0">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C28" s="0" t="s">
         <v>6</v>
@@ -933,10 +936,10 @@
     </row>
     <row r="29">
       <c r="A29" s="0">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C29" s="0" t="s">
         <v>6</v>
@@ -950,10 +953,10 @@
     </row>
     <row r="30">
       <c r="A30" s="0">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B30" s="0" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C30" s="0" t="s">
         <v>6</v>
@@ -967,10 +970,10 @@
     </row>
     <row r="31">
       <c r="A31" s="0">
-        <v>25</v>
+        <v>84</v>
       </c>
       <c r="B31" s="0" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C31" s="0" t="s">
         <v>6</v>
@@ -979,15 +982,15 @@
         <v>7</v>
       </c>
       <c r="E31" s="0" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="0">
-        <v>57</v>
+        <v>25</v>
       </c>
       <c r="B32" s="0" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C32" s="0" t="s">
         <v>6</v>
@@ -996,15 +999,15 @@
         <v>7</v>
       </c>
       <c r="E32" s="0" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="0">
-        <v>65</v>
+        <v>57</v>
       </c>
       <c r="B33" s="0" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C33" s="0" t="s">
         <v>6</v>
@@ -1018,10 +1021,10 @@
     </row>
     <row r="34">
       <c r="A34" s="0">
-        <v>58</v>
+        <v>65</v>
       </c>
       <c r="B34" s="0" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C34" s="0" t="s">
         <v>6</v>
@@ -1035,10 +1038,10 @@
     </row>
     <row r="35">
       <c r="A35" s="0">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="B35" s="0" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C35" s="0" t="s">
         <v>6</v>
@@ -1052,10 +1055,10 @@
     </row>
     <row r="36">
       <c r="A36" s="0">
-        <v>26</v>
+        <v>61</v>
       </c>
       <c r="B36" s="0" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C36" s="0" t="s">
         <v>6</v>
@@ -1064,15 +1067,15 @@
         <v>7</v>
       </c>
       <c r="E36" s="0" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="0">
-        <v>43</v>
+        <v>26</v>
       </c>
       <c r="B37" s="0" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C37" s="0" t="s">
         <v>6</v>
@@ -1081,15 +1084,15 @@
         <v>7</v>
       </c>
       <c r="E37" s="0" t="s">
-        <v>53</v>
+        <v>22</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="0">
-        <v>74</v>
+        <v>43</v>
       </c>
       <c r="B38" s="0" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C38" s="0" t="s">
         <v>6</v>
@@ -1098,15 +1101,15 @@
         <v>7</v>
       </c>
       <c r="E38" s="0" t="s">
-        <v>10</v>
+        <v>53</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="0">
-        <v>29</v>
+        <v>74</v>
       </c>
       <c r="B39" s="0" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C39" s="0" t="s">
         <v>6</v>
@@ -1115,15 +1118,15 @@
         <v>7</v>
       </c>
       <c r="E39" s="0" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="0">
-        <v>47</v>
+        <v>29</v>
       </c>
       <c r="B40" s="0" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C40" s="0" t="s">
         <v>6</v>
@@ -1132,23 +1135,40 @@
         <v>7</v>
       </c>
       <c r="E40" s="0" t="s">
-        <v>57</v>
+        <v>22</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="0">
+        <v>47</v>
+      </c>
+      <c r="B41" s="0" t="s">
+        <v>56</v>
+      </c>
+      <c r="C41" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D41" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E41" s="0" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" s="0">
         <v>60</v>
       </c>
-      <c r="B41" s="0" t="s">
+      <c r="B42" s="0" t="s">
         <v>58</v>
       </c>
-      <c r="C41" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="D41" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="E41" s="0" t="s">
+      <c r="C42" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D42" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E42" s="0" t="s">
         <v>10</v>
       </c>
     </row>
@@ -2025,7 +2045,7 @@
         <v>7</v>
       </c>
       <c r="F2" s="0">
-        <v>89</v>
+        <v>90</v>
       </c>
     </row>
     <row r="3">

</xml_diff>

<commit_message>
test cases for applying/removing color to grayscale
</commit_message>
<xml_diff>
--- a/paint_todo.xlsx
+++ b/paint_todo.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="107">
   <si>
     <t>Id</t>
   </si>
@@ -29,38 +29,18 @@
   </si>
   <si>
     <t>Created</t>
-  </si>
-  <si>
-    <t xml:space="preserve">set and check tolerance for "black" and "white"
-- "blacks" will be left untouched
-- "whites" will be treated as pure white, which will in effect alter them to white</t>
-  </si>
-  <si>
-    <t>Todo</t>
-  </si>
-  <si>
-    <t>Task</t>
-  </si>
-  <si>
-    <t>8/12/2018</t>
-  </si>
-  <si>
-    <t>new color: enter an rgb value</t>
-  </si>
-  <si>
-    <t>8/24/2018</t>
-  </si>
-  <si>
-    <t>new color: enter a hexadecimal value</t>
-  </si>
-  <si>
-    <t>new color: enter an hsv value</t>
   </si>
   <si>
     <t xml:space="preserve">design test that generates value scale for many different colors, easy to scan with the eye
 - for instance, sometimes the adjusted color gets darker than the lightest "black", leaving a paler ring around it</t>
   </si>
   <si>
+    <t>Todo</t>
+  </si>
+  <si>
+    <t>Task</t>
+  </si>
+  <si>
     <t>8/22/2018</t>
   </si>
   <si>
@@ -68,9 +48,6 @@
   </si>
   <si>
     <t>8/11/2018</t>
-  </si>
-  <si>
-    <t>refactor WithoutHaste.Drawing.Colors HSV to use ints instead of floats (0-360, 0-100, 0-100)</t>
   </si>
   <si>
     <t>refactor all history actions and panels to use proper events instead of delegate properties</t>
@@ -92,6 +69,9 @@
   <si>
     <t xml:space="preserve">bug: Palette &gt; New &gt; Done
 get error because no filename to open in main form</t>
+  </si>
+  <si>
+    <t>8/24/2018</t>
   </si>
   <si>
     <t xml:space="preserve">make a MasterImage class
@@ -100,6 +80,15 @@
   </si>
   <si>
     <t>8/23/2018</t>
+  </si>
+  <si>
+    <t xml:space="preserve">to be consistent with System.Convert naming standards
+update ConvertColors
+- To&lt;Type&gt;(FromType)
+- &lt;FromType&gt;To&lt;Type&gt;(list of generic params)</t>
+  </si>
+  <si>
+    <t>name all Settings properties in OneImageForm with prefix "Setting" for consistency</t>
   </si>
   <si>
     <t xml:space="preserve">prompt to save if image has changed since last save
@@ -112,6 +101,20 @@
   </si>
   <si>
     <t>full documentation of Perpetual Paint</t>
+  </si>
+  <si>
+    <t>in public projects, make a Release directory to put each Version into</t>
+  </si>
+  <si>
+    <t>8/26/2018</t>
+  </si>
+  <si>
+    <t xml:space="preserve">set and check tolerance for "black" and "white"
+- "blacks" will be left untouched
+- "whites" will be treated as pure white, which will in effect alter them to white</t>
+  </si>
+  <si>
+    <t>8/12/2018</t>
   </si>
   <si>
     <t xml:space="preserve">documentation: include request for sample palette files for the specific formats/color spaces I can't verify because I don't have a test file to load
@@ -233,6 +236,24 @@
     <t>Done</t>
   </si>
   <si>
+    <t xml:space="preserve">having problems with imprecise color format conversions
+it's really important they be perfectly reversible</t>
+  </si>
+  <si>
+    <t xml:space="preserve">refactor WithoutHaste.Drawing.Colors HSV to use ints instead of floats (0-360, 0-100, 0-100)
+CANCELLED
+more research online shows that float is proper for HSV</t>
+  </si>
+  <si>
+    <t>new color: enter an hsv value</t>
+  </si>
+  <si>
+    <t>new color: enter a hexadecimal value</t>
+  </si>
+  <si>
+    <t>new color: enter an rgb value</t>
+  </si>
+  <si>
     <t>edit palette: display rgb/hexdecimal/hsv values of selected color</t>
   </si>
   <si>
@@ -381,24 +402,6 @@
   </si>
   <si>
     <t>Bug</t>
-  </si>
-  <si>
-    <t xml:space="preserve">to be consistent with System.Convert naming standards
-update ConvertColors
-- To&lt;Type&gt;(FromType)
-- &lt;FromType&gt;To&lt;Type&gt;(list of generic params)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">having problems with imprecise color format conversions
-it's really important they be perfectly reversible</t>
-  </si>
-  <si>
-    <t xml:space="preserve">refactor WithoutHaste.Drawing.Colors HSV to use ints instead of floats (0-360, 0-100, 0-100)
-CANCELLED
-more research online shows that float is proper for HSV</t>
-  </si>
-  <si>
-    <t>name all Settings properties in OneImageForm with prefix "Setting" for consistency</t>
   </si>
 </sst>
 </file>
@@ -451,7 +454,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:F42"/>
+  <dimension ref="A1:F43"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -480,7 +483,7 @@
         <v>50</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="C2" s="0" t="s">
         <v>6</v>
@@ -489,7 +492,7 @@
         <v>7</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
     </row>
     <row r="3">
@@ -497,7 +500,7 @@
         <v>34</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="C3" s="0" t="s">
         <v>6</v>
@@ -506,7 +509,7 @@
         <v>7</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4">
@@ -514,7 +517,7 @@
         <v>87</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="C4" s="0" t="s">
         <v>6</v>
@@ -523,7 +526,7 @@
         <v>7</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
     </row>
     <row r="5">
@@ -531,7 +534,7 @@
         <v>49</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="C5" s="0" t="s">
         <v>6</v>
@@ -540,7 +543,7 @@
         <v>7</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
     </row>
     <row r="6">
@@ -548,7 +551,7 @@
         <v>21</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="C6" s="0" t="s">
         <v>6</v>
@@ -557,7 +560,7 @@
         <v>7</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
     </row>
     <row r="7">
@@ -565,7 +568,7 @@
         <v>86</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="C7" s="0" t="s">
         <v>6</v>
@@ -574,7 +577,7 @@
         <v>7</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
     </row>
     <row r="8">
@@ -582,7 +585,7 @@
         <v>54</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="C8" s="0" t="s">
         <v>6</v>
@@ -591,7 +594,7 @@
         <v>7</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
     </row>
     <row r="9">
@@ -599,7 +602,7 @@
         <v>88</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>102</v>
+        <v>20</v>
       </c>
       <c r="C9" s="0" t="s">
         <v>6</v>
@@ -608,7 +611,7 @@
         <v>7</v>
       </c>
       <c r="E9" s="0" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
     </row>
     <row r="10">
@@ -616,7 +619,7 @@
         <v>90</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>105</v>
+        <v>21</v>
       </c>
       <c r="C10" s="0" t="s">
         <v>6</v>
@@ -625,7 +628,7 @@
         <v>7</v>
       </c>
       <c r="E10" s="0" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
     </row>
     <row r="11">
@@ -633,7 +636,7 @@
         <v>53</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="C11" s="0" t="s">
         <v>6</v>
@@ -642,7 +645,7 @@
         <v>7</v>
       </c>
       <c r="E11" s="0" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
     </row>
     <row r="12">
@@ -650,7 +653,7 @@
         <v>51</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="C12" s="0" t="s">
         <v>6</v>
@@ -659,7 +662,7 @@
         <v>7</v>
       </c>
       <c r="E12" s="0" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
     </row>
     <row r="13">
@@ -667,7 +670,7 @@
         <v>76</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="C13" s="0" t="s">
         <v>6</v>
@@ -676,15 +679,15 @@
         <v>7</v>
       </c>
       <c r="E13" s="0" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="0">
-        <v>35</v>
+        <v>91</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>5</v>
+        <v>25</v>
       </c>
       <c r="C14" s="0" t="s">
         <v>6</v>
@@ -693,15 +696,15 @@
         <v>7</v>
       </c>
       <c r="E14" s="0" t="s">
-        <v>8</v>
+        <v>26</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="0">
-        <v>79</v>
+        <v>35</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C15" s="0" t="s">
         <v>6</v>
@@ -710,15 +713,15 @@
         <v>7</v>
       </c>
       <c r="E15" s="0" t="s">
-        <v>10</v>
+        <v>28</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="0">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C16" s="0" t="s">
         <v>6</v>
@@ -727,15 +730,15 @@
         <v>7</v>
       </c>
       <c r="E16" s="0" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="0">
-        <v>80</v>
+        <v>85</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C17" s="0" t="s">
         <v>6</v>
@@ -744,15 +747,15 @@
         <v>7</v>
       </c>
       <c r="E17" s="0" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="0">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C18" s="0" t="s">
         <v>6</v>
@@ -761,15 +764,15 @@
         <v>7</v>
       </c>
       <c r="E18" s="0" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="0">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C19" s="0" t="s">
         <v>6</v>
@@ -778,15 +781,15 @@
         <v>7</v>
       </c>
       <c r="E19" s="0" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="0">
-        <v>52</v>
+        <v>78</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C20" s="0" t="s">
         <v>6</v>
@@ -795,15 +798,15 @@
         <v>7</v>
       </c>
       <c r="E20" s="0" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="0">
-        <v>27</v>
+        <v>52</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C21" s="0" t="s">
         <v>6</v>
@@ -812,15 +815,15 @@
         <v>7</v>
       </c>
       <c r="E21" s="0" t="s">
-        <v>22</v>
+        <v>8</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="0">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C22" s="0" t="s">
         <v>6</v>
@@ -829,15 +832,15 @@
         <v>7</v>
       </c>
       <c r="E22" s="0" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="0">
-        <v>19</v>
+        <v>28</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C23" s="0" t="s">
         <v>6</v>
@@ -846,15 +849,15 @@
         <v>7</v>
       </c>
       <c r="E23" s="0" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="0">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C24" s="0" t="s">
         <v>6</v>
@@ -863,15 +866,15 @@
         <v>7</v>
       </c>
       <c r="E24" s="0" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="0">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C25" s="0" t="s">
         <v>6</v>
@@ -880,15 +883,15 @@
         <v>7</v>
       </c>
       <c r="E25" s="0" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="0">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C26" s="0" t="s">
         <v>6</v>
@@ -897,15 +900,15 @@
         <v>7</v>
       </c>
       <c r="E26" s="0" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="0">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C27" s="0" t="s">
         <v>6</v>
@@ -914,15 +917,15 @@
         <v>7</v>
       </c>
       <c r="E27" s="0" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="0">
-        <v>81</v>
+        <v>18</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C28" s="0" t="s">
         <v>6</v>
@@ -931,15 +934,15 @@
         <v>7</v>
       </c>
       <c r="E28" s="0" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="0">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C29" s="0" t="s">
         <v>6</v>
@@ -948,15 +951,15 @@
         <v>7</v>
       </c>
       <c r="E29" s="0" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="0">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B30" s="0" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C30" s="0" t="s">
         <v>6</v>
@@ -965,15 +968,15 @@
         <v>7</v>
       </c>
       <c r="E30" s="0" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="0">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B31" s="0" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C31" s="0" t="s">
         <v>6</v>
@@ -982,15 +985,15 @@
         <v>7</v>
       </c>
       <c r="E31" s="0" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="0">
-        <v>25</v>
+        <v>84</v>
       </c>
       <c r="B32" s="0" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C32" s="0" t="s">
         <v>6</v>
@@ -999,15 +1002,15 @@
         <v>7</v>
       </c>
       <c r="E32" s="0" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="0">
-        <v>57</v>
+        <v>25</v>
       </c>
       <c r="B33" s="0" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C33" s="0" t="s">
         <v>6</v>
@@ -1016,15 +1019,15 @@
         <v>7</v>
       </c>
       <c r="E33" s="0" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="0">
-        <v>65</v>
+        <v>57</v>
       </c>
       <c r="B34" s="0" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C34" s="0" t="s">
         <v>6</v>
@@ -1033,15 +1036,15 @@
         <v>7</v>
       </c>
       <c r="E34" s="0" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="0">
-        <v>58</v>
+        <v>65</v>
       </c>
       <c r="B35" s="0" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C35" s="0" t="s">
         <v>6</v>
@@ -1050,15 +1053,15 @@
         <v>7</v>
       </c>
       <c r="E35" s="0" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="0">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="B36" s="0" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C36" s="0" t="s">
         <v>6</v>
@@ -1067,15 +1070,15 @@
         <v>7</v>
       </c>
       <c r="E36" s="0" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="0">
-        <v>26</v>
+        <v>61</v>
       </c>
       <c r="B37" s="0" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C37" s="0" t="s">
         <v>6</v>
@@ -1084,15 +1087,15 @@
         <v>7</v>
       </c>
       <c r="E37" s="0" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="0">
-        <v>43</v>
+        <v>26</v>
       </c>
       <c r="B38" s="0" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C38" s="0" t="s">
         <v>6</v>
@@ -1101,15 +1104,15 @@
         <v>7</v>
       </c>
       <c r="E38" s="0" t="s">
-        <v>53</v>
+        <v>15</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="0">
-        <v>74</v>
+        <v>43</v>
       </c>
       <c r="B39" s="0" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C39" s="0" t="s">
         <v>6</v>
@@ -1118,15 +1121,15 @@
         <v>7</v>
       </c>
       <c r="E39" s="0" t="s">
-        <v>10</v>
+        <v>53</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="0">
-        <v>29</v>
+        <v>74</v>
       </c>
       <c r="B40" s="0" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C40" s="0" t="s">
         <v>6</v>
@@ -1135,15 +1138,15 @@
         <v>7</v>
       </c>
       <c r="E40" s="0" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="0">
-        <v>47</v>
+        <v>29</v>
       </c>
       <c r="B41" s="0" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C41" s="0" t="s">
         <v>6</v>
@@ -1152,24 +1155,41 @@
         <v>7</v>
       </c>
       <c r="E41" s="0" t="s">
-        <v>57</v>
+        <v>15</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="0">
+        <v>47</v>
+      </c>
+      <c r="B42" s="0" t="s">
+        <v>56</v>
+      </c>
+      <c r="C42" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D42" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E42" s="0" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" s="0">
         <v>60</v>
       </c>
-      <c r="B42" s="0" t="s">
+      <c r="B43" s="0" t="s">
         <v>58</v>
       </c>
-      <c r="C42" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="D42" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="E42" s="0" t="s">
-        <v>10</v>
+      <c r="C43" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D43" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E43" s="0" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>
@@ -1210,7 +1230,7 @@
         <v>89</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>103</v>
+        <v>60</v>
       </c>
       <c r="C2" s="0" t="s">
         <v>59</v>
@@ -1219,10 +1239,10 @@
         <v>7</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3">
@@ -1230,7 +1250,7 @@
         <v>59</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>104</v>
+        <v>61</v>
       </c>
       <c r="C3" s="0" t="s">
         <v>59</v>
@@ -1239,10 +1259,10 @@
         <v>7</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="F3" s="0" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
     </row>
     <row r="4">
@@ -1250,19 +1270,19 @@
         <v>69</v>
       </c>
       <c r="B4" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>59</v>
+      </c>
+      <c r="D4" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E4" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="F4" s="0" t="s">
         <v>12</v>
-      </c>
-      <c r="C4" s="0" t="s">
-        <v>59</v>
-      </c>
-      <c r="D4" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="E4" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="F4" s="0" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="5">
@@ -1270,7 +1290,7 @@
         <v>68</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>11</v>
+        <v>63</v>
       </c>
       <c r="C5" s="0" t="s">
         <v>59</v>
@@ -1279,10 +1299,10 @@
         <v>7</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="F5" s="0" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
     </row>
     <row r="6">
@@ -1290,7 +1310,7 @@
         <v>67</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>9</v>
+        <v>64</v>
       </c>
       <c r="C6" s="0" t="s">
         <v>59</v>
@@ -1299,10 +1319,10 @@
         <v>7</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="F6" s="0" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
     </row>
     <row r="7">
@@ -1310,7 +1330,7 @@
         <v>71</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>60</v>
+        <v>65</v>
       </c>
       <c r="C7" s="0" t="s">
         <v>59</v>
@@ -1319,10 +1339,10 @@
         <v>7</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="F7" s="0" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
     </row>
     <row r="8">
@@ -1330,7 +1350,7 @@
         <v>24</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>61</v>
+        <v>66</v>
       </c>
       <c r="C8" s="0" t="s">
         <v>59</v>
@@ -1339,10 +1359,10 @@
         <v>7</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="F8" s="0" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
     </row>
     <row r="9">
@@ -1350,7 +1370,7 @@
         <v>75</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>62</v>
+        <v>67</v>
       </c>
       <c r="C9" s="0" t="s">
         <v>59</v>
@@ -1359,10 +1379,10 @@
         <v>7</v>
       </c>
       <c r="E9" s="0" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="F9" s="0" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
     </row>
     <row r="10">
@@ -1370,7 +1390,7 @@
         <v>55</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>63</v>
+        <v>68</v>
       </c>
       <c r="C10" s="0" t="s">
         <v>59</v>
@@ -1379,10 +1399,10 @@
         <v>7</v>
       </c>
       <c r="E10" s="0" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="F10" s="0" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
     </row>
     <row r="11">
@@ -1390,7 +1410,7 @@
         <v>56</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>64</v>
+        <v>69</v>
       </c>
       <c r="C11" s="0" t="s">
         <v>59</v>
@@ -1399,10 +1419,10 @@
         <v>7</v>
       </c>
       <c r="E11" s="0" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="F11" s="0" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
     </row>
     <row r="12">
@@ -1410,7 +1430,7 @@
         <v>72</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="C12" s="0" t="s">
         <v>59</v>
@@ -1419,10 +1439,10 @@
         <v>7</v>
       </c>
       <c r="E12" s="0" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="F12" s="0" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
     </row>
     <row r="13">
@@ -1430,7 +1450,7 @@
         <v>66</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>66</v>
+        <v>71</v>
       </c>
       <c r="C13" s="0" t="s">
         <v>59</v>
@@ -1439,10 +1459,10 @@
         <v>7</v>
       </c>
       <c r="E13" s="0" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="F13" s="0" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
     </row>
     <row r="14">
@@ -1450,7 +1470,7 @@
         <v>62</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>67</v>
+        <v>72</v>
       </c>
       <c r="C14" s="0" t="s">
         <v>59</v>
@@ -1459,10 +1479,10 @@
         <v>7</v>
       </c>
       <c r="E14" s="0" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="F14" s="0" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
     </row>
     <row r="15">
@@ -1470,7 +1490,7 @@
         <v>70</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
       <c r="C15" s="0" t="s">
         <v>59</v>
@@ -1479,10 +1499,10 @@
         <v>7</v>
       </c>
       <c r="E15" s="0" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="F15" s="0" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
     </row>
     <row r="16">
@@ -1490,7 +1510,7 @@
         <v>64</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>69</v>
+        <v>74</v>
       </c>
       <c r="C16" s="0" t="s">
         <v>59</v>
@@ -1499,10 +1519,10 @@
         <v>7</v>
       </c>
       <c r="E16" s="0" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="F16" s="0" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
     </row>
     <row r="17">
@@ -1510,7 +1530,7 @@
         <v>63</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>70</v>
+        <v>75</v>
       </c>
       <c r="C17" s="0" t="s">
         <v>59</v>
@@ -1519,10 +1539,10 @@
         <v>7</v>
       </c>
       <c r="E17" s="0" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="F17" s="0" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
     </row>
     <row r="18">
@@ -1530,7 +1550,7 @@
         <v>13</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>71</v>
+        <v>76</v>
       </c>
       <c r="C18" s="0" t="s">
         <v>59</v>
@@ -1539,10 +1559,10 @@
         <v>7</v>
       </c>
       <c r="E18" s="0" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="F18" s="0" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
     </row>
     <row r="19">
@@ -1550,7 +1570,7 @@
         <v>42</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>72</v>
+        <v>77</v>
       </c>
       <c r="C19" s="0" t="s">
         <v>59</v>
@@ -1562,7 +1582,7 @@
         <v>53</v>
       </c>
       <c r="F19" s="0" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
     </row>
     <row r="20">
@@ -1570,7 +1590,7 @@
         <v>33</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="C20" s="0" t="s">
         <v>59</v>
@@ -1579,10 +1599,10 @@
         <v>7</v>
       </c>
       <c r="E20" s="0" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="F20" s="0" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
     </row>
     <row r="21">
@@ -1590,7 +1610,7 @@
         <v>48</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>74</v>
+        <v>79</v>
       </c>
       <c r="C21" s="0" t="s">
         <v>59</v>
@@ -1599,10 +1619,10 @@
         <v>7</v>
       </c>
       <c r="E21" s="0" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="F21" s="0" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
     </row>
     <row r="22">
@@ -1610,7 +1630,7 @@
         <v>37</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>75</v>
+        <v>80</v>
       </c>
       <c r="C22" s="0" t="s">
         <v>59</v>
@@ -1619,10 +1639,10 @@
         <v>7</v>
       </c>
       <c r="E22" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="F22" s="0" t="s">
         <v>8</v>
-      </c>
-      <c r="F22" s="0" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="23">
@@ -1630,7 +1650,7 @@
         <v>38</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>76</v>
+        <v>81</v>
       </c>
       <c r="C23" s="0" t="s">
         <v>59</v>
@@ -1639,7 +1659,7 @@
         <v>7</v>
       </c>
       <c r="E23" s="0" t="s">
-        <v>8</v>
+        <v>28</v>
       </c>
       <c r="F23" s="0" t="s">
         <v>57</v>
@@ -1650,7 +1670,7 @@
         <v>46</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>77</v>
+        <v>82</v>
       </c>
       <c r="C24" s="0" t="s">
         <v>59</v>
@@ -1659,7 +1679,7 @@
         <v>7</v>
       </c>
       <c r="E24" s="0" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="F24" s="0" t="s">
         <v>57</v>
@@ -1670,7 +1690,7 @@
         <v>45</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="C25" s="0" t="s">
         <v>59</v>
@@ -1690,7 +1710,7 @@
         <v>44</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>80</v>
+        <v>85</v>
       </c>
       <c r="C26" s="0" t="s">
         <v>59</v>
@@ -1710,7 +1730,7 @@
         <v>41</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>81</v>
+        <v>86</v>
       </c>
       <c r="C27" s="0" t="s">
         <v>59</v>
@@ -1722,7 +1742,7 @@
         <v>53</v>
       </c>
       <c r="F27" s="0" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
     </row>
     <row r="28">
@@ -1730,7 +1750,7 @@
         <v>36</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
       <c r="C28" s="0" t="s">
         <v>59</v>
@@ -1739,10 +1759,10 @@
         <v>7</v>
       </c>
       <c r="E28" s="0" t="s">
-        <v>8</v>
+        <v>28</v>
       </c>
       <c r="F28" s="0" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
     </row>
     <row r="29">
@@ -1750,7 +1770,7 @@
         <v>11</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>83</v>
+        <v>88</v>
       </c>
       <c r="C29" s="0" t="s">
         <v>59</v>
@@ -1759,7 +1779,7 @@
         <v>7</v>
       </c>
       <c r="E29" s="0" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="F29" s="0" t="s">
         <v>53</v>
@@ -1770,7 +1790,7 @@
         <v>40</v>
       </c>
       <c r="B30" s="0" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="C30" s="0" t="s">
         <v>59</v>
@@ -1779,7 +1799,7 @@
         <v>7</v>
       </c>
       <c r="E30" s="0" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="F30" s="0" t="s">
         <v>53</v>
@@ -1790,7 +1810,7 @@
         <v>39</v>
       </c>
       <c r="B31" s="0" t="s">
-        <v>86</v>
+        <v>91</v>
       </c>
       <c r="C31" s="0" t="s">
         <v>59</v>
@@ -1799,7 +1819,7 @@
         <v>7</v>
       </c>
       <c r="E31" s="0" t="s">
-        <v>8</v>
+        <v>28</v>
       </c>
       <c r="F31" s="0" t="s">
         <v>53</v>
@@ -1810,7 +1830,7 @@
         <v>32</v>
       </c>
       <c r="B32" s="0" t="s">
-        <v>87</v>
+        <v>92</v>
       </c>
       <c r="C32" s="0" t="s">
         <v>59</v>
@@ -1819,10 +1839,10 @@
         <v>7</v>
       </c>
       <c r="E32" s="0" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="F32" s="0" t="s">
-        <v>8</v>
+        <v>28</v>
       </c>
     </row>
     <row r="33">
@@ -1830,7 +1850,7 @@
         <v>31</v>
       </c>
       <c r="B33" s="0" t="s">
-        <v>88</v>
+        <v>93</v>
       </c>
       <c r="C33" s="0" t="s">
         <v>59</v>
@@ -1839,10 +1859,10 @@
         <v>7</v>
       </c>
       <c r="E33" s="0" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="F33" s="0" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
     </row>
     <row r="34">
@@ -1850,7 +1870,7 @@
         <v>20</v>
       </c>
       <c r="B34" s="0" t="s">
-        <v>89</v>
+        <v>94</v>
       </c>
       <c r="C34" s="0" t="s">
         <v>59</v>
@@ -1859,10 +1879,10 @@
         <v>7</v>
       </c>
       <c r="E34" s="0" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="F34" s="0" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
     </row>
     <row r="35">
@@ -1870,7 +1890,7 @@
         <v>9</v>
       </c>
       <c r="B35" s="0" t="s">
-        <v>90</v>
+        <v>95</v>
       </c>
       <c r="C35" s="0" t="s">
         <v>59</v>
@@ -1879,10 +1899,10 @@
         <v>7</v>
       </c>
       <c r="E35" s="0" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="F35" s="0" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
     </row>
     <row r="36">
@@ -1890,7 +1910,7 @@
         <v>8</v>
       </c>
       <c r="B36" s="0" t="s">
-        <v>91</v>
+        <v>96</v>
       </c>
       <c r="C36" s="0" t="s">
         <v>59</v>
@@ -1899,10 +1919,10 @@
         <v>7</v>
       </c>
       <c r="E36" s="0" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="F36" s="0" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
     </row>
     <row r="37">
@@ -1910,7 +1930,7 @@
         <v>4</v>
       </c>
       <c r="B37" s="0" t="s">
-        <v>92</v>
+        <v>97</v>
       </c>
       <c r="C37" s="0" t="s">
         <v>59</v>
@@ -1919,10 +1939,10 @@
         <v>7</v>
       </c>
       <c r="E37" s="0" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="F37" s="0" t="s">
-        <v>93</v>
+        <v>98</v>
       </c>
     </row>
     <row r="38">
@@ -1930,7 +1950,7 @@
         <v>3</v>
       </c>
       <c r="B38" s="0" t="s">
-        <v>94</v>
+        <v>99</v>
       </c>
       <c r="C38" s="0" t="s">
         <v>59</v>
@@ -1939,10 +1959,10 @@
         <v>7</v>
       </c>
       <c r="E38" s="0" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="F38" s="0" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
     </row>
     <row r="39">
@@ -1950,7 +1970,7 @@
         <v>30</v>
       </c>
       <c r="B39" s="0" t="s">
-        <v>95</v>
+        <v>100</v>
       </c>
       <c r="C39" s="0" t="s">
         <v>59</v>
@@ -1959,10 +1979,10 @@
         <v>7</v>
       </c>
       <c r="E39" s="0" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="F39" s="0" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
     </row>
     <row r="40">
@@ -1970,7 +1990,7 @@
         <v>2</v>
       </c>
       <c r="B40" s="0" t="s">
-        <v>96</v>
+        <v>101</v>
       </c>
       <c r="C40" s="0" t="s">
         <v>59</v>
@@ -1979,10 +1999,10 @@
         <v>7</v>
       </c>
       <c r="E40" s="0" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="F40" s="0" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
     </row>
     <row r="41">
@@ -1990,7 +2010,7 @@
         <v>1</v>
       </c>
       <c r="B41" s="0" t="s">
-        <v>97</v>
+        <v>102</v>
       </c>
       <c r="C41" s="0" t="s">
         <v>59</v>
@@ -1999,10 +2019,10 @@
         <v>7</v>
       </c>
       <c r="E41" s="0" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="F41" s="0" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>
@@ -2023,7 +2043,7 @@
         <v>2</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>98</v>
+        <v>103</v>
       </c>
       <c r="C1" s="2"/>
       <c r="D1" s="2" t="s">
@@ -2031,7 +2051,7 @@
       </c>
       <c r="E1" s="2"/>
       <c r="F1" s="2" t="s">
-        <v>99</v>
+        <v>104</v>
       </c>
     </row>
     <row r="2">
@@ -2039,13 +2059,13 @@
         <v>6</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>98</v>
+        <v>103</v>
       </c>
       <c r="D2" s="0" t="s">
         <v>7</v>
       </c>
       <c r="F2" s="0">
-        <v>90</v>
+        <v>91</v>
       </c>
     </row>
     <row r="3">
@@ -2053,10 +2073,10 @@
         <v>59</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>100</v>
+        <v>105</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>101</v>
+        <v>106</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
refactor: use new testable library
</commit_message>
<xml_diff>
--- a/paint_todo.xlsx
+++ b/paint_todo.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="112">
   <si>
     <t>Id</t>
   </si>
@@ -402,6 +402,24 @@
   </si>
   <si>
     <t>Bug</t>
+  </si>
+  <si>
+    <t>eyedrop tool: select color in palette, by selecting color on image</t>
+  </si>
+  <si>
+    <t>eyedrop tool: select color in palette, by selecting color on image (select palest color in regio)</t>
+  </si>
+  <si>
+    <t>eyedrop tool: select color in palette, by selecting color on image (select palest color in colored region)</t>
+  </si>
+  <si>
+    <t>file &gt; Save</t>
+  </si>
+  <si>
+    <t xml:space="preserve">keyboard shortcuts:
+save (image or palette)
+undo (image or palette)
+redo (image or palette)</t>
   </si>
 </sst>
 </file>
@@ -454,7 +472,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:F43"/>
+  <dimension ref="A1:F45"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -480,10 +498,10 @@
     </row>
     <row r="2">
       <c r="A2" s="0">
-        <v>50</v>
+        <v>34</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="C2" s="0" t="s">
         <v>6</v>
@@ -492,15 +510,15 @@
         <v>7</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="0">
-        <v>34</v>
+        <v>93</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>9</v>
+        <v>110</v>
       </c>
       <c r="C3" s="0" t="s">
         <v>6</v>
@@ -509,15 +527,15 @@
         <v>7</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>10</v>
+        <v>26</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="0">
-        <v>87</v>
+        <v>94</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>11</v>
+        <v>111</v>
       </c>
       <c r="C4" s="0" t="s">
         <v>6</v>
@@ -526,15 +544,15 @@
         <v>7</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>12</v>
+        <v>26</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="0">
-        <v>49</v>
+        <v>87</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C5" s="0" t="s">
         <v>6</v>
@@ -543,15 +561,15 @@
         <v>7</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="0">
-        <v>21</v>
+        <v>49</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C6" s="0" t="s">
         <v>6</v>
@@ -560,15 +578,15 @@
         <v>7</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="0">
-        <v>86</v>
+        <v>21</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C7" s="0" t="s">
         <v>6</v>
@@ -577,15 +595,15 @@
         <v>7</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="0">
-        <v>54</v>
+        <v>86</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C8" s="0" t="s">
         <v>6</v>
@@ -594,15 +612,15 @@
         <v>7</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="0">
-        <v>88</v>
+        <v>54</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C9" s="0" t="s">
         <v>6</v>
@@ -611,15 +629,15 @@
         <v>7</v>
       </c>
       <c r="E9" s="0" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="0">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C10" s="0" t="s">
         <v>6</v>
@@ -633,10 +651,10 @@
     </row>
     <row r="11">
       <c r="A11" s="0">
-        <v>53</v>
+        <v>90</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C11" s="0" t="s">
         <v>6</v>
@@ -645,15 +663,15 @@
         <v>7</v>
       </c>
       <c r="E11" s="0" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="0">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C12" s="0" t="s">
         <v>6</v>
@@ -662,15 +680,15 @@
         <v>7</v>
       </c>
       <c r="E12" s="0" t="s">
-        <v>8</v>
+        <v>19</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="0">
-        <v>76</v>
+        <v>92</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>24</v>
+        <v>109</v>
       </c>
       <c r="C13" s="0" t="s">
         <v>6</v>
@@ -679,15 +697,15 @@
         <v>7</v>
       </c>
       <c r="E13" s="0" t="s">
-        <v>17</v>
+        <v>26</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="0">
-        <v>91</v>
+        <v>51</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C14" s="0" t="s">
         <v>6</v>
@@ -696,15 +714,15 @@
         <v>7</v>
       </c>
       <c r="E14" s="0" t="s">
-        <v>26</v>
+        <v>8</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="0">
-        <v>35</v>
+        <v>76</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="C15" s="0" t="s">
         <v>6</v>
@@ -713,15 +731,15 @@
         <v>7</v>
       </c>
       <c r="E15" s="0" t="s">
-        <v>28</v>
+        <v>17</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="0">
-        <v>79</v>
+        <v>91</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="C16" s="0" t="s">
         <v>6</v>
@@ -730,15 +748,15 @@
         <v>7</v>
       </c>
       <c r="E16" s="0" t="s">
-        <v>17</v>
+        <v>26</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="0">
-        <v>85</v>
+        <v>35</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="C17" s="0" t="s">
         <v>6</v>
@@ -747,15 +765,15 @@
         <v>7</v>
       </c>
       <c r="E17" s="0" t="s">
-        <v>17</v>
+        <v>28</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="0">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C18" s="0" t="s">
         <v>6</v>
@@ -769,10 +787,10 @@
     </row>
     <row r="19">
       <c r="A19" s="0">
-        <v>77</v>
+        <v>85</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C19" s="0" t="s">
         <v>6</v>
@@ -786,10 +804,10 @@
     </row>
     <row r="20">
       <c r="A20" s="0">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C20" s="0" t="s">
         <v>6</v>
@@ -803,10 +821,10 @@
     </row>
     <row r="21">
       <c r="A21" s="0">
-        <v>52</v>
+        <v>77</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C21" s="0" t="s">
         <v>6</v>
@@ -815,15 +833,15 @@
         <v>7</v>
       </c>
       <c r="E21" s="0" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="0">
-        <v>27</v>
+        <v>78</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C22" s="0" t="s">
         <v>6</v>
@@ -832,15 +850,15 @@
         <v>7</v>
       </c>
       <c r="E22" s="0" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="0">
-        <v>28</v>
+        <v>52</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C23" s="0" t="s">
         <v>6</v>
@@ -849,15 +867,15 @@
         <v>7</v>
       </c>
       <c r="E23" s="0" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="0">
-        <v>19</v>
+        <v>27</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C24" s="0" t="s">
         <v>6</v>
@@ -871,10 +889,10 @@
     </row>
     <row r="25">
       <c r="A25" s="0">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C25" s="0" t="s">
         <v>6</v>
@@ -888,10 +906,10 @@
     </row>
     <row r="26">
       <c r="A26" s="0">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C26" s="0" t="s">
         <v>6</v>
@@ -905,10 +923,10 @@
     </row>
     <row r="27">
       <c r="A27" s="0">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C27" s="0" t="s">
         <v>6</v>
@@ -922,10 +940,10 @@
     </row>
     <row r="28">
       <c r="A28" s="0">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C28" s="0" t="s">
         <v>6</v>
@@ -939,10 +957,10 @@
     </row>
     <row r="29">
       <c r="A29" s="0">
-        <v>81</v>
+        <v>17</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C29" s="0" t="s">
         <v>6</v>
@@ -951,15 +969,15 @@
         <v>7</v>
       </c>
       <c r="E29" s="0" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="0">
-        <v>82</v>
+        <v>18</v>
       </c>
       <c r="B30" s="0" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C30" s="0" t="s">
         <v>6</v>
@@ -968,15 +986,15 @@
         <v>7</v>
       </c>
       <c r="E30" s="0" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="0">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B31" s="0" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C31" s="0" t="s">
         <v>6</v>
@@ -990,10 +1008,10 @@
     </row>
     <row r="32">
       <c r="A32" s="0">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B32" s="0" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C32" s="0" t="s">
         <v>6</v>
@@ -1007,10 +1025,10 @@
     </row>
     <row r="33">
       <c r="A33" s="0">
-        <v>25</v>
+        <v>83</v>
       </c>
       <c r="B33" s="0" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C33" s="0" t="s">
         <v>6</v>
@@ -1019,15 +1037,15 @@
         <v>7</v>
       </c>
       <c r="E33" s="0" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="0">
-        <v>57</v>
+        <v>84</v>
       </c>
       <c r="B34" s="0" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C34" s="0" t="s">
         <v>6</v>
@@ -1041,10 +1059,10 @@
     </row>
     <row r="35">
       <c r="A35" s="0">
-        <v>65</v>
+        <v>25</v>
       </c>
       <c r="B35" s="0" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C35" s="0" t="s">
         <v>6</v>
@@ -1053,15 +1071,15 @@
         <v>7</v>
       </c>
       <c r="E35" s="0" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="0">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B36" s="0" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C36" s="0" t="s">
         <v>6</v>
@@ -1075,10 +1093,10 @@
     </row>
     <row r="37">
       <c r="A37" s="0">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="B37" s="0" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C37" s="0" t="s">
         <v>6</v>
@@ -1092,10 +1110,10 @@
     </row>
     <row r="38">
       <c r="A38" s="0">
-        <v>26</v>
+        <v>58</v>
       </c>
       <c r="B38" s="0" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C38" s="0" t="s">
         <v>6</v>
@@ -1104,15 +1122,15 @@
         <v>7</v>
       </c>
       <c r="E38" s="0" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="0">
-        <v>43</v>
+        <v>61</v>
       </c>
       <c r="B39" s="0" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C39" s="0" t="s">
         <v>6</v>
@@ -1121,15 +1139,15 @@
         <v>7</v>
       </c>
       <c r="E39" s="0" t="s">
-        <v>53</v>
+        <v>17</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="0">
-        <v>74</v>
+        <v>26</v>
       </c>
       <c r="B40" s="0" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C40" s="0" t="s">
         <v>6</v>
@@ -1138,15 +1156,15 @@
         <v>7</v>
       </c>
       <c r="E40" s="0" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="0">
-        <v>29</v>
+        <v>43</v>
       </c>
       <c r="B41" s="0" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="C41" s="0" t="s">
         <v>6</v>
@@ -1155,15 +1173,15 @@
         <v>7</v>
       </c>
       <c r="E41" s="0" t="s">
-        <v>15</v>
+        <v>53</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="0">
-        <v>47</v>
+        <v>74</v>
       </c>
       <c r="B42" s="0" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C42" s="0" t="s">
         <v>6</v>
@@ -1172,23 +1190,57 @@
         <v>7</v>
       </c>
       <c r="E42" s="0" t="s">
-        <v>57</v>
+        <v>17</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" s="0">
+        <v>29</v>
+      </c>
+      <c r="B43" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="C43" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D43" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E43" s="0" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" s="0">
+        <v>47</v>
+      </c>
+      <c r="B44" s="0" t="s">
+        <v>56</v>
+      </c>
+      <c r="C44" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D44" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E44" s="0" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" s="0">
         <v>60</v>
       </c>
-      <c r="B43" s="0" t="s">
+      <c r="B45" s="0" t="s">
         <v>58</v>
       </c>
-      <c r="C43" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="D43" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="E43" s="0" t="s">
+      <c r="C45" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D45" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E45" s="0" t="s">
         <v>17</v>
       </c>
     </row>
@@ -1199,7 +1251,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:F41"/>
+  <dimension ref="A1:F42"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1227,10 +1279,10 @@
     </row>
     <row r="2">
       <c r="A2" s="0">
-        <v>89</v>
+        <v>50</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>60</v>
+        <v>5</v>
       </c>
       <c r="C2" s="0" t="s">
         <v>59</v>
@@ -1239,18 +1291,18 @@
         <v>7</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>12</v>
+        <v>26</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="0">
-        <v>59</v>
+        <v>89</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C3" s="0" t="s">
         <v>59</v>
@@ -1259,7 +1311,7 @@
         <v>7</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="F3" s="0" t="s">
         <v>12</v>
@@ -1267,10 +1319,10 @@
     </row>
     <row r="4">
       <c r="A4" s="0">
-        <v>69</v>
+        <v>59</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C4" s="0" t="s">
         <v>59</v>
@@ -1287,10 +1339,10 @@
     </row>
     <row r="5">
       <c r="A5" s="0">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C5" s="0" t="s">
         <v>59</v>
@@ -1307,10 +1359,10 @@
     </row>
     <row r="6">
       <c r="A6" s="0">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C6" s="0" t="s">
         <v>59</v>
@@ -1327,10 +1379,10 @@
     </row>
     <row r="7">
       <c r="A7" s="0">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C7" s="0" t="s">
         <v>59</v>
@@ -1342,15 +1394,15 @@
         <v>17</v>
       </c>
       <c r="F7" s="0" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="0">
-        <v>24</v>
+        <v>71</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C8" s="0" t="s">
         <v>59</v>
@@ -1359,7 +1411,7 @@
         <v>7</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="F8" s="0" t="s">
         <v>17</v>
@@ -1367,10 +1419,10 @@
     </row>
     <row r="9">
       <c r="A9" s="0">
-        <v>75</v>
+        <v>24</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C9" s="0" t="s">
         <v>59</v>
@@ -1379,7 +1431,7 @@
         <v>7</v>
       </c>
       <c r="E9" s="0" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="F9" s="0" t="s">
         <v>17</v>
@@ -1387,10 +1439,10 @@
     </row>
     <row r="10">
       <c r="A10" s="0">
-        <v>55</v>
+        <v>75</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C10" s="0" t="s">
         <v>59</v>
@@ -1399,7 +1451,7 @@
         <v>7</v>
       </c>
       <c r="E10" s="0" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="F10" s="0" t="s">
         <v>17</v>
@@ -1407,10 +1459,10 @@
     </row>
     <row r="11">
       <c r="A11" s="0">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C11" s="0" t="s">
         <v>59</v>
@@ -1427,10 +1479,10 @@
     </row>
     <row r="12">
       <c r="A12" s="0">
-        <v>72</v>
+        <v>56</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C12" s="0" t="s">
         <v>59</v>
@@ -1439,7 +1491,7 @@
         <v>7</v>
       </c>
       <c r="E12" s="0" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="F12" s="0" t="s">
         <v>17</v>
@@ -1447,10 +1499,10 @@
     </row>
     <row r="13">
       <c r="A13" s="0">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C13" s="0" t="s">
         <v>59</v>
@@ -1467,10 +1519,10 @@
     </row>
     <row r="14">
       <c r="A14" s="0">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C14" s="0" t="s">
         <v>59</v>
@@ -1487,10 +1539,10 @@
     </row>
     <row r="15">
       <c r="A15" s="0">
-        <v>70</v>
+        <v>62</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C15" s="0" t="s">
         <v>59</v>
@@ -1507,10 +1559,10 @@
     </row>
     <row r="16">
       <c r="A16" s="0">
-        <v>64</v>
+        <v>70</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C16" s="0" t="s">
         <v>59</v>
@@ -1527,10 +1579,10 @@
     </row>
     <row r="17">
       <c r="A17" s="0">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C17" s="0" t="s">
         <v>59</v>
@@ -1547,10 +1599,10 @@
     </row>
     <row r="18">
       <c r="A18" s="0">
-        <v>13</v>
+        <v>63</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C18" s="0" t="s">
         <v>59</v>
@@ -1559,7 +1611,7 @@
         <v>7</v>
       </c>
       <c r="E18" s="0" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="F18" s="0" t="s">
         <v>17</v>
@@ -1567,10 +1619,10 @@
     </row>
     <row r="19">
       <c r="A19" s="0">
-        <v>42</v>
+        <v>13</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C19" s="0" t="s">
         <v>59</v>
@@ -1579,18 +1631,18 @@
         <v>7</v>
       </c>
       <c r="E19" s="0" t="s">
-        <v>53</v>
+        <v>15</v>
       </c>
       <c r="F19" s="0" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="0">
-        <v>33</v>
+        <v>42</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C20" s="0" t="s">
         <v>59</v>
@@ -1599,7 +1651,7 @@
         <v>7</v>
       </c>
       <c r="E20" s="0" t="s">
-        <v>10</v>
+        <v>53</v>
       </c>
       <c r="F20" s="0" t="s">
         <v>19</v>
@@ -1607,10 +1659,10 @@
     </row>
     <row r="21">
       <c r="A21" s="0">
-        <v>48</v>
+        <v>33</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C21" s="0" t="s">
         <v>59</v>
@@ -1619,18 +1671,18 @@
         <v>7</v>
       </c>
       <c r="E21" s="0" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="F21" s="0" t="s">
-        <v>8</v>
+        <v>19</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="0">
-        <v>37</v>
+        <v>48</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C22" s="0" t="s">
         <v>59</v>
@@ -1639,7 +1691,7 @@
         <v>7</v>
       </c>
       <c r="E22" s="0" t="s">
-        <v>28</v>
+        <v>8</v>
       </c>
       <c r="F22" s="0" t="s">
         <v>8</v>
@@ -1647,10 +1699,10 @@
     </row>
     <row r="23">
       <c r="A23" s="0">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C23" s="0" t="s">
         <v>59</v>
@@ -1662,15 +1714,15 @@
         <v>28</v>
       </c>
       <c r="F23" s="0" t="s">
-        <v>57</v>
+        <v>8</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="0">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C24" s="0" t="s">
         <v>59</v>
@@ -1679,7 +1731,7 @@
         <v>7</v>
       </c>
       <c r="E24" s="0" t="s">
-        <v>83</v>
+        <v>28</v>
       </c>
       <c r="F24" s="0" t="s">
         <v>57</v>
@@ -1687,10 +1739,10 @@
     </row>
     <row r="25">
       <c r="A25" s="0">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C25" s="0" t="s">
         <v>59</v>
@@ -1699,7 +1751,7 @@
         <v>7</v>
       </c>
       <c r="E25" s="0" t="s">
-        <v>53</v>
+        <v>83</v>
       </c>
       <c r="F25" s="0" t="s">
         <v>57</v>
@@ -1707,10 +1759,10 @@
     </row>
     <row r="26">
       <c r="A26" s="0">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C26" s="0" t="s">
         <v>59</v>
@@ -1727,10 +1779,10 @@
     </row>
     <row r="27">
       <c r="A27" s="0">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C27" s="0" t="s">
         <v>59</v>
@@ -1742,15 +1794,15 @@
         <v>53</v>
       </c>
       <c r="F27" s="0" t="s">
-        <v>83</v>
+        <v>57</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="0">
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C28" s="0" t="s">
         <v>59</v>
@@ -1759,7 +1811,7 @@
         <v>7</v>
       </c>
       <c r="E28" s="0" t="s">
-        <v>28</v>
+        <v>53</v>
       </c>
       <c r="F28" s="0" t="s">
         <v>83</v>
@@ -1767,10 +1819,10 @@
     </row>
     <row r="29">
       <c r="A29" s="0">
-        <v>11</v>
+        <v>36</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C29" s="0" t="s">
         <v>59</v>
@@ -1779,18 +1831,18 @@
         <v>7</v>
       </c>
       <c r="E29" s="0" t="s">
-        <v>15</v>
+        <v>28</v>
       </c>
       <c r="F29" s="0" t="s">
-        <v>53</v>
+        <v>83</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="0">
-        <v>40</v>
+        <v>11</v>
       </c>
       <c r="B30" s="0" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C30" s="0" t="s">
         <v>59</v>
@@ -1799,7 +1851,7 @@
         <v>7</v>
       </c>
       <c r="E30" s="0" t="s">
-        <v>90</v>
+        <v>15</v>
       </c>
       <c r="F30" s="0" t="s">
         <v>53</v>
@@ -1807,10 +1859,10 @@
     </row>
     <row r="31">
       <c r="A31" s="0">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B31" s="0" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C31" s="0" t="s">
         <v>59</v>
@@ -1819,7 +1871,7 @@
         <v>7</v>
       </c>
       <c r="E31" s="0" t="s">
-        <v>28</v>
+        <v>90</v>
       </c>
       <c r="F31" s="0" t="s">
         <v>53</v>
@@ -1827,10 +1879,10 @@
     </row>
     <row r="32">
       <c r="A32" s="0">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="B32" s="0" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C32" s="0" t="s">
         <v>59</v>
@@ -1839,18 +1891,18 @@
         <v>7</v>
       </c>
       <c r="E32" s="0" t="s">
-        <v>10</v>
+        <v>28</v>
       </c>
       <c r="F32" s="0" t="s">
-        <v>28</v>
+        <v>53</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="0">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B33" s="0" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C33" s="0" t="s">
         <v>59</v>
@@ -1862,15 +1914,15 @@
         <v>10</v>
       </c>
       <c r="F33" s="0" t="s">
-        <v>10</v>
+        <v>28</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="0">
-        <v>20</v>
+        <v>31</v>
       </c>
       <c r="B34" s="0" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C34" s="0" t="s">
         <v>59</v>
@@ -1879,7 +1931,7 @@
         <v>7</v>
       </c>
       <c r="E34" s="0" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="F34" s="0" t="s">
         <v>10</v>
@@ -1887,10 +1939,10 @@
     </row>
     <row r="35">
       <c r="A35" s="0">
-        <v>9</v>
+        <v>20</v>
       </c>
       <c r="B35" s="0" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C35" s="0" t="s">
         <v>59</v>
@@ -1907,10 +1959,10 @@
     </row>
     <row r="36">
       <c r="A36" s="0">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B36" s="0" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C36" s="0" t="s">
         <v>59</v>
@@ -1927,10 +1979,10 @@
     </row>
     <row r="37">
       <c r="A37" s="0">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="B37" s="0" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C37" s="0" t="s">
         <v>59</v>
@@ -1942,15 +1994,15 @@
         <v>15</v>
       </c>
       <c r="F37" s="0" t="s">
-        <v>98</v>
+        <v>10</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="0">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B38" s="0" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C38" s="0" t="s">
         <v>59</v>
@@ -1962,15 +2014,15 @@
         <v>15</v>
       </c>
       <c r="F38" s="0" t="s">
-        <v>15</v>
+        <v>98</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="0">
-        <v>30</v>
+        <v>3</v>
       </c>
       <c r="B39" s="0" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C39" s="0" t="s">
         <v>59</v>
@@ -1987,10 +2039,10 @@
     </row>
     <row r="40">
       <c r="A40" s="0">
-        <v>2</v>
+        <v>30</v>
       </c>
       <c r="B40" s="0" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C40" s="0" t="s">
         <v>59</v>
@@ -2007,21 +2059,41 @@
     </row>
     <row r="41">
       <c r="A41" s="0">
+        <v>2</v>
+      </c>
+      <c r="B41" s="0" t="s">
+        <v>101</v>
+      </c>
+      <c r="C41" s="0" t="s">
+        <v>59</v>
+      </c>
+      <c r="D41" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E41" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="F41" s="0" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" s="0">
         <v>1</v>
       </c>
-      <c r="B41" s="0" t="s">
+      <c r="B42" s="0" t="s">
         <v>102</v>
       </c>
-      <c r="C41" s="0" t="s">
-        <v>59</v>
-      </c>
-      <c r="D41" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="E41" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="F41" s="0" t="s">
+      <c r="C42" s="0" t="s">
+        <v>59</v>
+      </c>
+      <c r="D42" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E42" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="F42" s="0" t="s">
         <v>15</v>
       </c>
     </row>
@@ -2065,7 +2137,7 @@
         <v>7</v>
       </c>
       <c r="F2" s="0">
-        <v>91</v>
+        <v>94</v>
       </c>
     </row>
     <row r="3">

</xml_diff>

<commit_message>
zoom: keep scrollbars at min or max if they are already there
</commit_message>
<xml_diff>
--- a/paint_todo.xlsx
+++ b/paint_todo.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="113">
   <si>
     <t>Id</t>
   </si>
@@ -420,6 +420,9 @@
 save (image or palette)
 undo (image or palette)
 redo (image or palette)</t>
+  </si>
+  <si>
+    <t>continue refactoring business logic out of RequestColorWorker</t>
   </si>
 </sst>
 </file>
@@ -498,10 +501,10 @@
     </row>
     <row r="2">
       <c r="A2" s="0">
-        <v>34</v>
+        <v>93</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>9</v>
+        <v>110</v>
       </c>
       <c r="C2" s="0" t="s">
         <v>6</v>
@@ -510,15 +513,15 @@
         <v>7</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>10</v>
+        <v>26</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="0">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="C3" s="0" t="s">
         <v>6</v>
@@ -532,10 +535,10 @@
     </row>
     <row r="4">
       <c r="A4" s="0">
-        <v>94</v>
+        <v>87</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>111</v>
+        <v>11</v>
       </c>
       <c r="C4" s="0" t="s">
         <v>6</v>
@@ -544,15 +547,15 @@
         <v>7</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>26</v>
+        <v>12</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="0">
-        <v>87</v>
+        <v>49</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C5" s="0" t="s">
         <v>6</v>
@@ -561,15 +564,15 @@
         <v>7</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="0">
-        <v>49</v>
+        <v>21</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C6" s="0" t="s">
         <v>6</v>
@@ -578,15 +581,15 @@
         <v>7</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="0">
-        <v>21</v>
+        <v>86</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C7" s="0" t="s">
         <v>6</v>
@@ -595,15 +598,15 @@
         <v>7</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="0">
-        <v>86</v>
+        <v>54</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C8" s="0" t="s">
         <v>6</v>
@@ -612,15 +615,15 @@
         <v>7</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="0">
-        <v>54</v>
+        <v>88</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C9" s="0" t="s">
         <v>6</v>
@@ -629,15 +632,15 @@
         <v>7</v>
       </c>
       <c r="E9" s="0" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="0">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C10" s="0" t="s">
         <v>6</v>
@@ -651,10 +654,10 @@
     </row>
     <row r="11">
       <c r="A11" s="0">
-        <v>90</v>
+        <v>95</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>21</v>
+        <v>112</v>
       </c>
       <c r="C11" s="0" t="s">
         <v>6</v>
@@ -663,7 +666,7 @@
         <v>7</v>
       </c>
       <c r="E11" s="0" t="s">
-        <v>12</v>
+        <v>26</v>
       </c>
     </row>
     <row r="12">
@@ -1251,7 +1254,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:F42"/>
+  <dimension ref="A1:F43"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1279,10 +1282,10 @@
     </row>
     <row r="2">
       <c r="A2" s="0">
-        <v>50</v>
+        <v>34</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="C2" s="0" t="s">
         <v>59</v>
@@ -1291,7 +1294,7 @@
         <v>7</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="F2" s="0" t="s">
         <v>26</v>
@@ -1299,10 +1302,10 @@
     </row>
     <row r="3">
       <c r="A3" s="0">
-        <v>89</v>
+        <v>50</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>60</v>
+        <v>5</v>
       </c>
       <c r="C3" s="0" t="s">
         <v>59</v>
@@ -1311,18 +1314,18 @@
         <v>7</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="F3" s="0" t="s">
-        <v>12</v>
+        <v>26</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="0">
-        <v>59</v>
+        <v>89</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C4" s="0" t="s">
         <v>59</v>
@@ -1331,7 +1334,7 @@
         <v>7</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="F4" s="0" t="s">
         <v>12</v>
@@ -1339,10 +1342,10 @@
     </row>
     <row r="5">
       <c r="A5" s="0">
-        <v>69</v>
+        <v>59</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C5" s="0" t="s">
         <v>59</v>
@@ -1359,10 +1362,10 @@
     </row>
     <row r="6">
       <c r="A6" s="0">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C6" s="0" t="s">
         <v>59</v>
@@ -1379,10 +1382,10 @@
     </row>
     <row r="7">
       <c r="A7" s="0">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C7" s="0" t="s">
         <v>59</v>
@@ -1399,10 +1402,10 @@
     </row>
     <row r="8">
       <c r="A8" s="0">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C8" s="0" t="s">
         <v>59</v>
@@ -1414,15 +1417,15 @@
         <v>17</v>
       </c>
       <c r="F8" s="0" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="0">
-        <v>24</v>
+        <v>71</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C9" s="0" t="s">
         <v>59</v>
@@ -1431,7 +1434,7 @@
         <v>7</v>
       </c>
       <c r="E9" s="0" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="F9" s="0" t="s">
         <v>17</v>
@@ -1439,10 +1442,10 @@
     </row>
     <row r="10">
       <c r="A10" s="0">
-        <v>75</v>
+        <v>24</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C10" s="0" t="s">
         <v>59</v>
@@ -1451,7 +1454,7 @@
         <v>7</v>
       </c>
       <c r="E10" s="0" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="F10" s="0" t="s">
         <v>17</v>
@@ -1459,10 +1462,10 @@
     </row>
     <row r="11">
       <c r="A11" s="0">
-        <v>55</v>
+        <v>75</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C11" s="0" t="s">
         <v>59</v>
@@ -1471,7 +1474,7 @@
         <v>7</v>
       </c>
       <c r="E11" s="0" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="F11" s="0" t="s">
         <v>17</v>
@@ -1479,10 +1482,10 @@
     </row>
     <row r="12">
       <c r="A12" s="0">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C12" s="0" t="s">
         <v>59</v>
@@ -1499,10 +1502,10 @@
     </row>
     <row r="13">
       <c r="A13" s="0">
-        <v>72</v>
+        <v>56</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C13" s="0" t="s">
         <v>59</v>
@@ -1511,7 +1514,7 @@
         <v>7</v>
       </c>
       <c r="E13" s="0" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="F13" s="0" t="s">
         <v>17</v>
@@ -1519,10 +1522,10 @@
     </row>
     <row r="14">
       <c r="A14" s="0">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C14" s="0" t="s">
         <v>59</v>
@@ -1539,10 +1542,10 @@
     </row>
     <row r="15">
       <c r="A15" s="0">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C15" s="0" t="s">
         <v>59</v>
@@ -1559,10 +1562,10 @@
     </row>
     <row r="16">
       <c r="A16" s="0">
-        <v>70</v>
+        <v>62</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C16" s="0" t="s">
         <v>59</v>
@@ -1579,10 +1582,10 @@
     </row>
     <row r="17">
       <c r="A17" s="0">
-        <v>64</v>
+        <v>70</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C17" s="0" t="s">
         <v>59</v>
@@ -1599,10 +1602,10 @@
     </row>
     <row r="18">
       <c r="A18" s="0">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C18" s="0" t="s">
         <v>59</v>
@@ -1619,10 +1622,10 @@
     </row>
     <row r="19">
       <c r="A19" s="0">
-        <v>13</v>
+        <v>63</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C19" s="0" t="s">
         <v>59</v>
@@ -1631,7 +1634,7 @@
         <v>7</v>
       </c>
       <c r="E19" s="0" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="F19" s="0" t="s">
         <v>17</v>
@@ -1639,10 +1642,10 @@
     </row>
     <row r="20">
       <c r="A20" s="0">
-        <v>42</v>
+        <v>13</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C20" s="0" t="s">
         <v>59</v>
@@ -1651,18 +1654,18 @@
         <v>7</v>
       </c>
       <c r="E20" s="0" t="s">
-        <v>53</v>
+        <v>15</v>
       </c>
       <c r="F20" s="0" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="0">
-        <v>33</v>
+        <v>42</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C21" s="0" t="s">
         <v>59</v>
@@ -1671,7 +1674,7 @@
         <v>7</v>
       </c>
       <c r="E21" s="0" t="s">
-        <v>10</v>
+        <v>53</v>
       </c>
       <c r="F21" s="0" t="s">
         <v>19</v>
@@ -1679,10 +1682,10 @@
     </row>
     <row r="22">
       <c r="A22" s="0">
-        <v>48</v>
+        <v>33</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C22" s="0" t="s">
         <v>59</v>
@@ -1691,18 +1694,18 @@
         <v>7</v>
       </c>
       <c r="E22" s="0" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="F22" s="0" t="s">
-        <v>8</v>
+        <v>19</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="0">
-        <v>37</v>
+        <v>48</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C23" s="0" t="s">
         <v>59</v>
@@ -1711,7 +1714,7 @@
         <v>7</v>
       </c>
       <c r="E23" s="0" t="s">
-        <v>28</v>
+        <v>8</v>
       </c>
       <c r="F23" s="0" t="s">
         <v>8</v>
@@ -1719,10 +1722,10 @@
     </row>
     <row r="24">
       <c r="A24" s="0">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C24" s="0" t="s">
         <v>59</v>
@@ -1734,15 +1737,15 @@
         <v>28</v>
       </c>
       <c r="F24" s="0" t="s">
-        <v>57</v>
+        <v>8</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="0">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C25" s="0" t="s">
         <v>59</v>
@@ -1751,7 +1754,7 @@
         <v>7</v>
       </c>
       <c r="E25" s="0" t="s">
-        <v>83</v>
+        <v>28</v>
       </c>
       <c r="F25" s="0" t="s">
         <v>57</v>
@@ -1759,10 +1762,10 @@
     </row>
     <row r="26">
       <c r="A26" s="0">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C26" s="0" t="s">
         <v>59</v>
@@ -1771,7 +1774,7 @@
         <v>7</v>
       </c>
       <c r="E26" s="0" t="s">
-        <v>53</v>
+        <v>83</v>
       </c>
       <c r="F26" s="0" t="s">
         <v>57</v>
@@ -1779,10 +1782,10 @@
     </row>
     <row r="27">
       <c r="A27" s="0">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C27" s="0" t="s">
         <v>59</v>
@@ -1799,10 +1802,10 @@
     </row>
     <row r="28">
       <c r="A28" s="0">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C28" s="0" t="s">
         <v>59</v>
@@ -1814,15 +1817,15 @@
         <v>53</v>
       </c>
       <c r="F28" s="0" t="s">
-        <v>83</v>
+        <v>57</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="0">
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C29" s="0" t="s">
         <v>59</v>
@@ -1831,7 +1834,7 @@
         <v>7</v>
       </c>
       <c r="E29" s="0" t="s">
-        <v>28</v>
+        <v>53</v>
       </c>
       <c r="F29" s="0" t="s">
         <v>83</v>
@@ -1839,10 +1842,10 @@
     </row>
     <row r="30">
       <c r="A30" s="0">
-        <v>11</v>
+        <v>36</v>
       </c>
       <c r="B30" s="0" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C30" s="0" t="s">
         <v>59</v>
@@ -1851,18 +1854,18 @@
         <v>7</v>
       </c>
       <c r="E30" s="0" t="s">
-        <v>15</v>
+        <v>28</v>
       </c>
       <c r="F30" s="0" t="s">
-        <v>53</v>
+        <v>83</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="0">
-        <v>40</v>
+        <v>11</v>
       </c>
       <c r="B31" s="0" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C31" s="0" t="s">
         <v>59</v>
@@ -1871,7 +1874,7 @@
         <v>7</v>
       </c>
       <c r="E31" s="0" t="s">
-        <v>90</v>
+        <v>15</v>
       </c>
       <c r="F31" s="0" t="s">
         <v>53</v>
@@ -1879,10 +1882,10 @@
     </row>
     <row r="32">
       <c r="A32" s="0">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B32" s="0" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C32" s="0" t="s">
         <v>59</v>
@@ -1891,7 +1894,7 @@
         <v>7</v>
       </c>
       <c r="E32" s="0" t="s">
-        <v>28</v>
+        <v>90</v>
       </c>
       <c r="F32" s="0" t="s">
         <v>53</v>
@@ -1899,10 +1902,10 @@
     </row>
     <row r="33">
       <c r="A33" s="0">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="B33" s="0" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C33" s="0" t="s">
         <v>59</v>
@@ -1911,18 +1914,18 @@
         <v>7</v>
       </c>
       <c r="E33" s="0" t="s">
-        <v>10</v>
+        <v>28</v>
       </c>
       <c r="F33" s="0" t="s">
-        <v>28</v>
+        <v>53</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="0">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B34" s="0" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C34" s="0" t="s">
         <v>59</v>
@@ -1934,15 +1937,15 @@
         <v>10</v>
       </c>
       <c r="F34" s="0" t="s">
-        <v>10</v>
+        <v>28</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="0">
-        <v>20</v>
+        <v>31</v>
       </c>
       <c r="B35" s="0" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C35" s="0" t="s">
         <v>59</v>
@@ -1951,7 +1954,7 @@
         <v>7</v>
       </c>
       <c r="E35" s="0" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="F35" s="0" t="s">
         <v>10</v>
@@ -1959,10 +1962,10 @@
     </row>
     <row r="36">
       <c r="A36" s="0">
-        <v>9</v>
+        <v>20</v>
       </c>
       <c r="B36" s="0" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C36" s="0" t="s">
         <v>59</v>
@@ -1979,10 +1982,10 @@
     </row>
     <row r="37">
       <c r="A37" s="0">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B37" s="0" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C37" s="0" t="s">
         <v>59</v>
@@ -1999,10 +2002,10 @@
     </row>
     <row r="38">
       <c r="A38" s="0">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="B38" s="0" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C38" s="0" t="s">
         <v>59</v>
@@ -2014,15 +2017,15 @@
         <v>15</v>
       </c>
       <c r="F38" s="0" t="s">
-        <v>98</v>
+        <v>10</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="0">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B39" s="0" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C39" s="0" t="s">
         <v>59</v>
@@ -2034,15 +2037,15 @@
         <v>15</v>
       </c>
       <c r="F39" s="0" t="s">
-        <v>15</v>
+        <v>98</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="0">
-        <v>30</v>
+        <v>3</v>
       </c>
       <c r="B40" s="0" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C40" s="0" t="s">
         <v>59</v>
@@ -2059,10 +2062,10 @@
     </row>
     <row r="41">
       <c r="A41" s="0">
-        <v>2</v>
+        <v>30</v>
       </c>
       <c r="B41" s="0" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C41" s="0" t="s">
         <v>59</v>
@@ -2079,21 +2082,41 @@
     </row>
     <row r="42">
       <c r="A42" s="0">
+        <v>2</v>
+      </c>
+      <c r="B42" s="0" t="s">
+        <v>101</v>
+      </c>
+      <c r="C42" s="0" t="s">
+        <v>59</v>
+      </c>
+      <c r="D42" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E42" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="F42" s="0" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" s="0">
         <v>1</v>
       </c>
-      <c r="B42" s="0" t="s">
+      <c r="B43" s="0" t="s">
         <v>102</v>
       </c>
-      <c r="C42" s="0" t="s">
-        <v>59</v>
-      </c>
-      <c r="D42" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="E42" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="F42" s="0" t="s">
+      <c r="C43" s="0" t="s">
+        <v>59</v>
+      </c>
+      <c r="D43" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E43" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="F43" s="0" t="s">
         <v>15</v>
       </c>
     </row>
@@ -2137,7 +2160,7 @@
         <v>7</v>
       </c>
       <c r="F2" s="0">
-        <v>94</v>
+        <v>95</v>
       </c>
     </row>
     <row r="3">

</xml_diff>

<commit_message>
bug fix: open bitmap then save to same location; keyboard shortcut Open Image, Save Image
</commit_message>
<xml_diff>
--- a/paint_todo.xlsx
+++ b/paint_todo.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="114">
   <si>
     <t>Id</t>
   </si>
@@ -423,6 +423,13 @@
   </si>
   <si>
     <t>continue refactoring business logic out of RequestColorWorker</t>
+  </si>
+  <si>
+    <t xml:space="preserve">keyboard shortcuts:
+open (image)
+save (image or palette)
+undo (image or palette)
+redo (image or palette)</t>
   </si>
 </sst>
 </file>
@@ -504,7 +511,7 @@
         <v>94</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="C2" s="0" t="s">
         <v>6</v>
@@ -2163,7 +2170,7 @@
         <v>7</v>
       </c>
       <c r="F2" s="0">
-        <v>95</v>
+        <v>96</v>
       </c>
     </row>
     <row r="3">

</xml_diff>

<commit_message>
edit palette: shortcut keys
</commit_message>
<xml_diff>
--- a/paint_todo.xlsx
+++ b/paint_todo.xlsx
@@ -482,7 +482,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:F44"/>
+  <dimension ref="A1:F43"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -508,10 +508,10 @@
     </row>
     <row r="2">
       <c r="A2" s="0">
-        <v>94</v>
+        <v>87</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>113</v>
+        <v>11</v>
       </c>
       <c r="C2" s="0" t="s">
         <v>6</v>
@@ -520,15 +520,15 @@
         <v>7</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>26</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="0">
-        <v>87</v>
+        <v>49</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C3" s="0" t="s">
         <v>6</v>
@@ -537,15 +537,15 @@
         <v>7</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="0">
-        <v>49</v>
+        <v>21</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C4" s="0" t="s">
         <v>6</v>
@@ -554,15 +554,15 @@
         <v>7</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="0">
-        <v>21</v>
+        <v>86</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C5" s="0" t="s">
         <v>6</v>
@@ -571,15 +571,15 @@
         <v>7</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="0">
-        <v>86</v>
+        <v>54</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C6" s="0" t="s">
         <v>6</v>
@@ -588,15 +588,15 @@
         <v>7</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="0">
-        <v>54</v>
+        <v>88</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C7" s="0" t="s">
         <v>6</v>
@@ -605,15 +605,15 @@
         <v>7</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="0">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C8" s="0" t="s">
         <v>6</v>
@@ -627,10 +627,10 @@
     </row>
     <row r="9">
       <c r="A9" s="0">
-        <v>90</v>
+        <v>95</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>21</v>
+        <v>112</v>
       </c>
       <c r="C9" s="0" t="s">
         <v>6</v>
@@ -639,15 +639,15 @@
         <v>7</v>
       </c>
       <c r="E9" s="0" t="s">
-        <v>12</v>
+        <v>26</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="0">
-        <v>95</v>
+        <v>53</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>112</v>
+        <v>22</v>
       </c>
       <c r="C10" s="0" t="s">
         <v>6</v>
@@ -656,15 +656,15 @@
         <v>7</v>
       </c>
       <c r="E10" s="0" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="0">
-        <v>53</v>
+        <v>92</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>22</v>
+        <v>109</v>
       </c>
       <c r="C11" s="0" t="s">
         <v>6</v>
@@ -673,15 +673,15 @@
         <v>7</v>
       </c>
       <c r="E11" s="0" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="0">
-        <v>92</v>
+        <v>51</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>109</v>
+        <v>23</v>
       </c>
       <c r="C12" s="0" t="s">
         <v>6</v>
@@ -690,15 +690,15 @@
         <v>7</v>
       </c>
       <c r="E12" s="0" t="s">
-        <v>26</v>
+        <v>8</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="0">
-        <v>51</v>
+        <v>76</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C13" s="0" t="s">
         <v>6</v>
@@ -707,15 +707,15 @@
         <v>7</v>
       </c>
       <c r="E13" s="0" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="0">
-        <v>76</v>
+        <v>91</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C14" s="0" t="s">
         <v>6</v>
@@ -724,15 +724,15 @@
         <v>7</v>
       </c>
       <c r="E14" s="0" t="s">
-        <v>17</v>
+        <v>26</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="0">
-        <v>91</v>
+        <v>35</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="C15" s="0" t="s">
         <v>6</v>
@@ -741,15 +741,15 @@
         <v>7</v>
       </c>
       <c r="E15" s="0" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="0">
-        <v>35</v>
+        <v>79</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C16" s="0" t="s">
         <v>6</v>
@@ -758,15 +758,15 @@
         <v>7</v>
       </c>
       <c r="E16" s="0" t="s">
-        <v>28</v>
+        <v>17</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="0">
-        <v>79</v>
+        <v>85</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C17" s="0" t="s">
         <v>6</v>
@@ -780,10 +780,10 @@
     </row>
     <row r="18">
       <c r="A18" s="0">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C18" s="0" t="s">
         <v>6</v>
@@ -797,10 +797,10 @@
     </row>
     <row r="19">
       <c r="A19" s="0">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C19" s="0" t="s">
         <v>6</v>
@@ -814,10 +814,10 @@
     </row>
     <row r="20">
       <c r="A20" s="0">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C20" s="0" t="s">
         <v>6</v>
@@ -831,10 +831,10 @@
     </row>
     <row r="21">
       <c r="A21" s="0">
-        <v>78</v>
+        <v>52</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C21" s="0" t="s">
         <v>6</v>
@@ -843,15 +843,15 @@
         <v>7</v>
       </c>
       <c r="E21" s="0" t="s">
-        <v>17</v>
+        <v>8</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="0">
-        <v>52</v>
+        <v>27</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C22" s="0" t="s">
         <v>6</v>
@@ -860,15 +860,15 @@
         <v>7</v>
       </c>
       <c r="E22" s="0" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="0">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C23" s="0" t="s">
         <v>6</v>
@@ -882,10 +882,10 @@
     </row>
     <row r="24">
       <c r="A24" s="0">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C24" s="0" t="s">
         <v>6</v>
@@ -899,10 +899,10 @@
     </row>
     <row r="25">
       <c r="A25" s="0">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C25" s="0" t="s">
         <v>6</v>
@@ -916,10 +916,10 @@
     </row>
     <row r="26">
       <c r="A26" s="0">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C26" s="0" t="s">
         <v>6</v>
@@ -933,10 +933,10 @@
     </row>
     <row r="27">
       <c r="A27" s="0">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C27" s="0" t="s">
         <v>6</v>
@@ -950,10 +950,10 @@
     </row>
     <row r="28">
       <c r="A28" s="0">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C28" s="0" t="s">
         <v>6</v>
@@ -967,10 +967,10 @@
     </row>
     <row r="29">
       <c r="A29" s="0">
-        <v>18</v>
+        <v>81</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C29" s="0" t="s">
         <v>6</v>
@@ -979,15 +979,15 @@
         <v>7</v>
       </c>
       <c r="E29" s="0" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="0">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B30" s="0" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C30" s="0" t="s">
         <v>6</v>
@@ -1001,10 +1001,10 @@
     </row>
     <row r="31">
       <c r="A31" s="0">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="B31" s="0" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C31" s="0" t="s">
         <v>6</v>
@@ -1018,10 +1018,10 @@
     </row>
     <row r="32">
       <c r="A32" s="0">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B32" s="0" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C32" s="0" t="s">
         <v>6</v>
@@ -1035,10 +1035,10 @@
     </row>
     <row r="33">
       <c r="A33" s="0">
-        <v>84</v>
+        <v>25</v>
       </c>
       <c r="B33" s="0" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C33" s="0" t="s">
         <v>6</v>
@@ -1047,15 +1047,15 @@
         <v>7</v>
       </c>
       <c r="E33" s="0" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="0">
-        <v>25</v>
+        <v>57</v>
       </c>
       <c r="B34" s="0" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C34" s="0" t="s">
         <v>6</v>
@@ -1064,15 +1064,15 @@
         <v>7</v>
       </c>
       <c r="E34" s="0" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="0">
-        <v>57</v>
+        <v>65</v>
       </c>
       <c r="B35" s="0" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C35" s="0" t="s">
         <v>6</v>
@@ -1086,10 +1086,10 @@
     </row>
     <row r="36">
       <c r="A36" s="0">
-        <v>65</v>
+        <v>58</v>
       </c>
       <c r="B36" s="0" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C36" s="0" t="s">
         <v>6</v>
@@ -1103,10 +1103,10 @@
     </row>
     <row r="37">
       <c r="A37" s="0">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="B37" s="0" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C37" s="0" t="s">
         <v>6</v>
@@ -1120,10 +1120,10 @@
     </row>
     <row r="38">
       <c r="A38" s="0">
-        <v>61</v>
+        <v>26</v>
       </c>
       <c r="B38" s="0" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C38" s="0" t="s">
         <v>6</v>
@@ -1132,15 +1132,15 @@
         <v>7</v>
       </c>
       <c r="E38" s="0" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="0">
-        <v>26</v>
+        <v>43</v>
       </c>
       <c r="B39" s="0" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C39" s="0" t="s">
         <v>6</v>
@@ -1149,15 +1149,15 @@
         <v>7</v>
       </c>
       <c r="E39" s="0" t="s">
-        <v>15</v>
+        <v>53</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="0">
-        <v>43</v>
+        <v>74</v>
       </c>
       <c r="B40" s="0" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="C40" s="0" t="s">
         <v>6</v>
@@ -1166,15 +1166,15 @@
         <v>7</v>
       </c>
       <c r="E40" s="0" t="s">
-        <v>53</v>
+        <v>17</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="0">
-        <v>74</v>
+        <v>29</v>
       </c>
       <c r="B41" s="0" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C41" s="0" t="s">
         <v>6</v>
@@ -1183,15 +1183,15 @@
         <v>7</v>
       </c>
       <c r="E41" s="0" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="0">
-        <v>29</v>
+        <v>47</v>
       </c>
       <c r="B42" s="0" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C42" s="0" t="s">
         <v>6</v>
@@ -1200,15 +1200,15 @@
         <v>7</v>
       </c>
       <c r="E42" s="0" t="s">
-        <v>15</v>
+        <v>57</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" s="0">
-        <v>47</v>
+        <v>60</v>
       </c>
       <c r="B43" s="0" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="C43" s="0" t="s">
         <v>6</v>
@@ -1217,23 +1217,6 @@
         <v>7</v>
       </c>
       <c r="E43" s="0" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="44">
-      <c r="A44" s="0">
-        <v>60</v>
-      </c>
-      <c r="B44" s="0" t="s">
-        <v>58</v>
-      </c>
-      <c r="C44" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="D44" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="E44" s="0" t="s">
         <v>17</v>
       </c>
     </row>
@@ -1244,7 +1227,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:F44"/>
+  <dimension ref="A1:F45"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1272,10 +1255,10 @@
     </row>
     <row r="2">
       <c r="A2" s="0">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
       <c r="C2" s="0" t="s">
         <v>59</v>
@@ -1292,10 +1275,10 @@
     </row>
     <row r="3">
       <c r="A3" s="0">
-        <v>34</v>
+        <v>93</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>9</v>
+        <v>110</v>
       </c>
       <c r="C3" s="0" t="s">
         <v>59</v>
@@ -1304,7 +1287,7 @@
         <v>7</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>10</v>
+        <v>26</v>
       </c>
       <c r="F3" s="0" t="s">
         <v>26</v>
@@ -1312,10 +1295,10 @@
     </row>
     <row r="4">
       <c r="A4" s="0">
-        <v>50</v>
+        <v>34</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="C4" s="0" t="s">
         <v>59</v>
@@ -1324,7 +1307,7 @@
         <v>7</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="F4" s="0" t="s">
         <v>26</v>
@@ -1332,10 +1315,10 @@
     </row>
     <row r="5">
       <c r="A5" s="0">
-        <v>89</v>
+        <v>50</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>60</v>
+        <v>5</v>
       </c>
       <c r="C5" s="0" t="s">
         <v>59</v>
@@ -1344,18 +1327,18 @@
         <v>7</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="F5" s="0" t="s">
-        <v>12</v>
+        <v>26</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="0">
-        <v>59</v>
+        <v>89</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C6" s="0" t="s">
         <v>59</v>
@@ -1364,7 +1347,7 @@
         <v>7</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="F6" s="0" t="s">
         <v>12</v>
@@ -1372,10 +1355,10 @@
     </row>
     <row r="7">
       <c r="A7" s="0">
-        <v>69</v>
+        <v>59</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C7" s="0" t="s">
         <v>59</v>
@@ -1392,10 +1375,10 @@
     </row>
     <row r="8">
       <c r="A8" s="0">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C8" s="0" t="s">
         <v>59</v>
@@ -1412,10 +1395,10 @@
     </row>
     <row r="9">
       <c r="A9" s="0">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C9" s="0" t="s">
         <v>59</v>
@@ -1432,10 +1415,10 @@
     </row>
     <row r="10">
       <c r="A10" s="0">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C10" s="0" t="s">
         <v>59</v>
@@ -1447,15 +1430,15 @@
         <v>17</v>
       </c>
       <c r="F10" s="0" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="0">
-        <v>24</v>
+        <v>71</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C11" s="0" t="s">
         <v>59</v>
@@ -1464,7 +1447,7 @@
         <v>7</v>
       </c>
       <c r="E11" s="0" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="F11" s="0" t="s">
         <v>17</v>
@@ -1472,10 +1455,10 @@
     </row>
     <row r="12">
       <c r="A12" s="0">
-        <v>75</v>
+        <v>24</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C12" s="0" t="s">
         <v>59</v>
@@ -1484,7 +1467,7 @@
         <v>7</v>
       </c>
       <c r="E12" s="0" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="F12" s="0" t="s">
         <v>17</v>
@@ -1492,10 +1475,10 @@
     </row>
     <row r="13">
       <c r="A13" s="0">
-        <v>55</v>
+        <v>75</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C13" s="0" t="s">
         <v>59</v>
@@ -1504,7 +1487,7 @@
         <v>7</v>
       </c>
       <c r="E13" s="0" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="F13" s="0" t="s">
         <v>17</v>
@@ -1512,10 +1495,10 @@
     </row>
     <row r="14">
       <c r="A14" s="0">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C14" s="0" t="s">
         <v>59</v>
@@ -1532,10 +1515,10 @@
     </row>
     <row r="15">
       <c r="A15" s="0">
-        <v>72</v>
+        <v>56</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C15" s="0" t="s">
         <v>59</v>
@@ -1544,7 +1527,7 @@
         <v>7</v>
       </c>
       <c r="E15" s="0" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="F15" s="0" t="s">
         <v>17</v>
@@ -1552,10 +1535,10 @@
     </row>
     <row r="16">
       <c r="A16" s="0">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C16" s="0" t="s">
         <v>59</v>
@@ -1572,10 +1555,10 @@
     </row>
     <row r="17">
       <c r="A17" s="0">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C17" s="0" t="s">
         <v>59</v>
@@ -1592,10 +1575,10 @@
     </row>
     <row r="18">
       <c r="A18" s="0">
-        <v>70</v>
+        <v>62</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C18" s="0" t="s">
         <v>59</v>
@@ -1612,10 +1595,10 @@
     </row>
     <row r="19">
       <c r="A19" s="0">
-        <v>64</v>
+        <v>70</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C19" s="0" t="s">
         <v>59</v>
@@ -1632,10 +1615,10 @@
     </row>
     <row r="20">
       <c r="A20" s="0">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C20" s="0" t="s">
         <v>59</v>
@@ -1652,10 +1635,10 @@
     </row>
     <row r="21">
       <c r="A21" s="0">
-        <v>13</v>
+        <v>63</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C21" s="0" t="s">
         <v>59</v>
@@ -1664,7 +1647,7 @@
         <v>7</v>
       </c>
       <c r="E21" s="0" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="F21" s="0" t="s">
         <v>17</v>
@@ -1672,10 +1655,10 @@
     </row>
     <row r="22">
       <c r="A22" s="0">
-        <v>42</v>
+        <v>13</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C22" s="0" t="s">
         <v>59</v>
@@ -1684,18 +1667,18 @@
         <v>7</v>
       </c>
       <c r="E22" s="0" t="s">
-        <v>53</v>
+        <v>15</v>
       </c>
       <c r="F22" s="0" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="0">
-        <v>33</v>
+        <v>42</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C23" s="0" t="s">
         <v>59</v>
@@ -1704,7 +1687,7 @@
         <v>7</v>
       </c>
       <c r="E23" s="0" t="s">
-        <v>10</v>
+        <v>53</v>
       </c>
       <c r="F23" s="0" t="s">
         <v>19</v>
@@ -1712,10 +1695,10 @@
     </row>
     <row r="24">
       <c r="A24" s="0">
-        <v>48</v>
+        <v>33</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C24" s="0" t="s">
         <v>59</v>
@@ -1724,18 +1707,18 @@
         <v>7</v>
       </c>
       <c r="E24" s="0" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="F24" s="0" t="s">
-        <v>8</v>
+        <v>19</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="0">
-        <v>37</v>
+        <v>48</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C25" s="0" t="s">
         <v>59</v>
@@ -1744,7 +1727,7 @@
         <v>7</v>
       </c>
       <c r="E25" s="0" t="s">
-        <v>28</v>
+        <v>8</v>
       </c>
       <c r="F25" s="0" t="s">
         <v>8</v>
@@ -1752,10 +1735,10 @@
     </row>
     <row r="26">
       <c r="A26" s="0">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C26" s="0" t="s">
         <v>59</v>
@@ -1767,15 +1750,15 @@
         <v>28</v>
       </c>
       <c r="F26" s="0" t="s">
-        <v>57</v>
+        <v>8</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="0">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C27" s="0" t="s">
         <v>59</v>
@@ -1784,7 +1767,7 @@
         <v>7</v>
       </c>
       <c r="E27" s="0" t="s">
-        <v>83</v>
+        <v>28</v>
       </c>
       <c r="F27" s="0" t="s">
         <v>57</v>
@@ -1792,10 +1775,10 @@
     </row>
     <row r="28">
       <c r="A28" s="0">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C28" s="0" t="s">
         <v>59</v>
@@ -1804,7 +1787,7 @@
         <v>7</v>
       </c>
       <c r="E28" s="0" t="s">
-        <v>53</v>
+        <v>83</v>
       </c>
       <c r="F28" s="0" t="s">
         <v>57</v>
@@ -1812,10 +1795,10 @@
     </row>
     <row r="29">
       <c r="A29" s="0">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C29" s="0" t="s">
         <v>59</v>
@@ -1832,10 +1815,10 @@
     </row>
     <row r="30">
       <c r="A30" s="0">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="B30" s="0" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C30" s="0" t="s">
         <v>59</v>
@@ -1847,15 +1830,15 @@
         <v>53</v>
       </c>
       <c r="F30" s="0" t="s">
-        <v>83</v>
+        <v>57</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="0">
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="B31" s="0" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C31" s="0" t="s">
         <v>59</v>
@@ -1864,7 +1847,7 @@
         <v>7</v>
       </c>
       <c r="E31" s="0" t="s">
-        <v>28</v>
+        <v>53</v>
       </c>
       <c r="F31" s="0" t="s">
         <v>83</v>
@@ -1872,10 +1855,10 @@
     </row>
     <row r="32">
       <c r="A32" s="0">
-        <v>11</v>
+        <v>36</v>
       </c>
       <c r="B32" s="0" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C32" s="0" t="s">
         <v>59</v>
@@ -1884,18 +1867,18 @@
         <v>7</v>
       </c>
       <c r="E32" s="0" t="s">
-        <v>15</v>
+        <v>28</v>
       </c>
       <c r="F32" s="0" t="s">
-        <v>53</v>
+        <v>83</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="0">
-        <v>40</v>
+        <v>11</v>
       </c>
       <c r="B33" s="0" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C33" s="0" t="s">
         <v>59</v>
@@ -1904,7 +1887,7 @@
         <v>7</v>
       </c>
       <c r="E33" s="0" t="s">
-        <v>90</v>
+        <v>15</v>
       </c>
       <c r="F33" s="0" t="s">
         <v>53</v>
@@ -1912,10 +1895,10 @@
     </row>
     <row r="34">
       <c r="A34" s="0">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B34" s="0" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C34" s="0" t="s">
         <v>59</v>
@@ -1924,7 +1907,7 @@
         <v>7</v>
       </c>
       <c r="E34" s="0" t="s">
-        <v>28</v>
+        <v>90</v>
       </c>
       <c r="F34" s="0" t="s">
         <v>53</v>
@@ -1932,10 +1915,10 @@
     </row>
     <row r="35">
       <c r="A35" s="0">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="B35" s="0" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C35" s="0" t="s">
         <v>59</v>
@@ -1944,18 +1927,18 @@
         <v>7</v>
       </c>
       <c r="E35" s="0" t="s">
-        <v>10</v>
+        <v>28</v>
       </c>
       <c r="F35" s="0" t="s">
-        <v>28</v>
+        <v>53</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="0">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B36" s="0" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C36" s="0" t="s">
         <v>59</v>
@@ -1967,15 +1950,15 @@
         <v>10</v>
       </c>
       <c r="F36" s="0" t="s">
-        <v>10</v>
+        <v>28</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="0">
-        <v>20</v>
+        <v>31</v>
       </c>
       <c r="B37" s="0" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C37" s="0" t="s">
         <v>59</v>
@@ -1984,7 +1967,7 @@
         <v>7</v>
       </c>
       <c r="E37" s="0" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="F37" s="0" t="s">
         <v>10</v>
@@ -1992,10 +1975,10 @@
     </row>
     <row r="38">
       <c r="A38" s="0">
-        <v>9</v>
+        <v>20</v>
       </c>
       <c r="B38" s="0" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C38" s="0" t="s">
         <v>59</v>
@@ -2012,10 +1995,10 @@
     </row>
     <row r="39">
       <c r="A39" s="0">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B39" s="0" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C39" s="0" t="s">
         <v>59</v>
@@ -2032,10 +2015,10 @@
     </row>
     <row r="40">
       <c r="A40" s="0">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="B40" s="0" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C40" s="0" t="s">
         <v>59</v>
@@ -2047,15 +2030,15 @@
         <v>15</v>
       </c>
       <c r="F40" s="0" t="s">
-        <v>98</v>
+        <v>10</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="0">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B41" s="0" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C41" s="0" t="s">
         <v>59</v>
@@ -2067,15 +2050,15 @@
         <v>15</v>
       </c>
       <c r="F41" s="0" t="s">
-        <v>15</v>
+        <v>98</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="0">
-        <v>30</v>
+        <v>3</v>
       </c>
       <c r="B42" s="0" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C42" s="0" t="s">
         <v>59</v>
@@ -2092,10 +2075,10 @@
     </row>
     <row r="43">
       <c r="A43" s="0">
-        <v>2</v>
+        <v>30</v>
       </c>
       <c r="B43" s="0" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C43" s="0" t="s">
         <v>59</v>
@@ -2112,21 +2095,41 @@
     </row>
     <row r="44">
       <c r="A44" s="0">
+        <v>2</v>
+      </c>
+      <c r="B44" s="0" t="s">
+        <v>101</v>
+      </c>
+      <c r="C44" s="0" t="s">
+        <v>59</v>
+      </c>
+      <c r="D44" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E44" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="F44" s="0" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" s="0">
         <v>1</v>
       </c>
-      <c r="B44" s="0" t="s">
+      <c r="B45" s="0" t="s">
         <v>102</v>
       </c>
-      <c r="C44" s="0" t="s">
-        <v>59</v>
-      </c>
-      <c r="D44" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="E44" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="F44" s="0" t="s">
+      <c r="C45" s="0" t="s">
+        <v>59</v>
+      </c>
+      <c r="D45" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E45" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="F45" s="0" t="s">
         <v>15</v>
       </c>
     </row>

</xml_diff>

<commit_message>
refactor: panels to use events instead of EventHandler properties
</commit_message>
<xml_diff>
--- a/paint_todo.xlsx
+++ b/paint_todo.xlsx
@@ -494,7 +494,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:F45"/>
+  <dimension ref="A1:F44"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -520,10 +520,10 @@
     </row>
     <row r="2">
       <c r="A2" s="0">
-        <v>100</v>
+        <v>49</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>117</v>
+        <v>13</v>
       </c>
       <c r="C2" s="0" t="s">
         <v>6</v>
@@ -532,15 +532,15 @@
         <v>7</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>26</v>
+        <v>8</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="0">
-        <v>49</v>
+        <v>21</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C3" s="0" t="s">
         <v>6</v>
@@ -549,15 +549,15 @@
         <v>7</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="0">
-        <v>21</v>
+        <v>86</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C4" s="0" t="s">
         <v>6</v>
@@ -566,15 +566,15 @@
         <v>7</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="0">
-        <v>86</v>
+        <v>54</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C5" s="0" t="s">
         <v>6</v>
@@ -583,15 +583,15 @@
         <v>7</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="0">
-        <v>54</v>
+        <v>88</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C6" s="0" t="s">
         <v>6</v>
@@ -600,15 +600,15 @@
         <v>7</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="0">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C7" s="0" t="s">
         <v>6</v>
@@ -622,10 +622,10 @@
     </row>
     <row r="8">
       <c r="A8" s="0">
-        <v>90</v>
+        <v>95</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>21</v>
+        <v>112</v>
       </c>
       <c r="C8" s="0" t="s">
         <v>6</v>
@@ -634,15 +634,15 @@
         <v>7</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>12</v>
+        <v>26</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="0">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="C9" s="0" t="s">
         <v>6</v>
@@ -656,10 +656,10 @@
     </row>
     <row r="10">
       <c r="A10" s="0">
-        <v>97</v>
+        <v>53</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>114</v>
+        <v>22</v>
       </c>
       <c r="C10" s="0" t="s">
         <v>6</v>
@@ -668,15 +668,15 @@
         <v>7</v>
       </c>
       <c r="E10" s="0" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="0">
-        <v>53</v>
+        <v>92</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>22</v>
+        <v>109</v>
       </c>
       <c r="C11" s="0" t="s">
         <v>6</v>
@@ -685,15 +685,15 @@
         <v>7</v>
       </c>
       <c r="E11" s="0" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="0">
-        <v>92</v>
+        <v>51</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>109</v>
+        <v>23</v>
       </c>
       <c r="C12" s="0" t="s">
         <v>6</v>
@@ -702,15 +702,15 @@
         <v>7</v>
       </c>
       <c r="E12" s="0" t="s">
-        <v>26</v>
+        <v>8</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="0">
-        <v>51</v>
+        <v>76</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C13" s="0" t="s">
         <v>6</v>
@@ -719,15 +719,15 @@
         <v>7</v>
       </c>
       <c r="E13" s="0" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="0">
-        <v>76</v>
+        <v>91</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C14" s="0" t="s">
         <v>6</v>
@@ -736,15 +736,15 @@
         <v>7</v>
       </c>
       <c r="E14" s="0" t="s">
-        <v>17</v>
+        <v>26</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="0">
-        <v>91</v>
+        <v>35</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="C15" s="0" t="s">
         <v>6</v>
@@ -753,15 +753,15 @@
         <v>7</v>
       </c>
       <c r="E15" s="0" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="0">
-        <v>35</v>
+        <v>79</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C16" s="0" t="s">
         <v>6</v>
@@ -770,15 +770,15 @@
         <v>7</v>
       </c>
       <c r="E16" s="0" t="s">
-        <v>28</v>
+        <v>17</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="0">
-        <v>79</v>
+        <v>85</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C17" s="0" t="s">
         <v>6</v>
@@ -792,10 +792,10 @@
     </row>
     <row r="18">
       <c r="A18" s="0">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C18" s="0" t="s">
         <v>6</v>
@@ -809,10 +809,10 @@
     </row>
     <row r="19">
       <c r="A19" s="0">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C19" s="0" t="s">
         <v>6</v>
@@ -826,10 +826,10 @@
     </row>
     <row r="20">
       <c r="A20" s="0">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C20" s="0" t="s">
         <v>6</v>
@@ -843,10 +843,10 @@
     </row>
     <row r="21">
       <c r="A21" s="0">
-        <v>78</v>
+        <v>52</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C21" s="0" t="s">
         <v>6</v>
@@ -855,15 +855,15 @@
         <v>7</v>
       </c>
       <c r="E21" s="0" t="s">
-        <v>17</v>
+        <v>8</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="0">
-        <v>52</v>
+        <v>27</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C22" s="0" t="s">
         <v>6</v>
@@ -872,15 +872,15 @@
         <v>7</v>
       </c>
       <c r="E22" s="0" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="0">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C23" s="0" t="s">
         <v>6</v>
@@ -894,10 +894,10 @@
     </row>
     <row r="24">
       <c r="A24" s="0">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C24" s="0" t="s">
         <v>6</v>
@@ -911,10 +911,10 @@
     </row>
     <row r="25">
       <c r="A25" s="0">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C25" s="0" t="s">
         <v>6</v>
@@ -928,10 +928,10 @@
     </row>
     <row r="26">
       <c r="A26" s="0">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C26" s="0" t="s">
         <v>6</v>
@@ -945,10 +945,10 @@
     </row>
     <row r="27">
       <c r="A27" s="0">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C27" s="0" t="s">
         <v>6</v>
@@ -962,10 +962,10 @@
     </row>
     <row r="28">
       <c r="A28" s="0">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C28" s="0" t="s">
         <v>6</v>
@@ -979,10 +979,10 @@
     </row>
     <row r="29">
       <c r="A29" s="0">
-        <v>18</v>
+        <v>99</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>41</v>
+        <v>115</v>
       </c>
       <c r="C29" s="0" t="s">
         <v>6</v>
@@ -991,15 +991,15 @@
         <v>7</v>
       </c>
       <c r="E29" s="0" t="s">
-        <v>15</v>
+        <v>26</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="0">
-        <v>99</v>
+        <v>81</v>
       </c>
       <c r="B30" s="0" t="s">
-        <v>115</v>
+        <v>42</v>
       </c>
       <c r="C30" s="0" t="s">
         <v>6</v>
@@ -1008,15 +1008,15 @@
         <v>7</v>
       </c>
       <c r="E30" s="0" t="s">
-        <v>26</v>
+        <v>17</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="0">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B31" s="0" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C31" s="0" t="s">
         <v>6</v>
@@ -1030,10 +1030,10 @@
     </row>
     <row r="32">
       <c r="A32" s="0">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="B32" s="0" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C32" s="0" t="s">
         <v>6</v>
@@ -1047,10 +1047,10 @@
     </row>
     <row r="33">
       <c r="A33" s="0">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B33" s="0" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C33" s="0" t="s">
         <v>6</v>
@@ -1064,10 +1064,10 @@
     </row>
     <row r="34">
       <c r="A34" s="0">
-        <v>84</v>
+        <v>25</v>
       </c>
       <c r="B34" s="0" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C34" s="0" t="s">
         <v>6</v>
@@ -1076,15 +1076,15 @@
         <v>7</v>
       </c>
       <c r="E34" s="0" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="0">
-        <v>25</v>
+        <v>57</v>
       </c>
       <c r="B35" s="0" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C35" s="0" t="s">
         <v>6</v>
@@ -1093,15 +1093,15 @@
         <v>7</v>
       </c>
       <c r="E35" s="0" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="0">
-        <v>57</v>
+        <v>65</v>
       </c>
       <c r="B36" s="0" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C36" s="0" t="s">
         <v>6</v>
@@ -1115,10 +1115,10 @@
     </row>
     <row r="37">
       <c r="A37" s="0">
-        <v>65</v>
+        <v>58</v>
       </c>
       <c r="B37" s="0" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C37" s="0" t="s">
         <v>6</v>
@@ -1132,10 +1132,10 @@
     </row>
     <row r="38">
       <c r="A38" s="0">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="B38" s="0" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C38" s="0" t="s">
         <v>6</v>
@@ -1149,10 +1149,10 @@
     </row>
     <row r="39">
       <c r="A39" s="0">
-        <v>61</v>
+        <v>26</v>
       </c>
       <c r="B39" s="0" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C39" s="0" t="s">
         <v>6</v>
@@ -1161,15 +1161,15 @@
         <v>7</v>
       </c>
       <c r="E39" s="0" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="0">
-        <v>26</v>
+        <v>43</v>
       </c>
       <c r="B40" s="0" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C40" s="0" t="s">
         <v>6</v>
@@ -1178,15 +1178,15 @@
         <v>7</v>
       </c>
       <c r="E40" s="0" t="s">
-        <v>15</v>
+        <v>53</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="0">
-        <v>43</v>
+        <v>74</v>
       </c>
       <c r="B41" s="0" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="C41" s="0" t="s">
         <v>6</v>
@@ -1195,15 +1195,15 @@
         <v>7</v>
       </c>
       <c r="E41" s="0" t="s">
-        <v>53</v>
+        <v>17</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="0">
-        <v>74</v>
+        <v>29</v>
       </c>
       <c r="B42" s="0" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C42" s="0" t="s">
         <v>6</v>
@@ -1212,15 +1212,15 @@
         <v>7</v>
       </c>
       <c r="E42" s="0" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" s="0">
-        <v>29</v>
+        <v>47</v>
       </c>
       <c r="B43" s="0" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C43" s="0" t="s">
         <v>6</v>
@@ -1229,15 +1229,15 @@
         <v>7</v>
       </c>
       <c r="E43" s="0" t="s">
-        <v>15</v>
+        <v>57</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" s="0">
-        <v>47</v>
+        <v>60</v>
       </c>
       <c r="B44" s="0" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="C44" s="0" t="s">
         <v>6</v>
@@ -1246,23 +1246,6 @@
         <v>7</v>
       </c>
       <c r="E44" s="0" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="45">
-      <c r="A45" s="0">
-        <v>60</v>
-      </c>
-      <c r="B45" s="0" t="s">
-        <v>58</v>
-      </c>
-      <c r="C45" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="D45" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="E45" s="0" t="s">
         <v>17</v>
       </c>
     </row>
@@ -1273,7 +1256,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:F46"/>
+  <dimension ref="A1:F47"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1301,10 +1284,10 @@
     </row>
     <row r="2">
       <c r="A2" s="0">
-        <v>87</v>
+        <v>100</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="C2" s="0" t="s">
         <v>59</v>
@@ -1313,7 +1296,7 @@
         <v>7</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>12</v>
+        <v>26</v>
       </c>
       <c r="F2" s="0" t="s">
         <v>26</v>
@@ -1321,10 +1304,10 @@
     </row>
     <row r="3">
       <c r="A3" s="0">
-        <v>94</v>
+        <v>87</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="C3" s="0" t="s">
         <v>59</v>
@@ -1333,7 +1316,7 @@
         <v>7</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>26</v>
+        <v>12</v>
       </c>
       <c r="F3" s="0" t="s">
         <v>26</v>
@@ -1341,10 +1324,10 @@
     </row>
     <row r="4">
       <c r="A4" s="0">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
       <c r="C4" s="0" t="s">
         <v>59</v>
@@ -1361,10 +1344,10 @@
     </row>
     <row r="5">
       <c r="A5" s="0">
-        <v>34</v>
+        <v>93</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>9</v>
+        <v>110</v>
       </c>
       <c r="C5" s="0" t="s">
         <v>59</v>
@@ -1373,7 +1356,7 @@
         <v>7</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>10</v>
+        <v>26</v>
       </c>
       <c r="F5" s="0" t="s">
         <v>26</v>
@@ -1381,10 +1364,10 @@
     </row>
     <row r="6">
       <c r="A6" s="0">
-        <v>50</v>
+        <v>34</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="C6" s="0" t="s">
         <v>59</v>
@@ -1393,7 +1376,7 @@
         <v>7</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="F6" s="0" t="s">
         <v>26</v>
@@ -1401,10 +1384,10 @@
     </row>
     <row r="7">
       <c r="A7" s="0">
-        <v>89</v>
+        <v>50</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>60</v>
+        <v>5</v>
       </c>
       <c r="C7" s="0" t="s">
         <v>59</v>
@@ -1413,18 +1396,18 @@
         <v>7</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="F7" s="0" t="s">
-        <v>12</v>
+        <v>26</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="0">
-        <v>59</v>
+        <v>89</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C8" s="0" t="s">
         <v>59</v>
@@ -1433,7 +1416,7 @@
         <v>7</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="F8" s="0" t="s">
         <v>12</v>
@@ -1441,10 +1424,10 @@
     </row>
     <row r="9">
       <c r="A9" s="0">
-        <v>69</v>
+        <v>59</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C9" s="0" t="s">
         <v>59</v>
@@ -1461,10 +1444,10 @@
     </row>
     <row r="10">
       <c r="A10" s="0">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C10" s="0" t="s">
         <v>59</v>
@@ -1481,10 +1464,10 @@
     </row>
     <row r="11">
       <c r="A11" s="0">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C11" s="0" t="s">
         <v>59</v>
@@ -1501,10 +1484,10 @@
     </row>
     <row r="12">
       <c r="A12" s="0">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C12" s="0" t="s">
         <v>59</v>
@@ -1516,15 +1499,15 @@
         <v>17</v>
       </c>
       <c r="F12" s="0" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="0">
-        <v>24</v>
+        <v>71</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C13" s="0" t="s">
         <v>59</v>
@@ -1533,7 +1516,7 @@
         <v>7</v>
       </c>
       <c r="E13" s="0" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="F13" s="0" t="s">
         <v>17</v>
@@ -1541,10 +1524,10 @@
     </row>
     <row r="14">
       <c r="A14" s="0">
-        <v>75</v>
+        <v>24</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C14" s="0" t="s">
         <v>59</v>
@@ -1553,7 +1536,7 @@
         <v>7</v>
       </c>
       <c r="E14" s="0" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="F14" s="0" t="s">
         <v>17</v>
@@ -1561,10 +1544,10 @@
     </row>
     <row r="15">
       <c r="A15" s="0">
-        <v>55</v>
+        <v>75</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C15" s="0" t="s">
         <v>59</v>
@@ -1573,7 +1556,7 @@
         <v>7</v>
       </c>
       <c r="E15" s="0" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="F15" s="0" t="s">
         <v>17</v>
@@ -1581,10 +1564,10 @@
     </row>
     <row r="16">
       <c r="A16" s="0">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C16" s="0" t="s">
         <v>59</v>
@@ -1601,10 +1584,10 @@
     </row>
     <row r="17">
       <c r="A17" s="0">
-        <v>72</v>
+        <v>56</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C17" s="0" t="s">
         <v>59</v>
@@ -1613,7 +1596,7 @@
         <v>7</v>
       </c>
       <c r="E17" s="0" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="F17" s="0" t="s">
         <v>17</v>
@@ -1621,10 +1604,10 @@
     </row>
     <row r="18">
       <c r="A18" s="0">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C18" s="0" t="s">
         <v>59</v>
@@ -1641,10 +1624,10 @@
     </row>
     <row r="19">
       <c r="A19" s="0">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C19" s="0" t="s">
         <v>59</v>
@@ -1661,10 +1644,10 @@
     </row>
     <row r="20">
       <c r="A20" s="0">
-        <v>70</v>
+        <v>62</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C20" s="0" t="s">
         <v>59</v>
@@ -1681,10 +1664,10 @@
     </row>
     <row r="21">
       <c r="A21" s="0">
-        <v>64</v>
+        <v>70</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C21" s="0" t="s">
         <v>59</v>
@@ -1701,10 +1684,10 @@
     </row>
     <row r="22">
       <c r="A22" s="0">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C22" s="0" t="s">
         <v>59</v>
@@ -1721,10 +1704,10 @@
     </row>
     <row r="23">
       <c r="A23" s="0">
-        <v>13</v>
+        <v>63</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C23" s="0" t="s">
         <v>59</v>
@@ -1733,7 +1716,7 @@
         <v>7</v>
       </c>
       <c r="E23" s="0" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="F23" s="0" t="s">
         <v>17</v>
@@ -1741,10 +1724,10 @@
     </row>
     <row r="24">
       <c r="A24" s="0">
-        <v>42</v>
+        <v>13</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C24" s="0" t="s">
         <v>59</v>
@@ -1753,18 +1736,18 @@
         <v>7</v>
       </c>
       <c r="E24" s="0" t="s">
-        <v>53</v>
+        <v>15</v>
       </c>
       <c r="F24" s="0" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="0">
-        <v>33</v>
+        <v>42</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C25" s="0" t="s">
         <v>59</v>
@@ -1773,7 +1756,7 @@
         <v>7</v>
       </c>
       <c r="E25" s="0" t="s">
-        <v>10</v>
+        <v>53</v>
       </c>
       <c r="F25" s="0" t="s">
         <v>19</v>
@@ -1781,10 +1764,10 @@
     </row>
     <row r="26">
       <c r="A26" s="0">
-        <v>48</v>
+        <v>33</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C26" s="0" t="s">
         <v>59</v>
@@ -1793,18 +1776,18 @@
         <v>7</v>
       </c>
       <c r="E26" s="0" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="F26" s="0" t="s">
-        <v>8</v>
+        <v>19</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="0">
-        <v>37</v>
+        <v>48</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C27" s="0" t="s">
         <v>59</v>
@@ -1813,7 +1796,7 @@
         <v>7</v>
       </c>
       <c r="E27" s="0" t="s">
-        <v>28</v>
+        <v>8</v>
       </c>
       <c r="F27" s="0" t="s">
         <v>8</v>
@@ -1821,10 +1804,10 @@
     </row>
     <row r="28">
       <c r="A28" s="0">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C28" s="0" t="s">
         <v>59</v>
@@ -1836,15 +1819,15 @@
         <v>28</v>
       </c>
       <c r="F28" s="0" t="s">
-        <v>57</v>
+        <v>8</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="0">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C29" s="0" t="s">
         <v>59</v>
@@ -1853,7 +1836,7 @@
         <v>7</v>
       </c>
       <c r="E29" s="0" t="s">
-        <v>83</v>
+        <v>28</v>
       </c>
       <c r="F29" s="0" t="s">
         <v>57</v>
@@ -1861,10 +1844,10 @@
     </row>
     <row r="30">
       <c r="A30" s="0">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B30" s="0" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C30" s="0" t="s">
         <v>59</v>
@@ -1873,7 +1856,7 @@
         <v>7</v>
       </c>
       <c r="E30" s="0" t="s">
-        <v>53</v>
+        <v>83</v>
       </c>
       <c r="F30" s="0" t="s">
         <v>57</v>
@@ -1881,10 +1864,10 @@
     </row>
     <row r="31">
       <c r="A31" s="0">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B31" s="0" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C31" s="0" t="s">
         <v>59</v>
@@ -1901,10 +1884,10 @@
     </row>
     <row r="32">
       <c r="A32" s="0">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="B32" s="0" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C32" s="0" t="s">
         <v>59</v>
@@ -1916,15 +1899,15 @@
         <v>53</v>
       </c>
       <c r="F32" s="0" t="s">
-        <v>83</v>
+        <v>57</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="0">
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="B33" s="0" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C33" s="0" t="s">
         <v>59</v>
@@ -1933,7 +1916,7 @@
         <v>7</v>
       </c>
       <c r="E33" s="0" t="s">
-        <v>28</v>
+        <v>53</v>
       </c>
       <c r="F33" s="0" t="s">
         <v>83</v>
@@ -1941,10 +1924,10 @@
     </row>
     <row r="34">
       <c r="A34" s="0">
-        <v>11</v>
+        <v>36</v>
       </c>
       <c r="B34" s="0" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C34" s="0" t="s">
         <v>59</v>
@@ -1953,18 +1936,18 @@
         <v>7</v>
       </c>
       <c r="E34" s="0" t="s">
-        <v>15</v>
+        <v>28</v>
       </c>
       <c r="F34" s="0" t="s">
-        <v>53</v>
+        <v>83</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="0">
-        <v>40</v>
+        <v>11</v>
       </c>
       <c r="B35" s="0" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C35" s="0" t="s">
         <v>59</v>
@@ -1973,7 +1956,7 @@
         <v>7</v>
       </c>
       <c r="E35" s="0" t="s">
-        <v>90</v>
+        <v>15</v>
       </c>
       <c r="F35" s="0" t="s">
         <v>53</v>
@@ -1981,10 +1964,10 @@
     </row>
     <row r="36">
       <c r="A36" s="0">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B36" s="0" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C36" s="0" t="s">
         <v>59</v>
@@ -1993,7 +1976,7 @@
         <v>7</v>
       </c>
       <c r="E36" s="0" t="s">
-        <v>28</v>
+        <v>90</v>
       </c>
       <c r="F36" s="0" t="s">
         <v>53</v>
@@ -2001,10 +1984,10 @@
     </row>
     <row r="37">
       <c r="A37" s="0">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="B37" s="0" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C37" s="0" t="s">
         <v>59</v>
@@ -2013,18 +1996,18 @@
         <v>7</v>
       </c>
       <c r="E37" s="0" t="s">
-        <v>10</v>
+        <v>28</v>
       </c>
       <c r="F37" s="0" t="s">
-        <v>28</v>
+        <v>53</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="0">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B38" s="0" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C38" s="0" t="s">
         <v>59</v>
@@ -2036,15 +2019,15 @@
         <v>10</v>
       </c>
       <c r="F38" s="0" t="s">
-        <v>10</v>
+        <v>28</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="0">
-        <v>20</v>
+        <v>31</v>
       </c>
       <c r="B39" s="0" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C39" s="0" t="s">
         <v>59</v>
@@ -2053,7 +2036,7 @@
         <v>7</v>
       </c>
       <c r="E39" s="0" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="F39" s="0" t="s">
         <v>10</v>
@@ -2061,10 +2044,10 @@
     </row>
     <row r="40">
       <c r="A40" s="0">
-        <v>9</v>
+        <v>20</v>
       </c>
       <c r="B40" s="0" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C40" s="0" t="s">
         <v>59</v>
@@ -2081,10 +2064,10 @@
     </row>
     <row r="41">
       <c r="A41" s="0">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B41" s="0" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C41" s="0" t="s">
         <v>59</v>
@@ -2101,10 +2084,10 @@
     </row>
     <row r="42">
       <c r="A42" s="0">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="B42" s="0" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C42" s="0" t="s">
         <v>59</v>
@@ -2116,15 +2099,15 @@
         <v>15</v>
       </c>
       <c r="F42" s="0" t="s">
-        <v>98</v>
+        <v>10</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" s="0">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B43" s="0" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C43" s="0" t="s">
         <v>59</v>
@@ -2136,15 +2119,15 @@
         <v>15</v>
       </c>
       <c r="F43" s="0" t="s">
-        <v>15</v>
+        <v>98</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" s="0">
-        <v>30</v>
+        <v>3</v>
       </c>
       <c r="B44" s="0" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C44" s="0" t="s">
         <v>59</v>
@@ -2161,10 +2144,10 @@
     </row>
     <row r="45">
       <c r="A45" s="0">
-        <v>2</v>
+        <v>30</v>
       </c>
       <c r="B45" s="0" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C45" s="0" t="s">
         <v>59</v>
@@ -2181,21 +2164,41 @@
     </row>
     <row r="46">
       <c r="A46" s="0">
+        <v>2</v>
+      </c>
+      <c r="B46" s="0" t="s">
+        <v>101</v>
+      </c>
+      <c r="C46" s="0" t="s">
+        <v>59</v>
+      </c>
+      <c r="D46" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E46" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="F46" s="0" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" s="0">
         <v>1</v>
       </c>
-      <c r="B46" s="0" t="s">
+      <c r="B47" s="0" t="s">
         <v>102</v>
       </c>
-      <c r="C46" s="0" t="s">
-        <v>59</v>
-      </c>
-      <c r="D46" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="E46" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="F46" s="0" t="s">
+      <c r="C47" s="0" t="s">
+        <v>59</v>
+      </c>
+      <c r="D47" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E47" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="F47" s="0" t="s">
         <v>15</v>
       </c>
     </row>

</xml_diff>

<commit_message>
refactor: move Edit Palette controls to WithoutHaste.Windows.GUI project
</commit_message>
<xml_diff>
--- a/paint_todo.xlsx
+++ b/paint_todo.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="119">
   <si>
     <t>Id</t>
   </si>
@@ -442,6 +442,11 @@
   </si>
   <si>
     <t>refactor all panels to use proper events instead of delegate properties</t>
+  </si>
+  <si>
+    <t xml:space="preserve">when resizing windows, default behavior is to keep the same section of image in the viewing pane
+- so expanding window would in effect zoom in
+CANCELLED</t>
   </si>
 </sst>
 </file>
@@ -494,7 +499,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:F44"/>
+  <dimension ref="A1:F43"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -520,10 +525,10 @@
     </row>
     <row r="2">
       <c r="A2" s="0">
-        <v>49</v>
+        <v>86</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="C2" s="0" t="s">
         <v>6</v>
@@ -532,15 +537,15 @@
         <v>7</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="0">
-        <v>21</v>
+        <v>54</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="C3" s="0" t="s">
         <v>6</v>
@@ -549,15 +554,15 @@
         <v>7</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="0">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="C4" s="0" t="s">
         <v>6</v>
@@ -566,15 +571,15 @@
         <v>7</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="0">
-        <v>54</v>
+        <v>90</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="C5" s="0" t="s">
         <v>6</v>
@@ -583,15 +588,15 @@
         <v>7</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="0">
-        <v>88</v>
+        <v>95</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>20</v>
+        <v>112</v>
       </c>
       <c r="C6" s="0" t="s">
         <v>6</v>
@@ -600,15 +605,15 @@
         <v>7</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>12</v>
+        <v>26</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="0">
-        <v>90</v>
+        <v>97</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>21</v>
+        <v>114</v>
       </c>
       <c r="C7" s="0" t="s">
         <v>6</v>
@@ -617,15 +622,15 @@
         <v>7</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>12</v>
+        <v>26</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="0">
-        <v>95</v>
+        <v>53</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>112</v>
+        <v>22</v>
       </c>
       <c r="C8" s="0" t="s">
         <v>6</v>
@@ -634,15 +639,15 @@
         <v>7</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="0">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="C9" s="0" t="s">
         <v>6</v>
@@ -656,10 +661,10 @@
     </row>
     <row r="10">
       <c r="A10" s="0">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C10" s="0" t="s">
         <v>6</v>
@@ -668,15 +673,15 @@
         <v>7</v>
       </c>
       <c r="E10" s="0" t="s">
-        <v>19</v>
+        <v>8</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="0">
-        <v>92</v>
+        <v>76</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>109</v>
+        <v>24</v>
       </c>
       <c r="C11" s="0" t="s">
         <v>6</v>
@@ -685,15 +690,15 @@
         <v>7</v>
       </c>
       <c r="E11" s="0" t="s">
-        <v>26</v>
+        <v>17</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="0">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>23</v>
+        <v>13</v>
       </c>
       <c r="C12" s="0" t="s">
         <v>6</v>
@@ -707,10 +712,10 @@
     </row>
     <row r="13">
       <c r="A13" s="0">
-        <v>76</v>
+        <v>91</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C13" s="0" t="s">
         <v>6</v>
@@ -719,15 +724,15 @@
         <v>7</v>
       </c>
       <c r="E13" s="0" t="s">
-        <v>17</v>
+        <v>26</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="0">
-        <v>91</v>
+        <v>35</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="C14" s="0" t="s">
         <v>6</v>
@@ -736,15 +741,15 @@
         <v>7</v>
       </c>
       <c r="E14" s="0" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="0">
-        <v>35</v>
+        <v>79</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C15" s="0" t="s">
         <v>6</v>
@@ -753,15 +758,15 @@
         <v>7</v>
       </c>
       <c r="E15" s="0" t="s">
-        <v>28</v>
+        <v>17</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="0">
-        <v>79</v>
+        <v>85</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C16" s="0" t="s">
         <v>6</v>
@@ -775,10 +780,10 @@
     </row>
     <row r="17">
       <c r="A17" s="0">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C17" s="0" t="s">
         <v>6</v>
@@ -792,10 +797,10 @@
     </row>
     <row r="18">
       <c r="A18" s="0">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C18" s="0" t="s">
         <v>6</v>
@@ -809,10 +814,10 @@
     </row>
     <row r="19">
       <c r="A19" s="0">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C19" s="0" t="s">
         <v>6</v>
@@ -826,10 +831,10 @@
     </row>
     <row r="20">
       <c r="A20" s="0">
-        <v>78</v>
+        <v>52</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C20" s="0" t="s">
         <v>6</v>
@@ -838,15 +843,15 @@
         <v>7</v>
       </c>
       <c r="E20" s="0" t="s">
-        <v>17</v>
+        <v>8</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="0">
-        <v>52</v>
+        <v>27</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C21" s="0" t="s">
         <v>6</v>
@@ -855,15 +860,15 @@
         <v>7</v>
       </c>
       <c r="E21" s="0" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="0">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C22" s="0" t="s">
         <v>6</v>
@@ -877,10 +882,10 @@
     </row>
     <row r="23">
       <c r="A23" s="0">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C23" s="0" t="s">
         <v>6</v>
@@ -894,10 +899,10 @@
     </row>
     <row r="24">
       <c r="A24" s="0">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C24" s="0" t="s">
         <v>6</v>
@@ -911,10 +916,10 @@
     </row>
     <row r="25">
       <c r="A25" s="0">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C25" s="0" t="s">
         <v>6</v>
@@ -928,10 +933,10 @@
     </row>
     <row r="26">
       <c r="A26" s="0">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C26" s="0" t="s">
         <v>6</v>
@@ -945,10 +950,10 @@
     </row>
     <row r="27">
       <c r="A27" s="0">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C27" s="0" t="s">
         <v>6</v>
@@ -962,10 +967,10 @@
     </row>
     <row r="28">
       <c r="A28" s="0">
-        <v>18</v>
+        <v>99</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>41</v>
+        <v>115</v>
       </c>
       <c r="C28" s="0" t="s">
         <v>6</v>
@@ -974,15 +979,15 @@
         <v>7</v>
       </c>
       <c r="E28" s="0" t="s">
-        <v>15</v>
+        <v>26</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="0">
-        <v>99</v>
+        <v>81</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>115</v>
+        <v>42</v>
       </c>
       <c r="C29" s="0" t="s">
         <v>6</v>
@@ -991,15 +996,15 @@
         <v>7</v>
       </c>
       <c r="E29" s="0" t="s">
-        <v>26</v>
+        <v>17</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="0">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B30" s="0" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C30" s="0" t="s">
         <v>6</v>
@@ -1013,10 +1018,10 @@
     </row>
     <row r="31">
       <c r="A31" s="0">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="B31" s="0" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C31" s="0" t="s">
         <v>6</v>
@@ -1030,10 +1035,10 @@
     </row>
     <row r="32">
       <c r="A32" s="0">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B32" s="0" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C32" s="0" t="s">
         <v>6</v>
@@ -1047,10 +1052,10 @@
     </row>
     <row r="33">
       <c r="A33" s="0">
-        <v>84</v>
+        <v>25</v>
       </c>
       <c r="B33" s="0" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C33" s="0" t="s">
         <v>6</v>
@@ -1059,15 +1064,15 @@
         <v>7</v>
       </c>
       <c r="E33" s="0" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="0">
-        <v>25</v>
+        <v>57</v>
       </c>
       <c r="B34" s="0" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C34" s="0" t="s">
         <v>6</v>
@@ -1076,15 +1081,15 @@
         <v>7</v>
       </c>
       <c r="E34" s="0" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="0">
-        <v>57</v>
+        <v>65</v>
       </c>
       <c r="B35" s="0" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C35" s="0" t="s">
         <v>6</v>
@@ -1098,10 +1103,10 @@
     </row>
     <row r="36">
       <c r="A36" s="0">
-        <v>65</v>
+        <v>58</v>
       </c>
       <c r="B36" s="0" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C36" s="0" t="s">
         <v>6</v>
@@ -1115,10 +1120,10 @@
     </row>
     <row r="37">
       <c r="A37" s="0">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="B37" s="0" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C37" s="0" t="s">
         <v>6</v>
@@ -1132,10 +1137,10 @@
     </row>
     <row r="38">
       <c r="A38" s="0">
-        <v>61</v>
+        <v>26</v>
       </c>
       <c r="B38" s="0" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C38" s="0" t="s">
         <v>6</v>
@@ -1144,15 +1149,15 @@
         <v>7</v>
       </c>
       <c r="E38" s="0" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="0">
-        <v>26</v>
+        <v>43</v>
       </c>
       <c r="B39" s="0" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C39" s="0" t="s">
         <v>6</v>
@@ -1161,15 +1166,15 @@
         <v>7</v>
       </c>
       <c r="E39" s="0" t="s">
-        <v>15</v>
+        <v>53</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="0">
-        <v>43</v>
+        <v>74</v>
       </c>
       <c r="B40" s="0" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="C40" s="0" t="s">
         <v>6</v>
@@ -1178,15 +1183,15 @@
         <v>7</v>
       </c>
       <c r="E40" s="0" t="s">
-        <v>53</v>
+        <v>17</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="0">
-        <v>74</v>
+        <v>29</v>
       </c>
       <c r="B41" s="0" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C41" s="0" t="s">
         <v>6</v>
@@ -1195,15 +1200,15 @@
         <v>7</v>
       </c>
       <c r="E41" s="0" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="0">
-        <v>29</v>
+        <v>47</v>
       </c>
       <c r="B42" s="0" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C42" s="0" t="s">
         <v>6</v>
@@ -1212,15 +1217,15 @@
         <v>7</v>
       </c>
       <c r="E42" s="0" t="s">
-        <v>15</v>
+        <v>57</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" s="0">
-        <v>47</v>
+        <v>60</v>
       </c>
       <c r="B43" s="0" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="C43" s="0" t="s">
         <v>6</v>
@@ -1229,23 +1234,6 @@
         <v>7</v>
       </c>
       <c r="E43" s="0" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="44">
-      <c r="A44" s="0">
-        <v>60</v>
-      </c>
-      <c r="B44" s="0" t="s">
-        <v>58</v>
-      </c>
-      <c r="C44" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="D44" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="E44" s="0" t="s">
         <v>17</v>
       </c>
     </row>
@@ -1256,7 +1244,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:F47"/>
+  <dimension ref="A1:F48"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1284,10 +1272,10 @@
     </row>
     <row r="2">
       <c r="A2" s="0">
-        <v>100</v>
+        <v>21</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="C2" s="0" t="s">
         <v>59</v>
@@ -1296,7 +1284,7 @@
         <v>7</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>26</v>
+        <v>15</v>
       </c>
       <c r="F2" s="0" t="s">
         <v>26</v>
@@ -1304,10 +1292,10 @@
     </row>
     <row r="3">
       <c r="A3" s="0">
-        <v>87</v>
+        <v>100</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="C3" s="0" t="s">
         <v>59</v>
@@ -1316,7 +1304,7 @@
         <v>7</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>12</v>
+        <v>26</v>
       </c>
       <c r="F3" s="0" t="s">
         <v>26</v>
@@ -1324,10 +1312,10 @@
     </row>
     <row r="4">
       <c r="A4" s="0">
-        <v>94</v>
+        <v>87</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="C4" s="0" t="s">
         <v>59</v>
@@ -1336,7 +1324,7 @@
         <v>7</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>26</v>
+        <v>12</v>
       </c>
       <c r="F4" s="0" t="s">
         <v>26</v>
@@ -1344,10 +1332,10 @@
     </row>
     <row r="5">
       <c r="A5" s="0">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
       <c r="C5" s="0" t="s">
         <v>59</v>
@@ -1364,10 +1352,10 @@
     </row>
     <row r="6">
       <c r="A6" s="0">
-        <v>34</v>
+        <v>93</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>9</v>
+        <v>110</v>
       </c>
       <c r="C6" s="0" t="s">
         <v>59</v>
@@ -1376,7 +1364,7 @@
         <v>7</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>10</v>
+        <v>26</v>
       </c>
       <c r="F6" s="0" t="s">
         <v>26</v>
@@ -1384,10 +1372,10 @@
     </row>
     <row r="7">
       <c r="A7" s="0">
-        <v>50</v>
+        <v>34</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="C7" s="0" t="s">
         <v>59</v>
@@ -1396,7 +1384,7 @@
         <v>7</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="F7" s="0" t="s">
         <v>26</v>
@@ -1404,10 +1392,10 @@
     </row>
     <row r="8">
       <c r="A8" s="0">
-        <v>89</v>
+        <v>50</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>60</v>
+        <v>5</v>
       </c>
       <c r="C8" s="0" t="s">
         <v>59</v>
@@ -1416,18 +1404,18 @@
         <v>7</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="F8" s="0" t="s">
-        <v>12</v>
+        <v>26</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="0">
-        <v>59</v>
+        <v>89</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C9" s="0" t="s">
         <v>59</v>
@@ -1436,7 +1424,7 @@
         <v>7</v>
       </c>
       <c r="E9" s="0" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="F9" s="0" t="s">
         <v>12</v>
@@ -1444,10 +1432,10 @@
     </row>
     <row r="10">
       <c r="A10" s="0">
-        <v>69</v>
+        <v>59</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C10" s="0" t="s">
         <v>59</v>
@@ -1464,10 +1452,10 @@
     </row>
     <row r="11">
       <c r="A11" s="0">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C11" s="0" t="s">
         <v>59</v>
@@ -1484,10 +1472,10 @@
     </row>
     <row r="12">
       <c r="A12" s="0">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C12" s="0" t="s">
         <v>59</v>
@@ -1504,10 +1492,10 @@
     </row>
     <row r="13">
       <c r="A13" s="0">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C13" s="0" t="s">
         <v>59</v>
@@ -1519,15 +1507,15 @@
         <v>17</v>
       </c>
       <c r="F13" s="0" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="0">
-        <v>24</v>
+        <v>71</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C14" s="0" t="s">
         <v>59</v>
@@ -1536,7 +1524,7 @@
         <v>7</v>
       </c>
       <c r="E14" s="0" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="F14" s="0" t="s">
         <v>17</v>
@@ -1544,10 +1532,10 @@
     </row>
     <row r="15">
       <c r="A15" s="0">
-        <v>75</v>
+        <v>24</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C15" s="0" t="s">
         <v>59</v>
@@ -1556,7 +1544,7 @@
         <v>7</v>
       </c>
       <c r="E15" s="0" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="F15" s="0" t="s">
         <v>17</v>
@@ -1564,10 +1552,10 @@
     </row>
     <row r="16">
       <c r="A16" s="0">
-        <v>55</v>
+        <v>75</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C16" s="0" t="s">
         <v>59</v>
@@ -1576,7 +1564,7 @@
         <v>7</v>
       </c>
       <c r="E16" s="0" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="F16" s="0" t="s">
         <v>17</v>
@@ -1584,10 +1572,10 @@
     </row>
     <row r="17">
       <c r="A17" s="0">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C17" s="0" t="s">
         <v>59</v>
@@ -1604,10 +1592,10 @@
     </row>
     <row r="18">
       <c r="A18" s="0">
-        <v>72</v>
+        <v>56</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C18" s="0" t="s">
         <v>59</v>
@@ -1616,7 +1604,7 @@
         <v>7</v>
       </c>
       <c r="E18" s="0" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="F18" s="0" t="s">
         <v>17</v>
@@ -1624,10 +1612,10 @@
     </row>
     <row r="19">
       <c r="A19" s="0">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C19" s="0" t="s">
         <v>59</v>
@@ -1644,10 +1632,10 @@
     </row>
     <row r="20">
       <c r="A20" s="0">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C20" s="0" t="s">
         <v>59</v>
@@ -1664,10 +1652,10 @@
     </row>
     <row r="21">
       <c r="A21" s="0">
-        <v>70</v>
+        <v>62</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C21" s="0" t="s">
         <v>59</v>
@@ -1684,10 +1672,10 @@
     </row>
     <row r="22">
       <c r="A22" s="0">
-        <v>64</v>
+        <v>70</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C22" s="0" t="s">
         <v>59</v>
@@ -1704,10 +1692,10 @@
     </row>
     <row r="23">
       <c r="A23" s="0">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C23" s="0" t="s">
         <v>59</v>
@@ -1724,10 +1712,10 @@
     </row>
     <row r="24">
       <c r="A24" s="0">
-        <v>13</v>
+        <v>63</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C24" s="0" t="s">
         <v>59</v>
@@ -1736,7 +1724,7 @@
         <v>7</v>
       </c>
       <c r="E24" s="0" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="F24" s="0" t="s">
         <v>17</v>
@@ -1744,10 +1732,10 @@
     </row>
     <row r="25">
       <c r="A25" s="0">
-        <v>42</v>
+        <v>13</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C25" s="0" t="s">
         <v>59</v>
@@ -1756,18 +1744,18 @@
         <v>7</v>
       </c>
       <c r="E25" s="0" t="s">
-        <v>53</v>
+        <v>15</v>
       </c>
       <c r="F25" s="0" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="0">
-        <v>33</v>
+        <v>42</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C26" s="0" t="s">
         <v>59</v>
@@ -1776,7 +1764,7 @@
         <v>7</v>
       </c>
       <c r="E26" s="0" t="s">
-        <v>10</v>
+        <v>53</v>
       </c>
       <c r="F26" s="0" t="s">
         <v>19</v>
@@ -1784,10 +1772,10 @@
     </row>
     <row r="27">
       <c r="A27" s="0">
-        <v>48</v>
+        <v>33</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C27" s="0" t="s">
         <v>59</v>
@@ -1796,18 +1784,18 @@
         <v>7</v>
       </c>
       <c r="E27" s="0" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="F27" s="0" t="s">
-        <v>8</v>
+        <v>19</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="0">
-        <v>37</v>
+        <v>48</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C28" s="0" t="s">
         <v>59</v>
@@ -1816,7 +1804,7 @@
         <v>7</v>
       </c>
       <c r="E28" s="0" t="s">
-        <v>28</v>
+        <v>8</v>
       </c>
       <c r="F28" s="0" t="s">
         <v>8</v>
@@ -1824,10 +1812,10 @@
     </row>
     <row r="29">
       <c r="A29" s="0">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C29" s="0" t="s">
         <v>59</v>
@@ -1839,15 +1827,15 @@
         <v>28</v>
       </c>
       <c r="F29" s="0" t="s">
-        <v>57</v>
+        <v>8</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="0">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="B30" s="0" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C30" s="0" t="s">
         <v>59</v>
@@ -1856,7 +1844,7 @@
         <v>7</v>
       </c>
       <c r="E30" s="0" t="s">
-        <v>83</v>
+        <v>28</v>
       </c>
       <c r="F30" s="0" t="s">
         <v>57</v>
@@ -1864,10 +1852,10 @@
     </row>
     <row r="31">
       <c r="A31" s="0">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B31" s="0" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C31" s="0" t="s">
         <v>59</v>
@@ -1876,7 +1864,7 @@
         <v>7</v>
       </c>
       <c r="E31" s="0" t="s">
-        <v>53</v>
+        <v>83</v>
       </c>
       <c r="F31" s="0" t="s">
         <v>57</v>
@@ -1884,10 +1872,10 @@
     </row>
     <row r="32">
       <c r="A32" s="0">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B32" s="0" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C32" s="0" t="s">
         <v>59</v>
@@ -1904,10 +1892,10 @@
     </row>
     <row r="33">
       <c r="A33" s="0">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="B33" s="0" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C33" s="0" t="s">
         <v>59</v>
@@ -1919,15 +1907,15 @@
         <v>53</v>
       </c>
       <c r="F33" s="0" t="s">
-        <v>83</v>
+        <v>57</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="0">
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="B34" s="0" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C34" s="0" t="s">
         <v>59</v>
@@ -1936,7 +1924,7 @@
         <v>7</v>
       </c>
       <c r="E34" s="0" t="s">
-        <v>28</v>
+        <v>53</v>
       </c>
       <c r="F34" s="0" t="s">
         <v>83</v>
@@ -1944,10 +1932,10 @@
     </row>
     <row r="35">
       <c r="A35" s="0">
-        <v>11</v>
+        <v>36</v>
       </c>
       <c r="B35" s="0" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C35" s="0" t="s">
         <v>59</v>
@@ -1956,18 +1944,18 @@
         <v>7</v>
       </c>
       <c r="E35" s="0" t="s">
-        <v>15</v>
+        <v>28</v>
       </c>
       <c r="F35" s="0" t="s">
-        <v>53</v>
+        <v>83</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="0">
-        <v>40</v>
+        <v>11</v>
       </c>
       <c r="B36" s="0" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C36" s="0" t="s">
         <v>59</v>
@@ -1976,7 +1964,7 @@
         <v>7</v>
       </c>
       <c r="E36" s="0" t="s">
-        <v>90</v>
+        <v>15</v>
       </c>
       <c r="F36" s="0" t="s">
         <v>53</v>
@@ -1984,10 +1972,10 @@
     </row>
     <row r="37">
       <c r="A37" s="0">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B37" s="0" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C37" s="0" t="s">
         <v>59</v>
@@ -1996,7 +1984,7 @@
         <v>7</v>
       </c>
       <c r="E37" s="0" t="s">
-        <v>28</v>
+        <v>90</v>
       </c>
       <c r="F37" s="0" t="s">
         <v>53</v>
@@ -2004,10 +1992,10 @@
     </row>
     <row r="38">
       <c r="A38" s="0">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="B38" s="0" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C38" s="0" t="s">
         <v>59</v>
@@ -2016,18 +2004,18 @@
         <v>7</v>
       </c>
       <c r="E38" s="0" t="s">
-        <v>10</v>
+        <v>28</v>
       </c>
       <c r="F38" s="0" t="s">
-        <v>28</v>
+        <v>53</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="0">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B39" s="0" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C39" s="0" t="s">
         <v>59</v>
@@ -2039,15 +2027,15 @@
         <v>10</v>
       </c>
       <c r="F39" s="0" t="s">
-        <v>10</v>
+        <v>28</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="0">
-        <v>20</v>
+        <v>31</v>
       </c>
       <c r="B40" s="0" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C40" s="0" t="s">
         <v>59</v>
@@ -2056,7 +2044,7 @@
         <v>7</v>
       </c>
       <c r="E40" s="0" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="F40" s="0" t="s">
         <v>10</v>
@@ -2064,10 +2052,10 @@
     </row>
     <row r="41">
       <c r="A41" s="0">
-        <v>9</v>
+        <v>20</v>
       </c>
       <c r="B41" s="0" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C41" s="0" t="s">
         <v>59</v>
@@ -2084,10 +2072,10 @@
     </row>
     <row r="42">
       <c r="A42" s="0">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B42" s="0" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C42" s="0" t="s">
         <v>59</v>
@@ -2104,10 +2092,10 @@
     </row>
     <row r="43">
       <c r="A43" s="0">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="B43" s="0" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C43" s="0" t="s">
         <v>59</v>
@@ -2119,15 +2107,15 @@
         <v>15</v>
       </c>
       <c r="F43" s="0" t="s">
-        <v>98</v>
+        <v>10</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" s="0">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B44" s="0" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C44" s="0" t="s">
         <v>59</v>
@@ -2139,15 +2127,15 @@
         <v>15</v>
       </c>
       <c r="F44" s="0" t="s">
-        <v>15</v>
+        <v>98</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" s="0">
-        <v>30</v>
+        <v>3</v>
       </c>
       <c r="B45" s="0" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C45" s="0" t="s">
         <v>59</v>
@@ -2164,10 +2152,10 @@
     </row>
     <row r="46">
       <c r="A46" s="0">
-        <v>2</v>
+        <v>30</v>
       </c>
       <c r="B46" s="0" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C46" s="0" t="s">
         <v>59</v>
@@ -2184,21 +2172,41 @@
     </row>
     <row r="47">
       <c r="A47" s="0">
+        <v>2</v>
+      </c>
+      <c r="B47" s="0" t="s">
+        <v>101</v>
+      </c>
+      <c r="C47" s="0" t="s">
+        <v>59</v>
+      </c>
+      <c r="D47" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E47" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="F47" s="0" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" s="0">
         <v>1</v>
       </c>
-      <c r="B47" s="0" t="s">
+      <c r="B48" s="0" t="s">
         <v>102</v>
       </c>
-      <c r="C47" s="0" t="s">
-        <v>59</v>
-      </c>
-      <c r="D47" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="E47" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="F47" s="0" t="s">
+      <c r="C48" s="0" t="s">
+        <v>59</v>
+      </c>
+      <c r="D48" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E48" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="F48" s="0" t="s">
         <v>15</v>
       </c>
     </row>

</xml_diff>

<commit_message>
refactor: use WithoutHaste.Windows.GUI IconManager
</commit_message>
<xml_diff>
--- a/paint_todo.xlsx
+++ b/paint_todo.xlsx
@@ -499,7 +499,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:F43"/>
+  <dimension ref="A1:F42"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -610,10 +610,10 @@
     </row>
     <row r="7">
       <c r="A7" s="0">
-        <v>97</v>
+        <v>53</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>114</v>
+        <v>22</v>
       </c>
       <c r="C7" s="0" t="s">
         <v>6</v>
@@ -622,15 +622,15 @@
         <v>7</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="0">
-        <v>53</v>
+        <v>92</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>22</v>
+        <v>109</v>
       </c>
       <c r="C8" s="0" t="s">
         <v>6</v>
@@ -639,15 +639,15 @@
         <v>7</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="0">
-        <v>92</v>
+        <v>51</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>109</v>
+        <v>23</v>
       </c>
       <c r="C9" s="0" t="s">
         <v>6</v>
@@ -656,15 +656,15 @@
         <v>7</v>
       </c>
       <c r="E9" s="0" t="s">
-        <v>26</v>
+        <v>8</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="0">
-        <v>51</v>
+        <v>76</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C10" s="0" t="s">
         <v>6</v>
@@ -673,15 +673,15 @@
         <v>7</v>
       </c>
       <c r="E10" s="0" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="0">
-        <v>76</v>
+        <v>49</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>24</v>
+        <v>13</v>
       </c>
       <c r="C11" s="0" t="s">
         <v>6</v>
@@ -690,15 +690,15 @@
         <v>7</v>
       </c>
       <c r="E11" s="0" t="s">
-        <v>17</v>
+        <v>8</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="0">
-        <v>49</v>
+        <v>91</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>13</v>
+        <v>25</v>
       </c>
       <c r="C12" s="0" t="s">
         <v>6</v>
@@ -707,15 +707,15 @@
         <v>7</v>
       </c>
       <c r="E12" s="0" t="s">
-        <v>8</v>
+        <v>26</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="0">
-        <v>91</v>
+        <v>35</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="C13" s="0" t="s">
         <v>6</v>
@@ -724,15 +724,15 @@
         <v>7</v>
       </c>
       <c r="E13" s="0" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="0">
-        <v>35</v>
+        <v>79</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C14" s="0" t="s">
         <v>6</v>
@@ -741,15 +741,15 @@
         <v>7</v>
       </c>
       <c r="E14" s="0" t="s">
-        <v>28</v>
+        <v>17</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="0">
-        <v>79</v>
+        <v>85</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C15" s="0" t="s">
         <v>6</v>
@@ -763,10 +763,10 @@
     </row>
     <row r="16">
       <c r="A16" s="0">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C16" s="0" t="s">
         <v>6</v>
@@ -780,10 +780,10 @@
     </row>
     <row r="17">
       <c r="A17" s="0">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C17" s="0" t="s">
         <v>6</v>
@@ -797,10 +797,10 @@
     </row>
     <row r="18">
       <c r="A18" s="0">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C18" s="0" t="s">
         <v>6</v>
@@ -814,10 +814,10 @@
     </row>
     <row r="19">
       <c r="A19" s="0">
-        <v>78</v>
+        <v>52</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C19" s="0" t="s">
         <v>6</v>
@@ -826,15 +826,15 @@
         <v>7</v>
       </c>
       <c r="E19" s="0" t="s">
-        <v>17</v>
+        <v>8</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="0">
-        <v>52</v>
+        <v>27</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C20" s="0" t="s">
         <v>6</v>
@@ -843,15 +843,15 @@
         <v>7</v>
       </c>
       <c r="E20" s="0" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="0">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C21" s="0" t="s">
         <v>6</v>
@@ -865,10 +865,10 @@
     </row>
     <row r="22">
       <c r="A22" s="0">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C22" s="0" t="s">
         <v>6</v>
@@ -882,10 +882,10 @@
     </row>
     <row r="23">
       <c r="A23" s="0">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C23" s="0" t="s">
         <v>6</v>
@@ -899,10 +899,10 @@
     </row>
     <row r="24">
       <c r="A24" s="0">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C24" s="0" t="s">
         <v>6</v>
@@ -916,10 +916,10 @@
     </row>
     <row r="25">
       <c r="A25" s="0">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C25" s="0" t="s">
         <v>6</v>
@@ -933,10 +933,10 @@
     </row>
     <row r="26">
       <c r="A26" s="0">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C26" s="0" t="s">
         <v>6</v>
@@ -950,10 +950,10 @@
     </row>
     <row r="27">
       <c r="A27" s="0">
-        <v>18</v>
+        <v>99</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>41</v>
+        <v>115</v>
       </c>
       <c r="C27" s="0" t="s">
         <v>6</v>
@@ -962,15 +962,15 @@
         <v>7</v>
       </c>
       <c r="E27" s="0" t="s">
-        <v>15</v>
+        <v>26</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="0">
-        <v>99</v>
+        <v>81</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>115</v>
+        <v>42</v>
       </c>
       <c r="C28" s="0" t="s">
         <v>6</v>
@@ -979,15 +979,15 @@
         <v>7</v>
       </c>
       <c r="E28" s="0" t="s">
-        <v>26</v>
+        <v>17</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="0">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C29" s="0" t="s">
         <v>6</v>
@@ -1001,10 +1001,10 @@
     </row>
     <row r="30">
       <c r="A30" s="0">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="B30" s="0" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C30" s="0" t="s">
         <v>6</v>
@@ -1018,10 +1018,10 @@
     </row>
     <row r="31">
       <c r="A31" s="0">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B31" s="0" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C31" s="0" t="s">
         <v>6</v>
@@ -1035,10 +1035,10 @@
     </row>
     <row r="32">
       <c r="A32" s="0">
-        <v>84</v>
+        <v>25</v>
       </c>
       <c r="B32" s="0" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C32" s="0" t="s">
         <v>6</v>
@@ -1047,15 +1047,15 @@
         <v>7</v>
       </c>
       <c r="E32" s="0" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="0">
-        <v>25</v>
+        <v>57</v>
       </c>
       <c r="B33" s="0" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C33" s="0" t="s">
         <v>6</v>
@@ -1064,15 +1064,15 @@
         <v>7</v>
       </c>
       <c r="E33" s="0" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="0">
-        <v>57</v>
+        <v>65</v>
       </c>
       <c r="B34" s="0" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C34" s="0" t="s">
         <v>6</v>
@@ -1086,10 +1086,10 @@
     </row>
     <row r="35">
       <c r="A35" s="0">
-        <v>65</v>
+        <v>58</v>
       </c>
       <c r="B35" s="0" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C35" s="0" t="s">
         <v>6</v>
@@ -1103,10 +1103,10 @@
     </row>
     <row r="36">
       <c r="A36" s="0">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="B36" s="0" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C36" s="0" t="s">
         <v>6</v>
@@ -1120,10 +1120,10 @@
     </row>
     <row r="37">
       <c r="A37" s="0">
-        <v>61</v>
+        <v>26</v>
       </c>
       <c r="B37" s="0" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C37" s="0" t="s">
         <v>6</v>
@@ -1132,15 +1132,15 @@
         <v>7</v>
       </c>
       <c r="E37" s="0" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="0">
-        <v>26</v>
+        <v>43</v>
       </c>
       <c r="B38" s="0" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C38" s="0" t="s">
         <v>6</v>
@@ -1149,15 +1149,15 @@
         <v>7</v>
       </c>
       <c r="E38" s="0" t="s">
-        <v>15</v>
+        <v>53</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="0">
-        <v>43</v>
+        <v>74</v>
       </c>
       <c r="B39" s="0" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="C39" s="0" t="s">
         <v>6</v>
@@ -1166,15 +1166,15 @@
         <v>7</v>
       </c>
       <c r="E39" s="0" t="s">
-        <v>53</v>
+        <v>17</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="0">
-        <v>74</v>
+        <v>29</v>
       </c>
       <c r="B40" s="0" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C40" s="0" t="s">
         <v>6</v>
@@ -1183,15 +1183,15 @@
         <v>7</v>
       </c>
       <c r="E40" s="0" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="0">
-        <v>29</v>
+        <v>47</v>
       </c>
       <c r="B41" s="0" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C41" s="0" t="s">
         <v>6</v>
@@ -1200,15 +1200,15 @@
         <v>7</v>
       </c>
       <c r="E41" s="0" t="s">
-        <v>15</v>
+        <v>57</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="0">
-        <v>47</v>
+        <v>60</v>
       </c>
       <c r="B42" s="0" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="C42" s="0" t="s">
         <v>6</v>
@@ -1217,23 +1217,6 @@
         <v>7</v>
       </c>
       <c r="E42" s="0" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="43">
-      <c r="A43" s="0">
-        <v>60</v>
-      </c>
-      <c r="B43" s="0" t="s">
-        <v>58</v>
-      </c>
-      <c r="C43" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="D43" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="E43" s="0" t="s">
         <v>17</v>
       </c>
     </row>
@@ -1244,7 +1227,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:F48"/>
+  <dimension ref="A1:F49"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1272,10 +1255,10 @@
     </row>
     <row r="2">
       <c r="A2" s="0">
-        <v>21</v>
+        <v>97</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="C2" s="0" t="s">
         <v>59</v>
@@ -1284,7 +1267,7 @@
         <v>7</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>15</v>
+        <v>26</v>
       </c>
       <c r="F2" s="0" t="s">
         <v>26</v>
@@ -1292,10 +1275,10 @@
     </row>
     <row r="3">
       <c r="A3" s="0">
-        <v>100</v>
+        <v>21</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="C3" s="0" t="s">
         <v>59</v>
@@ -1304,7 +1287,7 @@
         <v>7</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>26</v>
+        <v>15</v>
       </c>
       <c r="F3" s="0" t="s">
         <v>26</v>
@@ -1312,10 +1295,10 @@
     </row>
     <row r="4">
       <c r="A4" s="0">
-        <v>87</v>
+        <v>100</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="C4" s="0" t="s">
         <v>59</v>
@@ -1324,7 +1307,7 @@
         <v>7</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>12</v>
+        <v>26</v>
       </c>
       <c r="F4" s="0" t="s">
         <v>26</v>
@@ -1332,10 +1315,10 @@
     </row>
     <row r="5">
       <c r="A5" s="0">
-        <v>94</v>
+        <v>87</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="C5" s="0" t="s">
         <v>59</v>
@@ -1344,7 +1327,7 @@
         <v>7</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>26</v>
+        <v>12</v>
       </c>
       <c r="F5" s="0" t="s">
         <v>26</v>
@@ -1352,10 +1335,10 @@
     </row>
     <row r="6">
       <c r="A6" s="0">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
       <c r="C6" s="0" t="s">
         <v>59</v>
@@ -1372,10 +1355,10 @@
     </row>
     <row r="7">
       <c r="A7" s="0">
-        <v>34</v>
+        <v>93</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>9</v>
+        <v>110</v>
       </c>
       <c r="C7" s="0" t="s">
         <v>59</v>
@@ -1384,7 +1367,7 @@
         <v>7</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>10</v>
+        <v>26</v>
       </c>
       <c r="F7" s="0" t="s">
         <v>26</v>
@@ -1392,10 +1375,10 @@
     </row>
     <row r="8">
       <c r="A8" s="0">
-        <v>50</v>
+        <v>34</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="C8" s="0" t="s">
         <v>59</v>
@@ -1404,7 +1387,7 @@
         <v>7</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="F8" s="0" t="s">
         <v>26</v>
@@ -1412,10 +1395,10 @@
     </row>
     <row r="9">
       <c r="A9" s="0">
-        <v>89</v>
+        <v>50</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>60</v>
+        <v>5</v>
       </c>
       <c r="C9" s="0" t="s">
         <v>59</v>
@@ -1424,18 +1407,18 @@
         <v>7</v>
       </c>
       <c r="E9" s="0" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="F9" s="0" t="s">
-        <v>12</v>
+        <v>26</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="0">
-        <v>59</v>
+        <v>89</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C10" s="0" t="s">
         <v>59</v>
@@ -1444,7 +1427,7 @@
         <v>7</v>
       </c>
       <c r="E10" s="0" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="F10" s="0" t="s">
         <v>12</v>
@@ -1452,10 +1435,10 @@
     </row>
     <row r="11">
       <c r="A11" s="0">
-        <v>69</v>
+        <v>59</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C11" s="0" t="s">
         <v>59</v>
@@ -1472,10 +1455,10 @@
     </row>
     <row r="12">
       <c r="A12" s="0">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C12" s="0" t="s">
         <v>59</v>
@@ -1492,10 +1475,10 @@
     </row>
     <row r="13">
       <c r="A13" s="0">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C13" s="0" t="s">
         <v>59</v>
@@ -1512,10 +1495,10 @@
     </row>
     <row r="14">
       <c r="A14" s="0">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C14" s="0" t="s">
         <v>59</v>
@@ -1527,15 +1510,15 @@
         <v>17</v>
       </c>
       <c r="F14" s="0" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="0">
-        <v>24</v>
+        <v>71</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C15" s="0" t="s">
         <v>59</v>
@@ -1544,7 +1527,7 @@
         <v>7</v>
       </c>
       <c r="E15" s="0" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="F15" s="0" t="s">
         <v>17</v>
@@ -1552,10 +1535,10 @@
     </row>
     <row r="16">
       <c r="A16" s="0">
-        <v>75</v>
+        <v>24</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C16" s="0" t="s">
         <v>59</v>
@@ -1564,7 +1547,7 @@
         <v>7</v>
       </c>
       <c r="E16" s="0" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="F16" s="0" t="s">
         <v>17</v>
@@ -1572,10 +1555,10 @@
     </row>
     <row r="17">
       <c r="A17" s="0">
-        <v>55</v>
+        <v>75</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C17" s="0" t="s">
         <v>59</v>
@@ -1584,7 +1567,7 @@
         <v>7</v>
       </c>
       <c r="E17" s="0" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="F17" s="0" t="s">
         <v>17</v>
@@ -1592,10 +1575,10 @@
     </row>
     <row r="18">
       <c r="A18" s="0">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C18" s="0" t="s">
         <v>59</v>
@@ -1612,10 +1595,10 @@
     </row>
     <row r="19">
       <c r="A19" s="0">
-        <v>72</v>
+        <v>56</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C19" s="0" t="s">
         <v>59</v>
@@ -1624,7 +1607,7 @@
         <v>7</v>
       </c>
       <c r="E19" s="0" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="F19" s="0" t="s">
         <v>17</v>
@@ -1632,10 +1615,10 @@
     </row>
     <row r="20">
       <c r="A20" s="0">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C20" s="0" t="s">
         <v>59</v>
@@ -1652,10 +1635,10 @@
     </row>
     <row r="21">
       <c r="A21" s="0">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C21" s="0" t="s">
         <v>59</v>
@@ -1672,10 +1655,10 @@
     </row>
     <row r="22">
       <c r="A22" s="0">
-        <v>70</v>
+        <v>62</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C22" s="0" t="s">
         <v>59</v>
@@ -1692,10 +1675,10 @@
     </row>
     <row r="23">
       <c r="A23" s="0">
-        <v>64</v>
+        <v>70</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C23" s="0" t="s">
         <v>59</v>
@@ -1712,10 +1695,10 @@
     </row>
     <row r="24">
       <c r="A24" s="0">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C24" s="0" t="s">
         <v>59</v>
@@ -1732,10 +1715,10 @@
     </row>
     <row r="25">
       <c r="A25" s="0">
-        <v>13</v>
+        <v>63</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C25" s="0" t="s">
         <v>59</v>
@@ -1744,7 +1727,7 @@
         <v>7</v>
       </c>
       <c r="E25" s="0" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="F25" s="0" t="s">
         <v>17</v>
@@ -1752,10 +1735,10 @@
     </row>
     <row r="26">
       <c r="A26" s="0">
-        <v>42</v>
+        <v>13</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C26" s="0" t="s">
         <v>59</v>
@@ -1764,18 +1747,18 @@
         <v>7</v>
       </c>
       <c r="E26" s="0" t="s">
-        <v>53</v>
+        <v>15</v>
       </c>
       <c r="F26" s="0" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="0">
-        <v>33</v>
+        <v>42</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C27" s="0" t="s">
         <v>59</v>
@@ -1784,7 +1767,7 @@
         <v>7</v>
       </c>
       <c r="E27" s="0" t="s">
-        <v>10</v>
+        <v>53</v>
       </c>
       <c r="F27" s="0" t="s">
         <v>19</v>
@@ -1792,10 +1775,10 @@
     </row>
     <row r="28">
       <c r="A28" s="0">
-        <v>48</v>
+        <v>33</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C28" s="0" t="s">
         <v>59</v>
@@ -1804,18 +1787,18 @@
         <v>7</v>
       </c>
       <c r="E28" s="0" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="F28" s="0" t="s">
-        <v>8</v>
+        <v>19</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="0">
-        <v>37</v>
+        <v>48</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C29" s="0" t="s">
         <v>59</v>
@@ -1824,7 +1807,7 @@
         <v>7</v>
       </c>
       <c r="E29" s="0" t="s">
-        <v>28</v>
+        <v>8</v>
       </c>
       <c r="F29" s="0" t="s">
         <v>8</v>
@@ -1832,10 +1815,10 @@
     </row>
     <row r="30">
       <c r="A30" s="0">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B30" s="0" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C30" s="0" t="s">
         <v>59</v>
@@ -1847,15 +1830,15 @@
         <v>28</v>
       </c>
       <c r="F30" s="0" t="s">
-        <v>57</v>
+        <v>8</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="0">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="B31" s="0" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C31" s="0" t="s">
         <v>59</v>
@@ -1864,7 +1847,7 @@
         <v>7</v>
       </c>
       <c r="E31" s="0" t="s">
-        <v>83</v>
+        <v>28</v>
       </c>
       <c r="F31" s="0" t="s">
         <v>57</v>
@@ -1872,10 +1855,10 @@
     </row>
     <row r="32">
       <c r="A32" s="0">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B32" s="0" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C32" s="0" t="s">
         <v>59</v>
@@ -1884,7 +1867,7 @@
         <v>7</v>
       </c>
       <c r="E32" s="0" t="s">
-        <v>53</v>
+        <v>83</v>
       </c>
       <c r="F32" s="0" t="s">
         <v>57</v>
@@ -1892,10 +1875,10 @@
     </row>
     <row r="33">
       <c r="A33" s="0">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B33" s="0" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C33" s="0" t="s">
         <v>59</v>
@@ -1912,10 +1895,10 @@
     </row>
     <row r="34">
       <c r="A34" s="0">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="B34" s="0" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C34" s="0" t="s">
         <v>59</v>
@@ -1927,15 +1910,15 @@
         <v>53</v>
       </c>
       <c r="F34" s="0" t="s">
-        <v>83</v>
+        <v>57</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="0">
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="B35" s="0" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C35" s="0" t="s">
         <v>59</v>
@@ -1944,7 +1927,7 @@
         <v>7</v>
       </c>
       <c r="E35" s="0" t="s">
-        <v>28</v>
+        <v>53</v>
       </c>
       <c r="F35" s="0" t="s">
         <v>83</v>
@@ -1952,10 +1935,10 @@
     </row>
     <row r="36">
       <c r="A36" s="0">
-        <v>11</v>
+        <v>36</v>
       </c>
       <c r="B36" s="0" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C36" s="0" t="s">
         <v>59</v>
@@ -1964,18 +1947,18 @@
         <v>7</v>
       </c>
       <c r="E36" s="0" t="s">
-        <v>15</v>
+        <v>28</v>
       </c>
       <c r="F36" s="0" t="s">
-        <v>53</v>
+        <v>83</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="0">
-        <v>40</v>
+        <v>11</v>
       </c>
       <c r="B37" s="0" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C37" s="0" t="s">
         <v>59</v>
@@ -1984,7 +1967,7 @@
         <v>7</v>
       </c>
       <c r="E37" s="0" t="s">
-        <v>90</v>
+        <v>15</v>
       </c>
       <c r="F37" s="0" t="s">
         <v>53</v>
@@ -1992,10 +1975,10 @@
     </row>
     <row r="38">
       <c r="A38" s="0">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B38" s="0" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C38" s="0" t="s">
         <v>59</v>
@@ -2004,7 +1987,7 @@
         <v>7</v>
       </c>
       <c r="E38" s="0" t="s">
-        <v>28</v>
+        <v>90</v>
       </c>
       <c r="F38" s="0" t="s">
         <v>53</v>
@@ -2012,10 +1995,10 @@
     </row>
     <row r="39">
       <c r="A39" s="0">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="B39" s="0" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C39" s="0" t="s">
         <v>59</v>
@@ -2024,18 +2007,18 @@
         <v>7</v>
       </c>
       <c r="E39" s="0" t="s">
-        <v>10</v>
+        <v>28</v>
       </c>
       <c r="F39" s="0" t="s">
-        <v>28</v>
+        <v>53</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="0">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B40" s="0" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C40" s="0" t="s">
         <v>59</v>
@@ -2047,15 +2030,15 @@
         <v>10</v>
       </c>
       <c r="F40" s="0" t="s">
-        <v>10</v>
+        <v>28</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="0">
-        <v>20</v>
+        <v>31</v>
       </c>
       <c r="B41" s="0" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C41" s="0" t="s">
         <v>59</v>
@@ -2064,7 +2047,7 @@
         <v>7</v>
       </c>
       <c r="E41" s="0" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="F41" s="0" t="s">
         <v>10</v>
@@ -2072,10 +2055,10 @@
     </row>
     <row r="42">
       <c r="A42" s="0">
-        <v>9</v>
+        <v>20</v>
       </c>
       <c r="B42" s="0" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C42" s="0" t="s">
         <v>59</v>
@@ -2092,10 +2075,10 @@
     </row>
     <row r="43">
       <c r="A43" s="0">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B43" s="0" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C43" s="0" t="s">
         <v>59</v>
@@ -2112,10 +2095,10 @@
     </row>
     <row r="44">
       <c r="A44" s="0">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="B44" s="0" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C44" s="0" t="s">
         <v>59</v>
@@ -2127,15 +2110,15 @@
         <v>15</v>
       </c>
       <c r="F44" s="0" t="s">
-        <v>98</v>
+        <v>10</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" s="0">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B45" s="0" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C45" s="0" t="s">
         <v>59</v>
@@ -2147,15 +2130,15 @@
         <v>15</v>
       </c>
       <c r="F45" s="0" t="s">
-        <v>15</v>
+        <v>98</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" s="0">
-        <v>30</v>
+        <v>3</v>
       </c>
       <c r="B46" s="0" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C46" s="0" t="s">
         <v>59</v>
@@ -2172,10 +2155,10 @@
     </row>
     <row r="47">
       <c r="A47" s="0">
-        <v>2</v>
+        <v>30</v>
       </c>
       <c r="B47" s="0" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C47" s="0" t="s">
         <v>59</v>
@@ -2192,21 +2175,41 @@
     </row>
     <row r="48">
       <c r="A48" s="0">
+        <v>2</v>
+      </c>
+      <c r="B48" s="0" t="s">
+        <v>101</v>
+      </c>
+      <c r="C48" s="0" t="s">
+        <v>59</v>
+      </c>
+      <c r="D48" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E48" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="F48" s="0" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" s="0">
         <v>1</v>
       </c>
-      <c r="B48" s="0" t="s">
+      <c r="B49" s="0" t="s">
         <v>102</v>
       </c>
-      <c r="C48" s="0" t="s">
-        <v>59</v>
-      </c>
-      <c r="D48" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="E48" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="F48" s="0" t="s">
+      <c r="C49" s="0" t="s">
+        <v>59</v>
+      </c>
+      <c r="D49" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E49" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="F49" s="0" t="s">
         <v>15</v>
       </c>
     </row>

</xml_diff>

<commit_message>
bug fix: don't try to load palette with no filename
</commit_message>
<xml_diff>
--- a/paint_todo.xlsx
+++ b/paint_todo.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="120">
   <si>
     <t>Id</t>
   </si>
@@ -447,6 +447,9 @@
     <t xml:space="preserve">when resizing windows, default behavior is to keep the same section of image in the viewing pane
 - so expanding window would in effect zoom in
 CANCELLED</t>
+  </si>
+  <si>
+    <t>walk through Edit Palette panels and events and make sure its all right</t>
   </si>
 </sst>
 </file>
@@ -525,10 +528,10 @@
     </row>
     <row r="2">
       <c r="A2" s="0">
-        <v>86</v>
+        <v>54</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C2" s="0" t="s">
         <v>6</v>
@@ -537,15 +540,15 @@
         <v>7</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="0">
-        <v>54</v>
+        <v>88</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C3" s="0" t="s">
         <v>6</v>
@@ -554,15 +557,15 @@
         <v>7</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="0">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C4" s="0" t="s">
         <v>6</v>
@@ -576,10 +579,10 @@
     </row>
     <row r="5">
       <c r="A5" s="0">
-        <v>90</v>
+        <v>95</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>21</v>
+        <v>112</v>
       </c>
       <c r="C5" s="0" t="s">
         <v>6</v>
@@ -588,15 +591,15 @@
         <v>7</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>12</v>
+        <v>26</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="0">
-        <v>95</v>
+        <v>53</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>112</v>
+        <v>22</v>
       </c>
       <c r="C6" s="0" t="s">
         <v>6</v>
@@ -605,15 +608,15 @@
         <v>7</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="0">
-        <v>53</v>
+        <v>92</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>22</v>
+        <v>109</v>
       </c>
       <c r="C7" s="0" t="s">
         <v>6</v>
@@ -622,15 +625,15 @@
         <v>7</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="0">
-        <v>92</v>
+        <v>101</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>109</v>
+        <v>119</v>
       </c>
       <c r="C8" s="0" t="s">
         <v>6</v>
@@ -1227,7 +1230,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:F49"/>
+  <dimension ref="A1:F50"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1255,10 +1258,10 @@
     </row>
     <row r="2">
       <c r="A2" s="0">
-        <v>97</v>
+        <v>86</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>114</v>
+        <v>16</v>
       </c>
       <c r="C2" s="0" t="s">
         <v>59</v>
@@ -1267,7 +1270,7 @@
         <v>7</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>26</v>
+        <v>17</v>
       </c>
       <c r="F2" s="0" t="s">
         <v>26</v>
@@ -1275,10 +1278,10 @@
     </row>
     <row r="3">
       <c r="A3" s="0">
-        <v>21</v>
+        <v>97</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="C3" s="0" t="s">
         <v>59</v>
@@ -1287,7 +1290,7 @@
         <v>7</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>15</v>
+        <v>26</v>
       </c>
       <c r="F3" s="0" t="s">
         <v>26</v>
@@ -1295,10 +1298,10 @@
     </row>
     <row r="4">
       <c r="A4" s="0">
-        <v>100</v>
+        <v>21</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="C4" s="0" t="s">
         <v>59</v>
@@ -1307,7 +1310,7 @@
         <v>7</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>26</v>
+        <v>15</v>
       </c>
       <c r="F4" s="0" t="s">
         <v>26</v>
@@ -1315,10 +1318,10 @@
     </row>
     <row r="5">
       <c r="A5" s="0">
-        <v>87</v>
+        <v>100</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="C5" s="0" t="s">
         <v>59</v>
@@ -1327,7 +1330,7 @@
         <v>7</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>12</v>
+        <v>26</v>
       </c>
       <c r="F5" s="0" t="s">
         <v>26</v>
@@ -1335,10 +1338,10 @@
     </row>
     <row r="6">
       <c r="A6" s="0">
-        <v>94</v>
+        <v>87</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="C6" s="0" t="s">
         <v>59</v>
@@ -1347,7 +1350,7 @@
         <v>7</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>26</v>
+        <v>12</v>
       </c>
       <c r="F6" s="0" t="s">
         <v>26</v>
@@ -1355,10 +1358,10 @@
     </row>
     <row r="7">
       <c r="A7" s="0">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
       <c r="C7" s="0" t="s">
         <v>59</v>
@@ -1375,10 +1378,10 @@
     </row>
     <row r="8">
       <c r="A8" s="0">
-        <v>34</v>
+        <v>93</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>9</v>
+        <v>110</v>
       </c>
       <c r="C8" s="0" t="s">
         <v>59</v>
@@ -1387,7 +1390,7 @@
         <v>7</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>10</v>
+        <v>26</v>
       </c>
       <c r="F8" s="0" t="s">
         <v>26</v>
@@ -1395,10 +1398,10 @@
     </row>
     <row r="9">
       <c r="A9" s="0">
-        <v>50</v>
+        <v>34</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="C9" s="0" t="s">
         <v>59</v>
@@ -1407,7 +1410,7 @@
         <v>7</v>
       </c>
       <c r="E9" s="0" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="F9" s="0" t="s">
         <v>26</v>
@@ -1415,10 +1418,10 @@
     </row>
     <row r="10">
       <c r="A10" s="0">
-        <v>89</v>
+        <v>50</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>60</v>
+        <v>5</v>
       </c>
       <c r="C10" s="0" t="s">
         <v>59</v>
@@ -1427,18 +1430,18 @@
         <v>7</v>
       </c>
       <c r="E10" s="0" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="F10" s="0" t="s">
-        <v>12</v>
+        <v>26</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="0">
-        <v>59</v>
+        <v>89</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C11" s="0" t="s">
         <v>59</v>
@@ -1447,7 +1450,7 @@
         <v>7</v>
       </c>
       <c r="E11" s="0" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="F11" s="0" t="s">
         <v>12</v>
@@ -1455,10 +1458,10 @@
     </row>
     <row r="12">
       <c r="A12" s="0">
-        <v>69</v>
+        <v>59</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C12" s="0" t="s">
         <v>59</v>
@@ -1475,10 +1478,10 @@
     </row>
     <row r="13">
       <c r="A13" s="0">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C13" s="0" t="s">
         <v>59</v>
@@ -1495,10 +1498,10 @@
     </row>
     <row r="14">
       <c r="A14" s="0">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C14" s="0" t="s">
         <v>59</v>
@@ -1515,10 +1518,10 @@
     </row>
     <row r="15">
       <c r="A15" s="0">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C15" s="0" t="s">
         <v>59</v>
@@ -1530,15 +1533,15 @@
         <v>17</v>
       </c>
       <c r="F15" s="0" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="0">
-        <v>24</v>
+        <v>71</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C16" s="0" t="s">
         <v>59</v>
@@ -1547,7 +1550,7 @@
         <v>7</v>
       </c>
       <c r="E16" s="0" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="F16" s="0" t="s">
         <v>17</v>
@@ -1555,10 +1558,10 @@
     </row>
     <row r="17">
       <c r="A17" s="0">
-        <v>75</v>
+        <v>24</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C17" s="0" t="s">
         <v>59</v>
@@ -1567,7 +1570,7 @@
         <v>7</v>
       </c>
       <c r="E17" s="0" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="F17" s="0" t="s">
         <v>17</v>
@@ -1575,10 +1578,10 @@
     </row>
     <row r="18">
       <c r="A18" s="0">
-        <v>55</v>
+        <v>75</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C18" s="0" t="s">
         <v>59</v>
@@ -1587,7 +1590,7 @@
         <v>7</v>
       </c>
       <c r="E18" s="0" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="F18" s="0" t="s">
         <v>17</v>
@@ -1595,10 +1598,10 @@
     </row>
     <row r="19">
       <c r="A19" s="0">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C19" s="0" t="s">
         <v>59</v>
@@ -1615,10 +1618,10 @@
     </row>
     <row r="20">
       <c r="A20" s="0">
-        <v>72</v>
+        <v>56</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C20" s="0" t="s">
         <v>59</v>
@@ -1627,7 +1630,7 @@
         <v>7</v>
       </c>
       <c r="E20" s="0" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="F20" s="0" t="s">
         <v>17</v>
@@ -1635,10 +1638,10 @@
     </row>
     <row r="21">
       <c r="A21" s="0">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C21" s="0" t="s">
         <v>59</v>
@@ -1655,10 +1658,10 @@
     </row>
     <row r="22">
       <c r="A22" s="0">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C22" s="0" t="s">
         <v>59</v>
@@ -1675,10 +1678,10 @@
     </row>
     <row r="23">
       <c r="A23" s="0">
-        <v>70</v>
+        <v>62</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C23" s="0" t="s">
         <v>59</v>
@@ -1695,10 +1698,10 @@
     </row>
     <row r="24">
       <c r="A24" s="0">
-        <v>64</v>
+        <v>70</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C24" s="0" t="s">
         <v>59</v>
@@ -1715,10 +1718,10 @@
     </row>
     <row r="25">
       <c r="A25" s="0">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C25" s="0" t="s">
         <v>59</v>
@@ -1735,10 +1738,10 @@
     </row>
     <row r="26">
       <c r="A26" s="0">
-        <v>13</v>
+        <v>63</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C26" s="0" t="s">
         <v>59</v>
@@ -1747,7 +1750,7 @@
         <v>7</v>
       </c>
       <c r="E26" s="0" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="F26" s="0" t="s">
         <v>17</v>
@@ -1755,10 +1758,10 @@
     </row>
     <row r="27">
       <c r="A27" s="0">
-        <v>42</v>
+        <v>13</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C27" s="0" t="s">
         <v>59</v>
@@ -1767,18 +1770,18 @@
         <v>7</v>
       </c>
       <c r="E27" s="0" t="s">
-        <v>53</v>
+        <v>15</v>
       </c>
       <c r="F27" s="0" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="0">
-        <v>33</v>
+        <v>42</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C28" s="0" t="s">
         <v>59</v>
@@ -1787,7 +1790,7 @@
         <v>7</v>
       </c>
       <c r="E28" s="0" t="s">
-        <v>10</v>
+        <v>53</v>
       </c>
       <c r="F28" s="0" t="s">
         <v>19</v>
@@ -1795,10 +1798,10 @@
     </row>
     <row r="29">
       <c r="A29" s="0">
-        <v>48</v>
+        <v>33</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C29" s="0" t="s">
         <v>59</v>
@@ -1807,18 +1810,18 @@
         <v>7</v>
       </c>
       <c r="E29" s="0" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="F29" s="0" t="s">
-        <v>8</v>
+        <v>19</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="0">
-        <v>37</v>
+        <v>48</v>
       </c>
       <c r="B30" s="0" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C30" s="0" t="s">
         <v>59</v>
@@ -1827,7 +1830,7 @@
         <v>7</v>
       </c>
       <c r="E30" s="0" t="s">
-        <v>28</v>
+        <v>8</v>
       </c>
       <c r="F30" s="0" t="s">
         <v>8</v>
@@ -1835,10 +1838,10 @@
     </row>
     <row r="31">
       <c r="A31" s="0">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B31" s="0" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C31" s="0" t="s">
         <v>59</v>
@@ -1850,15 +1853,15 @@
         <v>28</v>
       </c>
       <c r="F31" s="0" t="s">
-        <v>57</v>
+        <v>8</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="0">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="B32" s="0" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C32" s="0" t="s">
         <v>59</v>
@@ -1867,7 +1870,7 @@
         <v>7</v>
       </c>
       <c r="E32" s="0" t="s">
-        <v>83</v>
+        <v>28</v>
       </c>
       <c r="F32" s="0" t="s">
         <v>57</v>
@@ -1875,10 +1878,10 @@
     </row>
     <row r="33">
       <c r="A33" s="0">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B33" s="0" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C33" s="0" t="s">
         <v>59</v>
@@ -1887,7 +1890,7 @@
         <v>7</v>
       </c>
       <c r="E33" s="0" t="s">
-        <v>53</v>
+        <v>83</v>
       </c>
       <c r="F33" s="0" t="s">
         <v>57</v>
@@ -1895,10 +1898,10 @@
     </row>
     <row r="34">
       <c r="A34" s="0">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B34" s="0" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C34" s="0" t="s">
         <v>59</v>
@@ -1915,10 +1918,10 @@
     </row>
     <row r="35">
       <c r="A35" s="0">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="B35" s="0" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C35" s="0" t="s">
         <v>59</v>
@@ -1930,15 +1933,15 @@
         <v>53</v>
       </c>
       <c r="F35" s="0" t="s">
-        <v>83</v>
+        <v>57</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="0">
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="B36" s="0" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C36" s="0" t="s">
         <v>59</v>
@@ -1947,7 +1950,7 @@
         <v>7</v>
       </c>
       <c r="E36" s="0" t="s">
-        <v>28</v>
+        <v>53</v>
       </c>
       <c r="F36" s="0" t="s">
         <v>83</v>
@@ -1955,10 +1958,10 @@
     </row>
     <row r="37">
       <c r="A37" s="0">
-        <v>11</v>
+        <v>36</v>
       </c>
       <c r="B37" s="0" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C37" s="0" t="s">
         <v>59</v>
@@ -1967,18 +1970,18 @@
         <v>7</v>
       </c>
       <c r="E37" s="0" t="s">
-        <v>15</v>
+        <v>28</v>
       </c>
       <c r="F37" s="0" t="s">
-        <v>53</v>
+        <v>83</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="0">
-        <v>40</v>
+        <v>11</v>
       </c>
       <c r="B38" s="0" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C38" s="0" t="s">
         <v>59</v>
@@ -1987,7 +1990,7 @@
         <v>7</v>
       </c>
       <c r="E38" s="0" t="s">
-        <v>90</v>
+        <v>15</v>
       </c>
       <c r="F38" s="0" t="s">
         <v>53</v>
@@ -1995,10 +1998,10 @@
     </row>
     <row r="39">
       <c r="A39" s="0">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B39" s="0" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C39" s="0" t="s">
         <v>59</v>
@@ -2007,7 +2010,7 @@
         <v>7</v>
       </c>
       <c r="E39" s="0" t="s">
-        <v>28</v>
+        <v>90</v>
       </c>
       <c r="F39" s="0" t="s">
         <v>53</v>
@@ -2015,10 +2018,10 @@
     </row>
     <row r="40">
       <c r="A40" s="0">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="B40" s="0" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C40" s="0" t="s">
         <v>59</v>
@@ -2027,18 +2030,18 @@
         <v>7</v>
       </c>
       <c r="E40" s="0" t="s">
-        <v>10</v>
+        <v>28</v>
       </c>
       <c r="F40" s="0" t="s">
-        <v>28</v>
+        <v>53</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="0">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B41" s="0" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C41" s="0" t="s">
         <v>59</v>
@@ -2050,15 +2053,15 @@
         <v>10</v>
       </c>
       <c r="F41" s="0" t="s">
-        <v>10</v>
+        <v>28</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="0">
-        <v>20</v>
+        <v>31</v>
       </c>
       <c r="B42" s="0" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C42" s="0" t="s">
         <v>59</v>
@@ -2067,7 +2070,7 @@
         <v>7</v>
       </c>
       <c r="E42" s="0" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="F42" s="0" t="s">
         <v>10</v>
@@ -2075,10 +2078,10 @@
     </row>
     <row r="43">
       <c r="A43" s="0">
-        <v>9</v>
+        <v>20</v>
       </c>
       <c r="B43" s="0" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C43" s="0" t="s">
         <v>59</v>
@@ -2095,10 +2098,10 @@
     </row>
     <row r="44">
       <c r="A44" s="0">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B44" s="0" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C44" s="0" t="s">
         <v>59</v>
@@ -2115,10 +2118,10 @@
     </row>
     <row r="45">
       <c r="A45" s="0">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="B45" s="0" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C45" s="0" t="s">
         <v>59</v>
@@ -2130,15 +2133,15 @@
         <v>15</v>
       </c>
       <c r="F45" s="0" t="s">
-        <v>98</v>
+        <v>10</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" s="0">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B46" s="0" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C46" s="0" t="s">
         <v>59</v>
@@ -2150,15 +2153,15 @@
         <v>15</v>
       </c>
       <c r="F46" s="0" t="s">
-        <v>15</v>
+        <v>98</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" s="0">
-        <v>30</v>
+        <v>3</v>
       </c>
       <c r="B47" s="0" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C47" s="0" t="s">
         <v>59</v>
@@ -2175,10 +2178,10 @@
     </row>
     <row r="48">
       <c r="A48" s="0">
-        <v>2</v>
+        <v>30</v>
       </c>
       <c r="B48" s="0" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C48" s="0" t="s">
         <v>59</v>
@@ -2195,21 +2198,41 @@
     </row>
     <row r="49">
       <c r="A49" s="0">
+        <v>2</v>
+      </c>
+      <c r="B49" s="0" t="s">
+        <v>101</v>
+      </c>
+      <c r="C49" s="0" t="s">
+        <v>59</v>
+      </c>
+      <c r="D49" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E49" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="F49" s="0" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" s="0">
         <v>1</v>
       </c>
-      <c r="B49" s="0" t="s">
+      <c r="B50" s="0" t="s">
         <v>102</v>
       </c>
-      <c r="C49" s="0" t="s">
-        <v>59</v>
-      </c>
-      <c r="D49" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="E49" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="F49" s="0" t="s">
+      <c r="C50" s="0" t="s">
+        <v>59</v>
+      </c>
+      <c r="D50" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E50" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="F50" s="0" t="s">
         <v>15</v>
       </c>
     </row>
@@ -2253,7 +2276,7 @@
         <v>7</v>
       </c>
       <c r="F2" s="0">
-        <v>100</v>
+        <v>101</v>
       </c>
     </row>
     <row r="3">

</xml_diff>

<commit_message>
refactor: consistent naming of setting properties
</commit_message>
<xml_diff>
--- a/paint_todo.xlsx
+++ b/paint_todo.xlsx
@@ -502,7 +502,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:F42"/>
+  <dimension ref="A1:F40"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -545,10 +545,10 @@
     </row>
     <row r="3">
       <c r="A3" s="0">
-        <v>88</v>
+        <v>95</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>20</v>
+        <v>112</v>
       </c>
       <c r="C3" s="0" t="s">
         <v>6</v>
@@ -557,15 +557,15 @@
         <v>7</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>12</v>
+        <v>26</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="0">
-        <v>90</v>
+        <v>53</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C4" s="0" t="s">
         <v>6</v>
@@ -574,15 +574,15 @@
         <v>7</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="0">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="C5" s="0" t="s">
         <v>6</v>
@@ -596,10 +596,10 @@
     </row>
     <row r="6">
       <c r="A6" s="0">
-        <v>53</v>
+        <v>101</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>22</v>
+        <v>119</v>
       </c>
       <c r="C6" s="0" t="s">
         <v>6</v>
@@ -608,15 +608,15 @@
         <v>7</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="0">
-        <v>92</v>
+        <v>51</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>109</v>
+        <v>23</v>
       </c>
       <c r="C7" s="0" t="s">
         <v>6</v>
@@ -625,15 +625,15 @@
         <v>7</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>26</v>
+        <v>8</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="0">
-        <v>101</v>
+        <v>76</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>119</v>
+        <v>24</v>
       </c>
       <c r="C8" s="0" t="s">
         <v>6</v>
@@ -642,15 +642,15 @@
         <v>7</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>26</v>
+        <v>17</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="0">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>23</v>
+        <v>13</v>
       </c>
       <c r="C9" s="0" t="s">
         <v>6</v>
@@ -664,10 +664,10 @@
     </row>
     <row r="10">
       <c r="A10" s="0">
-        <v>76</v>
+        <v>91</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C10" s="0" t="s">
         <v>6</v>
@@ -676,15 +676,15 @@
         <v>7</v>
       </c>
       <c r="E10" s="0" t="s">
-        <v>17</v>
+        <v>26</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="0">
-        <v>49</v>
+        <v>35</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>13</v>
+        <v>27</v>
       </c>
       <c r="C11" s="0" t="s">
         <v>6</v>
@@ -693,15 +693,15 @@
         <v>7</v>
       </c>
       <c r="E11" s="0" t="s">
-        <v>8</v>
+        <v>28</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="0">
-        <v>91</v>
+        <v>79</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="C12" s="0" t="s">
         <v>6</v>
@@ -710,15 +710,15 @@
         <v>7</v>
       </c>
       <c r="E12" s="0" t="s">
-        <v>26</v>
+        <v>17</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="0">
-        <v>35</v>
+        <v>85</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="C13" s="0" t="s">
         <v>6</v>
@@ -727,15 +727,15 @@
         <v>7</v>
       </c>
       <c r="E13" s="0" t="s">
-        <v>28</v>
+        <v>17</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="0">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="C14" s="0" t="s">
         <v>6</v>
@@ -749,10 +749,10 @@
     </row>
     <row r="15">
       <c r="A15" s="0">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="C15" s="0" t="s">
         <v>6</v>
@@ -766,10 +766,10 @@
     </row>
     <row r="16">
       <c r="A16" s="0">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="C16" s="0" t="s">
         <v>6</v>
@@ -783,10 +783,10 @@
     </row>
     <row r="17">
       <c r="A17" s="0">
-        <v>77</v>
+        <v>52</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C17" s="0" t="s">
         <v>6</v>
@@ -795,15 +795,15 @@
         <v>7</v>
       </c>
       <c r="E17" s="0" t="s">
-        <v>17</v>
+        <v>8</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="0">
-        <v>78</v>
+        <v>27</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="C18" s="0" t="s">
         <v>6</v>
@@ -812,15 +812,15 @@
         <v>7</v>
       </c>
       <c r="E18" s="0" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="0">
-        <v>52</v>
+        <v>28</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="C19" s="0" t="s">
         <v>6</v>
@@ -829,15 +829,15 @@
         <v>7</v>
       </c>
       <c r="E19" s="0" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="0">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="C20" s="0" t="s">
         <v>6</v>
@@ -851,10 +851,10 @@
     </row>
     <row r="21">
       <c r="A21" s="0">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="C21" s="0" t="s">
         <v>6</v>
@@ -868,10 +868,10 @@
     </row>
     <row r="22">
       <c r="A22" s="0">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="C22" s="0" t="s">
         <v>6</v>
@@ -885,10 +885,10 @@
     </row>
     <row r="23">
       <c r="A23" s="0">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="C23" s="0" t="s">
         <v>6</v>
@@ -902,10 +902,10 @@
     </row>
     <row r="24">
       <c r="A24" s="0">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C24" s="0" t="s">
         <v>6</v>
@@ -919,10 +919,10 @@
     </row>
     <row r="25">
       <c r="A25" s="0">
-        <v>17</v>
+        <v>99</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>40</v>
+        <v>115</v>
       </c>
       <c r="C25" s="0" t="s">
         <v>6</v>
@@ -931,15 +931,15 @@
         <v>7</v>
       </c>
       <c r="E25" s="0" t="s">
-        <v>15</v>
+        <v>26</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="0">
-        <v>18</v>
+        <v>81</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C26" s="0" t="s">
         <v>6</v>
@@ -948,15 +948,15 @@
         <v>7</v>
       </c>
       <c r="E26" s="0" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="0">
-        <v>99</v>
+        <v>82</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>115</v>
+        <v>43</v>
       </c>
       <c r="C27" s="0" t="s">
         <v>6</v>
@@ -965,15 +965,15 @@
         <v>7</v>
       </c>
       <c r="E27" s="0" t="s">
-        <v>26</v>
+        <v>17</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="0">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="C28" s="0" t="s">
         <v>6</v>
@@ -987,10 +987,10 @@
     </row>
     <row r="29">
       <c r="A29" s="0">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="C29" s="0" t="s">
         <v>6</v>
@@ -1004,10 +1004,10 @@
     </row>
     <row r="30">
       <c r="A30" s="0">
-        <v>83</v>
+        <v>25</v>
       </c>
       <c r="B30" s="0" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="C30" s="0" t="s">
         <v>6</v>
@@ -1016,15 +1016,15 @@
         <v>7</v>
       </c>
       <c r="E30" s="0" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="0">
-        <v>84</v>
+        <v>57</v>
       </c>
       <c r="B31" s="0" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="C31" s="0" t="s">
         <v>6</v>
@@ -1038,10 +1038,10 @@
     </row>
     <row r="32">
       <c r="A32" s="0">
-        <v>25</v>
+        <v>65</v>
       </c>
       <c r="B32" s="0" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="C32" s="0" t="s">
         <v>6</v>
@@ -1050,15 +1050,15 @@
         <v>7</v>
       </c>
       <c r="E32" s="0" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="0">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B33" s="0" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="C33" s="0" t="s">
         <v>6</v>
@@ -1072,10 +1072,10 @@
     </row>
     <row r="34">
       <c r="A34" s="0">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="B34" s="0" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="C34" s="0" t="s">
         <v>6</v>
@@ -1089,10 +1089,10 @@
     </row>
     <row r="35">
       <c r="A35" s="0">
-        <v>58</v>
+        <v>26</v>
       </c>
       <c r="B35" s="0" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="C35" s="0" t="s">
         <v>6</v>
@@ -1101,15 +1101,15 @@
         <v>7</v>
       </c>
       <c r="E35" s="0" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="0">
-        <v>61</v>
+        <v>43</v>
       </c>
       <c r="B36" s="0" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="C36" s="0" t="s">
         <v>6</v>
@@ -1118,15 +1118,15 @@
         <v>7</v>
       </c>
       <c r="E36" s="0" t="s">
-        <v>17</v>
+        <v>53</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="0">
-        <v>26</v>
+        <v>74</v>
       </c>
       <c r="B37" s="0" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="C37" s="0" t="s">
         <v>6</v>
@@ -1135,15 +1135,15 @@
         <v>7</v>
       </c>
       <c r="E37" s="0" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="0">
-        <v>43</v>
+        <v>29</v>
       </c>
       <c r="B38" s="0" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="C38" s="0" t="s">
         <v>6</v>
@@ -1152,15 +1152,15 @@
         <v>7</v>
       </c>
       <c r="E38" s="0" t="s">
-        <v>53</v>
+        <v>15</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="0">
-        <v>74</v>
+        <v>47</v>
       </c>
       <c r="B39" s="0" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="C39" s="0" t="s">
         <v>6</v>
@@ -1169,15 +1169,15 @@
         <v>7</v>
       </c>
       <c r="E39" s="0" t="s">
-        <v>17</v>
+        <v>57</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="0">
-        <v>29</v>
+        <v>60</v>
       </c>
       <c r="B40" s="0" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="C40" s="0" t="s">
         <v>6</v>
@@ -1186,40 +1186,6 @@
         <v>7</v>
       </c>
       <c r="E40" s="0" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="41">
-      <c r="A41" s="0">
-        <v>47</v>
-      </c>
-      <c r="B41" s="0" t="s">
-        <v>56</v>
-      </c>
-      <c r="C41" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="D41" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="E41" s="0" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="42">
-      <c r="A42" s="0">
-        <v>60</v>
-      </c>
-      <c r="B42" s="0" t="s">
-        <v>58</v>
-      </c>
-      <c r="C42" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="D42" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="E42" s="0" t="s">
         <v>17</v>
       </c>
     </row>
@@ -1230,7 +1196,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:F50"/>
+  <dimension ref="A1:F52"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1258,10 +1224,10 @@
     </row>
     <row r="2">
       <c r="A2" s="0">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="C2" s="0" t="s">
         <v>59</v>
@@ -1270,7 +1236,7 @@
         <v>7</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="F2" s="0" t="s">
         <v>26</v>
@@ -1278,10 +1244,10 @@
     </row>
     <row r="3">
       <c r="A3" s="0">
-        <v>97</v>
+        <v>88</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>114</v>
+        <v>20</v>
       </c>
       <c r="C3" s="0" t="s">
         <v>59</v>
@@ -1290,7 +1256,7 @@
         <v>7</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>26</v>
+        <v>12</v>
       </c>
       <c r="F3" s="0" t="s">
         <v>26</v>
@@ -1298,10 +1264,10 @@
     </row>
     <row r="4">
       <c r="A4" s="0">
-        <v>21</v>
+        <v>86</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>118</v>
+        <v>16</v>
       </c>
       <c r="C4" s="0" t="s">
         <v>59</v>
@@ -1310,7 +1276,7 @@
         <v>7</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="F4" s="0" t="s">
         <v>26</v>
@@ -1318,10 +1284,10 @@
     </row>
     <row r="5">
       <c r="A5" s="0">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="C5" s="0" t="s">
         <v>59</v>
@@ -1338,10 +1304,10 @@
     </row>
     <row r="6">
       <c r="A6" s="0">
-        <v>87</v>
+        <v>21</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="C6" s="0" t="s">
         <v>59</v>
@@ -1350,7 +1316,7 @@
         <v>7</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="F6" s="0" t="s">
         <v>26</v>
@@ -1358,10 +1324,10 @@
     </row>
     <row r="7">
       <c r="A7" s="0">
-        <v>94</v>
+        <v>100</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>113</v>
+        <v>117</v>
       </c>
       <c r="C7" s="0" t="s">
         <v>59</v>
@@ -1378,10 +1344,10 @@
     </row>
     <row r="8">
       <c r="A8" s="0">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>110</v>
+        <v>116</v>
       </c>
       <c r="C8" s="0" t="s">
         <v>59</v>
@@ -1390,7 +1356,7 @@
         <v>7</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>26</v>
+        <v>12</v>
       </c>
       <c r="F8" s="0" t="s">
         <v>26</v>
@@ -1398,10 +1364,10 @@
     </row>
     <row r="9">
       <c r="A9" s="0">
-        <v>34</v>
+        <v>94</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>9</v>
+        <v>113</v>
       </c>
       <c r="C9" s="0" t="s">
         <v>59</v>
@@ -1410,7 +1376,7 @@
         <v>7</v>
       </c>
       <c r="E9" s="0" t="s">
-        <v>10</v>
+        <v>26</v>
       </c>
       <c r="F9" s="0" t="s">
         <v>26</v>
@@ -1418,10 +1384,10 @@
     </row>
     <row r="10">
       <c r="A10" s="0">
-        <v>50</v>
+        <v>93</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>5</v>
+        <v>110</v>
       </c>
       <c r="C10" s="0" t="s">
         <v>59</v>
@@ -1430,7 +1396,7 @@
         <v>7</v>
       </c>
       <c r="E10" s="0" t="s">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="F10" s="0" t="s">
         <v>26</v>
@@ -1438,10 +1404,10 @@
     </row>
     <row r="11">
       <c r="A11" s="0">
-        <v>89</v>
+        <v>34</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>60</v>
+        <v>9</v>
       </c>
       <c r="C11" s="0" t="s">
         <v>59</v>
@@ -1450,18 +1416,18 @@
         <v>7</v>
       </c>
       <c r="E11" s="0" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="F11" s="0" t="s">
-        <v>12</v>
+        <v>26</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="0">
-        <v>59</v>
+        <v>50</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>61</v>
+        <v>5</v>
       </c>
       <c r="C12" s="0" t="s">
         <v>59</v>
@@ -1470,18 +1436,18 @@
         <v>7</v>
       </c>
       <c r="E12" s="0" t="s">
-        <v>17</v>
+        <v>8</v>
       </c>
       <c r="F12" s="0" t="s">
-        <v>12</v>
+        <v>26</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="0">
-        <v>69</v>
+        <v>89</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C13" s="0" t="s">
         <v>59</v>
@@ -1490,7 +1456,7 @@
         <v>7</v>
       </c>
       <c r="E13" s="0" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="F13" s="0" t="s">
         <v>12</v>
@@ -1498,10 +1464,10 @@
     </row>
     <row r="14">
       <c r="A14" s="0">
-        <v>68</v>
+        <v>59</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C14" s="0" t="s">
         <v>59</v>
@@ -1518,10 +1484,10 @@
     </row>
     <row r="15">
       <c r="A15" s="0">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C15" s="0" t="s">
         <v>59</v>
@@ -1538,10 +1504,10 @@
     </row>
     <row r="16">
       <c r="A16" s="0">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C16" s="0" t="s">
         <v>59</v>
@@ -1553,15 +1519,15 @@
         <v>17</v>
       </c>
       <c r="F16" s="0" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="0">
-        <v>24</v>
+        <v>67</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C17" s="0" t="s">
         <v>59</v>
@@ -1570,18 +1536,18 @@
         <v>7</v>
       </c>
       <c r="E17" s="0" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="F17" s="0" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="0">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C18" s="0" t="s">
         <v>59</v>
@@ -1598,10 +1564,10 @@
     </row>
     <row r="19">
       <c r="A19" s="0">
-        <v>55</v>
+        <v>24</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C19" s="0" t="s">
         <v>59</v>
@@ -1610,7 +1576,7 @@
         <v>7</v>
       </c>
       <c r="E19" s="0" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="F19" s="0" t="s">
         <v>17</v>
@@ -1618,10 +1584,10 @@
     </row>
     <row r="20">
       <c r="A20" s="0">
-        <v>56</v>
+        <v>75</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C20" s="0" t="s">
         <v>59</v>
@@ -1630,7 +1596,7 @@
         <v>7</v>
       </c>
       <c r="E20" s="0" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="F20" s="0" t="s">
         <v>17</v>
@@ -1638,10 +1604,10 @@
     </row>
     <row r="21">
       <c r="A21" s="0">
-        <v>72</v>
+        <v>55</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C21" s="0" t="s">
         <v>59</v>
@@ -1650,7 +1616,7 @@
         <v>7</v>
       </c>
       <c r="E21" s="0" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="F21" s="0" t="s">
         <v>17</v>
@@ -1658,10 +1624,10 @@
     </row>
     <row r="22">
       <c r="A22" s="0">
-        <v>66</v>
+        <v>56</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C22" s="0" t="s">
         <v>59</v>
@@ -1670,7 +1636,7 @@
         <v>7</v>
       </c>
       <c r="E22" s="0" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="F22" s="0" t="s">
         <v>17</v>
@@ -1678,10 +1644,10 @@
     </row>
     <row r="23">
       <c r="A23" s="0">
-        <v>62</v>
+        <v>72</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C23" s="0" t="s">
         <v>59</v>
@@ -1698,10 +1664,10 @@
     </row>
     <row r="24">
       <c r="A24" s="0">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C24" s="0" t="s">
         <v>59</v>
@@ -1718,10 +1684,10 @@
     </row>
     <row r="25">
       <c r="A25" s="0">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C25" s="0" t="s">
         <v>59</v>
@@ -1738,10 +1704,10 @@
     </row>
     <row r="26">
       <c r="A26" s="0">
-        <v>63</v>
+        <v>70</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C26" s="0" t="s">
         <v>59</v>
@@ -1758,10 +1724,10 @@
     </row>
     <row r="27">
       <c r="A27" s="0">
-        <v>13</v>
+        <v>64</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C27" s="0" t="s">
         <v>59</v>
@@ -1770,7 +1736,7 @@
         <v>7</v>
       </c>
       <c r="E27" s="0" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="F27" s="0" t="s">
         <v>17</v>
@@ -1778,10 +1744,10 @@
     </row>
     <row r="28">
       <c r="A28" s="0">
-        <v>42</v>
+        <v>63</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C28" s="0" t="s">
         <v>59</v>
@@ -1790,18 +1756,18 @@
         <v>7</v>
       </c>
       <c r="E28" s="0" t="s">
-        <v>53</v>
+        <v>17</v>
       </c>
       <c r="F28" s="0" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="0">
-        <v>33</v>
+        <v>13</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C29" s="0" t="s">
         <v>59</v>
@@ -1810,18 +1776,18 @@
         <v>7</v>
       </c>
       <c r="E29" s="0" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="F29" s="0" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="0">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="B30" s="0" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C30" s="0" t="s">
         <v>59</v>
@@ -1830,18 +1796,18 @@
         <v>7</v>
       </c>
       <c r="E30" s="0" t="s">
-        <v>8</v>
+        <v>53</v>
       </c>
       <c r="F30" s="0" t="s">
-        <v>8</v>
+        <v>19</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="0">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="B31" s="0" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C31" s="0" t="s">
         <v>59</v>
@@ -1850,18 +1816,18 @@
         <v>7</v>
       </c>
       <c r="E31" s="0" t="s">
-        <v>28</v>
+        <v>10</v>
       </c>
       <c r="F31" s="0" t="s">
-        <v>8</v>
+        <v>19</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="0">
-        <v>38</v>
+        <v>48</v>
       </c>
       <c r="B32" s="0" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C32" s="0" t="s">
         <v>59</v>
@@ -1870,18 +1836,18 @@
         <v>7</v>
       </c>
       <c r="E32" s="0" t="s">
-        <v>28</v>
+        <v>8</v>
       </c>
       <c r="F32" s="0" t="s">
-        <v>57</v>
+        <v>8</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="0">
-        <v>46</v>
+        <v>37</v>
       </c>
       <c r="B33" s="0" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C33" s="0" t="s">
         <v>59</v>
@@ -1890,18 +1856,18 @@
         <v>7</v>
       </c>
       <c r="E33" s="0" t="s">
-        <v>83</v>
+        <v>28</v>
       </c>
       <c r="F33" s="0" t="s">
-        <v>57</v>
+        <v>8</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="0">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="B34" s="0" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="C34" s="0" t="s">
         <v>59</v>
@@ -1910,7 +1876,7 @@
         <v>7</v>
       </c>
       <c r="E34" s="0" t="s">
-        <v>53</v>
+        <v>28</v>
       </c>
       <c r="F34" s="0" t="s">
         <v>57</v>
@@ -1918,10 +1884,10 @@
     </row>
     <row r="35">
       <c r="A35" s="0">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="B35" s="0" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="C35" s="0" t="s">
         <v>59</v>
@@ -1930,7 +1896,7 @@
         <v>7</v>
       </c>
       <c r="E35" s="0" t="s">
-        <v>53</v>
+        <v>83</v>
       </c>
       <c r="F35" s="0" t="s">
         <v>57</v>
@@ -1938,10 +1904,10 @@
     </row>
     <row r="36">
       <c r="A36" s="0">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="B36" s="0" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C36" s="0" t="s">
         <v>59</v>
@@ -1953,15 +1919,15 @@
         <v>53</v>
       </c>
       <c r="F36" s="0" t="s">
-        <v>83</v>
+        <v>57</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="0">
-        <v>36</v>
+        <v>44</v>
       </c>
       <c r="B37" s="0" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C37" s="0" t="s">
         <v>59</v>
@@ -1970,18 +1936,18 @@
         <v>7</v>
       </c>
       <c r="E37" s="0" t="s">
-        <v>28</v>
+        <v>53</v>
       </c>
       <c r="F37" s="0" t="s">
-        <v>83</v>
+        <v>57</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="0">
-        <v>11</v>
+        <v>41</v>
       </c>
       <c r="B38" s="0" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C38" s="0" t="s">
         <v>59</v>
@@ -1990,18 +1956,18 @@
         <v>7</v>
       </c>
       <c r="E38" s="0" t="s">
-        <v>15</v>
+        <v>53</v>
       </c>
       <c r="F38" s="0" t="s">
-        <v>53</v>
+        <v>83</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="0">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="B39" s="0" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C39" s="0" t="s">
         <v>59</v>
@@ -2010,18 +1976,18 @@
         <v>7</v>
       </c>
       <c r="E39" s="0" t="s">
-        <v>90</v>
+        <v>28</v>
       </c>
       <c r="F39" s="0" t="s">
-        <v>53</v>
+        <v>83</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="0">
-        <v>39</v>
+        <v>11</v>
       </c>
       <c r="B40" s="0" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="C40" s="0" t="s">
         <v>59</v>
@@ -2030,7 +1996,7 @@
         <v>7</v>
       </c>
       <c r="E40" s="0" t="s">
-        <v>28</v>
+        <v>15</v>
       </c>
       <c r="F40" s="0" t="s">
         <v>53</v>
@@ -2038,10 +2004,10 @@
     </row>
     <row r="41">
       <c r="A41" s="0">
-        <v>32</v>
+        <v>40</v>
       </c>
       <c r="B41" s="0" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="C41" s="0" t="s">
         <v>59</v>
@@ -2050,18 +2016,18 @@
         <v>7</v>
       </c>
       <c r="E41" s="0" t="s">
-        <v>10</v>
+        <v>90</v>
       </c>
       <c r="F41" s="0" t="s">
-        <v>28</v>
+        <v>53</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="0">
-        <v>31</v>
+        <v>39</v>
       </c>
       <c r="B42" s="0" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C42" s="0" t="s">
         <v>59</v>
@@ -2070,18 +2036,18 @@
         <v>7</v>
       </c>
       <c r="E42" s="0" t="s">
-        <v>10</v>
+        <v>28</v>
       </c>
       <c r="F42" s="0" t="s">
-        <v>10</v>
+        <v>53</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" s="0">
-        <v>20</v>
+        <v>32</v>
       </c>
       <c r="B43" s="0" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C43" s="0" t="s">
         <v>59</v>
@@ -2090,18 +2056,18 @@
         <v>7</v>
       </c>
       <c r="E43" s="0" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="F43" s="0" t="s">
-        <v>10</v>
+        <v>28</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" s="0">
-        <v>9</v>
+        <v>31</v>
       </c>
       <c r="B44" s="0" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C44" s="0" t="s">
         <v>59</v>
@@ -2110,7 +2076,7 @@
         <v>7</v>
       </c>
       <c r="E44" s="0" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="F44" s="0" t="s">
         <v>10</v>
@@ -2118,10 +2084,10 @@
     </row>
     <row r="45">
       <c r="A45" s="0">
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="B45" s="0" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C45" s="0" t="s">
         <v>59</v>
@@ -2138,10 +2104,10 @@
     </row>
     <row r="46">
       <c r="A46" s="0">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="B46" s="0" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C46" s="0" t="s">
         <v>59</v>
@@ -2153,15 +2119,15 @@
         <v>15</v>
       </c>
       <c r="F46" s="0" t="s">
-        <v>98</v>
+        <v>10</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" s="0">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="B47" s="0" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="C47" s="0" t="s">
         <v>59</v>
@@ -2173,15 +2139,15 @@
         <v>15</v>
       </c>
       <c r="F47" s="0" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" s="0">
-        <v>30</v>
+        <v>4</v>
       </c>
       <c r="B48" s="0" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="C48" s="0" t="s">
         <v>59</v>
@@ -2193,15 +2159,15 @@
         <v>15</v>
       </c>
       <c r="F48" s="0" t="s">
-        <v>15</v>
+        <v>98</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" s="0">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B49" s="0" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C49" s="0" t="s">
         <v>59</v>
@@ -2218,21 +2184,61 @@
     </row>
     <row r="50">
       <c r="A50" s="0">
+        <v>30</v>
+      </c>
+      <c r="B50" s="0" t="s">
+        <v>100</v>
+      </c>
+      <c r="C50" s="0" t="s">
+        <v>59</v>
+      </c>
+      <c r="D50" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E50" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="F50" s="0" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" s="0">
+        <v>2</v>
+      </c>
+      <c r="B51" s="0" t="s">
+        <v>101</v>
+      </c>
+      <c r="C51" s="0" t="s">
+        <v>59</v>
+      </c>
+      <c r="D51" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E51" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="F51" s="0" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" s="0">
         <v>1</v>
       </c>
-      <c r="B50" s="0" t="s">
+      <c r="B52" s="0" t="s">
         <v>102</v>
       </c>
-      <c r="C50" s="0" t="s">
-        <v>59</v>
-      </c>
-      <c r="D50" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="E50" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="F50" s="0" t="s">
+      <c r="C52" s="0" t="s">
+        <v>59</v>
+      </c>
+      <c r="D52" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E52" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="F52" s="0" t="s">
         <v>15</v>
       </c>
     </row>

</xml_diff>

<commit_message>
determine all regions before coloring
</commit_message>
<xml_diff>
--- a/paint_todo.xlsx
+++ b/paint_todo.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="125">
   <si>
     <t>Id</t>
   </si>
@@ -87,16 +87,22 @@
     <t>8/12/2018</t>
   </si>
   <si>
+    <t>make the withouthaste,com/thanks page with link to Patron</t>
+  </si>
+  <si>
+    <t>8/30/2018</t>
+  </si>
+  <si>
     <t xml:space="preserve">libraries:
 if library relies on specific verion of another library, that needs to be documented</t>
-  </si>
-  <si>
-    <t>8/30/2018</t>
   </si>
   <si>
     <t xml:space="preserve">documentation: include request for sample palette files for the specific formats/color spaces I can't verify because I don't have a test file to load
 - maybe in the actual error messages from the library, too
 - like, send me the file you are trying to read so I can add support for it</t>
+  </si>
+  <si>
+    <t>put links to license on library pages</t>
   </si>
   <si>
     <t>what license should the libraries and this program be under?</t>
@@ -170,6 +176,14 @@
     <t>VERSION 1.5: PROJECTS</t>
   </si>
   <si>
+    <t xml:space="preserve">project file is a config file
+the palette filename
+list of b/w image filename associated with color image filename (so grayscale can always be refreshed from the original)</t>
+  </si>
+  <si>
+    <t>9/1/2018</t>
+  </si>
+  <si>
     <t xml:space="preserve">secondary optional form
 open multiple files
 select one to see and edit in main form</t>
@@ -455,12 +469,6 @@
   </si>
   <si>
     <t>Bug</t>
-  </si>
-  <si>
-    <t>put links to license on library pages</t>
-  </si>
-  <si>
-    <t>make the withouthaste,com/thanks page with link to Patron</t>
   </si>
 </sst>
 </file>
@@ -513,7 +521,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:F44"/>
+  <dimension ref="A1:F45"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -695,7 +703,7 @@
         <v>107</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>122</v>
+        <v>21</v>
       </c>
       <c r="C11" s="0" t="s">
         <v>6</v>
@@ -712,7 +720,7 @@
         <v>105</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="C12" s="0" t="s">
         <v>6</v>
@@ -729,7 +737,7 @@
         <v>79</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C13" s="0" t="s">
         <v>6</v>
@@ -746,7 +754,7 @@
         <v>106</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>121</v>
+        <v>25</v>
       </c>
       <c r="C14" s="0" t="s">
         <v>6</v>
@@ -763,7 +771,7 @@
         <v>103</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="C15" s="0" t="s">
         <v>6</v>
@@ -772,7 +780,7 @@
         <v>7</v>
       </c>
       <c r="E15" s="0" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
     </row>
     <row r="16">
@@ -780,7 +788,7 @@
         <v>102</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="C16" s="0" t="s">
         <v>6</v>
@@ -789,7 +797,7 @@
         <v>7</v>
       </c>
       <c r="E16" s="0" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
     </row>
     <row r="17">
@@ -797,7 +805,7 @@
         <v>85</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="C17" s="0" t="s">
         <v>6</v>
@@ -814,7 +822,7 @@
         <v>80</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="C18" s="0" t="s">
         <v>6</v>
@@ -831,7 +839,7 @@
         <v>77</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="C19" s="0" t="s">
         <v>6</v>
@@ -848,7 +856,7 @@
         <v>78</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="C20" s="0" t="s">
         <v>6</v>
@@ -865,7 +873,7 @@
         <v>52</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C21" s="0" t="s">
         <v>6</v>
@@ -882,7 +890,7 @@
         <v>27</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="C22" s="0" t="s">
         <v>6</v>
@@ -891,7 +899,7 @@
         <v>7</v>
       </c>
       <c r="E22" s="0" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
     </row>
     <row r="23">
@@ -899,7 +907,7 @@
         <v>28</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="C23" s="0" t="s">
         <v>6</v>
@@ -908,7 +916,7 @@
         <v>7</v>
       </c>
       <c r="E23" s="0" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
     </row>
     <row r="24">
@@ -916,7 +924,7 @@
         <v>19</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="C24" s="0" t="s">
         <v>6</v>
@@ -925,7 +933,7 @@
         <v>7</v>
       </c>
       <c r="E24" s="0" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
     </row>
     <row r="25">
@@ -933,7 +941,7 @@
         <v>22</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="C25" s="0" t="s">
         <v>6</v>
@@ -942,7 +950,7 @@
         <v>7</v>
       </c>
       <c r="E25" s="0" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
     </row>
     <row r="26">
@@ -950,7 +958,7 @@
         <v>16</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="C26" s="0" t="s">
         <v>6</v>
@@ -959,7 +967,7 @@
         <v>7</v>
       </c>
       <c r="E26" s="0" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
     </row>
     <row r="27">
@@ -967,7 +975,7 @@
         <v>17</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C27" s="0" t="s">
         <v>6</v>
@@ -976,7 +984,7 @@
         <v>7</v>
       </c>
       <c r="E27" s="0" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
     </row>
     <row r="28">
@@ -984,7 +992,7 @@
         <v>18</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="C28" s="0" t="s">
         <v>6</v>
@@ -993,7 +1001,7 @@
         <v>7</v>
       </c>
       <c r="E28" s="0" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
     </row>
     <row r="29">
@@ -1001,7 +1009,7 @@
         <v>99</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="C29" s="0" t="s">
         <v>6</v>
@@ -1018,7 +1026,7 @@
         <v>81</v>
       </c>
       <c r="B30" s="0" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="C30" s="0" t="s">
         <v>6</v>
@@ -1032,10 +1040,10 @@
     </row>
     <row r="31">
       <c r="A31" s="0">
-        <v>82</v>
+        <v>108</v>
       </c>
       <c r="B31" s="0" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="C31" s="0" t="s">
         <v>6</v>
@@ -1044,15 +1052,15 @@
         <v>7</v>
       </c>
       <c r="E31" s="0" t="s">
-        <v>16</v>
+        <v>46</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="0">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B32" s="0" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="C32" s="0" t="s">
         <v>6</v>
@@ -1066,10 +1074,10 @@
     </row>
     <row r="33">
       <c r="A33" s="0">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B33" s="0" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="C33" s="0" t="s">
         <v>6</v>
@@ -1083,10 +1091,10 @@
     </row>
     <row r="34">
       <c r="A34" s="0">
-        <v>25</v>
+        <v>84</v>
       </c>
       <c r="B34" s="0" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="C34" s="0" t="s">
         <v>6</v>
@@ -1095,15 +1103,15 @@
         <v>7</v>
       </c>
       <c r="E34" s="0" t="s">
-        <v>34</v>
+        <v>16</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="0">
-        <v>57</v>
+        <v>25</v>
       </c>
       <c r="B35" s="0" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="C35" s="0" t="s">
         <v>6</v>
@@ -1112,15 +1120,15 @@
         <v>7</v>
       </c>
       <c r="E35" s="0" t="s">
-        <v>16</v>
+        <v>36</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="0">
-        <v>65</v>
+        <v>57</v>
       </c>
       <c r="B36" s="0" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="C36" s="0" t="s">
         <v>6</v>
@@ -1134,10 +1142,10 @@
     </row>
     <row r="37">
       <c r="A37" s="0">
-        <v>58</v>
+        <v>65</v>
       </c>
       <c r="B37" s="0" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="C37" s="0" t="s">
         <v>6</v>
@@ -1151,10 +1159,10 @@
     </row>
     <row r="38">
       <c r="A38" s="0">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="B38" s="0" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="C38" s="0" t="s">
         <v>6</v>
@@ -1168,10 +1176,10 @@
     </row>
     <row r="39">
       <c r="A39" s="0">
-        <v>26</v>
+        <v>61</v>
       </c>
       <c r="B39" s="0" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="C39" s="0" t="s">
         <v>6</v>
@@ -1180,15 +1188,15 @@
         <v>7</v>
       </c>
       <c r="E39" s="0" t="s">
-        <v>34</v>
+        <v>16</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="0">
-        <v>43</v>
+        <v>26</v>
       </c>
       <c r="B40" s="0" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="C40" s="0" t="s">
         <v>6</v>
@@ -1197,15 +1205,15 @@
         <v>7</v>
       </c>
       <c r="E40" s="0" t="s">
-        <v>53</v>
+        <v>36</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="0">
-        <v>74</v>
+        <v>43</v>
       </c>
       <c r="B41" s="0" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="C41" s="0" t="s">
         <v>6</v>
@@ -1214,15 +1222,15 @@
         <v>7</v>
       </c>
       <c r="E41" s="0" t="s">
-        <v>16</v>
+        <v>57</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="0">
-        <v>29</v>
+        <v>74</v>
       </c>
       <c r="B42" s="0" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="C42" s="0" t="s">
         <v>6</v>
@@ -1231,15 +1239,15 @@
         <v>7</v>
       </c>
       <c r="E42" s="0" t="s">
-        <v>34</v>
+        <v>16</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" s="0">
-        <v>47</v>
+        <v>29</v>
       </c>
       <c r="B43" s="0" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="C43" s="0" t="s">
         <v>6</v>
@@ -1248,16 +1256,16 @@
         <v>7</v>
       </c>
       <c r="E43" s="0" t="s">
-        <v>57</v>
+        <v>36</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" s="0">
+        <v>47</v>
+      </c>
+      <c r="B44" s="0" t="s">
         <v>60</v>
       </c>
-      <c r="B44" s="0" t="s">
-        <v>58</v>
-      </c>
       <c r="C44" s="0" t="s">
         <v>6</v>
       </c>
@@ -1265,6 +1273,23 @@
         <v>7</v>
       </c>
       <c r="E44" s="0" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" s="0">
+        <v>60</v>
+      </c>
+      <c r="B45" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="C45" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D45" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E45" s="0" t="s">
         <v>16</v>
       </c>
     </row>
@@ -1298,7 +1323,7 @@
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
     </row>
     <row r="2">
@@ -1306,10 +1331,10 @@
         <v>92</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="D2" s="0" t="s">
         <v>7</v>
@@ -1326,16 +1351,16 @@
         <v>90</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="D3" s="0" t="s">
         <v>7</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="F3" s="0" t="s">
         <v>10</v>
@@ -1346,16 +1371,16 @@
         <v>88</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="D4" s="0" t="s">
         <v>7</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="F4" s="0" t="s">
         <v>10</v>
@@ -1366,10 +1391,10 @@
         <v>86</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="D5" s="0" t="s">
         <v>7</v>
@@ -1386,10 +1411,10 @@
         <v>97</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="D6" s="0" t="s">
         <v>7</v>
@@ -1406,16 +1431,16 @@
         <v>21</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="D7" s="0" t="s">
         <v>7</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="F7" s="0" t="s">
         <v>10</v>
@@ -1426,10 +1451,10 @@
         <v>100</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="D8" s="0" t="s">
         <v>7</v>
@@ -1446,16 +1471,16 @@
         <v>87</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="D9" s="0" t="s">
         <v>7</v>
       </c>
       <c r="E9" s="0" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="F9" s="0" t="s">
         <v>10</v>
@@ -1466,10 +1491,10 @@
         <v>94</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="D10" s="0" t="s">
         <v>7</v>
@@ -1486,10 +1511,10 @@
         <v>93</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="D11" s="0" t="s">
         <v>7</v>
@@ -1506,16 +1531,16 @@
         <v>34</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="D12" s="0" t="s">
         <v>7</v>
       </c>
       <c r="E12" s="0" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="F12" s="0" t="s">
         <v>10</v>
@@ -1526,10 +1551,10 @@
         <v>50</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="D13" s="0" t="s">
         <v>7</v>
@@ -1546,19 +1571,19 @@
         <v>89</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="D14" s="0" t="s">
         <v>7</v>
       </c>
       <c r="E14" s="0" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="F14" s="0" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
     </row>
     <row r="15">
@@ -1566,10 +1591,10 @@
         <v>59</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="D15" s="0" t="s">
         <v>7</v>
@@ -1578,7 +1603,7 @@
         <v>16</v>
       </c>
       <c r="F15" s="0" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
     </row>
     <row r="16">
@@ -1586,10 +1611,10 @@
         <v>69</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="D16" s="0" t="s">
         <v>7</v>
@@ -1598,7 +1623,7 @@
         <v>16</v>
       </c>
       <c r="F16" s="0" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
     </row>
     <row r="17">
@@ -1606,10 +1631,10 @@
         <v>68</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="D17" s="0" t="s">
         <v>7</v>
@@ -1618,7 +1643,7 @@
         <v>16</v>
       </c>
       <c r="F17" s="0" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
     </row>
     <row r="18">
@@ -1626,10 +1651,10 @@
         <v>67</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="D18" s="0" t="s">
         <v>7</v>
@@ -1638,7 +1663,7 @@
         <v>16</v>
       </c>
       <c r="F18" s="0" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
     </row>
     <row r="19">
@@ -1646,10 +1671,10 @@
         <v>71</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="D19" s="0" t="s">
         <v>7</v>
@@ -1666,16 +1691,16 @@
         <v>24</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="C20" s="0" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="D20" s="0" t="s">
         <v>7</v>
       </c>
       <c r="E20" s="0" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="F20" s="0" t="s">
         <v>16</v>
@@ -1686,10 +1711,10 @@
         <v>75</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="C21" s="0" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="D21" s="0" t="s">
         <v>7</v>
@@ -1706,10 +1731,10 @@
         <v>55</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="C22" s="0" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="D22" s="0" t="s">
         <v>7</v>
@@ -1726,10 +1751,10 @@
         <v>56</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="C23" s="0" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="D23" s="0" t="s">
         <v>7</v>
@@ -1746,10 +1771,10 @@
         <v>72</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
       <c r="C24" s="0" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="D24" s="0" t="s">
         <v>7</v>
@@ -1766,10 +1791,10 @@
         <v>66</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
       <c r="C25" s="0" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="D25" s="0" t="s">
         <v>7</v>
@@ -1786,10 +1811,10 @@
         <v>62</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="C26" s="0" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="D26" s="0" t="s">
         <v>7</v>
@@ -1806,10 +1831,10 @@
         <v>70</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>87</v>
+        <v>91</v>
       </c>
       <c r="C27" s="0" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="D27" s="0" t="s">
         <v>7</v>
@@ -1826,10 +1851,10 @@
         <v>64</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>88</v>
+        <v>92</v>
       </c>
       <c r="C28" s="0" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="D28" s="0" t="s">
         <v>7</v>
@@ -1846,10 +1871,10 @@
         <v>63</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>89</v>
+        <v>93</v>
       </c>
       <c r="C29" s="0" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="D29" s="0" t="s">
         <v>7</v>
@@ -1866,16 +1891,16 @@
         <v>13</v>
       </c>
       <c r="B30" s="0" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
       <c r="C30" s="0" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="D30" s="0" t="s">
         <v>7</v>
       </c>
       <c r="E30" s="0" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="F30" s="0" t="s">
         <v>16</v>
@@ -1886,16 +1911,16 @@
         <v>42</v>
       </c>
       <c r="B31" s="0" t="s">
-        <v>91</v>
+        <v>95</v>
       </c>
       <c r="C31" s="0" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="D31" s="0" t="s">
         <v>7</v>
       </c>
       <c r="E31" s="0" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="F31" s="0" t="s">
         <v>8</v>
@@ -1906,16 +1931,16 @@
         <v>33</v>
       </c>
       <c r="B32" s="0" t="s">
-        <v>92</v>
+        <v>96</v>
       </c>
       <c r="C32" s="0" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="D32" s="0" t="s">
         <v>7</v>
       </c>
       <c r="E32" s="0" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="F32" s="0" t="s">
         <v>8</v>
@@ -1926,10 +1951,10 @@
         <v>48</v>
       </c>
       <c r="B33" s="0" t="s">
-        <v>93</v>
+        <v>97</v>
       </c>
       <c r="C33" s="0" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="D33" s="0" t="s">
         <v>7</v>
@@ -1946,10 +1971,10 @@
         <v>37</v>
       </c>
       <c r="B34" s="0" t="s">
-        <v>94</v>
+        <v>98</v>
       </c>
       <c r="C34" s="0" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="D34" s="0" t="s">
         <v>7</v>
@@ -1966,10 +1991,10 @@
         <v>38</v>
       </c>
       <c r="B35" s="0" t="s">
-        <v>95</v>
+        <v>99</v>
       </c>
       <c r="C35" s="0" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="D35" s="0" t="s">
         <v>7</v>
@@ -1978,7 +2003,7 @@
         <v>20</v>
       </c>
       <c r="F35" s="0" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
     </row>
     <row r="36">
@@ -1986,19 +2011,19 @@
         <v>46</v>
       </c>
       <c r="B36" s="0" t="s">
-        <v>96</v>
+        <v>100</v>
       </c>
       <c r="C36" s="0" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="D36" s="0" t="s">
         <v>7</v>
       </c>
       <c r="E36" s="0" t="s">
-        <v>97</v>
+        <v>101</v>
       </c>
       <c r="F36" s="0" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
     </row>
     <row r="37">
@@ -2006,19 +2031,19 @@
         <v>45</v>
       </c>
       <c r="B37" s="0" t="s">
-        <v>98</v>
+        <v>102</v>
       </c>
       <c r="C37" s="0" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="D37" s="0" t="s">
         <v>7</v>
       </c>
       <c r="E37" s="0" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="F37" s="0" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
     </row>
     <row r="38">
@@ -2026,19 +2051,19 @@
         <v>44</v>
       </c>
       <c r="B38" s="0" t="s">
-        <v>99</v>
+        <v>103</v>
       </c>
       <c r="C38" s="0" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="D38" s="0" t="s">
         <v>7</v>
       </c>
       <c r="E38" s="0" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="F38" s="0" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
     </row>
     <row r="39">
@@ -2046,19 +2071,19 @@
         <v>41</v>
       </c>
       <c r="B39" s="0" t="s">
-        <v>100</v>
+        <v>104</v>
       </c>
       <c r="C39" s="0" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="D39" s="0" t="s">
         <v>7</v>
       </c>
       <c r="E39" s="0" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="F39" s="0" t="s">
-        <v>97</v>
+        <v>101</v>
       </c>
     </row>
     <row r="40">
@@ -2066,10 +2091,10 @@
         <v>36</v>
       </c>
       <c r="B40" s="0" t="s">
-        <v>101</v>
+        <v>105</v>
       </c>
       <c r="C40" s="0" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="D40" s="0" t="s">
         <v>7</v>
@@ -2078,7 +2103,7 @@
         <v>20</v>
       </c>
       <c r="F40" s="0" t="s">
-        <v>97</v>
+        <v>101</v>
       </c>
     </row>
     <row r="41">
@@ -2086,19 +2111,19 @@
         <v>11</v>
       </c>
       <c r="B41" s="0" t="s">
-        <v>102</v>
+        <v>106</v>
       </c>
       <c r="C41" s="0" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="D41" s="0" t="s">
         <v>7</v>
       </c>
       <c r="E41" s="0" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="F41" s="0" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
     </row>
     <row r="42">
@@ -2106,19 +2131,19 @@
         <v>40</v>
       </c>
       <c r="B42" s="0" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
       <c r="C42" s="0" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="D42" s="0" t="s">
         <v>7</v>
       </c>
       <c r="E42" s="0" t="s">
-        <v>104</v>
+        <v>108</v>
       </c>
       <c r="F42" s="0" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
     </row>
     <row r="43">
@@ -2126,10 +2151,10 @@
         <v>39</v>
       </c>
       <c r="B43" s="0" t="s">
-        <v>105</v>
+        <v>109</v>
       </c>
       <c r="C43" s="0" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="D43" s="0" t="s">
         <v>7</v>
@@ -2138,7 +2163,7 @@
         <v>20</v>
       </c>
       <c r="F43" s="0" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
     </row>
     <row r="44">
@@ -2146,16 +2171,16 @@
         <v>32</v>
       </c>
       <c r="B44" s="0" t="s">
-        <v>106</v>
+        <v>110</v>
       </c>
       <c r="C44" s="0" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="D44" s="0" t="s">
         <v>7</v>
       </c>
       <c r="E44" s="0" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="F44" s="0" t="s">
         <v>20</v>
@@ -2166,19 +2191,19 @@
         <v>31</v>
       </c>
       <c r="B45" s="0" t="s">
-        <v>107</v>
+        <v>111</v>
       </c>
       <c r="C45" s="0" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="D45" s="0" t="s">
         <v>7</v>
       </c>
       <c r="E45" s="0" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="F45" s="0" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
     </row>
     <row r="46">
@@ -2186,19 +2211,19 @@
         <v>20</v>
       </c>
       <c r="B46" s="0" t="s">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="C46" s="0" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="D46" s="0" t="s">
         <v>7</v>
       </c>
       <c r="E46" s="0" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="F46" s="0" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
     </row>
     <row r="47">
@@ -2206,19 +2231,19 @@
         <v>9</v>
       </c>
       <c r="B47" s="0" t="s">
-        <v>109</v>
+        <v>113</v>
       </c>
       <c r="C47" s="0" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="D47" s="0" t="s">
         <v>7</v>
       </c>
       <c r="E47" s="0" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="F47" s="0" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
     </row>
     <row r="48">
@@ -2226,19 +2251,19 @@
         <v>8</v>
       </c>
       <c r="B48" s="0" t="s">
-        <v>110</v>
+        <v>114</v>
       </c>
       <c r="C48" s="0" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="D48" s="0" t="s">
         <v>7</v>
       </c>
       <c r="E48" s="0" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="F48" s="0" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
     </row>
     <row r="49">
@@ -2246,19 +2271,19 @@
         <v>4</v>
       </c>
       <c r="B49" s="0" t="s">
-        <v>111</v>
+        <v>115</v>
       </c>
       <c r="C49" s="0" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="D49" s="0" t="s">
         <v>7</v>
       </c>
       <c r="E49" s="0" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="F49" s="0" t="s">
-        <v>112</v>
+        <v>116</v>
       </c>
     </row>
     <row r="50">
@@ -2266,19 +2291,19 @@
         <v>3</v>
       </c>
       <c r="B50" s="0" t="s">
-        <v>113</v>
+        <v>117</v>
       </c>
       <c r="C50" s="0" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="D50" s="0" t="s">
         <v>7</v>
       </c>
       <c r="E50" s="0" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="F50" s="0" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
     </row>
     <row r="51">
@@ -2286,19 +2311,19 @@
         <v>30</v>
       </c>
       <c r="B51" s="0" t="s">
-        <v>114</v>
+        <v>118</v>
       </c>
       <c r="C51" s="0" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="D51" s="0" t="s">
         <v>7</v>
       </c>
       <c r="E51" s="0" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="F51" s="0" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
     </row>
     <row r="52">
@@ -2306,19 +2331,19 @@
         <v>2</v>
       </c>
       <c r="B52" s="0" t="s">
-        <v>115</v>
+        <v>119</v>
       </c>
       <c r="C52" s="0" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="D52" s="0" t="s">
         <v>7</v>
       </c>
       <c r="E52" s="0" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="F52" s="0" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
     </row>
     <row r="53">
@@ -2326,19 +2351,19 @@
         <v>1</v>
       </c>
       <c r="B53" s="0" t="s">
-        <v>116</v>
+        <v>120</v>
       </c>
       <c r="C53" s="0" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="D53" s="0" t="s">
         <v>7</v>
       </c>
       <c r="E53" s="0" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="F53" s="0" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
     </row>
   </sheetData>
@@ -2359,7 +2384,7 @@
         <v>2</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>117</v>
+        <v>121</v>
       </c>
       <c r="C1" s="2"/>
       <c r="D1" s="2" t="s">
@@ -2367,7 +2392,7 @@
       </c>
       <c r="E1" s="2"/>
       <c r="F1" s="2" t="s">
-        <v>118</v>
+        <v>122</v>
       </c>
     </row>
     <row r="2">
@@ -2375,24 +2400,24 @@
         <v>6</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>117</v>
+        <v>121</v>
       </c>
       <c r="D2" s="0" t="s">
         <v>7</v>
       </c>
       <c r="F2" s="0">
-        <v>107</v>
+        <v>108</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="0" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>119</v>
+        <v>123</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>120</v>
+        <v>124</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
cancel loading of image
</commit_message>
<xml_diff>
--- a/paint_todo.xlsx
+++ b/paint_todo.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="126">
   <si>
     <t>Id</t>
   </si>
@@ -469,6 +469,12 @@
   </si>
   <si>
     <t>Bug</t>
+  </si>
+  <si>
+    <t xml:space="preserve">make a MasterImage class
+that one-time figures out all the regions in a background thread
+and provides that data to the color worker
+- finding 1 region at a time benchmarked at 10.7sec for tea shop cat</t>
   </si>
 </sst>
 </file>
@@ -550,7 +556,7 @@
         <v>54</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>5</v>
+        <v>125</v>
       </c>
       <c r="C2" s="0" t="s">
         <v>6</v>

</xml_diff>

<commit_message>
testing other algorithms for finding regions
</commit_message>
<xml_diff>
--- a/paint_todo.xlsx
+++ b/paint_todo.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="135">
   <si>
     <t>Id</t>
   </si>
@@ -475,6 +475,74 @@
 that one-time figures out all the regions in a background thread
 and provides that data to the color worker
 - finding 1 region at a time benchmarked at 10.7sec for tea shop cat</t>
+  </si>
+  <si>
+    <t xml:space="preserve">make a MasterImage class
+that one-time figures out all the regions in a background thread
+and provides that data to the color worker
+- finding 1 region at a time benchmarked at 10.7sec for tea shop cat - benchmarked at &gt;15min for rabbit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">make a MasterImage class
+that one-time figures out all the regions in a background thread
+and provides that data to the color worker
+- finding 1 region at a time benchmarked at 10.7sec for tea shop cat - benchmarked at &gt;15min for rabbit
+- leading edge method 12sec for cat</t>
+  </si>
+  <si>
+    <t xml:space="preserve">make a MasterImage class
+that one-time figures out all the regions in a background thread
+and provides that data to the color worker
+- finding 1 region at a time benchmarked at 10.7sec for tea shop cat - benchmarked at &gt;15min for rabbit
+- leading edge method 12sec for cat BUT rabit only took 4min22sec</t>
+  </si>
+  <si>
+    <t xml:space="preserve">make a MasterImage class
+that one-time figures out all the regions in a background thread
+and provides that data to the color worker
+- finding 1 region at a time benchmarked at 10.7sec for tea shop cat - benchmarked at &gt;15min for rabbit
+- leading edge method 12sec for cat BUT rabit only took 4min22sec
+- maybe I should select the method based on image size?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">make a MasterImage class
+that one-time figures out all the regions in a background thread
+and provides that data to the color worker
+- finding 1 region at a time benchmarked at 10.7sec for tea shop cat - benchmarked at &gt;15min for rabbit
+- leading edge method 
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">make a MasterImage class
+that one-time figures out all the regions in a background thread
+and provides that data to the color worker
+- finding 1 region at a time benchmarked at 10.7sec for tea shop cat - benchmarked at &gt;15min for rabbit
+- leading edge method still &gt;15min for rabbit
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">make a MasterImage class
+that one-time figures out all the regions in a background thread
+and provides that data to the color worker
+- finding 1 region at a time benchmarked at 10.7sec for tea shop cat - benchmarked at &gt;15min for rabbit
+- leading edge method still &gt;22min for rabbit
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">make a MasterImage class
+that one-time figures out all the regions in a background thread
+and provides that data to the color worker
+- finding 1 region at a time benchmarked at 10.7sec for tea shop cat - benchmarked at &gt;15min for rabbit
+- leading edge method still &gt;22min for rabbit and it was 10min for the cat
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">make a MasterImage class
+that one-time figures out all the regions in a background thread
+and provides that data to the color worker
+- A: finding 1 region at a time benchmarked at 10.7sec for tea shop cat - benchmarked at &gt;15min for rabbit
+- B: leading edge method still &gt;22min for rabbit and it was 10min for the cat (verified A still runs in 10sec on cat)
+</t>
   </si>
 </sst>
 </file>
@@ -556,7 +624,7 @@
         <v>54</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>125</v>
+        <v>134</v>
       </c>
       <c r="C2" s="0" t="s">
         <v>6</v>

</xml_diff>

<commit_message>
fixed performance issues when finding all regions on image load
</commit_message>
<xml_diff>
--- a/paint_todo.xlsx
+++ b/paint_todo.xlsx
@@ -31,9 +31,11 @@
     <t>Created</t>
   </si>
   <si>
-    <t xml:space="preserve">make a MasterImage class
-that one-time figures out all the regions in a background thread
-and provides that data to the color worker</t>
+    <t xml:space="preserve">benchmarking:
+- how long to simply count pixels?
+- how long to create 1 Point per pixel?
+- how long to GetPixel for each pixel?
+- how long to union set each pixel together?</t>
   </si>
   <si>
     <t>Todo</t>
@@ -42,7 +44,7 @@
     <t>Task</t>
   </si>
   <si>
-    <t>8/23/2018</t>
+    <t>9/10/2018</t>
   </si>
   <si>
     <t>continue refactoring business logic out of RequestColorWorker</t>
@@ -55,6 +57,9 @@
 - on closing program
 - on opening new image
 Add this tracking to MasterImage class</t>
+  </si>
+  <si>
+    <t>8/23/2018</t>
   </si>
   <si>
     <t>walk through Edit Palette panels and events and make sure its all right</t>
@@ -176,6 +181,16 @@
     <t>VERSION 1.5: PROJECTS</t>
   </si>
   <si>
+    <t xml:space="preserve">main form &gt; edit palette color
+option to edit with live preview in current image</t>
+  </si>
+  <si>
+    <t>9/6/2018</t>
+  </si>
+  <si>
+    <t>safe color swap in images (1 or multiple or all)</t>
+  </si>
+  <si>
     <t xml:space="preserve">project file is a config file
 the palette filename
 list of b/w image filename associated with color image filename (so grayscale can always be refreshed from the original)</t>
@@ -198,7 +213,14 @@
     <t>open project</t>
   </si>
   <si>
+    <t>display version number somewhere in GUI</t>
+  </si>
+  <si>
     <t>EVERYTHING BELOW HERE IS VERSION 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">keep some sort of Versions document
+- is there a suggested format?</t>
   </si>
   <si>
     <t xml:space="preserve">create custom trackbar control
@@ -250,6 +272,13 @@
     <t>Done</t>
   </si>
   <si>
+    <t xml:space="preserve">make a MasterImage class
+that one-time figures out all the regions in a background thread
+and provides that data to the color worker
+- A: finding 1 region at a time benchmarked at 10.7sec for tea shop cat - benchmarked at &gt;15min for rabbit
+- B: leading edge method still &gt;22min for rabbit and it was 10min for the cat (verified A still runs in 10sec on cat)</t>
+  </si>
+  <si>
     <t>eyedrop tool: select color in palette, by selecting color on image (select palest color in colored region)</t>
   </si>
   <si>
@@ -471,78 +500,24 @@
     <t>Bug</t>
   </si>
   <si>
-    <t xml:space="preserve">make a MasterImage class
-that one-time figures out all the regions in a background thread
-and provides that data to the color worker
-- finding 1 region at a time benchmarked at 10.7sec for tea shop cat</t>
-  </si>
-  <si>
-    <t xml:space="preserve">make a MasterImage class
-that one-time figures out all the regions in a background thread
-and provides that data to the color worker
-- finding 1 region at a time benchmarked at 10.7sec for tea shop cat - benchmarked at &gt;15min for rabbit</t>
-  </si>
-  <si>
-    <t xml:space="preserve">make a MasterImage class
-that one-time figures out all the regions in a background thread
-and provides that data to the color worker
-- finding 1 region at a time benchmarked at 10.7sec for tea shop cat - benchmarked at &gt;15min for rabbit
-- leading edge method 12sec for cat</t>
-  </si>
-  <si>
-    <t xml:space="preserve">make a MasterImage class
-that one-time figures out all the regions in a background thread
-and provides that data to the color worker
-- finding 1 region at a time benchmarked at 10.7sec for tea shop cat - benchmarked at &gt;15min for rabbit
-- leading edge method 12sec for cat BUT rabit only took 4min22sec</t>
-  </si>
-  <si>
-    <t xml:space="preserve">make a MasterImage class
-that one-time figures out all the regions in a background thread
-and provides that data to the color worker
-- finding 1 region at a time benchmarked at 10.7sec for tea shop cat - benchmarked at &gt;15min for rabbit
-- leading edge method 12sec for cat BUT rabit only took 4min22sec
-- maybe I should select the method based on image size?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">make a MasterImage class
-that one-time figures out all the regions in a background thread
-and provides that data to the color worker
-- finding 1 region at a time benchmarked at 10.7sec for tea shop cat - benchmarked at &gt;15min for rabbit
-- leading edge method 
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">make a MasterImage class
-that one-time figures out all the regions in a background thread
-and provides that data to the color worker
-- finding 1 region at a time benchmarked at 10.7sec for tea shop cat - benchmarked at &gt;15min for rabbit
-- leading edge method still &gt;15min for rabbit
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">make a MasterImage class
-that one-time figures out all the regions in a background thread
-and provides that data to the color worker
-- finding 1 region at a time benchmarked at 10.7sec for tea shop cat - benchmarked at &gt;15min for rabbit
-- leading edge method still &gt;22min for rabbit
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">make a MasterImage class
-that one-time figures out all the regions in a background thread
-and provides that data to the color worker
-- finding 1 region at a time benchmarked at 10.7sec for tea shop cat - benchmarked at &gt;15min for rabbit
-- leading edge method still &gt;22min for rabbit and it was 10min for the cat
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">make a MasterImage class
-that one-time figures out all the regions in a background thread
-and provides that data to the color worker
-- A: finding 1 region at a time benchmarked at 10.7sec for tea shop cat - benchmarked at &gt;15min for rabbit
-- B: leading edge method still &gt;22min for rabbit and it was 10min for the cat (verified A still runs in 10sec on cat)
-</t>
+    <t>replace Rabbit with smaller and better divided sample image</t>
+  </si>
+  <si>
+    <t xml:space="preserve">benchmarking:
+- how long to simply count pixels?
+- how long to create 1 Point per pixel?
+- how long to GetPixel for each pixel?
+- how long to union set each pixel together?
+looks like UnionWith operations are the problem</t>
+  </si>
+  <si>
+    <t xml:space="preserve">benchmarking:
+- how long to simply count pixels?
+- how long to create 1 Point per pixel?
+- how long to GetPixel for each pixel?
+- how long to union set each pixel together?
+looks like UnionWith operations are the problem
+- fixed it!</t>
   </si>
 </sst>
 </file>
@@ -595,7 +570,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:F45"/>
+  <dimension ref="A1:F36"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -621,10 +596,10 @@
     </row>
     <row r="2">
       <c r="A2" s="0">
-        <v>54</v>
+        <v>95</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>134</v>
+        <v>9</v>
       </c>
       <c r="C2" s="0" t="s">
         <v>6</v>
@@ -633,15 +608,15 @@
         <v>7</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="0">
-        <v>95</v>
+        <v>53</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C3" s="0" t="s">
         <v>6</v>
@@ -650,15 +625,15 @@
         <v>7</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="0">
-        <v>53</v>
+        <v>101</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C4" s="0" t="s">
         <v>6</v>
@@ -667,15 +642,15 @@
         <v>7</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="0">
-        <v>101</v>
+        <v>51</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>12</v>
+        <v>132</v>
       </c>
       <c r="C5" s="0" t="s">
         <v>6</v>
@@ -684,15 +659,15 @@
         <v>7</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="0">
-        <v>51</v>
+        <v>76</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="C6" s="0" t="s">
         <v>6</v>
@@ -701,15 +676,15 @@
         <v>7</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="0">
-        <v>76</v>
+        <v>35</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="C7" s="0" t="s">
         <v>6</v>
@@ -718,15 +693,15 @@
         <v>7</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="0">
-        <v>49</v>
+        <v>80</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>17</v>
+        <v>32</v>
       </c>
       <c r="C8" s="0" t="s">
         <v>6</v>
@@ -735,15 +710,15 @@
         <v>7</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="0">
-        <v>91</v>
+        <v>27</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>18</v>
+        <v>36</v>
       </c>
       <c r="C9" s="0" t="s">
         <v>6</v>
@@ -752,15 +727,15 @@
         <v>7</v>
       </c>
       <c r="E9" s="0" t="s">
-        <v>10</v>
+        <v>37</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="0">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>19</v>
+        <v>38</v>
       </c>
       <c r="C10" s="0" t="s">
         <v>6</v>
@@ -769,15 +744,15 @@
         <v>7</v>
       </c>
       <c r="E10" s="0" t="s">
-        <v>20</v>
+        <v>37</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="0">
-        <v>107</v>
+        <v>19</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>21</v>
+        <v>39</v>
       </c>
       <c r="C11" s="0" t="s">
         <v>6</v>
@@ -786,15 +761,15 @@
         <v>7</v>
       </c>
       <c r="E11" s="0" t="s">
-        <v>22</v>
+        <v>37</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="0">
-        <v>105</v>
+        <v>22</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>23</v>
+        <v>40</v>
       </c>
       <c r="C12" s="0" t="s">
         <v>6</v>
@@ -803,15 +778,15 @@
         <v>7</v>
       </c>
       <c r="E12" s="0" t="s">
-        <v>22</v>
+        <v>37</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="0">
-        <v>79</v>
+        <v>16</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>24</v>
+        <v>41</v>
       </c>
       <c r="C13" s="0" t="s">
         <v>6</v>
@@ -820,15 +795,15 @@
         <v>7</v>
       </c>
       <c r="E13" s="0" t="s">
-        <v>16</v>
+        <v>37</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="0">
-        <v>106</v>
+        <v>17</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>25</v>
+        <v>42</v>
       </c>
       <c r="C14" s="0" t="s">
         <v>6</v>
@@ -837,15 +812,15 @@
         <v>7</v>
       </c>
       <c r="E14" s="0" t="s">
-        <v>22</v>
+        <v>37</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="0">
-        <v>103</v>
+        <v>18</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>26</v>
+        <v>43</v>
       </c>
       <c r="C15" s="0" t="s">
         <v>6</v>
@@ -854,15 +829,15 @@
         <v>7</v>
       </c>
       <c r="E15" s="0" t="s">
-        <v>27</v>
+        <v>37</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="0">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>28</v>
+        <v>44</v>
       </c>
       <c r="C16" s="0" t="s">
         <v>6</v>
@@ -871,15 +846,15 @@
         <v>7</v>
       </c>
       <c r="E16" s="0" t="s">
-        <v>29</v>
+        <v>10</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="0">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>30</v>
+        <v>45</v>
       </c>
       <c r="C17" s="0" t="s">
         <v>6</v>
@@ -888,15 +863,15 @@
         <v>7</v>
       </c>
       <c r="E17" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="0">
-        <v>80</v>
+        <v>109</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>31</v>
+        <v>46</v>
       </c>
       <c r="C18" s="0" t="s">
         <v>6</v>
@@ -905,15 +880,15 @@
         <v>7</v>
       </c>
       <c r="E18" s="0" t="s">
-        <v>16</v>
+        <v>47</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="0">
-        <v>77</v>
+        <v>110</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>32</v>
+        <v>48</v>
       </c>
       <c r="C19" s="0" t="s">
         <v>6</v>
@@ -922,15 +897,15 @@
         <v>7</v>
       </c>
       <c r="E19" s="0" t="s">
-        <v>16</v>
+        <v>47</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="0">
-        <v>78</v>
+        <v>108</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>33</v>
+        <v>49</v>
       </c>
       <c r="C20" s="0" t="s">
         <v>6</v>
@@ -939,15 +914,15 @@
         <v>7</v>
       </c>
       <c r="E20" s="0" t="s">
-        <v>16</v>
+        <v>50</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="0">
-        <v>52</v>
+        <v>82</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>34</v>
+        <v>51</v>
       </c>
       <c r="C21" s="0" t="s">
         <v>6</v>
@@ -956,15 +931,15 @@
         <v>7</v>
       </c>
       <c r="E21" s="0" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="0">
-        <v>27</v>
+        <v>83</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>35</v>
+        <v>52</v>
       </c>
       <c r="C22" s="0" t="s">
         <v>6</v>
@@ -973,15 +948,15 @@
         <v>7</v>
       </c>
       <c r="E22" s="0" t="s">
-        <v>36</v>
+        <v>17</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="0">
-        <v>28</v>
+        <v>84</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>37</v>
+        <v>53</v>
       </c>
       <c r="C23" s="0" t="s">
         <v>6</v>
@@ -990,15 +965,15 @@
         <v>7</v>
       </c>
       <c r="E23" s="0" t="s">
-        <v>36</v>
+        <v>17</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="0">
-        <v>19</v>
+        <v>112</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>38</v>
+        <v>54</v>
       </c>
       <c r="C24" s="0" t="s">
         <v>6</v>
@@ -1007,15 +982,15 @@
         <v>7</v>
       </c>
       <c r="E24" s="0" t="s">
-        <v>36</v>
+        <v>47</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="0">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>39</v>
+        <v>55</v>
       </c>
       <c r="C25" s="0" t="s">
         <v>6</v>
@@ -1024,15 +999,15 @@
         <v>7</v>
       </c>
       <c r="E25" s="0" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="0">
-        <v>16</v>
+        <v>111</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>40</v>
+        <v>56</v>
       </c>
       <c r="C26" s="0" t="s">
         <v>6</v>
@@ -1041,15 +1016,15 @@
         <v>7</v>
       </c>
       <c r="E26" s="0" t="s">
-        <v>36</v>
+        <v>47</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="0">
-        <v>17</v>
+        <v>57</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>41</v>
+        <v>57</v>
       </c>
       <c r="C27" s="0" t="s">
         <v>6</v>
@@ -1058,15 +1033,15 @@
         <v>7</v>
       </c>
       <c r="E27" s="0" t="s">
-        <v>36</v>
+        <v>17</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="0">
-        <v>18</v>
+        <v>65</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>42</v>
+        <v>58</v>
       </c>
       <c r="C28" s="0" t="s">
         <v>6</v>
@@ -1075,15 +1050,15 @@
         <v>7</v>
       </c>
       <c r="E28" s="0" t="s">
-        <v>36</v>
+        <v>17</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="0">
-        <v>99</v>
+        <v>58</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>43</v>
+        <v>59</v>
       </c>
       <c r="C29" s="0" t="s">
         <v>6</v>
@@ -1092,15 +1067,15 @@
         <v>7</v>
       </c>
       <c r="E29" s="0" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="0">
-        <v>81</v>
+        <v>61</v>
       </c>
       <c r="B30" s="0" t="s">
-        <v>44</v>
+        <v>60</v>
       </c>
       <c r="C30" s="0" t="s">
         <v>6</v>
@@ -1109,15 +1084,15 @@
         <v>7</v>
       </c>
       <c r="E30" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="0">
-        <v>108</v>
+        <v>26</v>
       </c>
       <c r="B31" s="0" t="s">
-        <v>45</v>
+        <v>61</v>
       </c>
       <c r="C31" s="0" t="s">
         <v>6</v>
@@ -1126,15 +1101,15 @@
         <v>7</v>
       </c>
       <c r="E31" s="0" t="s">
-        <v>46</v>
+        <v>37</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="0">
-        <v>82</v>
+        <v>43</v>
       </c>
       <c r="B32" s="0" t="s">
-        <v>47</v>
+        <v>62</v>
       </c>
       <c r="C32" s="0" t="s">
         <v>6</v>
@@ -1143,15 +1118,15 @@
         <v>7</v>
       </c>
       <c r="E32" s="0" t="s">
-        <v>16</v>
+        <v>63</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="0">
-        <v>83</v>
+        <v>74</v>
       </c>
       <c r="B33" s="0" t="s">
-        <v>48</v>
+        <v>64</v>
       </c>
       <c r="C33" s="0" t="s">
         <v>6</v>
@@ -1160,15 +1135,15 @@
         <v>7</v>
       </c>
       <c r="E33" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="0">
-        <v>84</v>
+        <v>29</v>
       </c>
       <c r="B34" s="0" t="s">
-        <v>49</v>
+        <v>65</v>
       </c>
       <c r="C34" s="0" t="s">
         <v>6</v>
@@ -1177,15 +1152,15 @@
         <v>7</v>
       </c>
       <c r="E34" s="0" t="s">
-        <v>16</v>
+        <v>37</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="0">
-        <v>25</v>
+        <v>47</v>
       </c>
       <c r="B35" s="0" t="s">
-        <v>50</v>
+        <v>66</v>
       </c>
       <c r="C35" s="0" t="s">
         <v>6</v>
@@ -1194,15 +1169,15 @@
         <v>7</v>
       </c>
       <c r="E35" s="0" t="s">
-        <v>36</v>
+        <v>67</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="0">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="B36" s="0" t="s">
-        <v>51</v>
+        <v>68</v>
       </c>
       <c r="C36" s="0" t="s">
         <v>6</v>
@@ -1211,160 +1186,7 @@
         <v>7</v>
       </c>
       <c r="E36" s="0" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="37">
-      <c r="A37" s="0">
-        <v>65</v>
-      </c>
-      <c r="B37" s="0" t="s">
-        <v>52</v>
-      </c>
-      <c r="C37" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="D37" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="E37" s="0" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="38">
-      <c r="A38" s="0">
-        <v>58</v>
-      </c>
-      <c r="B38" s="0" t="s">
-        <v>53</v>
-      </c>
-      <c r="C38" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="D38" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="E38" s="0" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="39">
-      <c r="A39" s="0">
-        <v>61</v>
-      </c>
-      <c r="B39" s="0" t="s">
-        <v>54</v>
-      </c>
-      <c r="C39" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="D39" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="E39" s="0" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="40">
-      <c r="A40" s="0">
-        <v>26</v>
-      </c>
-      <c r="B40" s="0" t="s">
-        <v>55</v>
-      </c>
-      <c r="C40" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="D40" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="E40" s="0" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="41">
-      <c r="A41" s="0">
-        <v>43</v>
-      </c>
-      <c r="B41" s="0" t="s">
-        <v>56</v>
-      </c>
-      <c r="C41" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="D41" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="E41" s="0" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="42">
-      <c r="A42" s="0">
-        <v>74</v>
-      </c>
-      <c r="B42" s="0" t="s">
-        <v>58</v>
-      </c>
-      <c r="C42" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="D42" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="E42" s="0" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="43">
-      <c r="A43" s="0">
-        <v>29</v>
-      </c>
-      <c r="B43" s="0" t="s">
-        <v>59</v>
-      </c>
-      <c r="C43" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="D43" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="E43" s="0" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="44">
-      <c r="A44" s="0">
-        <v>47</v>
-      </c>
-      <c r="B44" s="0" t="s">
-        <v>60</v>
-      </c>
-      <c r="C44" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="D44" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="E44" s="0" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="45">
-      <c r="A45" s="0">
-        <v>60</v>
-      </c>
-      <c r="B45" s="0" t="s">
-        <v>62</v>
-      </c>
-      <c r="C45" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="D45" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="E45" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
   </sheetData>
@@ -1374,7 +1196,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:F53"/>
+  <dimension ref="A1:F62"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1397,198 +1219,198 @@
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>63</v>
+        <v>69</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="0">
-        <v>92</v>
+        <v>113</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>64</v>
+        <v>134</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>63</v>
+        <v>69</v>
       </c>
       <c r="D2" s="0" t="s">
         <v>7</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="0">
-        <v>90</v>
+        <v>78</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>65</v>
+        <v>34</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>63</v>
+        <v>69</v>
       </c>
       <c r="D3" s="0" t="s">
         <v>7</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>66</v>
+        <v>17</v>
       </c>
       <c r="F3" s="0" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="0">
-        <v>88</v>
+        <v>77</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>67</v>
+        <v>33</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>63</v>
+        <v>69</v>
       </c>
       <c r="D4" s="0" t="s">
         <v>7</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>66</v>
+        <v>17</v>
       </c>
       <c r="F4" s="0" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="0">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>68</v>
+        <v>31</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>63</v>
+        <v>69</v>
       </c>
       <c r="D5" s="0" t="s">
         <v>7</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="F5" s="0" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="0">
-        <v>97</v>
+        <v>106</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>69</v>
+        <v>26</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>63</v>
+        <v>69</v>
       </c>
       <c r="D6" s="0" t="s">
         <v>7</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>10</v>
+        <v>23</v>
       </c>
       <c r="F6" s="0" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="0">
-        <v>21</v>
+        <v>105</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>70</v>
+        <v>24</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>63</v>
+        <v>69</v>
       </c>
       <c r="D7" s="0" t="s">
         <v>7</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>36</v>
+        <v>23</v>
       </c>
       <c r="F7" s="0" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="0">
-        <v>100</v>
+        <v>107</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>71</v>
+        <v>22</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>63</v>
+        <v>69</v>
       </c>
       <c r="D8" s="0" t="s">
         <v>7</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>10</v>
+        <v>23</v>
       </c>
       <c r="F8" s="0" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="0">
-        <v>87</v>
+        <v>49</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>72</v>
+        <v>18</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>63</v>
+        <v>69</v>
       </c>
       <c r="D9" s="0" t="s">
         <v>7</v>
       </c>
       <c r="E9" s="0" t="s">
-        <v>66</v>
+        <v>15</v>
       </c>
       <c r="F9" s="0" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="0">
-        <v>94</v>
+        <v>54</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>63</v>
+        <v>69</v>
       </c>
       <c r="D10" s="0" t="s">
         <v>7</v>
       </c>
       <c r="E10" s="0" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="F10" s="0" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="0">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>63</v>
+        <v>69</v>
       </c>
       <c r="D11" s="0" t="s">
         <v>7</v>
@@ -1602,19 +1424,19 @@
     </row>
     <row r="12">
       <c r="A12" s="0">
-        <v>34</v>
+        <v>90</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>63</v>
+        <v>69</v>
       </c>
       <c r="D12" s="0" t="s">
         <v>7</v>
       </c>
       <c r="E12" s="0" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="F12" s="0" t="s">
         <v>10</v>
@@ -1622,19 +1444,19 @@
     </row>
     <row r="13">
       <c r="A13" s="0">
-        <v>50</v>
+        <v>88</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>63</v>
+        <v>69</v>
       </c>
       <c r="D13" s="0" t="s">
         <v>7</v>
       </c>
       <c r="E13" s="0" t="s">
-        <v>14</v>
+        <v>73</v>
       </c>
       <c r="F13" s="0" t="s">
         <v>10</v>
@@ -1642,802 +1464,982 @@
     </row>
     <row r="14">
       <c r="A14" s="0">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>63</v>
+        <v>69</v>
       </c>
       <c r="D14" s="0" t="s">
         <v>7</v>
       </c>
       <c r="E14" s="0" t="s">
-        <v>66</v>
+        <v>17</v>
       </c>
       <c r="F14" s="0" t="s">
-        <v>66</v>
+        <v>10</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="0">
-        <v>59</v>
+        <v>97</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>63</v>
+        <v>69</v>
       </c>
       <c r="D15" s="0" t="s">
         <v>7</v>
       </c>
       <c r="E15" s="0" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="F15" s="0" t="s">
-        <v>66</v>
+        <v>10</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="0">
-        <v>69</v>
+        <v>21</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>63</v>
+        <v>69</v>
       </c>
       <c r="D16" s="0" t="s">
         <v>7</v>
       </c>
       <c r="E16" s="0" t="s">
-        <v>16</v>
+        <v>37</v>
       </c>
       <c r="F16" s="0" t="s">
-        <v>66</v>
+        <v>10</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="0">
-        <v>68</v>
+        <v>100</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>63</v>
+        <v>69</v>
       </c>
       <c r="D17" s="0" t="s">
         <v>7</v>
       </c>
       <c r="E17" s="0" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="F17" s="0" t="s">
-        <v>66</v>
+        <v>10</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="0">
-        <v>67</v>
+        <v>87</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>63</v>
+        <v>69</v>
       </c>
       <c r="D18" s="0" t="s">
         <v>7</v>
       </c>
       <c r="E18" s="0" t="s">
-        <v>16</v>
+        <v>73</v>
       </c>
       <c r="F18" s="0" t="s">
-        <v>66</v>
+        <v>10</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="0">
-        <v>71</v>
+        <v>94</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>63</v>
+        <v>69</v>
       </c>
       <c r="D19" s="0" t="s">
         <v>7</v>
       </c>
       <c r="E19" s="0" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="F19" s="0" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="0">
-        <v>24</v>
+        <v>93</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="C20" s="0" t="s">
-        <v>63</v>
+        <v>69</v>
       </c>
       <c r="D20" s="0" t="s">
         <v>7</v>
       </c>
       <c r="E20" s="0" t="s">
-        <v>36</v>
+        <v>10</v>
       </c>
       <c r="F20" s="0" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="0">
-        <v>75</v>
+        <v>34</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="C21" s="0" t="s">
-        <v>63</v>
+        <v>69</v>
       </c>
       <c r="D21" s="0" t="s">
         <v>7</v>
       </c>
       <c r="E21" s="0" t="s">
-        <v>16</v>
+        <v>83</v>
       </c>
       <c r="F21" s="0" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="0">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C22" s="0" t="s">
-        <v>63</v>
+        <v>69</v>
       </c>
       <c r="D22" s="0" t="s">
         <v>7</v>
       </c>
       <c r="E22" s="0" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="F22" s="0" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="0">
-        <v>56</v>
+        <v>89</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C23" s="0" t="s">
-        <v>63</v>
+        <v>69</v>
       </c>
       <c r="D23" s="0" t="s">
         <v>7</v>
       </c>
       <c r="E23" s="0" t="s">
-        <v>8</v>
+        <v>73</v>
       </c>
       <c r="F23" s="0" t="s">
-        <v>16</v>
+        <v>73</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="0">
-        <v>72</v>
+        <v>59</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C24" s="0" t="s">
-        <v>63</v>
+        <v>69</v>
       </c>
       <c r="D24" s="0" t="s">
         <v>7</v>
       </c>
       <c r="E24" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="F24" s="0" t="s">
-        <v>16</v>
+        <v>73</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="0">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C25" s="0" t="s">
-        <v>63</v>
+        <v>69</v>
       </c>
       <c r="D25" s="0" t="s">
         <v>7</v>
       </c>
       <c r="E25" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="F25" s="0" t="s">
-        <v>16</v>
+        <v>73</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="0">
-        <v>62</v>
+        <v>68</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C26" s="0" t="s">
-        <v>63</v>
+        <v>69</v>
       </c>
       <c r="D26" s="0" t="s">
         <v>7</v>
       </c>
       <c r="E26" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="F26" s="0" t="s">
-        <v>16</v>
+        <v>73</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="0">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C27" s="0" t="s">
-        <v>63</v>
+        <v>69</v>
       </c>
       <c r="D27" s="0" t="s">
         <v>7</v>
       </c>
       <c r="E27" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="F27" s="0" t="s">
-        <v>16</v>
+        <v>73</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="0">
-        <v>64</v>
+        <v>71</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C28" s="0" t="s">
-        <v>63</v>
+        <v>69</v>
       </c>
       <c r="D28" s="0" t="s">
         <v>7</v>
       </c>
       <c r="E28" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="F28" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="0">
-        <v>63</v>
+        <v>24</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C29" s="0" t="s">
-        <v>63</v>
+        <v>69</v>
       </c>
       <c r="D29" s="0" t="s">
         <v>7</v>
       </c>
       <c r="E29" s="0" t="s">
-        <v>16</v>
+        <v>37</v>
       </c>
       <c r="F29" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="0">
-        <v>13</v>
+        <v>75</v>
       </c>
       <c r="B30" s="0" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C30" s="0" t="s">
-        <v>63</v>
+        <v>69</v>
       </c>
       <c r="D30" s="0" t="s">
         <v>7</v>
       </c>
       <c r="E30" s="0" t="s">
-        <v>36</v>
+        <v>17</v>
       </c>
       <c r="F30" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="0">
-        <v>42</v>
+        <v>55</v>
       </c>
       <c r="B31" s="0" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C31" s="0" t="s">
-        <v>63</v>
+        <v>69</v>
       </c>
       <c r="D31" s="0" t="s">
         <v>7</v>
       </c>
       <c r="E31" s="0" t="s">
-        <v>57</v>
+        <v>12</v>
       </c>
       <c r="F31" s="0" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="0">
-        <v>33</v>
+        <v>56</v>
       </c>
       <c r="B32" s="0" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C32" s="0" t="s">
-        <v>63</v>
+        <v>69</v>
       </c>
       <c r="D32" s="0" t="s">
         <v>7</v>
       </c>
       <c r="E32" s="0" t="s">
-        <v>76</v>
+        <v>12</v>
       </c>
       <c r="F32" s="0" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="0">
-        <v>48</v>
+        <v>72</v>
       </c>
       <c r="B33" s="0" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C33" s="0" t="s">
-        <v>63</v>
+        <v>69</v>
       </c>
       <c r="D33" s="0" t="s">
         <v>7</v>
       </c>
       <c r="E33" s="0" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="F33" s="0" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="0">
-        <v>37</v>
+        <v>66</v>
       </c>
       <c r="B34" s="0" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C34" s="0" t="s">
-        <v>63</v>
+        <v>69</v>
       </c>
       <c r="D34" s="0" t="s">
         <v>7</v>
       </c>
       <c r="E34" s="0" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="F34" s="0" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="0">
-        <v>38</v>
+        <v>62</v>
       </c>
       <c r="B35" s="0" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C35" s="0" t="s">
-        <v>63</v>
+        <v>69</v>
       </c>
       <c r="D35" s="0" t="s">
         <v>7</v>
       </c>
       <c r="E35" s="0" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="F35" s="0" t="s">
-        <v>61</v>
+        <v>17</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="0">
-        <v>46</v>
+        <v>70</v>
       </c>
       <c r="B36" s="0" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C36" s="0" t="s">
-        <v>63</v>
+        <v>69</v>
       </c>
       <c r="D36" s="0" t="s">
         <v>7</v>
       </c>
       <c r="E36" s="0" t="s">
-        <v>101</v>
+        <v>17</v>
       </c>
       <c r="F36" s="0" t="s">
-        <v>61</v>
+        <v>17</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="0">
-        <v>45</v>
+        <v>64</v>
       </c>
       <c r="B37" s="0" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="C37" s="0" t="s">
-        <v>63</v>
+        <v>69</v>
       </c>
       <c r="D37" s="0" t="s">
         <v>7</v>
       </c>
       <c r="E37" s="0" t="s">
-        <v>57</v>
+        <v>17</v>
       </c>
       <c r="F37" s="0" t="s">
-        <v>61</v>
+        <v>17</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="0">
-        <v>44</v>
+        <v>63</v>
       </c>
       <c r="B38" s="0" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="C38" s="0" t="s">
-        <v>63</v>
+        <v>69</v>
       </c>
       <c r="D38" s="0" t="s">
         <v>7</v>
       </c>
       <c r="E38" s="0" t="s">
-        <v>57</v>
+        <v>17</v>
       </c>
       <c r="F38" s="0" t="s">
-        <v>61</v>
+        <v>17</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="0">
-        <v>41</v>
+        <v>13</v>
       </c>
       <c r="B39" s="0" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="C39" s="0" t="s">
-        <v>63</v>
+        <v>69</v>
       </c>
       <c r="D39" s="0" t="s">
         <v>7</v>
       </c>
       <c r="E39" s="0" t="s">
-        <v>57</v>
+        <v>37</v>
       </c>
       <c r="F39" s="0" t="s">
-        <v>101</v>
+        <v>17</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="0">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="B40" s="0" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="C40" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="D40" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E40" s="0" t="s">
         <v>63</v>
       </c>
-      <c r="D40" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="E40" s="0" t="s">
-        <v>20</v>
-      </c>
       <c r="F40" s="0" t="s">
-        <v>101</v>
+        <v>12</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="0">
-        <v>11</v>
+        <v>33</v>
       </c>
       <c r="B41" s="0" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="C41" s="0" t="s">
-        <v>63</v>
+        <v>69</v>
       </c>
       <c r="D41" s="0" t="s">
         <v>7</v>
       </c>
       <c r="E41" s="0" t="s">
-        <v>36</v>
+        <v>83</v>
       </c>
       <c r="F41" s="0" t="s">
-        <v>57</v>
+        <v>12</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="0">
-        <v>40</v>
+        <v>48</v>
       </c>
       <c r="B42" s="0" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="C42" s="0" t="s">
-        <v>63</v>
+        <v>69</v>
       </c>
       <c r="D42" s="0" t="s">
         <v>7</v>
       </c>
       <c r="E42" s="0" t="s">
-        <v>108</v>
+        <v>15</v>
       </c>
       <c r="F42" s="0" t="s">
-        <v>57</v>
+        <v>15</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" s="0">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B43" s="0" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="C43" s="0" t="s">
-        <v>63</v>
+        <v>69</v>
       </c>
       <c r="D43" s="0" t="s">
         <v>7</v>
       </c>
       <c r="E43" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F43" s="0" t="s">
-        <v>57</v>
+        <v>15</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" s="0">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="B44" s="0" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="C44" s="0" t="s">
-        <v>63</v>
+        <v>69</v>
       </c>
       <c r="D44" s="0" t="s">
         <v>7</v>
       </c>
       <c r="E44" s="0" t="s">
-        <v>76</v>
+        <v>21</v>
       </c>
       <c r="F44" s="0" t="s">
-        <v>20</v>
+        <v>67</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" s="0">
-        <v>31</v>
+        <v>46</v>
       </c>
       <c r="B45" s="0" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="C45" s="0" t="s">
-        <v>63</v>
+        <v>69</v>
       </c>
       <c r="D45" s="0" t="s">
         <v>7</v>
       </c>
       <c r="E45" s="0" t="s">
-        <v>76</v>
+        <v>108</v>
       </c>
       <c r="F45" s="0" t="s">
-        <v>76</v>
+        <v>67</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" s="0">
-        <v>20</v>
+        <v>45</v>
       </c>
       <c r="B46" s="0" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="C46" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="D46" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E46" s="0" t="s">
         <v>63</v>
       </c>
-      <c r="D46" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="E46" s="0" t="s">
-        <v>36</v>
-      </c>
       <c r="F46" s="0" t="s">
-        <v>76</v>
+        <v>67</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" s="0">
-        <v>9</v>
+        <v>44</v>
       </c>
       <c r="B47" s="0" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="C47" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="D47" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E47" s="0" t="s">
         <v>63</v>
       </c>
-      <c r="D47" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="E47" s="0" t="s">
-        <v>36</v>
-      </c>
       <c r="F47" s="0" t="s">
-        <v>76</v>
+        <v>67</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" s="0">
-        <v>8</v>
+        <v>41</v>
       </c>
       <c r="B48" s="0" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="C48" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="D48" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E48" s="0" t="s">
         <v>63</v>
       </c>
-      <c r="D48" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="E48" s="0" t="s">
-        <v>36</v>
-      </c>
       <c r="F48" s="0" t="s">
-        <v>76</v>
+        <v>108</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" s="0">
-        <v>4</v>
+        <v>36</v>
       </c>
       <c r="B49" s="0" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="C49" s="0" t="s">
-        <v>63</v>
+        <v>69</v>
       </c>
       <c r="D49" s="0" t="s">
         <v>7</v>
       </c>
       <c r="E49" s="0" t="s">
-        <v>36</v>
+        <v>21</v>
       </c>
       <c r="F49" s="0" t="s">
-        <v>116</v>
+        <v>108</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" s="0">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="B50" s="0" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="C50" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="D50" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E50" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="F50" s="0" t="s">
         <v>63</v>
-      </c>
-      <c r="D50" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="E50" s="0" t="s">
-        <v>36</v>
-      </c>
-      <c r="F50" s="0" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" s="0">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="B51" s="0" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="C51" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="D51" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E51" s="0" t="s">
+        <v>115</v>
+      </c>
+      <c r="F51" s="0" t="s">
         <v>63</v>
-      </c>
-      <c r="D51" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="E51" s="0" t="s">
-        <v>36</v>
-      </c>
-      <c r="F51" s="0" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" s="0">
-        <v>2</v>
+        <v>39</v>
       </c>
       <c r="B52" s="0" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="C52" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="D52" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E52" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="F52" s="0" t="s">
         <v>63</v>
-      </c>
-      <c r="D52" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="E52" s="0" t="s">
-        <v>36</v>
-      </c>
-      <c r="F52" s="0" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" s="0">
+        <v>32</v>
+      </c>
+      <c r="B53" s="0" t="s">
+        <v>117</v>
+      </c>
+      <c r="C53" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="D53" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E53" s="0" t="s">
+        <v>83</v>
+      </c>
+      <c r="F53" s="0" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" s="0">
+        <v>31</v>
+      </c>
+      <c r="B54" s="0" t="s">
+        <v>118</v>
+      </c>
+      <c r="C54" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="D54" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E54" s="0" t="s">
+        <v>83</v>
+      </c>
+      <c r="F54" s="0" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" s="0">
+        <v>20</v>
+      </c>
+      <c r="B55" s="0" t="s">
+        <v>119</v>
+      </c>
+      <c r="C55" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="D55" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E55" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="F55" s="0" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" s="0">
+        <v>9</v>
+      </c>
+      <c r="B56" s="0" t="s">
+        <v>120</v>
+      </c>
+      <c r="C56" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="D56" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E56" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="F56" s="0" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" s="0">
+        <v>8</v>
+      </c>
+      <c r="B57" s="0" t="s">
+        <v>121</v>
+      </c>
+      <c r="C57" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="D57" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E57" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="F57" s="0" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" s="0">
+        <v>4</v>
+      </c>
+      <c r="B58" s="0" t="s">
+        <v>122</v>
+      </c>
+      <c r="C58" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="D58" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E58" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="F58" s="0" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" s="0">
+        <v>3</v>
+      </c>
+      <c r="B59" s="0" t="s">
+        <v>124</v>
+      </c>
+      <c r="C59" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="D59" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E59" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="F59" s="0" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" s="0">
+        <v>30</v>
+      </c>
+      <c r="B60" s="0" t="s">
+        <v>125</v>
+      </c>
+      <c r="C60" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="D60" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E60" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="F60" s="0" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" s="0">
+        <v>2</v>
+      </c>
+      <c r="B61" s="0" t="s">
+        <v>126</v>
+      </c>
+      <c r="C61" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="D61" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E61" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="F61" s="0" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" s="0">
         <v>1</v>
       </c>
-      <c r="B53" s="0" t="s">
-        <v>120</v>
-      </c>
-      <c r="C53" s="0" t="s">
-        <v>63</v>
-      </c>
-      <c r="D53" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="E53" s="0" t="s">
-        <v>36</v>
-      </c>
-      <c r="F53" s="0" t="s">
-        <v>36</v>
+      <c r="B62" s="0" t="s">
+        <v>127</v>
+      </c>
+      <c r="C62" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="D62" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E62" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="F62" s="0" t="s">
+        <v>37</v>
       </c>
     </row>
   </sheetData>
@@ -2458,7 +2460,7 @@
         <v>2</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>121</v>
+        <v>128</v>
       </c>
       <c r="C1" s="2"/>
       <c r="D1" s="2" t="s">
@@ -2466,7 +2468,7 @@
       </c>
       <c r="E1" s="2"/>
       <c r="F1" s="2" t="s">
-        <v>122</v>
+        <v>129</v>
       </c>
     </row>
     <row r="2">
@@ -2474,24 +2476,24 @@
         <v>6</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>121</v>
+        <v>128</v>
       </c>
       <c r="D2" s="0" t="s">
         <v>7</v>
       </c>
       <c r="F2" s="0">
-        <v>108</v>
+        <v>113</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="0" t="s">
-        <v>63</v>
+        <v>69</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>123</v>
+        <v>130</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>124</v>
+        <v>131</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
refactor: remove old FindRegions methods
</commit_message>
<xml_diff>
--- a/paint_todo.xlsx
+++ b/paint_todo.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="138">
   <si>
     <t>Id</t>
   </si>
@@ -518,6 +518,15 @@
 - how long to union set each pixel together?
 looks like UnionWith operations are the problem
 - fixed it!</t>
+  </si>
+  <si>
+    <t>remove old code for old find-regions logic</t>
+  </si>
+  <si>
+    <t>use mouse scroll for zoom in/out</t>
+  </si>
+  <si>
+    <t>drag and drop image to move it</t>
   </si>
 </sst>
 </file>
@@ -570,7 +579,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:F36"/>
+  <dimension ref="A1:F38"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -851,10 +860,10 @@
     </row>
     <row r="17">
       <c r="A17" s="0">
-        <v>81</v>
+        <v>115</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>45</v>
+        <v>136</v>
       </c>
       <c r="C17" s="0" t="s">
         <v>6</v>
@@ -863,15 +872,15 @@
         <v>7</v>
       </c>
       <c r="E17" s="0" t="s">
-        <v>17</v>
+        <v>8</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="0">
-        <v>109</v>
+        <v>116</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>46</v>
+        <v>137</v>
       </c>
       <c r="C18" s="0" t="s">
         <v>6</v>
@@ -880,15 +889,15 @@
         <v>7</v>
       </c>
       <c r="E18" s="0" t="s">
-        <v>47</v>
+        <v>8</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="0">
-        <v>110</v>
+        <v>81</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="C19" s="0" t="s">
         <v>6</v>
@@ -897,15 +906,15 @@
         <v>7</v>
       </c>
       <c r="E19" s="0" t="s">
-        <v>47</v>
+        <v>17</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="0">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C20" s="0" t="s">
         <v>6</v>
@@ -914,15 +923,15 @@
         <v>7</v>
       </c>
       <c r="E20" s="0" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="0">
-        <v>82</v>
+        <v>110</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="C21" s="0" t="s">
         <v>6</v>
@@ -931,15 +940,15 @@
         <v>7</v>
       </c>
       <c r="E21" s="0" t="s">
-        <v>17</v>
+        <v>47</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="0">
-        <v>83</v>
+        <v>108</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="C22" s="0" t="s">
         <v>6</v>
@@ -948,15 +957,15 @@
         <v>7</v>
       </c>
       <c r="E22" s="0" t="s">
-        <v>17</v>
+        <v>50</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="0">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C23" s="0" t="s">
         <v>6</v>
@@ -970,10 +979,10 @@
     </row>
     <row r="24">
       <c r="A24" s="0">
-        <v>112</v>
+        <v>83</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C24" s="0" t="s">
         <v>6</v>
@@ -982,15 +991,15 @@
         <v>7</v>
       </c>
       <c r="E24" s="0" t="s">
-        <v>47</v>
+        <v>17</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="0">
-        <v>25</v>
+        <v>84</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C25" s="0" t="s">
         <v>6</v>
@@ -999,15 +1008,15 @@
         <v>7</v>
       </c>
       <c r="E25" s="0" t="s">
-        <v>37</v>
+        <v>17</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="0">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C26" s="0" t="s">
         <v>6</v>
@@ -1021,10 +1030,10 @@
     </row>
     <row r="27">
       <c r="A27" s="0">
-        <v>57</v>
+        <v>25</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C27" s="0" t="s">
         <v>6</v>
@@ -1033,15 +1042,15 @@
         <v>7</v>
       </c>
       <c r="E27" s="0" t="s">
-        <v>17</v>
+        <v>37</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="0">
-        <v>65</v>
+        <v>111</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C28" s="0" t="s">
         <v>6</v>
@@ -1050,15 +1059,15 @@
         <v>7</v>
       </c>
       <c r="E28" s="0" t="s">
-        <v>17</v>
+        <v>47</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="0">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C29" s="0" t="s">
         <v>6</v>
@@ -1072,10 +1081,10 @@
     </row>
     <row r="30">
       <c r="A30" s="0">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="B30" s="0" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C30" s="0" t="s">
         <v>6</v>
@@ -1089,10 +1098,10 @@
     </row>
     <row r="31">
       <c r="A31" s="0">
-        <v>26</v>
+        <v>58</v>
       </c>
       <c r="B31" s="0" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C31" s="0" t="s">
         <v>6</v>
@@ -1101,15 +1110,15 @@
         <v>7</v>
       </c>
       <c r="E31" s="0" t="s">
-        <v>37</v>
+        <v>17</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="0">
-        <v>43</v>
+        <v>61</v>
       </c>
       <c r="B32" s="0" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C32" s="0" t="s">
         <v>6</v>
@@ -1118,15 +1127,15 @@
         <v>7</v>
       </c>
       <c r="E32" s="0" t="s">
-        <v>63</v>
+        <v>17</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="0">
-        <v>74</v>
+        <v>26</v>
       </c>
       <c r="B33" s="0" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="C33" s="0" t="s">
         <v>6</v>
@@ -1135,15 +1144,15 @@
         <v>7</v>
       </c>
       <c r="E33" s="0" t="s">
-        <v>17</v>
+        <v>37</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="0">
-        <v>29</v>
+        <v>43</v>
       </c>
       <c r="B34" s="0" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="C34" s="0" t="s">
         <v>6</v>
@@ -1152,15 +1161,15 @@
         <v>7</v>
       </c>
       <c r="E34" s="0" t="s">
-        <v>37</v>
+        <v>63</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="0">
-        <v>47</v>
+        <v>74</v>
       </c>
       <c r="B35" s="0" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C35" s="0" t="s">
         <v>6</v>
@@ -1169,23 +1178,57 @@
         <v>7</v>
       </c>
       <c r="E35" s="0" t="s">
-        <v>67</v>
+        <v>17</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="0">
+        <v>29</v>
+      </c>
+      <c r="B36" s="0" t="s">
+        <v>65</v>
+      </c>
+      <c r="C36" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D36" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E36" s="0" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" s="0">
+        <v>47</v>
+      </c>
+      <c r="B37" s="0" t="s">
+        <v>66</v>
+      </c>
+      <c r="C37" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D37" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E37" s="0" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" s="0">
         <v>60</v>
       </c>
-      <c r="B36" s="0" t="s">
+      <c r="B38" s="0" t="s">
         <v>68</v>
       </c>
-      <c r="C36" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="D36" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="E36" s="0" t="s">
+      <c r="C38" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D38" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E38" s="0" t="s">
         <v>17</v>
       </c>
     </row>
@@ -1196,7 +1239,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:F62"/>
+  <dimension ref="A1:F63"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1224,10 +1267,10 @@
     </row>
     <row r="2">
       <c r="A2" s="0">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="C2" s="0" t="s">
         <v>69</v>
@@ -1244,10 +1287,10 @@
     </row>
     <row r="3">
       <c r="A3" s="0">
-        <v>78</v>
+        <v>113</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>34</v>
+        <v>134</v>
       </c>
       <c r="C3" s="0" t="s">
         <v>69</v>
@@ -1256,7 +1299,7 @@
         <v>7</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>17</v>
+        <v>8</v>
       </c>
       <c r="F3" s="0" t="s">
         <v>8</v>
@@ -1264,10 +1307,10 @@
     </row>
     <row r="4">
       <c r="A4" s="0">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C4" s="0" t="s">
         <v>69</v>
@@ -1284,10 +1327,10 @@
     </row>
     <row r="5">
       <c r="A5" s="0">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="C5" s="0" t="s">
         <v>69</v>
@@ -1304,10 +1347,10 @@
     </row>
     <row r="6">
       <c r="A6" s="0">
-        <v>106</v>
+        <v>85</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="C6" s="0" t="s">
         <v>69</v>
@@ -1316,7 +1359,7 @@
         <v>7</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="F6" s="0" t="s">
         <v>8</v>
@@ -1324,10 +1367,10 @@
     </row>
     <row r="7">
       <c r="A7" s="0">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="C7" s="0" t="s">
         <v>69</v>
@@ -1344,10 +1387,10 @@
     </row>
     <row r="8">
       <c r="A8" s="0">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="C8" s="0" t="s">
         <v>69</v>
@@ -1364,10 +1407,10 @@
     </row>
     <row r="9">
       <c r="A9" s="0">
-        <v>49</v>
+        <v>107</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="C9" s="0" t="s">
         <v>69</v>
@@ -1376,7 +1419,7 @@
         <v>7</v>
       </c>
       <c r="E9" s="0" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="F9" s="0" t="s">
         <v>8</v>
@@ -1384,10 +1427,10 @@
     </row>
     <row r="10">
       <c r="A10" s="0">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>70</v>
+        <v>18</v>
       </c>
       <c r="C10" s="0" t="s">
         <v>69</v>
@@ -1396,7 +1439,7 @@
         <v>7</v>
       </c>
       <c r="E10" s="0" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="F10" s="0" t="s">
         <v>8</v>
@@ -1404,10 +1447,10 @@
     </row>
     <row r="11">
       <c r="A11" s="0">
-        <v>92</v>
+        <v>54</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C11" s="0" t="s">
         <v>69</v>
@@ -1416,18 +1459,18 @@
         <v>7</v>
       </c>
       <c r="E11" s="0" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="F11" s="0" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="0">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C12" s="0" t="s">
         <v>69</v>
@@ -1436,7 +1479,7 @@
         <v>7</v>
       </c>
       <c r="E12" s="0" t="s">
-        <v>73</v>
+        <v>10</v>
       </c>
       <c r="F12" s="0" t="s">
         <v>10</v>
@@ -1444,10 +1487,10 @@
     </row>
     <row r="13">
       <c r="A13" s="0">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C13" s="0" t="s">
         <v>69</v>
@@ -1464,10 +1507,10 @@
     </row>
     <row r="14">
       <c r="A14" s="0">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C14" s="0" t="s">
         <v>69</v>
@@ -1476,7 +1519,7 @@
         <v>7</v>
       </c>
       <c r="E14" s="0" t="s">
-        <v>17</v>
+        <v>73</v>
       </c>
       <c r="F14" s="0" t="s">
         <v>10</v>
@@ -1484,10 +1527,10 @@
     </row>
     <row r="15">
       <c r="A15" s="0">
-        <v>97</v>
+        <v>86</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C15" s="0" t="s">
         <v>69</v>
@@ -1496,7 +1539,7 @@
         <v>7</v>
       </c>
       <c r="E15" s="0" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="F15" s="0" t="s">
         <v>10</v>
@@ -1504,10 +1547,10 @@
     </row>
     <row r="16">
       <c r="A16" s="0">
-        <v>21</v>
+        <v>97</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C16" s="0" t="s">
         <v>69</v>
@@ -1516,7 +1559,7 @@
         <v>7</v>
       </c>
       <c r="E16" s="0" t="s">
-        <v>37</v>
+        <v>10</v>
       </c>
       <c r="F16" s="0" t="s">
         <v>10</v>
@@ -1524,10 +1567,10 @@
     </row>
     <row r="17">
       <c r="A17" s="0">
-        <v>100</v>
+        <v>21</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C17" s="0" t="s">
         <v>69</v>
@@ -1536,7 +1579,7 @@
         <v>7</v>
       </c>
       <c r="E17" s="0" t="s">
-        <v>10</v>
+        <v>37</v>
       </c>
       <c r="F17" s="0" t="s">
         <v>10</v>
@@ -1544,10 +1587,10 @@
     </row>
     <row r="18">
       <c r="A18" s="0">
-        <v>87</v>
+        <v>100</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C18" s="0" t="s">
         <v>69</v>
@@ -1556,7 +1599,7 @@
         <v>7</v>
       </c>
       <c r="E18" s="0" t="s">
-        <v>73</v>
+        <v>10</v>
       </c>
       <c r="F18" s="0" t="s">
         <v>10</v>
@@ -1564,10 +1607,10 @@
     </row>
     <row r="19">
       <c r="A19" s="0">
-        <v>94</v>
+        <v>87</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C19" s="0" t="s">
         <v>69</v>
@@ -1576,7 +1619,7 @@
         <v>7</v>
       </c>
       <c r="E19" s="0" t="s">
-        <v>10</v>
+        <v>73</v>
       </c>
       <c r="F19" s="0" t="s">
         <v>10</v>
@@ -1584,10 +1627,10 @@
     </row>
     <row r="20">
       <c r="A20" s="0">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C20" s="0" t="s">
         <v>69</v>
@@ -1604,10 +1647,10 @@
     </row>
     <row r="21">
       <c r="A21" s="0">
-        <v>34</v>
+        <v>93</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C21" s="0" t="s">
         <v>69</v>
@@ -1616,7 +1659,7 @@
         <v>7</v>
       </c>
       <c r="E21" s="0" t="s">
-        <v>83</v>
+        <v>10</v>
       </c>
       <c r="F21" s="0" t="s">
         <v>10</v>
@@ -1624,10 +1667,10 @@
     </row>
     <row r="22">
       <c r="A22" s="0">
-        <v>50</v>
+        <v>34</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C22" s="0" t="s">
         <v>69</v>
@@ -1636,7 +1679,7 @@
         <v>7</v>
       </c>
       <c r="E22" s="0" t="s">
-        <v>15</v>
+        <v>83</v>
       </c>
       <c r="F22" s="0" t="s">
         <v>10</v>
@@ -1644,10 +1687,10 @@
     </row>
     <row r="23">
       <c r="A23" s="0">
-        <v>89</v>
+        <v>50</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C23" s="0" t="s">
         <v>69</v>
@@ -1656,18 +1699,18 @@
         <v>7</v>
       </c>
       <c r="E23" s="0" t="s">
-        <v>73</v>
+        <v>15</v>
       </c>
       <c r="F23" s="0" t="s">
-        <v>73</v>
+        <v>10</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="0">
-        <v>59</v>
+        <v>89</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C24" s="0" t="s">
         <v>69</v>
@@ -1676,7 +1719,7 @@
         <v>7</v>
       </c>
       <c r="E24" s="0" t="s">
-        <v>17</v>
+        <v>73</v>
       </c>
       <c r="F24" s="0" t="s">
         <v>73</v>
@@ -1684,10 +1727,10 @@
     </row>
     <row r="25">
       <c r="A25" s="0">
-        <v>69</v>
+        <v>59</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C25" s="0" t="s">
         <v>69</v>
@@ -1704,10 +1747,10 @@
     </row>
     <row r="26">
       <c r="A26" s="0">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C26" s="0" t="s">
         <v>69</v>
@@ -1724,10 +1767,10 @@
     </row>
     <row r="27">
       <c r="A27" s="0">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C27" s="0" t="s">
         <v>69</v>
@@ -1744,10 +1787,10 @@
     </row>
     <row r="28">
       <c r="A28" s="0">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C28" s="0" t="s">
         <v>69</v>
@@ -1759,15 +1802,15 @@
         <v>17</v>
       </c>
       <c r="F28" s="0" t="s">
-        <v>17</v>
+        <v>73</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="0">
-        <v>24</v>
+        <v>71</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C29" s="0" t="s">
         <v>69</v>
@@ -1776,7 +1819,7 @@
         <v>7</v>
       </c>
       <c r="E29" s="0" t="s">
-        <v>37</v>
+        <v>17</v>
       </c>
       <c r="F29" s="0" t="s">
         <v>17</v>
@@ -1784,10 +1827,10 @@
     </row>
     <row r="30">
       <c r="A30" s="0">
-        <v>75</v>
+        <v>24</v>
       </c>
       <c r="B30" s="0" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C30" s="0" t="s">
         <v>69</v>
@@ -1796,7 +1839,7 @@
         <v>7</v>
       </c>
       <c r="E30" s="0" t="s">
-        <v>17</v>
+        <v>37</v>
       </c>
       <c r="F30" s="0" t="s">
         <v>17</v>
@@ -1804,10 +1847,10 @@
     </row>
     <row r="31">
       <c r="A31" s="0">
-        <v>55</v>
+        <v>75</v>
       </c>
       <c r="B31" s="0" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C31" s="0" t="s">
         <v>69</v>
@@ -1816,7 +1859,7 @@
         <v>7</v>
       </c>
       <c r="E31" s="0" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="F31" s="0" t="s">
         <v>17</v>
@@ -1824,10 +1867,10 @@
     </row>
     <row r="32">
       <c r="A32" s="0">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B32" s="0" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C32" s="0" t="s">
         <v>69</v>
@@ -1844,10 +1887,10 @@
     </row>
     <row r="33">
       <c r="A33" s="0">
-        <v>72</v>
+        <v>56</v>
       </c>
       <c r="B33" s="0" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C33" s="0" t="s">
         <v>69</v>
@@ -1856,7 +1899,7 @@
         <v>7</v>
       </c>
       <c r="E33" s="0" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="F33" s="0" t="s">
         <v>17</v>
@@ -1864,10 +1907,10 @@
     </row>
     <row r="34">
       <c r="A34" s="0">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="B34" s="0" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C34" s="0" t="s">
         <v>69</v>
@@ -1884,10 +1927,10 @@
     </row>
     <row r="35">
       <c r="A35" s="0">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="B35" s="0" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C35" s="0" t="s">
         <v>69</v>
@@ -1904,10 +1947,10 @@
     </row>
     <row r="36">
       <c r="A36" s="0">
-        <v>70</v>
+        <v>62</v>
       </c>
       <c r="B36" s="0" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C36" s="0" t="s">
         <v>69</v>
@@ -1924,10 +1967,10 @@
     </row>
     <row r="37">
       <c r="A37" s="0">
-        <v>64</v>
+        <v>70</v>
       </c>
       <c r="B37" s="0" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C37" s="0" t="s">
         <v>69</v>
@@ -1944,10 +1987,10 @@
     </row>
     <row r="38">
       <c r="A38" s="0">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B38" s="0" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C38" s="0" t="s">
         <v>69</v>
@@ -1964,10 +2007,10 @@
     </row>
     <row r="39">
       <c r="A39" s="0">
-        <v>13</v>
+        <v>63</v>
       </c>
       <c r="B39" s="0" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C39" s="0" t="s">
         <v>69</v>
@@ -1976,7 +2019,7 @@
         <v>7</v>
       </c>
       <c r="E39" s="0" t="s">
-        <v>37</v>
+        <v>17</v>
       </c>
       <c r="F39" s="0" t="s">
         <v>17</v>
@@ -1984,10 +2027,10 @@
     </row>
     <row r="40">
       <c r="A40" s="0">
-        <v>42</v>
+        <v>13</v>
       </c>
       <c r="B40" s="0" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C40" s="0" t="s">
         <v>69</v>
@@ -1996,18 +2039,18 @@
         <v>7</v>
       </c>
       <c r="E40" s="0" t="s">
-        <v>63</v>
+        <v>37</v>
       </c>
       <c r="F40" s="0" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="0">
-        <v>33</v>
+        <v>42</v>
       </c>
       <c r="B41" s="0" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C41" s="0" t="s">
         <v>69</v>
@@ -2016,7 +2059,7 @@
         <v>7</v>
       </c>
       <c r="E41" s="0" t="s">
-        <v>83</v>
+        <v>63</v>
       </c>
       <c r="F41" s="0" t="s">
         <v>12</v>
@@ -2024,10 +2067,10 @@
     </row>
     <row r="42">
       <c r="A42" s="0">
-        <v>48</v>
+        <v>33</v>
       </c>
       <c r="B42" s="0" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C42" s="0" t="s">
         <v>69</v>
@@ -2036,18 +2079,18 @@
         <v>7</v>
       </c>
       <c r="E42" s="0" t="s">
-        <v>15</v>
+        <v>83</v>
       </c>
       <c r="F42" s="0" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" s="0">
-        <v>37</v>
+        <v>48</v>
       </c>
       <c r="B43" s="0" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C43" s="0" t="s">
         <v>69</v>
@@ -2056,7 +2099,7 @@
         <v>7</v>
       </c>
       <c r="E43" s="0" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="F43" s="0" t="s">
         <v>15</v>
@@ -2064,10 +2107,10 @@
     </row>
     <row r="44">
       <c r="A44" s="0">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B44" s="0" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C44" s="0" t="s">
         <v>69</v>
@@ -2079,15 +2122,15 @@
         <v>21</v>
       </c>
       <c r="F44" s="0" t="s">
-        <v>67</v>
+        <v>15</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" s="0">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="B45" s="0" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C45" s="0" t="s">
         <v>69</v>
@@ -2096,7 +2139,7 @@
         <v>7</v>
       </c>
       <c r="E45" s="0" t="s">
-        <v>108</v>
+        <v>21</v>
       </c>
       <c r="F45" s="0" t="s">
         <v>67</v>
@@ -2104,10 +2147,10 @@
     </row>
     <row r="46">
       <c r="A46" s="0">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B46" s="0" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C46" s="0" t="s">
         <v>69</v>
@@ -2116,7 +2159,7 @@
         <v>7</v>
       </c>
       <c r="E46" s="0" t="s">
-        <v>63</v>
+        <v>108</v>
       </c>
       <c r="F46" s="0" t="s">
         <v>67</v>
@@ -2124,10 +2167,10 @@
     </row>
     <row r="47">
       <c r="A47" s="0">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B47" s="0" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C47" s="0" t="s">
         <v>69</v>
@@ -2144,10 +2187,10 @@
     </row>
     <row r="48">
       <c r="A48" s="0">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="B48" s="0" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C48" s="0" t="s">
         <v>69</v>
@@ -2159,15 +2202,15 @@
         <v>63</v>
       </c>
       <c r="F48" s="0" t="s">
-        <v>108</v>
+        <v>67</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" s="0">
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="B49" s="0" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C49" s="0" t="s">
         <v>69</v>
@@ -2176,7 +2219,7 @@
         <v>7</v>
       </c>
       <c r="E49" s="0" t="s">
-        <v>21</v>
+        <v>63</v>
       </c>
       <c r="F49" s="0" t="s">
         <v>108</v>
@@ -2184,10 +2227,10 @@
     </row>
     <row r="50">
       <c r="A50" s="0">
-        <v>11</v>
+        <v>36</v>
       </c>
       <c r="B50" s="0" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C50" s="0" t="s">
         <v>69</v>
@@ -2196,18 +2239,18 @@
         <v>7</v>
       </c>
       <c r="E50" s="0" t="s">
-        <v>37</v>
+        <v>21</v>
       </c>
       <c r="F50" s="0" t="s">
-        <v>63</v>
+        <v>108</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" s="0">
-        <v>40</v>
+        <v>11</v>
       </c>
       <c r="B51" s="0" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C51" s="0" t="s">
         <v>69</v>
@@ -2216,7 +2259,7 @@
         <v>7</v>
       </c>
       <c r="E51" s="0" t="s">
-        <v>115</v>
+        <v>37</v>
       </c>
       <c r="F51" s="0" t="s">
         <v>63</v>
@@ -2224,10 +2267,10 @@
     </row>
     <row r="52">
       <c r="A52" s="0">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B52" s="0" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="C52" s="0" t="s">
         <v>69</v>
@@ -2236,7 +2279,7 @@
         <v>7</v>
       </c>
       <c r="E52" s="0" t="s">
-        <v>21</v>
+        <v>115</v>
       </c>
       <c r="F52" s="0" t="s">
         <v>63</v>
@@ -2244,10 +2287,10 @@
     </row>
     <row r="53">
       <c r="A53" s="0">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="B53" s="0" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C53" s="0" t="s">
         <v>69</v>
@@ -2256,18 +2299,18 @@
         <v>7</v>
       </c>
       <c r="E53" s="0" t="s">
-        <v>83</v>
+        <v>21</v>
       </c>
       <c r="F53" s="0" t="s">
-        <v>21</v>
+        <v>63</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" s="0">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B54" s="0" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C54" s="0" t="s">
         <v>69</v>
@@ -2279,15 +2322,15 @@
         <v>83</v>
       </c>
       <c r="F54" s="0" t="s">
-        <v>83</v>
+        <v>21</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" s="0">
-        <v>20</v>
+        <v>31</v>
       </c>
       <c r="B55" s="0" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C55" s="0" t="s">
         <v>69</v>
@@ -2296,7 +2339,7 @@
         <v>7</v>
       </c>
       <c r="E55" s="0" t="s">
-        <v>37</v>
+        <v>83</v>
       </c>
       <c r="F55" s="0" t="s">
         <v>83</v>
@@ -2304,10 +2347,10 @@
     </row>
     <row r="56">
       <c r="A56" s="0">
-        <v>9</v>
+        <v>20</v>
       </c>
       <c r="B56" s="0" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C56" s="0" t="s">
         <v>69</v>
@@ -2324,10 +2367,10 @@
     </row>
     <row r="57">
       <c r="A57" s="0">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B57" s="0" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C57" s="0" t="s">
         <v>69</v>
@@ -2344,10 +2387,10 @@
     </row>
     <row r="58">
       <c r="A58" s="0">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="B58" s="0" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C58" s="0" t="s">
         <v>69</v>
@@ -2359,15 +2402,15 @@
         <v>37</v>
       </c>
       <c r="F58" s="0" t="s">
-        <v>123</v>
+        <v>83</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" s="0">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B59" s="0" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="C59" s="0" t="s">
         <v>69</v>
@@ -2379,15 +2422,15 @@
         <v>37</v>
       </c>
       <c r="F59" s="0" t="s">
-        <v>37</v>
+        <v>123</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" s="0">
-        <v>30</v>
+        <v>3</v>
       </c>
       <c r="B60" s="0" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C60" s="0" t="s">
         <v>69</v>
@@ -2404,10 +2447,10 @@
     </row>
     <row r="61">
       <c r="A61" s="0">
-        <v>2</v>
+        <v>30</v>
       </c>
       <c r="B61" s="0" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C61" s="0" t="s">
         <v>69</v>
@@ -2424,21 +2467,41 @@
     </row>
     <row r="62">
       <c r="A62" s="0">
+        <v>2</v>
+      </c>
+      <c r="B62" s="0" t="s">
+        <v>126</v>
+      </c>
+      <c r="C62" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="D62" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E62" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="F62" s="0" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" s="0">
         <v>1</v>
       </c>
-      <c r="B62" s="0" t="s">
+      <c r="B63" s="0" t="s">
         <v>127</v>
       </c>
-      <c r="C62" s="0" t="s">
-        <v>69</v>
-      </c>
-      <c r="D62" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="E62" s="0" t="s">
-        <v>37</v>
-      </c>
-      <c r="F62" s="0" t="s">
+      <c r="C63" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="D63" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E63" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="F63" s="0" t="s">
         <v>37</v>
       </c>
     </row>
@@ -2482,7 +2545,7 @@
         <v>7</v>
       </c>
       <c r="F2" s="0">
-        <v>113</v>
+        <v>116</v>
       </c>
     </row>
     <row r="3">

</xml_diff>

<commit_message>
prompt to save changes before closing image
</commit_message>
<xml_diff>
--- a/paint_todo.xlsx
+++ b/paint_todo.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="138">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="128">
   <si>
     <t>Id</t>
   </si>
@@ -31,11 +31,7 @@
     <t>Created</t>
   </si>
   <si>
-    <t xml:space="preserve">benchmarking:
-- how long to simply count pixels?
-- how long to create 1 Point per pixel?
-- how long to GetPixel for each pixel?
-- how long to union set each pixel together?</t>
+    <t>walk through Edit Palette panels and events and make sure its all right</t>
   </si>
   <si>
     <t>Todo</t>
@@ -44,28 +40,10 @@
     <t>Task</t>
   </si>
   <si>
-    <t>9/10/2018</t>
-  </si>
-  <si>
-    <t>continue refactoring business logic out of RequestColorWorker</t>
-  </si>
-  <si>
     <t>8/26/2018</t>
   </si>
   <si>
-    <t xml:space="preserve">prompt to save if image has changed since last save
-- on closing program
-- on opening new image
-Add this tracking to MasterImage class</t>
-  </si>
-  <si>
-    <t>8/23/2018</t>
-  </si>
-  <si>
-    <t>walk through Edit Palette panels and events and make sure its all right</t>
-  </si>
-  <si>
-    <t>replace Rabbit with smaller and better divided image</t>
+    <t>replace Rabbit with smaller and better divided sample image</t>
   </si>
   <si>
     <t>8/22/2018</t>
@@ -75,13 +53,6 @@
   </si>
   <si>
     <t>8/24/2018</t>
-  </si>
-  <si>
-    <t xml:space="preserve">applying color is pretty fast even on large image
-but removing the color is really slow</t>
-  </si>
-  <si>
-    <t>in public projects, make a Release directory to put each Version into</t>
   </si>
   <si>
     <t xml:space="preserve">set and check tolerance for "black" and "white"
@@ -92,57 +63,8 @@
     <t>8/12/2018</t>
   </si>
   <si>
-    <t>make the withouthaste,com/thanks page with link to Patron</t>
-  </si>
-  <si>
-    <t>8/30/2018</t>
-  </si>
-  <si>
-    <t xml:space="preserve">libraries:
-if library relies on specific verion of another library, that needs to be documented</t>
-  </si>
-  <si>
-    <t xml:space="preserve">documentation: include request for sample palette files for the specific formats/color spaces I can't verify because I don't have a test file to load
-- maybe in the actual error messages from the library, too
-- like, send me the file you are trying to read so I can add support for it</t>
-  </si>
-  <si>
-    <t>put links to license on library pages</t>
-  </si>
-  <si>
-    <t>what license should the libraries and this program be under?</t>
-  </si>
-  <si>
-    <t>8/29/2018</t>
-  </si>
-  <si>
-    <t xml:space="preserve">make more standard icons available in IconManager
-- new file
-- open file
-- save
-- cut, copy, paste
-- search</t>
-  </si>
-  <si>
-    <t>8/28/2018</t>
-  </si>
-  <si>
-    <t>put in top of documentation that program is being actively developed, so open to bug reports and feature requests</t>
-  </si>
-  <si>
     <t xml:space="preserve">in Paint documenation
 describe the use-case of converting between palette formats: open file, edit palette, save as new format</t>
-  </si>
-  <si>
-    <t>full documentation of support library Colors</t>
-  </si>
-  <si>
-    <t>full documentation of support library GUI</t>
-  </si>
-  <si>
-    <t xml:space="preserve">in documentation
-recommend user keeps an original b/w copy to go back to
-if conversion errors build up with lots of editing</t>
   </si>
   <si>
     <t xml:space="preserve">include support contact information
@@ -176,6 +98,15 @@
   </si>
   <si>
     <t>make sure all TODOs are cleared from project</t>
+  </si>
+  <si>
+    <t>use mouse scroll for zoom in/out</t>
+  </si>
+  <si>
+    <t>9/10/2018</t>
+  </si>
+  <si>
+    <t>drag and drop image to move it</t>
   </si>
   <si>
     <t>VERSION 1.5: PROJECTS</t>
@@ -272,243 +203,19 @@
     <t>Done</t>
   </si>
   <si>
-    <t xml:space="preserve">make a MasterImage class
-that one-time figures out all the regions in a background thread
-and provides that data to the color worker
-- A: finding 1 region at a time benchmarked at 10.7sec for tea shop cat - benchmarked at &gt;15min for rabbit
-- B: leading edge method still &gt;22min for rabbit and it was 10min for the cat (verified A still runs in 10sec on cat)</t>
-  </si>
-  <si>
-    <t>eyedrop tool: select color in palette, by selecting color on image (select palest color in colored region)</t>
-  </si>
-  <si>
-    <t>name all Settings properties in OneImageForm with prefix "Setting" for consistency</t>
-  </si>
-  <si>
-    <t>8/25/2018</t>
-  </si>
-  <si>
-    <t xml:space="preserve">to be consistent with System.Convert naming standards
-update ConvertColors
-- To&lt;Type&gt;(FromType)
-- &lt;FromType&gt;To&lt;Type&gt;(list of generic params)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">bug: Palette &gt; New &gt; Done
-get error because no filename to open in main form</t>
-  </si>
-  <si>
-    <t>refactor Edit Palette Panel (and everything under it) to WithoutHaste.Windows.GUI</t>
-  </si>
-  <si>
-    <t xml:space="preserve">when resizing windows, default behavior is to keep the same section of image in the viewing pane
-- so expanding window would in effect zoom in
-CANCELLED</t>
-  </si>
-  <si>
-    <t>refactor all panels to use proper events instead of delegate properties</t>
-  </si>
-  <si>
-    <t>refactor all history actions to use proper events instead of delegate properties</t>
-  </si>
-  <si>
-    <t xml:space="preserve">keyboard shortcuts:
-open (image)
-save (image or palette)
-undo (image or palette)
-redo (image or palette)</t>
-  </si>
-  <si>
-    <t>file &gt; Save</t>
-  </si>
-  <si>
-    <t>when zooming, if a scroll bar is all the way to min or max, keep it there</t>
-  </si>
-  <si>
-    <t>8/11/2018</t>
-  </si>
-  <si>
-    <t xml:space="preserve">design test that generates value scale for many different colors, easy to scan with the eye
-- for instance, sometimes the adjusted color gets darker than the lightest "black", leaving a paler ring around it</t>
-  </si>
-  <si>
-    <t xml:space="preserve">having problems with imprecise color format conversions
-it's really important they be perfectly reversible</t>
-  </si>
-  <si>
-    <t xml:space="preserve">refactor WithoutHaste.Drawing.Colors HSV to use ints instead of floats (0-360, 0-100, 0-100)
-CANCELLED
-more research online shows that float is proper for HSV</t>
-  </si>
-  <si>
-    <t>new color: enter an hsv value</t>
-  </si>
-  <si>
-    <t>new color: enter a hexadecimal value</t>
-  </si>
-  <si>
-    <t>new color: enter an rgb value</t>
-  </si>
-  <si>
-    <t>edit palette: display rgb/hexdecimal/hsv values of selected color</t>
-  </si>
-  <si>
-    <t xml:space="preserve">remember windows size from last closing
-- full screen vs not
-- default not-full-screen size
-open with this size</t>
-  </si>
-  <si>
-    <t>remember last open palette and reopen it next time program starts</t>
-  </si>
-  <si>
-    <t>use SwatchPanel object for main palette display</t>
-  </si>
-  <si>
-    <t>change names of dialog-only forms to XDialog</t>
-  </si>
-  <si>
-    <t>entirely new palette</t>
-  </si>
-  <si>
-    <t>edit palette: undo/redo all changes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">edit palette: save changes
-see updates in main form
-- save or lose changes on close</t>
-  </si>
-  <si>
-    <t>edit palette: add new color, but start from existing color</t>
-  </si>
-  <si>
-    <t>edit palette: edit color in place</t>
-  </si>
-  <si>
-    <t>edit palette: remove color</t>
-  </si>
-  <si>
-    <t xml:space="preserve">open edit palette mode
-- add swatches</t>
-  </si>
-  <si>
-    <t>bug: expanded palette covers part of picturebox and statuspanel</t>
-  </si>
-  <si>
-    <t>undo, redo coloring a section on the image</t>
-  </si>
-  <si>
-    <t xml:space="preserve">on error popup:
-display all nested errors</t>
-  </si>
-  <si>
-    <t xml:space="preserve">apply color over color without changing underlying values
-- change section back to grayscale
-- then to the new color</t>
-  </si>
-  <si>
-    <t>support applying color while zoomed in or out</t>
-  </si>
-  <si>
-    <t>add "100%" size button</t>
-  </si>
-  <si>
-    <t>8/16/2018</t>
-  </si>
-  <si>
-    <t xml:space="preserve">display closable modal "Please Wait" while coloring image
-- with "Cancel Color" option that will stop the thread and cancel the changes
-UPDATED: show status bar message</t>
-  </si>
-  <si>
-    <t xml:space="preserve">move coloring operations into another thread
-- queue incoming commands
-- handle one at a time in another thread, updating display between each one</t>
-  </si>
-  <si>
-    <t>bug: on some colors (oranges esp.) adjusting the saturation gives a too bright color - keep it in the gray range</t>
-  </si>
-  <si>
-    <t>what to rename ColorPalette library to so it does not conflict with object ColorPalette?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">save changes to image
-- bitmap
-- png
-- jpg</t>
-  </si>
-  <si>
-    <t>zoom in needs to keep pixels clear instead of letting it blur together</t>
-  </si>
-  <si>
-    <t>8/13/2018</t>
-  </si>
-  <si>
-    <t xml:space="preserve">bug: it isn't actually keeping the grayscale
-- wow, spent days debugging and it was just a test-line outside the area I was looking at</t>
-  </si>
-  <si>
-    <t>fill in a section of color on the image</t>
-  </si>
-  <si>
-    <t>select a palette color</t>
-  </si>
-  <si>
-    <t xml:space="preserve">program preference setting: how wide the palette area is
-- let user drag and drop divider to change palette width
-- minimum is 3 swatches, max is maybe 12
-- save setting and reuse on next progam open
-(maybe instead of drag-n-drop the border, there are little &lt; &gt; arrow buttons that will expand/contract space one swatch at a time)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">display a default palette along the side of the window
-- give it a vertical scroll when needed</t>
-  </si>
-  <si>
-    <t xml:space="preserve">build 1 to 3 default palettes
-- downloaded some Photoshop palettes</t>
-  </si>
-  <si>
-    <t>scroll horizontal and vertical when zoomed in</t>
-  </si>
-  <si>
-    <t>8/10/2018</t>
-  </si>
-  <si>
-    <t>zoom in and out of image</t>
-  </si>
-  <si>
-    <t>resize image to fit window as it resizes</t>
-  </si>
-  <si>
-    <t>open an image and display it in a window at default size</t>
-  </si>
-  <si>
-    <t xml:space="preserve">new window's console app
-- version 0 until minimum viable is complete</t>
-  </si>
-  <si>
-    <t>Active</t>
-  </si>
-  <si>
-    <t>Max Id</t>
-  </si>
-  <si>
-    <t>Inactive</t>
-  </si>
-  <si>
-    <t>Bug</t>
-  </si>
-  <si>
-    <t>replace Rabbit with smaller and better divided sample image</t>
-  </si>
-  <si>
-    <t xml:space="preserve">benchmarking:
-- how long to simply count pixels?
-- how long to create 1 Point per pixel?
-- how long to GetPixel for each pixel?
-- how long to union set each pixel together?
-looks like UnionWith operations are the problem</t>
+    <t xml:space="preserve">prompt to save if image has changed since last save
+- on closing program
+- on opening new image
+Add this tracking to MasterImage class</t>
+  </si>
+  <si>
+    <t>8/23/2018</t>
+  </si>
+  <si>
+    <t>9/12/2018</t>
+  </si>
+  <si>
+    <t>remove old code for old find-regions logic</t>
   </si>
   <si>
     <t xml:space="preserve">benchmarking:
@@ -520,13 +227,258 @@
 - fixed it!</t>
   </si>
   <si>
-    <t>remove old code for old find-regions logic</t>
-  </si>
-  <si>
-    <t>use mouse scroll for zoom in/out</t>
-  </si>
-  <si>
-    <t>drag and drop image to move it</t>
+    <t>full documentation of support library GUI</t>
+  </si>
+  <si>
+    <t>full documentation of support library Colors</t>
+  </si>
+  <si>
+    <t>put in top of documentation that program is being actively developed, so open to bug reports and feature requests</t>
+  </si>
+  <si>
+    <t>put links to license on library pages</t>
+  </si>
+  <si>
+    <t>8/30/2018</t>
+  </si>
+  <si>
+    <t xml:space="preserve">libraries:
+if library relies on specific verion of another library, that needs to be documented</t>
+  </si>
+  <si>
+    <t>make the withouthaste,com/thanks page with link to Patron</t>
+  </si>
+  <si>
+    <t xml:space="preserve">applying color is pretty fast even on large image
+but removing the color is really slow</t>
+  </si>
+  <si>
+    <t xml:space="preserve">make a MasterImage class
+that one-time figures out all the regions in a background thread
+and provides that data to the color worker
+- A: finding 1 region at a time benchmarked at 10.7sec for tea shop cat - benchmarked at &gt;15min for rabbit
+- B: leading edge method still &gt;22min for rabbit and it was 10min for the cat (verified A still runs in 10sec on cat)</t>
+  </si>
+  <si>
+    <t>eyedrop tool: select color in palette, by selecting color on image (select palest color in colored region)</t>
+  </si>
+  <si>
+    <t>name all Settings properties in OneImageForm with prefix "Setting" for consistency</t>
+  </si>
+  <si>
+    <t>8/25/2018</t>
+  </si>
+  <si>
+    <t xml:space="preserve">to be consistent with System.Convert naming standards
+update ConvertColors
+- To&lt;Type&gt;(FromType)
+- &lt;FromType&gt;To&lt;Type&gt;(list of generic params)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bug: Palette &gt; New &gt; Done
+get error because no filename to open in main form</t>
+  </si>
+  <si>
+    <t>refactor Edit Palette Panel (and everything under it) to WithoutHaste.Windows.GUI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">when resizing windows, default behavior is to keep the same section of image in the viewing pane
+- so expanding window would in effect zoom in
+CANCELLED</t>
+  </si>
+  <si>
+    <t>refactor all panels to use proper events instead of delegate properties</t>
+  </si>
+  <si>
+    <t>refactor all history actions to use proper events instead of delegate properties</t>
+  </si>
+  <si>
+    <t xml:space="preserve">keyboard shortcuts:
+open (image)
+save (image or palette)
+undo (image or palette)
+redo (image or palette)</t>
+  </si>
+  <si>
+    <t>file &gt; Save</t>
+  </si>
+  <si>
+    <t>when zooming, if a scroll bar is all the way to min or max, keep it there</t>
+  </si>
+  <si>
+    <t>8/11/2018</t>
+  </si>
+  <si>
+    <t xml:space="preserve">design test that generates value scale for many different colors, easy to scan with the eye
+- for instance, sometimes the adjusted color gets darker than the lightest "black", leaving a paler ring around it</t>
+  </si>
+  <si>
+    <t xml:space="preserve">having problems with imprecise color format conversions
+it's really important they be perfectly reversible</t>
+  </si>
+  <si>
+    <t xml:space="preserve">refactor WithoutHaste.Drawing.Colors HSV to use ints instead of floats (0-360, 0-100, 0-100)
+CANCELLED
+more research online shows that float is proper for HSV</t>
+  </si>
+  <si>
+    <t>new color: enter an hsv value</t>
+  </si>
+  <si>
+    <t>new color: enter a hexadecimal value</t>
+  </si>
+  <si>
+    <t>new color: enter an rgb value</t>
+  </si>
+  <si>
+    <t>edit palette: display rgb/hexdecimal/hsv values of selected color</t>
+  </si>
+  <si>
+    <t xml:space="preserve">remember windows size from last closing
+- full screen vs not
+- default not-full-screen size
+open with this size</t>
+  </si>
+  <si>
+    <t>remember last open palette and reopen it next time program starts</t>
+  </si>
+  <si>
+    <t>use SwatchPanel object for main palette display</t>
+  </si>
+  <si>
+    <t>change names of dialog-only forms to XDialog</t>
+  </si>
+  <si>
+    <t>entirely new palette</t>
+  </si>
+  <si>
+    <t>edit palette: undo/redo all changes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">edit palette: save changes
+see updates in main form
+- save or lose changes on close</t>
+  </si>
+  <si>
+    <t>edit palette: add new color, but start from existing color</t>
+  </si>
+  <si>
+    <t>edit palette: edit color in place</t>
+  </si>
+  <si>
+    <t>edit palette: remove color</t>
+  </si>
+  <si>
+    <t xml:space="preserve">open edit palette mode
+- add swatches</t>
+  </si>
+  <si>
+    <t>bug: expanded palette covers part of picturebox and statuspanel</t>
+  </si>
+  <si>
+    <t>undo, redo coloring a section on the image</t>
+  </si>
+  <si>
+    <t xml:space="preserve">on error popup:
+display all nested errors</t>
+  </si>
+  <si>
+    <t xml:space="preserve">apply color over color without changing underlying values
+- change section back to grayscale
+- then to the new color</t>
+  </si>
+  <si>
+    <t>support applying color while zoomed in or out</t>
+  </si>
+  <si>
+    <t>add "100%" size button</t>
+  </si>
+  <si>
+    <t>8/16/2018</t>
+  </si>
+  <si>
+    <t xml:space="preserve">display closable modal "Please Wait" while coloring image
+- with "Cancel Color" option that will stop the thread and cancel the changes
+UPDATED: show status bar message</t>
+  </si>
+  <si>
+    <t xml:space="preserve">move coloring operations into another thread
+- queue incoming commands
+- handle one at a time in another thread, updating display between each one</t>
+  </si>
+  <si>
+    <t>bug: on some colors (oranges esp.) adjusting the saturation gives a too bright color - keep it in the gray range</t>
+  </si>
+  <si>
+    <t>what to rename ColorPalette library to so it does not conflict with object ColorPalette?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">save changes to image
+- bitmap
+- png
+- jpg</t>
+  </si>
+  <si>
+    <t>zoom in needs to keep pixels clear instead of letting it blur together</t>
+  </si>
+  <si>
+    <t>8/13/2018</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bug: it isn't actually keeping the grayscale
+- wow, spent days debugging and it was just a test-line outside the area I was looking at</t>
+  </si>
+  <si>
+    <t>fill in a section of color on the image</t>
+  </si>
+  <si>
+    <t>select a palette color</t>
+  </si>
+  <si>
+    <t xml:space="preserve">program preference setting: how wide the palette area is
+- let user drag and drop divider to change palette width
+- minimum is 3 swatches, max is maybe 12
+- save setting and reuse on next progam open
+(maybe instead of drag-n-drop the border, there are little &lt; &gt; arrow buttons that will expand/contract space one swatch at a time)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">display a default palette along the side of the window
+- give it a vertical scroll when needed</t>
+  </si>
+  <si>
+    <t xml:space="preserve">build 1 to 3 default palettes
+- downloaded some Photoshop palettes</t>
+  </si>
+  <si>
+    <t>scroll horizontal and vertical when zoomed in</t>
+  </si>
+  <si>
+    <t>8/10/2018</t>
+  </si>
+  <si>
+    <t>zoom in and out of image</t>
+  </si>
+  <si>
+    <t>resize image to fit window as it resizes</t>
+  </si>
+  <si>
+    <t>open an image and display it in a window at default size</t>
+  </si>
+  <si>
+    <t xml:space="preserve">new window's console app
+- version 0 until minimum viable is complete</t>
+  </si>
+  <si>
+    <t>Active</t>
+  </si>
+  <si>
+    <t>Max Id</t>
+  </si>
+  <si>
+    <t>Inactive</t>
+  </si>
+  <si>
+    <t>Bug</t>
   </si>
 </sst>
 </file>
@@ -579,7 +531,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:F38"/>
+  <dimension ref="A1:F36"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -605,10 +557,10 @@
     </row>
     <row r="2">
       <c r="A2" s="0">
-        <v>95</v>
+        <v>101</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="C2" s="0" t="s">
         <v>6</v>
@@ -617,15 +569,15 @@
         <v>7</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="0">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C3" s="0" t="s">
         <v>6</v>
@@ -634,15 +586,15 @@
         <v>7</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="0">
-        <v>101</v>
+        <v>76</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C4" s="0" t="s">
         <v>6</v>
@@ -651,15 +603,15 @@
         <v>7</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="0">
-        <v>51</v>
+        <v>35</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>132</v>
+        <v>13</v>
       </c>
       <c r="C5" s="0" t="s">
         <v>6</v>
@@ -668,15 +620,15 @@
         <v>7</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="0">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C6" s="0" t="s">
         <v>6</v>
@@ -685,15 +637,15 @@
         <v>7</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="0">
-        <v>35</v>
+        <v>27</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="C7" s="0" t="s">
         <v>6</v>
@@ -702,15 +654,15 @@
         <v>7</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="0">
-        <v>80</v>
+        <v>28</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>32</v>
+        <v>18</v>
       </c>
       <c r="C8" s="0" t="s">
         <v>6</v>
@@ -724,10 +676,10 @@
     </row>
     <row r="9">
       <c r="A9" s="0">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>36</v>
+        <v>19</v>
       </c>
       <c r="C9" s="0" t="s">
         <v>6</v>
@@ -736,15 +688,15 @@
         <v>7</v>
       </c>
       <c r="E9" s="0" t="s">
-        <v>37</v>
+        <v>17</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="0">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>38</v>
+        <v>20</v>
       </c>
       <c r="C10" s="0" t="s">
         <v>6</v>
@@ -753,15 +705,15 @@
         <v>7</v>
       </c>
       <c r="E10" s="0" t="s">
-        <v>37</v>
+        <v>17</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="0">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>39</v>
+        <v>21</v>
       </c>
       <c r="C11" s="0" t="s">
         <v>6</v>
@@ -770,16 +722,16 @@
         <v>7</v>
       </c>
       <c r="E11" s="0" t="s">
-        <v>37</v>
+        <v>17</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="0">
+        <v>17</v>
+      </c>
+      <c r="B12" s="0" t="s">
         <v>22</v>
       </c>
-      <c r="B12" s="0" t="s">
-        <v>40</v>
-      </c>
       <c r="C12" s="0" t="s">
         <v>6</v>
       </c>
@@ -787,15 +739,15 @@
         <v>7</v>
       </c>
       <c r="E12" s="0" t="s">
-        <v>37</v>
+        <v>17</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="0">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>41</v>
+        <v>23</v>
       </c>
       <c r="C13" s="0" t="s">
         <v>6</v>
@@ -804,15 +756,15 @@
         <v>7</v>
       </c>
       <c r="E13" s="0" t="s">
-        <v>37</v>
+        <v>17</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="0">
-        <v>17</v>
+        <v>99</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>42</v>
+        <v>24</v>
       </c>
       <c r="C14" s="0" t="s">
         <v>6</v>
@@ -821,15 +773,15 @@
         <v>7</v>
       </c>
       <c r="E14" s="0" t="s">
-        <v>37</v>
+        <v>8</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="0">
-        <v>18</v>
+        <v>115</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>43</v>
+        <v>25</v>
       </c>
       <c r="C15" s="0" t="s">
         <v>6</v>
@@ -838,15 +790,15 @@
         <v>7</v>
       </c>
       <c r="E15" s="0" t="s">
-        <v>37</v>
+        <v>26</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="0">
-        <v>99</v>
+        <v>116</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>44</v>
+        <v>27</v>
       </c>
       <c r="C16" s="0" t="s">
         <v>6</v>
@@ -855,15 +807,15 @@
         <v>7</v>
       </c>
       <c r="E16" s="0" t="s">
-        <v>10</v>
+        <v>26</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="0">
-        <v>115</v>
+        <v>81</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>136</v>
+        <v>28</v>
       </c>
       <c r="C17" s="0" t="s">
         <v>6</v>
@@ -872,15 +824,15 @@
         <v>7</v>
       </c>
       <c r="E17" s="0" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="0">
-        <v>116</v>
+        <v>109</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>137</v>
+        <v>29</v>
       </c>
       <c r="C18" s="0" t="s">
         <v>6</v>
@@ -889,15 +841,15 @@
         <v>7</v>
       </c>
       <c r="E18" s="0" t="s">
-        <v>8</v>
+        <v>30</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="0">
-        <v>81</v>
+        <v>110</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>45</v>
+        <v>31</v>
       </c>
       <c r="C19" s="0" t="s">
         <v>6</v>
@@ -906,15 +858,15 @@
         <v>7</v>
       </c>
       <c r="E19" s="0" t="s">
-        <v>17</v>
+        <v>30</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="0">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>46</v>
+        <v>32</v>
       </c>
       <c r="C20" s="0" t="s">
         <v>6</v>
@@ -923,15 +875,15 @@
         <v>7</v>
       </c>
       <c r="E20" s="0" t="s">
-        <v>47</v>
+        <v>33</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="0">
-        <v>110</v>
+        <v>82</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>48</v>
+        <v>34</v>
       </c>
       <c r="C21" s="0" t="s">
         <v>6</v>
@@ -940,15 +892,15 @@
         <v>7</v>
       </c>
       <c r="E21" s="0" t="s">
-        <v>47</v>
+        <v>12</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="0">
-        <v>108</v>
+        <v>83</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>49</v>
+        <v>35</v>
       </c>
       <c r="C22" s="0" t="s">
         <v>6</v>
@@ -957,15 +909,15 @@
         <v>7</v>
       </c>
       <c r="E22" s="0" t="s">
-        <v>50</v>
+        <v>12</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="0">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>51</v>
+        <v>36</v>
       </c>
       <c r="C23" s="0" t="s">
         <v>6</v>
@@ -974,15 +926,15 @@
         <v>7</v>
       </c>
       <c r="E23" s="0" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="0">
-        <v>83</v>
+        <v>112</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>52</v>
+        <v>37</v>
       </c>
       <c r="C24" s="0" t="s">
         <v>6</v>
@@ -991,15 +943,15 @@
         <v>7</v>
       </c>
       <c r="E24" s="0" t="s">
-        <v>17</v>
+        <v>30</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="0">
-        <v>84</v>
+        <v>25</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>53</v>
+        <v>38</v>
       </c>
       <c r="C25" s="0" t="s">
         <v>6</v>
@@ -1013,10 +965,10 @@
     </row>
     <row r="26">
       <c r="A26" s="0">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>54</v>
+        <v>39</v>
       </c>
       <c r="C26" s="0" t="s">
         <v>6</v>
@@ -1025,15 +977,15 @@
         <v>7</v>
       </c>
       <c r="E26" s="0" t="s">
-        <v>47</v>
+        <v>30</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="0">
-        <v>25</v>
+        <v>57</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>55</v>
+        <v>40</v>
       </c>
       <c r="C27" s="0" t="s">
         <v>6</v>
@@ -1042,15 +994,15 @@
         <v>7</v>
       </c>
       <c r="E27" s="0" t="s">
-        <v>37</v>
+        <v>12</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="0">
-        <v>111</v>
+        <v>65</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>56</v>
+        <v>41</v>
       </c>
       <c r="C28" s="0" t="s">
         <v>6</v>
@@ -1059,15 +1011,15 @@
         <v>7</v>
       </c>
       <c r="E28" s="0" t="s">
-        <v>47</v>
+        <v>12</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="0">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>57</v>
+        <v>42</v>
       </c>
       <c r="C29" s="0" t="s">
         <v>6</v>
@@ -1076,15 +1028,15 @@
         <v>7</v>
       </c>
       <c r="E29" s="0" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="0">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="B30" s="0" t="s">
-        <v>58</v>
+        <v>43</v>
       </c>
       <c r="C30" s="0" t="s">
         <v>6</v>
@@ -1093,15 +1045,15 @@
         <v>7</v>
       </c>
       <c r="E30" s="0" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="0">
-        <v>58</v>
+        <v>26</v>
       </c>
       <c r="B31" s="0" t="s">
-        <v>59</v>
+        <v>44</v>
       </c>
       <c r="C31" s="0" t="s">
         <v>6</v>
@@ -1115,10 +1067,10 @@
     </row>
     <row r="32">
       <c r="A32" s="0">
-        <v>61</v>
+        <v>43</v>
       </c>
       <c r="B32" s="0" t="s">
-        <v>60</v>
+        <v>45</v>
       </c>
       <c r="C32" s="0" t="s">
         <v>6</v>
@@ -1127,15 +1079,15 @@
         <v>7</v>
       </c>
       <c r="E32" s="0" t="s">
-        <v>17</v>
+        <v>46</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="0">
-        <v>26</v>
+        <v>74</v>
       </c>
       <c r="B33" s="0" t="s">
-        <v>61</v>
+        <v>47</v>
       </c>
       <c r="C33" s="0" t="s">
         <v>6</v>
@@ -1144,15 +1096,15 @@
         <v>7</v>
       </c>
       <c r="E33" s="0" t="s">
-        <v>37</v>
+        <v>12</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="0">
-        <v>43</v>
+        <v>29</v>
       </c>
       <c r="B34" s="0" t="s">
-        <v>62</v>
+        <v>48</v>
       </c>
       <c r="C34" s="0" t="s">
         <v>6</v>
@@ -1161,15 +1113,15 @@
         <v>7</v>
       </c>
       <c r="E34" s="0" t="s">
-        <v>63</v>
+        <v>17</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="0">
-        <v>74</v>
+        <v>47</v>
       </c>
       <c r="B35" s="0" t="s">
-        <v>64</v>
+        <v>49</v>
       </c>
       <c r="C35" s="0" t="s">
         <v>6</v>
@@ -1178,15 +1130,15 @@
         <v>7</v>
       </c>
       <c r="E35" s="0" t="s">
-        <v>17</v>
+        <v>50</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="0">
-        <v>29</v>
+        <v>60</v>
       </c>
       <c r="B36" s="0" t="s">
-        <v>65</v>
+        <v>51</v>
       </c>
       <c r="C36" s="0" t="s">
         <v>6</v>
@@ -1195,41 +1147,7 @@
         <v>7</v>
       </c>
       <c r="E36" s="0" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="37">
-      <c r="A37" s="0">
-        <v>47</v>
-      </c>
-      <c r="B37" s="0" t="s">
-        <v>66</v>
-      </c>
-      <c r="C37" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="D37" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="E37" s="0" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="38">
-      <c r="A38" s="0">
-        <v>60</v>
-      </c>
-      <c r="B38" s="0" t="s">
-        <v>68</v>
-      </c>
-      <c r="C38" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="D38" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="E38" s="0" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>
@@ -1239,7 +1157,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:F63"/>
+  <dimension ref="A1:F64"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1262,598 +1180,598 @@
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>69</v>
+        <v>52</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="0">
-        <v>114</v>
+        <v>53</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>135</v>
+        <v>53</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>69</v>
+        <v>52</v>
       </c>
       <c r="D2" s="0" t="s">
         <v>7</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>8</v>
+        <v>54</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>8</v>
+        <v>55</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="0">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>134</v>
+        <v>56</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>69</v>
+        <v>52</v>
       </c>
       <c r="D3" s="0" t="s">
         <v>7</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="F3" s="0" t="s">
-        <v>8</v>
+        <v>26</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="0">
-        <v>78</v>
+        <v>113</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>34</v>
+        <v>57</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>69</v>
+        <v>52</v>
       </c>
       <c r="D4" s="0" t="s">
         <v>7</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>17</v>
+        <v>26</v>
       </c>
       <c r="F4" s="0" t="s">
-        <v>8</v>
+        <v>26</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="0">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>33</v>
+        <v>58</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>69</v>
+        <v>52</v>
       </c>
       <c r="D5" s="0" t="s">
         <v>7</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="F5" s="0" t="s">
-        <v>8</v>
+        <v>26</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="0">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>31</v>
+        <v>59</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>69</v>
+        <v>52</v>
       </c>
       <c r="D6" s="0" t="s">
         <v>7</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="F6" s="0" t="s">
-        <v>8</v>
+        <v>26</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="0">
-        <v>106</v>
+        <v>85</v>
       </c>
       <c r="B7" s="0" t="s">
+        <v>60</v>
+      </c>
+      <c r="C7" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="D7" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E7" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="F7" s="0" t="s">
         <v>26</v>
-      </c>
-      <c r="C7" s="0" t="s">
-        <v>69</v>
-      </c>
-      <c r="D7" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="E7" s="0" t="s">
-        <v>23</v>
-      </c>
-      <c r="F7" s="0" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="0">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>24</v>
+        <v>61</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>69</v>
+        <v>52</v>
       </c>
       <c r="D8" s="0" t="s">
         <v>7</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>23</v>
+        <v>62</v>
       </c>
       <c r="F8" s="0" t="s">
-        <v>8</v>
+        <v>26</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="0">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>22</v>
+        <v>63</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>69</v>
+        <v>52</v>
       </c>
       <c r="D9" s="0" t="s">
         <v>7</v>
       </c>
       <c r="E9" s="0" t="s">
-        <v>23</v>
+        <v>62</v>
       </c>
       <c r="F9" s="0" t="s">
-        <v>8</v>
+        <v>26</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="0">
-        <v>49</v>
+        <v>107</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>18</v>
+        <v>64</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>69</v>
+        <v>52</v>
       </c>
       <c r="D10" s="0" t="s">
         <v>7</v>
       </c>
       <c r="E10" s="0" t="s">
-        <v>15</v>
+        <v>62</v>
       </c>
       <c r="F10" s="0" t="s">
-        <v>8</v>
+        <v>26</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="0">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>69</v>
+        <v>52</v>
       </c>
       <c r="D11" s="0" t="s">
         <v>7</v>
       </c>
       <c r="E11" s="0" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="F11" s="0" t="s">
-        <v>8</v>
+        <v>26</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="0">
-        <v>92</v>
+        <v>54</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>69</v>
+        <v>52</v>
       </c>
       <c r="D12" s="0" t="s">
         <v>7</v>
       </c>
       <c r="E12" s="0" t="s">
-        <v>10</v>
+        <v>54</v>
       </c>
       <c r="F12" s="0" t="s">
-        <v>10</v>
+        <v>26</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="0">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>69</v>
+        <v>52</v>
       </c>
       <c r="D13" s="0" t="s">
         <v>7</v>
       </c>
       <c r="E13" s="0" t="s">
-        <v>73</v>
+        <v>8</v>
       </c>
       <c r="F13" s="0" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="0">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="C14" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="D14" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E14" s="0" t="s">
         <v>69</v>
       </c>
-      <c r="D14" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="E14" s="0" t="s">
-        <v>73</v>
-      </c>
       <c r="F14" s="0" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="0">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="C15" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="D15" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E15" s="0" t="s">
         <v>69</v>
       </c>
-      <c r="D15" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="E15" s="0" t="s">
-        <v>17</v>
-      </c>
       <c r="F15" s="0" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="0">
-        <v>97</v>
+        <v>86</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>69</v>
+        <v>52</v>
       </c>
       <c r="D16" s="0" t="s">
         <v>7</v>
       </c>
       <c r="E16" s="0" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="F16" s="0" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="0">
-        <v>21</v>
+        <v>97</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>69</v>
+        <v>52</v>
       </c>
       <c r="D17" s="0" t="s">
         <v>7</v>
       </c>
       <c r="E17" s="0" t="s">
-        <v>37</v>
+        <v>8</v>
       </c>
       <c r="F17" s="0" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="0">
-        <v>100</v>
+        <v>21</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>69</v>
+        <v>52</v>
       </c>
       <c r="D18" s="0" t="s">
         <v>7</v>
       </c>
       <c r="E18" s="0" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="F18" s="0" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="0">
-        <v>87</v>
+        <v>100</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>69</v>
+        <v>52</v>
       </c>
       <c r="D19" s="0" t="s">
         <v>7</v>
       </c>
       <c r="E19" s="0" t="s">
-        <v>73</v>
+        <v>8</v>
       </c>
       <c r="F19" s="0" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="0">
-        <v>94</v>
+        <v>87</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="C20" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="D20" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E20" s="0" t="s">
         <v>69</v>
       </c>
-      <c r="D20" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="E20" s="0" t="s">
-        <v>10</v>
-      </c>
       <c r="F20" s="0" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="0">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="C21" s="0" t="s">
-        <v>69</v>
+        <v>52</v>
       </c>
       <c r="D21" s="0" t="s">
         <v>7</v>
       </c>
       <c r="E21" s="0" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="F21" s="0" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="0">
-        <v>34</v>
+        <v>93</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="C22" s="0" t="s">
-        <v>69</v>
+        <v>52</v>
       </c>
       <c r="D22" s="0" t="s">
         <v>7</v>
       </c>
       <c r="E22" s="0" t="s">
-        <v>83</v>
+        <v>8</v>
       </c>
       <c r="F22" s="0" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="0">
-        <v>50</v>
+        <v>34</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="C23" s="0" t="s">
-        <v>69</v>
+        <v>52</v>
       </c>
       <c r="D23" s="0" t="s">
         <v>7</v>
       </c>
       <c r="E23" s="0" t="s">
-        <v>15</v>
+        <v>79</v>
       </c>
       <c r="F23" s="0" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="0">
-        <v>89</v>
+        <v>50</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="C24" s="0" t="s">
-        <v>69</v>
+        <v>52</v>
       </c>
       <c r="D24" s="0" t="s">
         <v>7</v>
       </c>
       <c r="E24" s="0" t="s">
-        <v>73</v>
+        <v>10</v>
       </c>
       <c r="F24" s="0" t="s">
-        <v>73</v>
+        <v>8</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="0">
-        <v>59</v>
+        <v>89</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="C25" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="D25" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E25" s="0" t="s">
         <v>69</v>
       </c>
-      <c r="D25" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="E25" s="0" t="s">
-        <v>17</v>
-      </c>
       <c r="F25" s="0" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="0">
+        <v>59</v>
+      </c>
+      <c r="B26" s="0" t="s">
+        <v>82</v>
+      </c>
+      <c r="C26" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="D26" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E26" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="F26" s="0" t="s">
         <v>69</v>
-      </c>
-      <c r="B26" s="0" t="s">
-        <v>87</v>
-      </c>
-      <c r="C26" s="0" t="s">
-        <v>69</v>
-      </c>
-      <c r="D26" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="E26" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="F26" s="0" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="0">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="C27" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="D27" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E27" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="F27" s="0" t="s">
         <v>69</v>
-      </c>
-      <c r="D27" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="E27" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="F27" s="0" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="0">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="C28" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="D28" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E28" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="F28" s="0" t="s">
         <v>69</v>
-      </c>
-      <c r="D28" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="E28" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="F28" s="0" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="0">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="C29" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="D29" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E29" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="F29" s="0" t="s">
         <v>69</v>
-      </c>
-      <c r="D29" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="E29" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="F29" s="0" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="0">
-        <v>24</v>
+        <v>71</v>
       </c>
       <c r="B30" s="0" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="C30" s="0" t="s">
-        <v>69</v>
+        <v>52</v>
       </c>
       <c r="D30" s="0" t="s">
         <v>7</v>
       </c>
       <c r="E30" s="0" t="s">
-        <v>37</v>
+        <v>12</v>
       </c>
       <c r="F30" s="0" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="0">
-        <v>75</v>
+        <v>24</v>
       </c>
       <c r="B31" s="0" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="C31" s="0" t="s">
-        <v>69</v>
+        <v>52</v>
       </c>
       <c r="D31" s="0" t="s">
         <v>7</v>
@@ -1862,18 +1780,18 @@
         <v>17</v>
       </c>
       <c r="F31" s="0" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="0">
-        <v>55</v>
+        <v>75</v>
       </c>
       <c r="B32" s="0" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="C32" s="0" t="s">
-        <v>69</v>
+        <v>52</v>
       </c>
       <c r="D32" s="0" t="s">
         <v>7</v>
@@ -1882,184 +1800,184 @@
         <v>12</v>
       </c>
       <c r="F32" s="0" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="0">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B33" s="0" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="C33" s="0" t="s">
-        <v>69</v>
+        <v>52</v>
       </c>
       <c r="D33" s="0" t="s">
         <v>7</v>
       </c>
       <c r="E33" s="0" t="s">
-        <v>12</v>
+        <v>54</v>
       </c>
       <c r="F33" s="0" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="0">
-        <v>72</v>
+        <v>56</v>
       </c>
       <c r="B34" s="0" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="C34" s="0" t="s">
-        <v>69</v>
+        <v>52</v>
       </c>
       <c r="D34" s="0" t="s">
         <v>7</v>
       </c>
       <c r="E34" s="0" t="s">
-        <v>17</v>
+        <v>54</v>
       </c>
       <c r="F34" s="0" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="0">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="B35" s="0" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="C35" s="0" t="s">
-        <v>69</v>
+        <v>52</v>
       </c>
       <c r="D35" s="0" t="s">
         <v>7</v>
       </c>
       <c r="E35" s="0" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="F35" s="0" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="0">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="B36" s="0" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="C36" s="0" t="s">
-        <v>69</v>
+        <v>52</v>
       </c>
       <c r="D36" s="0" t="s">
         <v>7</v>
       </c>
       <c r="E36" s="0" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="F36" s="0" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="0">
-        <v>70</v>
+        <v>62</v>
       </c>
       <c r="B37" s="0" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="C37" s="0" t="s">
-        <v>69</v>
+        <v>52</v>
       </c>
       <c r="D37" s="0" t="s">
         <v>7</v>
       </c>
       <c r="E37" s="0" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="F37" s="0" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="0">
-        <v>64</v>
+        <v>70</v>
       </c>
       <c r="B38" s="0" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="C38" s="0" t="s">
-        <v>69</v>
+        <v>52</v>
       </c>
       <c r="D38" s="0" t="s">
         <v>7</v>
       </c>
       <c r="E38" s="0" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="F38" s="0" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="0">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B39" s="0" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="C39" s="0" t="s">
-        <v>69</v>
+        <v>52</v>
       </c>
       <c r="D39" s="0" t="s">
         <v>7</v>
       </c>
       <c r="E39" s="0" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="F39" s="0" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="0">
-        <v>13</v>
+        <v>63</v>
       </c>
       <c r="B40" s="0" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="C40" s="0" t="s">
-        <v>69</v>
+        <v>52</v>
       </c>
       <c r="D40" s="0" t="s">
         <v>7</v>
       </c>
       <c r="E40" s="0" t="s">
-        <v>37</v>
+        <v>12</v>
       </c>
       <c r="F40" s="0" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="0">
-        <v>42</v>
+        <v>13</v>
       </c>
       <c r="B41" s="0" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="C41" s="0" t="s">
-        <v>69</v>
+        <v>52</v>
       </c>
       <c r="D41" s="0" t="s">
         <v>7</v>
       </c>
       <c r="E41" s="0" t="s">
-        <v>63</v>
+        <v>17</v>
       </c>
       <c r="F41" s="0" t="s">
         <v>12</v>
@@ -2067,442 +1985,462 @@
     </row>
     <row r="42">
       <c r="A42" s="0">
-        <v>33</v>
+        <v>42</v>
       </c>
       <c r="B42" s="0" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="C42" s="0" t="s">
-        <v>69</v>
+        <v>52</v>
       </c>
       <c r="D42" s="0" t="s">
         <v>7</v>
       </c>
       <c r="E42" s="0" t="s">
-        <v>83</v>
+        <v>46</v>
       </c>
       <c r="F42" s="0" t="s">
-        <v>12</v>
+        <v>54</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" s="0">
-        <v>48</v>
+        <v>33</v>
       </c>
       <c r="B43" s="0" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="C43" s="0" t="s">
-        <v>69</v>
+        <v>52</v>
       </c>
       <c r="D43" s="0" t="s">
         <v>7</v>
       </c>
       <c r="E43" s="0" t="s">
-        <v>15</v>
+        <v>79</v>
       </c>
       <c r="F43" s="0" t="s">
-        <v>15</v>
+        <v>54</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" s="0">
-        <v>37</v>
+        <v>48</v>
       </c>
       <c r="B44" s="0" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="C44" s="0" t="s">
-        <v>69</v>
+        <v>52</v>
       </c>
       <c r="D44" s="0" t="s">
         <v>7</v>
       </c>
       <c r="E44" s="0" t="s">
-        <v>21</v>
+        <v>10</v>
       </c>
       <c r="F44" s="0" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" s="0">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B45" s="0" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="C45" s="0" t="s">
-        <v>69</v>
+        <v>52</v>
       </c>
       <c r="D45" s="0" t="s">
         <v>7</v>
       </c>
       <c r="E45" s="0" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="F45" s="0" t="s">
-        <v>67</v>
+        <v>10</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" s="0">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="B46" s="0" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="C46" s="0" t="s">
-        <v>69</v>
+        <v>52</v>
       </c>
       <c r="D46" s="0" t="s">
         <v>7</v>
       </c>
       <c r="E46" s="0" t="s">
-        <v>108</v>
+        <v>14</v>
       </c>
       <c r="F46" s="0" t="s">
-        <v>67</v>
+        <v>50</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" s="0">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B47" s="0" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="C47" s="0" t="s">
-        <v>69</v>
+        <v>52</v>
       </c>
       <c r="D47" s="0" t="s">
         <v>7</v>
       </c>
       <c r="E47" s="0" t="s">
-        <v>63</v>
+        <v>104</v>
       </c>
       <c r="F47" s="0" t="s">
-        <v>67</v>
+        <v>50</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" s="0">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B48" s="0" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="C48" s="0" t="s">
-        <v>69</v>
+        <v>52</v>
       </c>
       <c r="D48" s="0" t="s">
         <v>7</v>
       </c>
       <c r="E48" s="0" t="s">
-        <v>63</v>
+        <v>46</v>
       </c>
       <c r="F48" s="0" t="s">
-        <v>67</v>
+        <v>50</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" s="0">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="B49" s="0" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="C49" s="0" t="s">
-        <v>69</v>
+        <v>52</v>
       </c>
       <c r="D49" s="0" t="s">
         <v>7</v>
       </c>
       <c r="E49" s="0" t="s">
-        <v>63</v>
+        <v>46</v>
       </c>
       <c r="F49" s="0" t="s">
-        <v>108</v>
+        <v>50</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" s="0">
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="B50" s="0" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="C50" s="0" t="s">
-        <v>69</v>
+        <v>52</v>
       </c>
       <c r="D50" s="0" t="s">
         <v>7</v>
       </c>
       <c r="E50" s="0" t="s">
-        <v>21</v>
+        <v>46</v>
       </c>
       <c r="F50" s="0" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" s="0">
-        <v>11</v>
+        <v>36</v>
       </c>
       <c r="B51" s="0" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="C51" s="0" t="s">
-        <v>69</v>
+        <v>52</v>
       </c>
       <c r="D51" s="0" t="s">
         <v>7</v>
       </c>
       <c r="E51" s="0" t="s">
-        <v>37</v>
+        <v>14</v>
       </c>
       <c r="F51" s="0" t="s">
-        <v>63</v>
+        <v>104</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" s="0">
-        <v>40</v>
+        <v>11</v>
       </c>
       <c r="B52" s="0" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="C52" s="0" t="s">
-        <v>69</v>
+        <v>52</v>
       </c>
       <c r="D52" s="0" t="s">
         <v>7</v>
       </c>
       <c r="E52" s="0" t="s">
-        <v>115</v>
+        <v>17</v>
       </c>
       <c r="F52" s="0" t="s">
-        <v>63</v>
+        <v>46</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" s="0">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B53" s="0" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="C53" s="0" t="s">
-        <v>69</v>
+        <v>52</v>
       </c>
       <c r="D53" s="0" t="s">
         <v>7</v>
       </c>
       <c r="E53" s="0" t="s">
-        <v>21</v>
+        <v>111</v>
       </c>
       <c r="F53" s="0" t="s">
-        <v>63</v>
+        <v>46</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" s="0">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="B54" s="0" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="C54" s="0" t="s">
-        <v>69</v>
+        <v>52</v>
       </c>
       <c r="D54" s="0" t="s">
         <v>7</v>
       </c>
       <c r="E54" s="0" t="s">
-        <v>83</v>
+        <v>14</v>
       </c>
       <c r="F54" s="0" t="s">
-        <v>21</v>
+        <v>46</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" s="0">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B55" s="0" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="C55" s="0" t="s">
-        <v>69</v>
+        <v>52</v>
       </c>
       <c r="D55" s="0" t="s">
         <v>7</v>
       </c>
       <c r="E55" s="0" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="F55" s="0" t="s">
-        <v>83</v>
+        <v>14</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" s="0">
-        <v>20</v>
+        <v>31</v>
       </c>
       <c r="B56" s="0" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="C56" s="0" t="s">
-        <v>69</v>
+        <v>52</v>
       </c>
       <c r="D56" s="0" t="s">
         <v>7</v>
       </c>
       <c r="E56" s="0" t="s">
-        <v>37</v>
+        <v>79</v>
       </c>
       <c r="F56" s="0" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" s="0">
-        <v>9</v>
+        <v>20</v>
       </c>
       <c r="B57" s="0" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="C57" s="0" t="s">
-        <v>69</v>
+        <v>52</v>
       </c>
       <c r="D57" s="0" t="s">
         <v>7</v>
       </c>
       <c r="E57" s="0" t="s">
-        <v>37</v>
+        <v>17</v>
       </c>
       <c r="F57" s="0" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" s="0">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B58" s="0" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="C58" s="0" t="s">
-        <v>69</v>
+        <v>52</v>
       </c>
       <c r="D58" s="0" t="s">
         <v>7</v>
       </c>
       <c r="E58" s="0" t="s">
-        <v>37</v>
+        <v>17</v>
       </c>
       <c r="F58" s="0" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" s="0">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="B59" s="0" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="C59" s="0" t="s">
-        <v>69</v>
+        <v>52</v>
       </c>
       <c r="D59" s="0" t="s">
         <v>7</v>
       </c>
       <c r="E59" s="0" t="s">
-        <v>37</v>
+        <v>17</v>
       </c>
       <c r="F59" s="0" t="s">
-        <v>123</v>
+        <v>79</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" s="0">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B60" s="0" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
       <c r="C60" s="0" t="s">
-        <v>69</v>
+        <v>52</v>
       </c>
       <c r="D60" s="0" t="s">
         <v>7</v>
       </c>
       <c r="E60" s="0" t="s">
-        <v>37</v>
+        <v>17</v>
       </c>
       <c r="F60" s="0" t="s">
-        <v>37</v>
+        <v>119</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" s="0">
-        <v>30</v>
+        <v>3</v>
       </c>
       <c r="B61" s="0" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="C61" s="0" t="s">
-        <v>69</v>
+        <v>52</v>
       </c>
       <c r="D61" s="0" t="s">
         <v>7</v>
       </c>
       <c r="E61" s="0" t="s">
-        <v>37</v>
+        <v>17</v>
       </c>
       <c r="F61" s="0" t="s">
-        <v>37</v>
+        <v>17</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" s="0">
-        <v>2</v>
+        <v>30</v>
       </c>
       <c r="B62" s="0" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="C62" s="0" t="s">
-        <v>69</v>
+        <v>52</v>
       </c>
       <c r="D62" s="0" t="s">
         <v>7</v>
       </c>
       <c r="E62" s="0" t="s">
-        <v>37</v>
+        <v>17</v>
       </c>
       <c r="F62" s="0" t="s">
-        <v>37</v>
+        <v>17</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" s="0">
+        <v>2</v>
+      </c>
+      <c r="B63" s="0" t="s">
+        <v>122</v>
+      </c>
+      <c r="C63" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="D63" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E63" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="F63" s="0" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" s="0">
         <v>1</v>
       </c>
-      <c r="B63" s="0" t="s">
-        <v>127</v>
-      </c>
-      <c r="C63" s="0" t="s">
-        <v>69</v>
-      </c>
-      <c r="D63" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="E63" s="0" t="s">
-        <v>37</v>
-      </c>
-      <c r="F63" s="0" t="s">
-        <v>37</v>
+      <c r="B64" s="0" t="s">
+        <v>123</v>
+      </c>
+      <c r="C64" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="D64" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E64" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="F64" s="0" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>
@@ -2523,7 +2461,7 @@
         <v>2</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="C1" s="2"/>
       <c r="D1" s="2" t="s">
@@ -2531,7 +2469,7 @@
       </c>
       <c r="E1" s="2"/>
       <c r="F1" s="2" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
     </row>
     <row r="2">
@@ -2539,7 +2477,7 @@
         <v>6</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="D2" s="0" t="s">
         <v>7</v>
@@ -2550,13 +2488,13 @@
     </row>
     <row r="3">
       <c r="A3" s="0" t="s">
-        <v>69</v>
+        <v>52</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
     </row>
   </sheetData>

</xml_diff>